<commit_message>
Hardware and software version index added
</commit_message>
<xml_diff>
--- a/hardware/BikeCounterPro/src/dataPackage/DataPackage.xlsx
+++ b/hardware/BikeCounterPro/src/dataPackage/DataPackage.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meier\Documents\Repos\lora\hardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meier\Documents\repos\lora\hardware\BikeCounterPro\src\dataPackage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797A9CEF-76B0-4804-BB36-33C2CC6CBE6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8209FCCC-4B59-4353-B97A-78EA8ADF4FC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="41172" yWindow="-108" windowWidth="41496" windowHeight="16896" xr2:uid="{CDF7A0A5-12B1-43F1-AFDE-54CA91221B4B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="96">
   <si>
     <t>minutes of day</t>
   </si>
@@ -302,6 +302,30 @@
   </si>
   <si>
     <t>Battery Voltage [V]</t>
+  </si>
+  <si>
+    <t>Software Version</t>
+  </si>
+  <si>
+    <t>Hardware Version</t>
+  </si>
+  <si>
+    <t>board v0.1</t>
+  </si>
+  <si>
+    <t>INR18650-29E</t>
+  </si>
+  <si>
+    <t>Samsung blue</t>
+  </si>
+  <si>
+    <t>Samsung pink</t>
+  </si>
+  <si>
+    <t>ICR18650-26J</t>
+  </si>
+  <si>
+    <t>Commit:</t>
   </si>
 </sst>
 </file>
@@ -554,13 +578,8 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -569,13 +588,16 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -605,6 +627,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -614,12 +639,11 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Gut" xfId="1" builtinId="26"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -648,7 +672,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1766,7 +1790,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2062,19 +2086,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{088FF0E6-8FE4-49E3-812F-B76B934E1ACD}">
-  <dimension ref="A1:H73"/>
+  <dimension ref="A1:S83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -2082,7 +2107,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -2091,12 +2116,12 @@
         <v>408</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -2104,7 +2129,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -2112,7 +2137,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -2121,604 +2146,771 @@
         <v>400</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>88</v>
       </c>
       <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11">
         <v>3</v>
       </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H11">
+        <v>4</v>
+      </c>
+      <c r="I11">
+        <v>5</v>
+      </c>
+      <c r="J11">
+        <v>6</v>
+      </c>
+      <c r="K11">
+        <v>7</v>
+      </c>
+      <c r="L11">
+        <v>8</v>
+      </c>
+      <c r="M11">
+        <v>9</v>
+      </c>
+      <c r="N11">
+        <v>10</v>
+      </c>
+      <c r="O11">
+        <v>11</v>
+      </c>
+      <c r="P11">
+        <v>12</v>
+      </c>
+      <c r="Q11">
+        <v>13</v>
+      </c>
+      <c r="R11">
+        <v>14</v>
+      </c>
+      <c r="S11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>32</v>
       </c>
       <c r="B12">
         <f>2^B11</f>
-        <v>8</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="4">
-        <f>B8-B11</f>
+        <f>B23-B11</f>
+        <v>393</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="G16">
+        <v>3</v>
+      </c>
+      <c r="H16">
+        <v>4</v>
+      </c>
+      <c r="I16">
+        <v>5</v>
+      </c>
+      <c r="J16">
+        <v>6</v>
+      </c>
+      <c r="K16">
+        <v>7</v>
+      </c>
+      <c r="L16">
+        <v>8</v>
+      </c>
+      <c r="M16">
+        <v>9</v>
+      </c>
+      <c r="N16">
+        <v>10</v>
+      </c>
+      <c r="O16">
+        <v>11</v>
+      </c>
+      <c r="P16">
+        <v>12</v>
+      </c>
+      <c r="Q16">
+        <v>13</v>
+      </c>
+      <c r="R16">
+        <v>14</v>
+      </c>
+      <c r="S16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17">
+        <f>2^B16</f>
+        <v>16</v>
+      </c>
+      <c r="D17" t="s">
+        <v>90</v>
+      </c>
+      <c r="E17" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="4">
+        <f>B13-B16</f>
+        <v>389</v>
+      </c>
+      <c r="D18" t="s">
+        <v>92</v>
+      </c>
+      <c r="E18" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E19" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>2</v>
+      </c>
+      <c r="G21">
+        <v>3</v>
+      </c>
+      <c r="H21">
+        <v>4</v>
+      </c>
+      <c r="I21">
+        <v>5</v>
+      </c>
+      <c r="J21">
+        <v>6</v>
+      </c>
+      <c r="K21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22">
+        <f>2^B21</f>
+        <v>8</v>
+      </c>
+      <c r="D22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="4">
+        <f>B8-B21</f>
         <v>397</v>
       </c>
-      <c r="D13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D14">
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>83</v>
+      </c>
+      <c r="B28">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D15">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>82</v>
-      </c>
-      <c r="D16">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>84</v>
+      </c>
+      <c r="B29">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30">
+        <f>B29-B28</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" s="20">
+        <f>B30/(2^B27-1)</f>
+        <v>4.8387096774193547E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" s="4">
+        <f>B18-B27</f>
+        <v>384</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>33</v>
+      </c>
+      <c r="B37">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>34</v>
+      </c>
+      <c r="B38">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B39">
+        <f>B38-B37</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>36</v>
+      </c>
+      <c r="B40" s="2">
+        <f>B39/(2^B36-1)</f>
+        <v>2.2580645161290325</v>
+      </c>
+      <c r="D40" s="2"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41" s="4">
+        <f>B32-B36</f>
+        <v>379</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
         <v>11</v>
       </c>
-      <c r="B17">
-        <v>5</v>
-      </c>
-      <c r="D17">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>83</v>
-      </c>
-      <c r="B18">
+      <c r="B45">
         <v>3</v>
       </c>
-      <c r="D18">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>84</v>
-      </c>
-      <c r="B19">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>85</v>
-      </c>
-      <c r="B20">
-        <f>B19-B18</f>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="40">
-        <f>B20/(2^B17-1)</f>
-        <v>4.8387096774193547E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="B46" s="2">
+        <f>100/(2^B45-1)</f>
+        <v>14.285714285714286</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="4">
-        <f>B13-B17</f>
-        <v>392</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>11</v>
-      </c>
-      <c r="B26">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27">
-        <v>-20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>34</v>
-      </c>
-      <c r="B28">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>35</v>
-      </c>
-      <c r="B29">
-        <f>B28-B27</f>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>36</v>
-      </c>
-      <c r="B30" s="2">
-        <f>B29/(2^B26-1)</f>
-        <v>2.2580645161290325</v>
-      </c>
-      <c r="D30" s="2"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>18</v>
-      </c>
-      <c r="B31" s="4">
-        <f>B22-B26</f>
-        <v>387</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>11</v>
-      </c>
-      <c r="B35">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>12</v>
-      </c>
-      <c r="B36" s="2">
-        <f>100/(2^B35-1)</f>
-        <v>14.285714285714286</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>18</v>
-      </c>
-      <c r="B37" s="4">
-        <f>B31-B35</f>
-        <v>384</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>11</v>
-      </c>
-      <c r="B41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>18</v>
-      </c>
-      <c r="B42" s="4">
-        <f>B37-B41</f>
-        <v>384</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B46" s="20"/>
-      <c r="C46" s="20"/>
-      <c r="D46" s="20"/>
-      <c r="E46" s="20"/>
-      <c r="F46" s="20"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B48" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>1</v>
-      </c>
-      <c r="B49">
-        <v>1440</v>
-      </c>
-      <c r="C49" t="s">
-        <v>3</v>
-      </c>
-      <c r="D49" s="3">
-        <f>B42/B50</f>
-        <v>34.909090909090907</v>
+      <c r="B47" s="4">
+        <f>B41-B45</f>
+        <v>376</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>11</v>
+      </c>
+      <c r="B51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>18</v>
+      </c>
+      <c r="B52" s="4">
+        <f>B47-B51</f>
+        <v>376</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B56" s="21"/>
+      <c r="C56" s="21"/>
+      <c r="D56" s="21"/>
+      <c r="E56" s="21"/>
+      <c r="F56" s="21"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B58" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>1</v>
+      </c>
+      <c r="B59">
+        <v>1440</v>
+      </c>
+      <c r="C59" t="s">
+        <v>3</v>
+      </c>
+      <c r="D59" s="3">
+        <f>B52/B60</f>
+        <v>34.18181818181818</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
         <v>2</v>
       </c>
-      <c r="B50">
+      <c r="B60">
         <v>11</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C60" t="s">
         <v>19</v>
       </c>
-      <c r="D50" s="14">
-        <f>ROUNDDOWN(D49,0)</f>
+      <c r="D60" s="14">
+        <f>ROUNDDOWN(D59,0)</f>
         <v>34</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B51">
-        <f>2^B50</f>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B61">
+        <f>2^B60</f>
         <v>2048</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C61" t="s">
         <v>18</v>
       </c>
-      <c r="D51">
-        <f>B42-D50*B50</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="20" t="s">
+      <c r="D61">
+        <f>B52-D60*B60</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B54" s="20"/>
-      <c r="C54" s="20"/>
-      <c r="D54" s="20"/>
-      <c r="E54" s="20"/>
-      <c r="F54" s="20"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="B56" s="13"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B57" s="13">
-        <v>3</v>
-      </c>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
-      <c r="F57" s="1"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B58" s="17">
-        <f>B42-B57</f>
-        <v>381</v>
-      </c>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
-      <c r="F59" s="1"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
-      <c r="F60" s="1"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B61" s="1">
-        <v>5</v>
-      </c>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
-      <c r="E61" s="1"/>
-      <c r="F61" s="1"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B62" s="1">
-        <f>2^B61</f>
-        <v>32</v>
-      </c>
-      <c r="C62" s="1"/>
-      <c r="D62" s="1"/>
-      <c r="E62" s="1"/>
-      <c r="F62" s="1"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" s="1"/>
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
-      <c r="E63" s="1"/>
-      <c r="F63" s="1"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B64" s="6">
-        <f>B58-B61</f>
-        <v>376</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D64" s="1">
-        <f>B64/8</f>
-        <v>47</v>
-      </c>
-      <c r="E64" s="1"/>
-      <c r="F64" s="1"/>
+      <c r="B64" s="21"/>
+      <c r="C64" s="21"/>
+      <c r="D64" s="21"/>
+      <c r="E64" s="21"/>
+      <c r="F64" s="21"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
       <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
       <c r="F65" s="1"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A66" s="1" t="s">
+      <c r="A66" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B66" s="13"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A67" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B67" s="13">
+        <v>3</v>
+      </c>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A68" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B68" s="17">
+        <f>B52-B67</f>
+        <v>373</v>
+      </c>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B71" s="1">
+        <v>5</v>
+      </c>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B72" s="1">
+        <f>2^B71</f>
+        <v>32</v>
+      </c>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B74" s="6">
+        <f>B68-B71</f>
+        <v>368</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D74" s="1">
+        <f>B74/8</f>
+        <v>46</v>
+      </c>
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
+      <c r="D75" s="1"/>
+      <c r="F75" s="1"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B76" t="s">
         <v>9</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C76" t="s">
         <v>7</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D76" t="s">
         <v>5</v>
       </c>
-      <c r="E66" t="s">
+      <c r="E76" t="s">
         <v>6</v>
       </c>
-      <c r="F66" t="s">
+      <c r="F76" t="s">
         <v>3</v>
       </c>
-      <c r="G66" t="s">
+      <c r="G76" t="s">
         <v>19</v>
       </c>
-      <c r="H66" t="s">
+      <c r="H76" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A67">
-        <v>0</v>
-      </c>
-      <c r="B67">
-        <v>1</v>
-      </c>
-      <c r="C67">
-        <f>B67*60</f>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>0</v>
+      </c>
+      <c r="B77">
+        <v>1</v>
+      </c>
+      <c r="C77">
+        <f>B77*60</f>
         <v>60</v>
       </c>
-      <c r="D67">
+      <c r="D77">
         <v>6</v>
       </c>
-      <c r="E67">
-        <f>2^D67</f>
+      <c r="E77">
+        <f>2^D77</f>
         <v>64</v>
       </c>
-      <c r="F67" s="3">
-        <f>$B$64/D67</f>
-        <v>62.666666666666664</v>
-      </c>
-      <c r="G67" s="5">
-        <f>ROUNDDOWN(F67,0)</f>
-        <v>62</v>
-      </c>
-      <c r="H67">
-        <f t="shared" ref="H67:H69" si="0">$B$64-G67*D67</f>
+      <c r="F77" s="3">
+        <f>$B$74/D77</f>
+        <v>61.333333333333336</v>
+      </c>
+      <c r="G77" s="5">
+        <f>ROUNDDOWN(F77,0)</f>
+        <v>61</v>
+      </c>
+      <c r="H77">
+        <f t="shared" ref="H77:H79" si="0">$B$74-G77*D77</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>1</v>
+      </c>
+      <c r="B78">
+        <v>2</v>
+      </c>
+      <c r="C78">
+        <f t="shared" ref="C78:C81" si="1">B78*60</f>
+        <v>120</v>
+      </c>
+      <c r="D78">
+        <v>7</v>
+      </c>
+      <c r="E78">
+        <f t="shared" ref="E78:E81" si="2">2^D78</f>
+        <v>128</v>
+      </c>
+      <c r="F78" s="3">
+        <f>$B$74/D78</f>
+        <v>52.571428571428569</v>
+      </c>
+      <c r="G78" s="5">
+        <f t="shared" ref="G78:G81" si="3">ROUNDDOWN(F78,0)</f>
+        <v>52</v>
+      </c>
+      <c r="H78">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A68">
-        <v>1</v>
-      </c>
-      <c r="B68">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A79">
         <v>2</v>
       </c>
-      <c r="C68">
-        <f t="shared" ref="C68:C71" si="1">B68*60</f>
-        <v>120</v>
-      </c>
-      <c r="D68">
-        <v>7</v>
-      </c>
-      <c r="E68">
-        <f t="shared" ref="E68:E71" si="2">2^D68</f>
-        <v>128</v>
-      </c>
-      <c r="F68" s="3">
-        <f>$B$64/D68</f>
-        <v>53.714285714285715</v>
-      </c>
-      <c r="G68" s="5">
-        <f t="shared" ref="G68:G71" si="3">ROUNDDOWN(F68,0)</f>
-        <v>53</v>
-      </c>
-      <c r="H68">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A69">
-        <v>2</v>
-      </c>
-      <c r="B69">
+      <c r="B79">
         <v>4</v>
       </c>
-      <c r="C69">
+      <c r="C79">
         <f t="shared" si="1"/>
         <v>240</v>
       </c>
-      <c r="D69">
+      <c r="D79">
         <v>8</v>
       </c>
-      <c r="E69">
+      <c r="E79">
         <f t="shared" si="2"/>
         <v>256</v>
       </c>
-      <c r="F69" s="3">
-        <f>$B$64/D69</f>
-        <v>47</v>
-      </c>
-      <c r="G69" s="5">
+      <c r="F79" s="3">
+        <f>$B$74/D79</f>
+        <v>46</v>
+      </c>
+      <c r="G79" s="5">
         <f t="shared" si="3"/>
-        <v>47</v>
-      </c>
-      <c r="H69">
+        <v>46</v>
+      </c>
+      <c r="H79">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A70">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A80">
         <v>3</v>
       </c>
-      <c r="B70">
+      <c r="B80">
         <v>8</v>
       </c>
-      <c r="C70">
+      <c r="C80">
         <f t="shared" si="1"/>
         <v>480</v>
       </c>
-      <c r="D70">
+      <c r="D80">
         <v>9</v>
       </c>
-      <c r="E70">
+      <c r="E80">
         <f t="shared" si="2"/>
         <v>512</v>
       </c>
-      <c r="F70" s="3">
-        <f>$B$64/D70</f>
-        <v>41.777777777777779</v>
-      </c>
-      <c r="G70" s="5">
+      <c r="F80" s="3">
+        <f>$B$74/D80</f>
+        <v>40.888888888888886</v>
+      </c>
+      <c r="G80" s="5">
         <f t="shared" si="3"/>
-        <v>41</v>
-      </c>
-      <c r="H70">
-        <f>$B$64-G70*D70</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A71">
+        <v>40</v>
+      </c>
+      <c r="H80">
+        <f>$B$74-G80*D80</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A81">
         <v>4</v>
       </c>
-      <c r="B71">
+      <c r="B81">
         <v>17</v>
       </c>
-      <c r="C71">
+      <c r="C81">
         <f t="shared" si="1"/>
         <v>1020</v>
       </c>
-      <c r="D71">
+      <c r="D81">
         <v>10</v>
       </c>
-      <c r="E71">
+      <c r="E81">
         <f t="shared" si="2"/>
         <v>1024</v>
       </c>
-      <c r="F71" s="3">
-        <f>$B$64/D71</f>
-        <v>37.6</v>
-      </c>
-      <c r="G71" s="5">
+      <c r="F81" s="3">
+        <f>$B$74/D81</f>
+        <v>36.799999999999997</v>
+      </c>
+      <c r="G81" s="5">
         <f t="shared" si="3"/>
-        <v>37</v>
-      </c>
-      <c r="H71">
-        <f>$B$64-G71*D71</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E72" s="3"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E73" s="3"/>
+        <v>36</v>
+      </c>
+      <c r="H81">
+        <f>$B$74-G81*D81</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E82" s="3"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E83" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A46:F46"/>
-    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="A56:F56"/>
+    <mergeCell ref="A64:F64"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2733,7 +2925,7 @@
       <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="32" width="4.21875" customWidth="1"/>
     <col min="33" max="150" width="3.109375" customWidth="1"/>
@@ -2949,82 +3141,82 @@
       <c r="S4" s="11"/>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
-      <c r="N5" s="26"/>
-      <c r="O5" s="26"/>
-      <c r="P5" s="26"/>
-      <c r="Q5" s="26"/>
-      <c r="R5" s="26"/>
-      <c r="S5" s="26"/>
-      <c r="T5" s="26"/>
-      <c r="U5" s="26"/>
-      <c r="V5" s="26"/>
-      <c r="W5" s="26"/>
-      <c r="X5" s="26"/>
-      <c r="Y5" s="26"/>
-      <c r="Z5" s="26"/>
-      <c r="AA5" s="26"/>
-      <c r="AB5" s="26"/>
-      <c r="AC5" s="26"/>
-      <c r="AD5" s="26"/>
-      <c r="AE5" s="26"/>
-      <c r="AF5" s="26"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="27"/>
+      <c r="N5" s="27"/>
+      <c r="O5" s="27"/>
+      <c r="P5" s="27"/>
+      <c r="Q5" s="27"/>
+      <c r="R5" s="27"/>
+      <c r="S5" s="27"/>
+      <c r="T5" s="27"/>
+      <c r="U5" s="27"/>
+      <c r="V5" s="27"/>
+      <c r="W5" s="27"/>
+      <c r="X5" s="27"/>
+      <c r="Y5" s="27"/>
+      <c r="Z5" s="27"/>
+      <c r="AA5" s="27"/>
+      <c r="AB5" s="27"/>
+      <c r="AC5" s="27"/>
+      <c r="AD5" s="27"/>
+      <c r="AE5" s="27"/>
+      <c r="AF5" s="27"/>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="27">
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26">
         <v>38</v>
       </c>
-      <c r="J6" s="27"/>
-      <c r="K6" s="27"/>
-      <c r="L6" s="27"/>
-      <c r="M6" s="27"/>
-      <c r="N6" s="27"/>
-      <c r="O6" s="27"/>
-      <c r="P6" s="27"/>
-      <c r="Q6" s="27">
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="26"/>
+      <c r="Q6" s="26">
         <v>73</v>
       </c>
-      <c r="R6" s="27"/>
-      <c r="S6" s="27"/>
-      <c r="T6" s="27"/>
-      <c r="U6" s="27"/>
-      <c r="V6" s="27"/>
-      <c r="W6" s="27"/>
-      <c r="X6" s="27"/>
-      <c r="Y6" s="27">
+      <c r="R6" s="26"/>
+      <c r="S6" s="26"/>
+      <c r="T6" s="26"/>
+      <c r="U6" s="26"/>
+      <c r="V6" s="26"/>
+      <c r="W6" s="26"/>
+      <c r="X6" s="26"/>
+      <c r="Y6" s="26">
         <v>88</v>
       </c>
-      <c r="Z6" s="27"/>
-      <c r="AA6" s="27"/>
-      <c r="AB6" s="27"/>
-      <c r="AC6" s="27"/>
-      <c r="AD6" s="27"/>
-      <c r="AE6" s="27"/>
-      <c r="AF6" s="27"/>
+      <c r="Z6" s="26"/>
+      <c r="AA6" s="26"/>
+      <c r="AB6" s="26"/>
+      <c r="AC6" s="26"/>
+      <c r="AD6" s="26"/>
+      <c r="AE6" s="26"/>
+      <c r="AF6" s="26"/>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A7" s="16">
@@ -3125,175 +3317,175 @@
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23" t="s">
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23" t="s">
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="O8" s="23"/>
-      <c r="P8" s="23"/>
-      <c r="Q8" s="23" t="s">
+      <c r="O8" s="22"/>
+      <c r="P8" s="22"/>
+      <c r="Q8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="R8" s="23"/>
-      <c r="S8" s="23"/>
-      <c r="T8" s="23" t="s">
+      <c r="R8" s="22"/>
+      <c r="S8" s="22"/>
+      <c r="T8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="U8" s="23"/>
-      <c r="V8" s="23"/>
-      <c r="W8" s="23"/>
-      <c r="X8" s="23"/>
-      <c r="Y8" s="23" t="s">
+      <c r="U8" s="22"/>
+      <c r="V8" s="22"/>
+      <c r="W8" s="22"/>
+      <c r="X8" s="22"/>
+      <c r="Y8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="Z8" s="23"/>
-      <c r="AA8" s="23"/>
-      <c r="AB8" s="23"/>
-      <c r="AC8" s="23"/>
-      <c r="AD8" s="23" t="s">
+      <c r="Z8" s="22"/>
+      <c r="AA8" s="22"/>
+      <c r="AB8" s="22"/>
+      <c r="AC8" s="22"/>
+      <c r="AD8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="AE8" s="23"/>
-      <c r="AF8" s="23"/>
+      <c r="AE8" s="22"/>
+      <c r="AF8" s="22"/>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A9" s="23">
+      <c r="A9" s="22">
         <v>10</v>
       </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23">
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22">
         <v>7</v>
       </c>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23">
-        <v>0</v>
-      </c>
-      <c r="O9" s="23"/>
-      <c r="P9" s="23"/>
-      <c r="Q9" s="23">
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22">
+        <v>0</v>
+      </c>
+      <c r="O9" s="22"/>
+      <c r="P9" s="22"/>
+      <c r="Q9" s="22">
         <v>3</v>
       </c>
-      <c r="R9" s="23"/>
-      <c r="S9" s="23"/>
-      <c r="T9" s="23">
+      <c r="R9" s="22"/>
+      <c r="S9" s="22"/>
+      <c r="T9" s="22">
         <v>19</v>
       </c>
-      <c r="U9" s="23"/>
-      <c r="V9" s="23"/>
-      <c r="W9" s="23"/>
-      <c r="X9" s="23"/>
-      <c r="Y9" s="23">
+      <c r="U9" s="22"/>
+      <c r="V9" s="22"/>
+      <c r="W9" s="22"/>
+      <c r="X9" s="22"/>
+      <c r="Y9" s="22">
         <v>17</v>
       </c>
-      <c r="Z9" s="23"/>
-      <c r="AA9" s="23"/>
-      <c r="AB9" s="23"/>
-      <c r="AC9" s="23"/>
-      <c r="AD9" s="23">
-        <v>0</v>
-      </c>
-      <c r="AE9" s="23"/>
-      <c r="AF9" s="23"/>
+      <c r="Z9" s="22"/>
+      <c r="AA9" s="22"/>
+      <c r="AB9" s="22"/>
+      <c r="AC9" s="22"/>
+      <c r="AD9" s="22">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="22"/>
+      <c r="AF9" s="22"/>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23" t="s">
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="J10" s="23"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="23"/>
-      <c r="M10" s="23"/>
-      <c r="N10" s="23" t="s">
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="O10" s="23"/>
-      <c r="P10" s="23"/>
-      <c r="Q10" s="23" t="s">
+      <c r="O10" s="22"/>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="R10" s="23"/>
-      <c r="S10" s="23"/>
-      <c r="T10" s="23" t="s">
+      <c r="R10" s="22"/>
+      <c r="S10" s="22"/>
+      <c r="T10" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="U10" s="23"/>
-      <c r="V10" s="23"/>
-      <c r="W10" s="23"/>
-      <c r="X10" s="23"/>
-      <c r="Y10" s="23" t="s">
+      <c r="U10" s="22"/>
+      <c r="V10" s="22"/>
+      <c r="W10" s="22"/>
+      <c r="X10" s="22"/>
+      <c r="Y10" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="Z10" s="23"/>
-      <c r="AA10" s="23"/>
-      <c r="AB10" s="23"/>
-      <c r="AC10" s="23"/>
-      <c r="AD10" s="23" t="s">
+      <c r="Z10" s="22"/>
+      <c r="AA10" s="22"/>
+      <c r="AB10" s="22"/>
+      <c r="AC10" s="22"/>
+      <c r="AD10" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="AE10" s="23"/>
-      <c r="AF10" s="23"/>
+      <c r="AE10" s="22"/>
+      <c r="AF10" s="22"/>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A11" s="23">
+      <c r="A11" s="22">
         <f>A9</f>
         <v>10</v>
       </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="24">
-        <f>'Data package'!$B$21*I9+'Data package'!$B$18</f>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="23">
+        <f>'Data package'!$B$31*I9+'Data package'!$B$28</f>
         <v>3.338709677419355</v>
       </c>
-      <c r="J11" s="24"/>
-      <c r="K11" s="24"/>
-      <c r="L11" s="24"/>
-      <c r="M11" s="24"/>
-      <c r="N11" s="21" t="str">
-        <f ca="1">LOOKUP(N9,'Data package'!$D$11:$D$18,'Data package'!$E$11:$E$21)</f>
-        <v>no error</v>
-      </c>
-      <c r="O11" s="21"/>
-      <c r="P11" s="21"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="24">
+        <f ca="1">LOOKUP(N9,'Data package'!$D$21:$D$24,'Data package'!$E$22:$E$31)</f>
+        <v>0</v>
+      </c>
+      <c r="O11" s="24"/>
+      <c r="P11" s="24"/>
       <c r="Q11" s="25">
         <f>100/(2^3-1)*Q9</f>
         <v>42.857142857142861</v>
@@ -3301,27 +3493,27 @@
       <c r="R11" s="25"/>
       <c r="S11" s="25"/>
       <c r="T11" s="25">
-        <f>'Data package'!$B$30*T9+'Data package'!$B$27</f>
+        <f>'Data package'!$B$40*T9+'Data package'!$B$37</f>
         <v>22.903225806451616</v>
       </c>
-      <c r="U11" s="21"/>
-      <c r="V11" s="21"/>
-      <c r="W11" s="21"/>
-      <c r="X11" s="21"/>
-      <c r="Y11" s="21">
+      <c r="U11" s="24"/>
+      <c r="V11" s="24"/>
+      <c r="W11" s="24"/>
+      <c r="X11" s="24"/>
+      <c r="Y11" s="24">
         <f>Y9</f>
         <v>17</v>
       </c>
-      <c r="Z11" s="21"/>
-      <c r="AA11" s="21"/>
-      <c r="AB11" s="21"/>
-      <c r="AC11" s="21"/>
-      <c r="AD11" s="21">
-        <f>LOOKUP(AD9,'Data package'!$A$67:$A$71,'Data package'!$B$67:$B$71)</f>
-        <v>1</v>
-      </c>
-      <c r="AE11" s="21"/>
-      <c r="AF11" s="21"/>
+      <c r="Z11" s="24"/>
+      <c r="AA11" s="24"/>
+      <c r="AB11" s="24"/>
+      <c r="AC11" s="24"/>
+      <c r="AD11" s="24">
+        <f>LOOKUP(AD9,'Data package'!$A$77:$A$81,'Data package'!$B$77:$B$81)</f>
+        <v>1</v>
+      </c>
+      <c r="AE11" s="24"/>
+      <c r="AF11" s="24"/>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
@@ -3337,82 +3529,82 @@
       <c r="K12" s="16"/>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A14" s="26" t="s">
+      <c r="A14" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="26"/>
-      <c r="M14" s="26"/>
-      <c r="N14" s="26"/>
-      <c r="O14" s="26"/>
-      <c r="P14" s="26"/>
-      <c r="Q14" s="26"/>
-      <c r="R14" s="26"/>
-      <c r="S14" s="26"/>
-      <c r="T14" s="26"/>
-      <c r="U14" s="26"/>
-      <c r="V14" s="26"/>
-      <c r="W14" s="26"/>
-      <c r="X14" s="26"/>
-      <c r="Y14" s="26"/>
-      <c r="Z14" s="26"/>
-      <c r="AA14" s="26"/>
-      <c r="AB14" s="26"/>
-      <c r="AC14" s="26"/>
-      <c r="AD14" s="26"/>
-      <c r="AE14" s="26"/>
-      <c r="AF14" s="26"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="27"/>
+      <c r="M14" s="27"/>
+      <c r="N14" s="27"/>
+      <c r="O14" s="27"/>
+      <c r="P14" s="27"/>
+      <c r="Q14" s="27"/>
+      <c r="R14" s="27"/>
+      <c r="S14" s="27"/>
+      <c r="T14" s="27"/>
+      <c r="U14" s="27"/>
+      <c r="V14" s="27"/>
+      <c r="W14" s="27"/>
+      <c r="X14" s="27"/>
+      <c r="Y14" s="27"/>
+      <c r="Z14" s="27"/>
+      <c r="AA14" s="27"/>
+      <c r="AB14" s="27"/>
+      <c r="AC14" s="27"/>
+      <c r="AD14" s="27"/>
+      <c r="AE14" s="27"/>
+      <c r="AF14" s="27"/>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="27" t="s">
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="J15" s="27"/>
-      <c r="K15" s="27"/>
-      <c r="L15" s="27"/>
-      <c r="M15" s="27"/>
-      <c r="N15" s="27"/>
-      <c r="O15" s="27"/>
-      <c r="P15" s="27"/>
-      <c r="Q15" s="27" t="s">
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="26"/>
+      <c r="O15" s="26"/>
+      <c r="P15" s="26"/>
+      <c r="Q15" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="R15" s="27"/>
-      <c r="S15" s="27"/>
-      <c r="T15" s="27"/>
-      <c r="U15" s="27"/>
-      <c r="V15" s="27"/>
-      <c r="W15" s="27"/>
-      <c r="X15" s="27"/>
-      <c r="Y15" s="27" t="s">
+      <c r="R15" s="26"/>
+      <c r="S15" s="26"/>
+      <c r="T15" s="26"/>
+      <c r="U15" s="26"/>
+      <c r="V15" s="26"/>
+      <c r="W15" s="26"/>
+      <c r="X15" s="26"/>
+      <c r="Y15" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="Z15" s="27"/>
-      <c r="AA15" s="27"/>
-      <c r="AB15" s="27"/>
-      <c r="AC15" s="27"/>
-      <c r="AD15" s="27"/>
-      <c r="AE15" s="27"/>
-      <c r="AF15" s="27"/>
+      <c r="Z15" s="26"/>
+      <c r="AA15" s="26"/>
+      <c r="AB15" s="26"/>
+      <c r="AC15" s="26"/>
+      <c r="AD15" s="26"/>
+      <c r="AE15" s="26"/>
+      <c r="AF15" s="26"/>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16" s="16">
@@ -3513,175 +3705,175 @@
       </c>
     </row>
     <row r="17" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23" t="s">
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="J17" s="23"/>
-      <c r="K17" s="23"/>
-      <c r="L17" s="23"/>
-      <c r="M17" s="23"/>
-      <c r="N17" s="23" t="s">
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22"/>
+      <c r="N17" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="O17" s="23"/>
-      <c r="P17" s="23"/>
-      <c r="Q17" s="23" t="s">
+      <c r="O17" s="22"/>
+      <c r="P17" s="22"/>
+      <c r="Q17" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="R17" s="23"/>
-      <c r="S17" s="23"/>
-      <c r="T17" s="23" t="s">
+      <c r="R17" s="22"/>
+      <c r="S17" s="22"/>
+      <c r="T17" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="U17" s="23"/>
-      <c r="V17" s="23"/>
-      <c r="W17" s="23"/>
-      <c r="X17" s="23"/>
-      <c r="Y17" s="23" t="s">
+      <c r="U17" s="22"/>
+      <c r="V17" s="22"/>
+      <c r="W17" s="22"/>
+      <c r="X17" s="22"/>
+      <c r="Y17" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="Z17" s="23"/>
-      <c r="AA17" s="23"/>
-      <c r="AB17" s="23"/>
-      <c r="AC17" s="23"/>
-      <c r="AD17" s="23" t="s">
+      <c r="Z17" s="22"/>
+      <c r="AA17" s="22"/>
+      <c r="AB17" s="22"/>
+      <c r="AC17" s="22"/>
+      <c r="AD17" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="AE17" s="23"/>
-      <c r="AF17" s="23"/>
+      <c r="AE17" s="22"/>
+      <c r="AF17" s="22"/>
     </row>
     <row r="18" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A18" s="23">
+      <c r="A18" s="22">
         <v>5</v>
       </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="23">
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22">
         <v>8</v>
       </c>
-      <c r="J18" s="23"/>
-      <c r="K18" s="23"/>
-      <c r="L18" s="23"/>
-      <c r="M18" s="23"/>
-      <c r="N18" s="23">
-        <v>0</v>
-      </c>
-      <c r="O18" s="23"/>
-      <c r="P18" s="23"/>
-      <c r="Q18" s="23">
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="22"/>
+      <c r="N18" s="22">
+        <v>0</v>
+      </c>
+      <c r="O18" s="22"/>
+      <c r="P18" s="22"/>
+      <c r="Q18" s="22">
         <v>3</v>
       </c>
-      <c r="R18" s="23"/>
-      <c r="S18" s="23"/>
-      <c r="T18" s="23">
+      <c r="R18" s="22"/>
+      <c r="S18" s="22"/>
+      <c r="T18" s="22">
         <v>19</v>
       </c>
-      <c r="U18" s="23"/>
-      <c r="V18" s="23"/>
-      <c r="W18" s="23"/>
-      <c r="X18" s="23"/>
-      <c r="Y18" s="23">
+      <c r="U18" s="22"/>
+      <c r="V18" s="22"/>
+      <c r="W18" s="22"/>
+      <c r="X18" s="22"/>
+      <c r="Y18" s="22">
         <v>17</v>
       </c>
-      <c r="Z18" s="23"/>
-      <c r="AA18" s="23"/>
-      <c r="AB18" s="23"/>
-      <c r="AC18" s="23"/>
-      <c r="AD18" s="23">
-        <v>0</v>
-      </c>
-      <c r="AE18" s="23"/>
-      <c r="AF18" s="23"/>
+      <c r="Z18" s="22"/>
+      <c r="AA18" s="22"/>
+      <c r="AB18" s="22"/>
+      <c r="AC18" s="22"/>
+      <c r="AD18" s="22">
+        <v>0</v>
+      </c>
+      <c r="AE18" s="22"/>
+      <c r="AF18" s="22"/>
     </row>
     <row r="19" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="23" t="s">
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="J19" s="23"/>
-      <c r="K19" s="23"/>
-      <c r="L19" s="23"/>
-      <c r="M19" s="23"/>
-      <c r="N19" s="23" t="s">
+      <c r="J19" s="22"/>
+      <c r="K19" s="22"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="22"/>
+      <c r="N19" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="O19" s="23"/>
-      <c r="P19" s="23"/>
-      <c r="Q19" s="23" t="s">
+      <c r="O19" s="22"/>
+      <c r="P19" s="22"/>
+      <c r="Q19" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="R19" s="23"/>
-      <c r="S19" s="23"/>
-      <c r="T19" s="23" t="s">
+      <c r="R19" s="22"/>
+      <c r="S19" s="22"/>
+      <c r="T19" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="U19" s="23"/>
-      <c r="V19" s="23"/>
-      <c r="W19" s="23"/>
-      <c r="X19" s="23"/>
-      <c r="Y19" s="23" t="s">
+      <c r="U19" s="22"/>
+      <c r="V19" s="22"/>
+      <c r="W19" s="22"/>
+      <c r="X19" s="22"/>
+      <c r="Y19" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="Z19" s="23"/>
-      <c r="AA19" s="23"/>
-      <c r="AB19" s="23"/>
-      <c r="AC19" s="23"/>
-      <c r="AD19" s="23" t="s">
+      <c r="Z19" s="22"/>
+      <c r="AA19" s="22"/>
+      <c r="AB19" s="22"/>
+      <c r="AC19" s="22"/>
+      <c r="AD19" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="AE19" s="23"/>
-      <c r="AF19" s="23"/>
+      <c r="AE19" s="22"/>
+      <c r="AF19" s="22"/>
     </row>
     <row r="20" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A20" s="23">
+      <c r="A20" s="22">
         <f>A18</f>
         <v>5</v>
       </c>
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="24">
-        <f>'Data package'!$B$21*I18+'Data package'!$B$18</f>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="23">
+        <f>'Data package'!$B$31*I18+'Data package'!$B$28</f>
         <v>3.3870967741935485</v>
       </c>
-      <c r="J20" s="24"/>
-      <c r="K20" s="24"/>
-      <c r="L20" s="24"/>
-      <c r="M20" s="24"/>
-      <c r="N20" s="21" t="str">
-        <f ca="1">LOOKUP(N18,'Data package'!$D$11:$D$18,'Data package'!$E$11:$E$21)</f>
-        <v>no error</v>
-      </c>
-      <c r="O20" s="21"/>
-      <c r="P20" s="21"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="23"/>
+      <c r="N20" s="24">
+        <f ca="1">LOOKUP(N18,'Data package'!$D$21:$D$24,'Data package'!$E$22:$E$31)</f>
+        <v>0</v>
+      </c>
+      <c r="O20" s="24"/>
+      <c r="P20" s="24"/>
       <c r="Q20" s="25">
         <f>100/(2^3-1)*Q18</f>
         <v>42.857142857142861</v>
@@ -3689,185 +3881,185 @@
       <c r="R20" s="25"/>
       <c r="S20" s="25"/>
       <c r="T20" s="25">
-        <f>'Data package'!$B$30*T18+'Data package'!$B$27</f>
+        <f>'Data package'!$B$40*T18+'Data package'!$B$37</f>
         <v>22.903225806451616</v>
       </c>
-      <c r="U20" s="21"/>
-      <c r="V20" s="21"/>
-      <c r="W20" s="21"/>
-      <c r="X20" s="21"/>
-      <c r="Y20" s="21">
+      <c r="U20" s="24"/>
+      <c r="V20" s="24"/>
+      <c r="W20" s="24"/>
+      <c r="X20" s="24"/>
+      <c r="Y20" s="24">
         <f>Y18</f>
         <v>17</v>
       </c>
-      <c r="Z20" s="21"/>
-      <c r="AA20" s="21"/>
-      <c r="AB20" s="21"/>
-      <c r="AC20" s="21"/>
-      <c r="AD20" s="21">
-        <f>LOOKUP(AD18,'Data package'!$A$67:$A$71,'Data package'!$B$67:$B$71)</f>
-        <v>1</v>
-      </c>
-      <c r="AE20" s="21"/>
-      <c r="AF20" s="21"/>
+      <c r="Z20" s="24"/>
+      <c r="AA20" s="24"/>
+      <c r="AB20" s="24"/>
+      <c r="AC20" s="24"/>
+      <c r="AD20" s="24">
+        <f>LOOKUP(AD18,'Data package'!$A$77:$A$81,'Data package'!$B$77:$B$81)</f>
+        <v>1</v>
+      </c>
+      <c r="AE20" s="24"/>
+      <c r="AF20" s="24"/>
     </row>
     <row r="23" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A23" s="26" t="s">
+      <c r="A23" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="26"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="26"/>
-      <c r="K23" s="26"/>
-      <c r="L23" s="26"/>
-      <c r="M23" s="26"/>
-      <c r="N23" s="26"/>
-      <c r="O23" s="26"/>
-      <c r="P23" s="26"/>
-      <c r="Q23" s="26"/>
-      <c r="R23" s="26"/>
-      <c r="S23" s="26"/>
-      <c r="T23" s="26"/>
-      <c r="U23" s="26"/>
-      <c r="V23" s="26"/>
-      <c r="W23" s="26"/>
-      <c r="X23" s="26"/>
-      <c r="Y23" s="26"/>
-      <c r="Z23" s="26"/>
-      <c r="AA23" s="26"/>
-      <c r="AB23" s="26"/>
-      <c r="AC23" s="26"/>
-      <c r="AD23" s="26"/>
-      <c r="AE23" s="26"/>
-      <c r="AF23" s="26"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="27"/>
+      <c r="M23" s="27"/>
+      <c r="N23" s="27"/>
+      <c r="O23" s="27"/>
+      <c r="P23" s="27"/>
+      <c r="Q23" s="27"/>
+      <c r="R23" s="27"/>
+      <c r="S23" s="27"/>
+      <c r="T23" s="27"/>
+      <c r="U23" s="27"/>
+      <c r="V23" s="27"/>
+      <c r="W23" s="27"/>
+      <c r="X23" s="27"/>
+      <c r="Y23" s="27"/>
+      <c r="Z23" s="27"/>
+      <c r="AA23" s="27"/>
+      <c r="AB23" s="27"/>
+      <c r="AC23" s="27"/>
+      <c r="AD23" s="27"/>
+      <c r="AE23" s="27"/>
+      <c r="AF23" s="27"/>
     </row>
     <row r="24" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A24" s="27" t="s">
+      <c r="A24" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="27"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27"/>
-      <c r="I24" s="27" t="s">
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="J24" s="27"/>
-      <c r="K24" s="27"/>
-      <c r="L24" s="27"/>
-      <c r="M24" s="27"/>
-      <c r="N24" s="27"/>
-      <c r="O24" s="27"/>
-      <c r="P24" s="27"/>
-      <c r="Q24" s="27" t="s">
+      <c r="J24" s="26"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="26"/>
+      <c r="M24" s="26"/>
+      <c r="N24" s="26"/>
+      <c r="O24" s="26"/>
+      <c r="P24" s="26"/>
+      <c r="Q24" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="R24" s="27"/>
-      <c r="S24" s="27"/>
-      <c r="T24" s="27"/>
-      <c r="U24" s="27"/>
-      <c r="V24" s="27"/>
-      <c r="W24" s="27"/>
-      <c r="X24" s="27"/>
-      <c r="Y24" s="27" t="s">
+      <c r="R24" s="26"/>
+      <c r="S24" s="26"/>
+      <c r="T24" s="26"/>
+      <c r="U24" s="26"/>
+      <c r="V24" s="26"/>
+      <c r="W24" s="26"/>
+      <c r="X24" s="26"/>
+      <c r="Y24" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="Z24" s="27"/>
-      <c r="AA24" s="27"/>
-      <c r="AB24" s="27"/>
-      <c r="AC24" s="27"/>
-      <c r="AD24" s="27"/>
-      <c r="AE24" s="27"/>
-      <c r="AF24" s="27"/>
-      <c r="AG24" s="22">
+      <c r="Z24" s="26"/>
+      <c r="AA24" s="26"/>
+      <c r="AB24" s="26"/>
+      <c r="AC24" s="26"/>
+      <c r="AD24" s="26"/>
+      <c r="AE24" s="26"/>
+      <c r="AF24" s="26"/>
+      <c r="AG24" s="37">
         <v>59</v>
       </c>
-      <c r="AH24" s="22"/>
-      <c r="AI24" s="22"/>
-      <c r="AJ24" s="22"/>
-      <c r="AK24" s="22"/>
-      <c r="AL24" s="22"/>
-      <c r="AM24" s="22"/>
-      <c r="AN24" s="22"/>
-      <c r="AO24" s="22">
+      <c r="AH24" s="37"/>
+      <c r="AI24" s="37"/>
+      <c r="AJ24" s="37"/>
+      <c r="AK24" s="37"/>
+      <c r="AL24" s="37"/>
+      <c r="AM24" s="37"/>
+      <c r="AN24" s="37"/>
+      <c r="AO24" s="37">
         <v>96</v>
       </c>
-      <c r="AP24" s="22"/>
-      <c r="AQ24" s="22"/>
-      <c r="AR24" s="22"/>
-      <c r="AS24" s="22"/>
-      <c r="AT24" s="22"/>
-      <c r="AU24" s="22"/>
-      <c r="AV24" s="22"/>
-      <c r="AW24" s="22">
+      <c r="AP24" s="37"/>
+      <c r="AQ24" s="37"/>
+      <c r="AR24" s="37"/>
+      <c r="AS24" s="37"/>
+      <c r="AT24" s="37"/>
+      <c r="AU24" s="37"/>
+      <c r="AV24" s="37"/>
+      <c r="AW24" s="37">
         <v>65</v>
       </c>
-      <c r="AX24" s="22"/>
-      <c r="AY24" s="22"/>
-      <c r="AZ24" s="22"/>
-      <c r="BA24" s="22"/>
-      <c r="BB24" s="22"/>
-      <c r="BC24" s="22"/>
-      <c r="BD24" s="22"/>
-      <c r="BE24" s="22" t="s">
+      <c r="AX24" s="37"/>
+      <c r="AY24" s="37"/>
+      <c r="AZ24" s="37"/>
+      <c r="BA24" s="37"/>
+      <c r="BB24" s="37"/>
+      <c r="BC24" s="37"/>
+      <c r="BD24" s="37"/>
+      <c r="BE24" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="BF24" s="22"/>
-      <c r="BG24" s="22"/>
-      <c r="BH24" s="22"/>
-      <c r="BI24" s="22"/>
-      <c r="BJ24" s="22"/>
-      <c r="BK24" s="22"/>
-      <c r="BL24" s="22"/>
-      <c r="BM24" s="22" t="s">
+      <c r="BF24" s="37"/>
+      <c r="BG24" s="37"/>
+      <c r="BH24" s="37"/>
+      <c r="BI24" s="37"/>
+      <c r="BJ24" s="37"/>
+      <c r="BK24" s="37"/>
+      <c r="BL24" s="37"/>
+      <c r="BM24" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="BN24" s="22"/>
-      <c r="BO24" s="22"/>
-      <c r="BP24" s="22"/>
-      <c r="BQ24" s="22"/>
-      <c r="BR24" s="22"/>
-      <c r="BS24" s="22"/>
-      <c r="BT24" s="22"/>
-      <c r="BU24" s="22">
+      <c r="BN24" s="37"/>
+      <c r="BO24" s="37"/>
+      <c r="BP24" s="37"/>
+      <c r="BQ24" s="37"/>
+      <c r="BR24" s="37"/>
+      <c r="BS24" s="37"/>
+      <c r="BT24" s="37"/>
+      <c r="BU24" s="37">
         <v>69</v>
       </c>
-      <c r="BV24" s="22"/>
-      <c r="BW24" s="22"/>
-      <c r="BX24" s="22"/>
-      <c r="BY24" s="22"/>
-      <c r="BZ24" s="22"/>
-      <c r="CA24" s="22"/>
-      <c r="CB24" s="22"/>
-      <c r="CC24" s="22" t="s">
+      <c r="BV24" s="37"/>
+      <c r="BW24" s="37"/>
+      <c r="BX24" s="37"/>
+      <c r="BY24" s="37"/>
+      <c r="BZ24" s="37"/>
+      <c r="CA24" s="37"/>
+      <c r="CB24" s="37"/>
+      <c r="CC24" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="CD24" s="22"/>
-      <c r="CE24" s="22"/>
-      <c r="CF24" s="22"/>
-      <c r="CG24" s="22"/>
-      <c r="CH24" s="22"/>
-      <c r="CI24" s="22"/>
-      <c r="CJ24" s="22"/>
-      <c r="CK24" s="22" t="s">
+      <c r="CD24" s="37"/>
+      <c r="CE24" s="37"/>
+      <c r="CF24" s="37"/>
+      <c r="CG24" s="37"/>
+      <c r="CH24" s="37"/>
+      <c r="CI24" s="37"/>
+      <c r="CJ24" s="37"/>
+      <c r="CK24" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="CL24" s="22"/>
-      <c r="CM24" s="22"/>
-      <c r="CN24" s="22"/>
-      <c r="CO24" s="22"/>
-      <c r="CP24" s="22"/>
-      <c r="CQ24" s="22"/>
-      <c r="CR24" s="22"/>
+      <c r="CL24" s="37"/>
+      <c r="CM24" s="37"/>
+      <c r="CN24" s="37"/>
+      <c r="CO24" s="37"/>
+      <c r="CP24" s="37"/>
+      <c r="CQ24" s="37"/>
+      <c r="CR24" s="37"/>
     </row>
     <row r="25" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A25" s="18">
@@ -4160,180 +4352,180 @@
       </c>
     </row>
     <row r="26" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="23"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="23" t="s">
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="J26" s="23"/>
-      <c r="K26" s="23"/>
-      <c r="L26" s="23"/>
-      <c r="M26" s="23"/>
-      <c r="N26" s="23" t="s">
+      <c r="J26" s="22"/>
+      <c r="K26" s="22"/>
+      <c r="L26" s="22"/>
+      <c r="M26" s="22"/>
+      <c r="N26" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="O26" s="23"/>
-      <c r="P26" s="23"/>
-      <c r="Q26" s="23" t="s">
+      <c r="O26" s="22"/>
+      <c r="P26" s="22"/>
+      <c r="Q26" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="R26" s="23"/>
-      <c r="S26" s="23"/>
-      <c r="T26" s="23" t="s">
+      <c r="R26" s="22"/>
+      <c r="S26" s="22"/>
+      <c r="T26" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="U26" s="23"/>
-      <c r="V26" s="23"/>
-      <c r="W26" s="23"/>
-      <c r="X26" s="23"/>
-      <c r="Y26" s="23" t="s">
+      <c r="U26" s="22"/>
+      <c r="V26" s="22"/>
+      <c r="W26" s="22"/>
+      <c r="X26" s="22"/>
+      <c r="Y26" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="Z26" s="23"/>
-      <c r="AA26" s="23"/>
-      <c r="AB26" s="23"/>
-      <c r="AC26" s="23"/>
-      <c r="AD26" s="23" t="s">
+      <c r="Z26" s="22"/>
+      <c r="AA26" s="22"/>
+      <c r="AB26" s="22"/>
+      <c r="AC26" s="22"/>
+      <c r="AD26" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="AE26" s="23"/>
-      <c r="AF26" s="23"/>
-      <c r="AG26" s="21" t="s">
+      <c r="AE26" s="22"/>
+      <c r="AF26" s="22"/>
+      <c r="AG26" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="AH26" s="21"/>
-      <c r="AI26" s="21"/>
-      <c r="AJ26" s="21"/>
-      <c r="AK26" s="21"/>
-      <c r="AL26" s="21"/>
-      <c r="AM26" s="21"/>
-      <c r="AN26" s="21"/>
-      <c r="AO26" s="21" t="s">
+      <c r="AH26" s="24"/>
+      <c r="AI26" s="24"/>
+      <c r="AJ26" s="24"/>
+      <c r="AK26" s="24"/>
+      <c r="AL26" s="24"/>
+      <c r="AM26" s="24"/>
+      <c r="AN26" s="24"/>
+      <c r="AO26" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="AP26" s="21"/>
-      <c r="AQ26" s="21"/>
-      <c r="AR26" s="21"/>
-      <c r="AS26" s="21"/>
-      <c r="AT26" s="21"/>
-      <c r="AU26" s="21"/>
-      <c r="AV26" s="21"/>
-      <c r="AW26" s="21" t="s">
+      <c r="AP26" s="24"/>
+      <c r="AQ26" s="24"/>
+      <c r="AR26" s="24"/>
+      <c r="AS26" s="24"/>
+      <c r="AT26" s="24"/>
+      <c r="AU26" s="24"/>
+      <c r="AV26" s="24"/>
+      <c r="AW26" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="AX26" s="21"/>
-      <c r="AY26" s="21"/>
-      <c r="AZ26" s="21"/>
-      <c r="BA26" s="21"/>
-      <c r="BB26" s="21"/>
-      <c r="BC26" s="21"/>
-      <c r="BD26" s="21"/>
-      <c r="BE26" s="21" t="s">
+      <c r="AX26" s="24"/>
+      <c r="AY26" s="24"/>
+      <c r="AZ26" s="24"/>
+      <c r="BA26" s="24"/>
+      <c r="BB26" s="24"/>
+      <c r="BC26" s="24"/>
+      <c r="BD26" s="24"/>
+      <c r="BE26" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="BF26" s="21"/>
-      <c r="BG26" s="21"/>
-      <c r="BH26" s="21"/>
-      <c r="BI26" s="21"/>
-      <c r="BJ26" s="21"/>
-      <c r="BK26" s="21"/>
-      <c r="BL26" s="21"/>
-      <c r="BM26" s="21" t="s">
+      <c r="BF26" s="24"/>
+      <c r="BG26" s="24"/>
+      <c r="BH26" s="24"/>
+      <c r="BI26" s="24"/>
+      <c r="BJ26" s="24"/>
+      <c r="BK26" s="24"/>
+      <c r="BL26" s="24"/>
+      <c r="BM26" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="BN26" s="21"/>
-      <c r="BO26" s="21"/>
-      <c r="BP26" s="21"/>
-      <c r="BQ26" s="21"/>
-      <c r="BR26" s="21"/>
-      <c r="BS26" s="21"/>
-      <c r="BT26" s="21"/>
-      <c r="BU26" s="21" t="s">
+      <c r="BN26" s="24"/>
+      <c r="BO26" s="24"/>
+      <c r="BP26" s="24"/>
+      <c r="BQ26" s="24"/>
+      <c r="BR26" s="24"/>
+      <c r="BS26" s="24"/>
+      <c r="BT26" s="24"/>
+      <c r="BU26" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="BV26" s="21"/>
-      <c r="BW26" s="21"/>
-      <c r="BX26" s="21"/>
-      <c r="BY26" s="21"/>
-      <c r="BZ26" s="21"/>
-      <c r="CA26" s="21"/>
-      <c r="CB26" s="21"/>
-      <c r="CC26" s="21" t="s">
+      <c r="BV26" s="24"/>
+      <c r="BW26" s="24"/>
+      <c r="BX26" s="24"/>
+      <c r="BY26" s="24"/>
+      <c r="BZ26" s="24"/>
+      <c r="CA26" s="24"/>
+      <c r="CB26" s="24"/>
+      <c r="CC26" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="CD26" s="21"/>
-      <c r="CE26" s="21"/>
-      <c r="CF26" s="21"/>
-      <c r="CG26" s="21"/>
-      <c r="CH26" s="21"/>
-      <c r="CI26" s="21"/>
-      <c r="CJ26" s="21"/>
-      <c r="CK26" s="21" t="s">
+      <c r="CD26" s="24"/>
+      <c r="CE26" s="24"/>
+      <c r="CF26" s="24"/>
+      <c r="CG26" s="24"/>
+      <c r="CH26" s="24"/>
+      <c r="CI26" s="24"/>
+      <c r="CJ26" s="24"/>
+      <c r="CK26" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="CL26" s="21"/>
-      <c r="CM26" s="21"/>
-      <c r="CN26" s="21"/>
-      <c r="CO26" s="21"/>
-      <c r="CP26" s="21"/>
-      <c r="CQ26" s="21"/>
-      <c r="CR26" s="21"/>
+      <c r="CL26" s="24"/>
+      <c r="CM26" s="24"/>
+      <c r="CN26" s="24"/>
+      <c r="CO26" s="24"/>
+      <c r="CP26" s="24"/>
+      <c r="CQ26" s="24"/>
+      <c r="CR26" s="24"/>
     </row>
     <row r="27" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A27" s="23">
+      <c r="A27" s="22">
         <v>10</v>
       </c>
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="23">
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22">
         <v>8</v>
       </c>
-      <c r="J27" s="23"/>
-      <c r="K27" s="23"/>
-      <c r="L27" s="23"/>
-      <c r="M27" s="23"/>
-      <c r="N27" s="23">
-        <v>0</v>
-      </c>
-      <c r="O27" s="23"/>
-      <c r="P27" s="23"/>
-      <c r="Q27" s="23">
+      <c r="J27" s="22"/>
+      <c r="K27" s="22"/>
+      <c r="L27" s="22"/>
+      <c r="M27" s="22"/>
+      <c r="N27" s="22">
+        <v>0</v>
+      </c>
+      <c r="O27" s="22"/>
+      <c r="P27" s="22"/>
+      <c r="Q27" s="22">
         <v>3</v>
       </c>
-      <c r="R27" s="23"/>
-      <c r="S27" s="23"/>
-      <c r="T27" s="23">
+      <c r="R27" s="22"/>
+      <c r="S27" s="22"/>
+      <c r="T27" s="22">
         <v>19</v>
       </c>
-      <c r="U27" s="23"/>
-      <c r="V27" s="23"/>
-      <c r="W27" s="23"/>
-      <c r="X27" s="23"/>
-      <c r="Y27" s="23">
+      <c r="U27" s="22"/>
+      <c r="V27" s="22"/>
+      <c r="W27" s="22"/>
+      <c r="X27" s="22"/>
+      <c r="Y27" s="22">
         <v>21</v>
       </c>
-      <c r="Z27" s="23"/>
-      <c r="AA27" s="23"/>
-      <c r="AB27" s="23"/>
-      <c r="AC27" s="23"/>
-      <c r="AD27" s="23">
-        <v>0</v>
-      </c>
-      <c r="AE27" s="23"/>
-      <c r="AF27" s="23"/>
+      <c r="Z27" s="22"/>
+      <c r="AA27" s="22"/>
+      <c r="AB27" s="22"/>
+      <c r="AC27" s="22"/>
+      <c r="AD27" s="22">
+        <v>0</v>
+      </c>
+      <c r="AE27" s="22"/>
+      <c r="AF27" s="22"/>
       <c r="AG27">
         <f>AN25</f>
         <v>1</v>
@@ -4592,159 +4784,159 @@
       </c>
     </row>
     <row r="28" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A28" s="23" t="s">
+      <c r="A28" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="23"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="23" t="s">
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="J28" s="23"/>
-      <c r="K28" s="23"/>
-      <c r="L28" s="23"/>
-      <c r="M28" s="23"/>
-      <c r="N28" s="23" t="s">
+      <c r="J28" s="22"/>
+      <c r="K28" s="22"/>
+      <c r="L28" s="22"/>
+      <c r="M28" s="22"/>
+      <c r="N28" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="O28" s="23"/>
-      <c r="P28" s="23"/>
-      <c r="Q28" s="23" t="s">
+      <c r="O28" s="22"/>
+      <c r="P28" s="22"/>
+      <c r="Q28" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="R28" s="23"/>
-      <c r="S28" s="23"/>
-      <c r="T28" s="23" t="s">
+      <c r="R28" s="22"/>
+      <c r="S28" s="22"/>
+      <c r="T28" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="U28" s="23"/>
-      <c r="V28" s="23"/>
-      <c r="W28" s="23"/>
-      <c r="X28" s="23"/>
-      <c r="Y28" s="23" t="s">
+      <c r="U28" s="22"/>
+      <c r="V28" s="22"/>
+      <c r="W28" s="22"/>
+      <c r="X28" s="22"/>
+      <c r="Y28" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="Z28" s="23"/>
-      <c r="AA28" s="23"/>
-      <c r="AB28" s="23"/>
-      <c r="AC28" s="23"/>
-      <c r="AD28" s="23" t="s">
+      <c r="Z28" s="22"/>
+      <c r="AA28" s="22"/>
+      <c r="AB28" s="22"/>
+      <c r="AC28" s="22"/>
+      <c r="AD28" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="AE28" s="23"/>
-      <c r="AF28" s="23"/>
-      <c r="AG28" s="21" t="s">
+      <c r="AE28" s="22"/>
+      <c r="AF28" s="22"/>
+      <c r="AG28" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="AH28" s="21"/>
-      <c r="AI28" s="21"/>
-      <c r="AJ28" s="21"/>
-      <c r="AK28" s="21"/>
-      <c r="AL28" s="21"/>
-      <c r="AM28" s="21" t="s">
+      <c r="AH28" s="24"/>
+      <c r="AI28" s="24"/>
+      <c r="AJ28" s="24"/>
+      <c r="AK28" s="24"/>
+      <c r="AL28" s="24"/>
+      <c r="AM28" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="AN28" s="21"/>
-      <c r="AO28" s="21"/>
-      <c r="AP28" s="21"/>
-      <c r="AQ28" s="21"/>
-      <c r="AR28" s="21"/>
-      <c r="AS28" s="21" t="s">
+      <c r="AN28" s="24"/>
+      <c r="AO28" s="24"/>
+      <c r="AP28" s="24"/>
+      <c r="AQ28" s="24"/>
+      <c r="AR28" s="24"/>
+      <c r="AS28" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="AT28" s="21"/>
-      <c r="AU28" s="21"/>
-      <c r="AV28" s="21"/>
-      <c r="AW28" s="21"/>
-      <c r="AX28" s="21"/>
-      <c r="AY28" s="21" t="s">
+      <c r="AT28" s="24"/>
+      <c r="AU28" s="24"/>
+      <c r="AV28" s="24"/>
+      <c r="AW28" s="24"/>
+      <c r="AX28" s="24"/>
+      <c r="AY28" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="AZ28" s="21"/>
-      <c r="BA28" s="21"/>
-      <c r="BB28" s="21"/>
-      <c r="BC28" s="21"/>
-      <c r="BD28" s="21"/>
-      <c r="BE28" s="21" t="s">
+      <c r="AZ28" s="24"/>
+      <c r="BA28" s="24"/>
+      <c r="BB28" s="24"/>
+      <c r="BC28" s="24"/>
+      <c r="BD28" s="24"/>
+      <c r="BE28" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="BF28" s="21"/>
-      <c r="BG28" s="21"/>
-      <c r="BH28" s="21"/>
-      <c r="BI28" s="21"/>
-      <c r="BJ28" s="21"/>
-      <c r="BK28" s="21" t="s">
+      <c r="BF28" s="24"/>
+      <c r="BG28" s="24"/>
+      <c r="BH28" s="24"/>
+      <c r="BI28" s="24"/>
+      <c r="BJ28" s="24"/>
+      <c r="BK28" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="BL28" s="21"/>
-      <c r="BM28" s="21"/>
-      <c r="BN28" s="21"/>
-      <c r="BO28" s="21"/>
-      <c r="BP28" s="21"/>
-      <c r="BQ28" s="21" t="s">
+      <c r="BL28" s="24"/>
+      <c r="BM28" s="24"/>
+      <c r="BN28" s="24"/>
+      <c r="BO28" s="24"/>
+      <c r="BP28" s="24"/>
+      <c r="BQ28" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="BR28" s="21"/>
-      <c r="BS28" s="21"/>
-      <c r="BT28" s="21"/>
-      <c r="BU28" s="21"/>
-      <c r="BV28" s="21"/>
-      <c r="BW28" s="21" t="s">
+      <c r="BR28" s="24"/>
+      <c r="BS28" s="24"/>
+      <c r="BT28" s="24"/>
+      <c r="BU28" s="24"/>
+      <c r="BV28" s="24"/>
+      <c r="BW28" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="BX28" s="21"/>
-      <c r="BY28" s="21"/>
-      <c r="BZ28" s="21"/>
-      <c r="CA28" s="21"/>
-      <c r="CB28" s="21"/>
-      <c r="CC28" s="21" t="s">
+      <c r="BX28" s="24"/>
+      <c r="BY28" s="24"/>
+      <c r="BZ28" s="24"/>
+      <c r="CA28" s="24"/>
+      <c r="CB28" s="24"/>
+      <c r="CC28" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="CD28" s="21"/>
-      <c r="CE28" s="21"/>
-      <c r="CF28" s="21"/>
-      <c r="CG28" s="21"/>
-      <c r="CH28" s="21"/>
-      <c r="CI28" s="21" t="s">
+      <c r="CD28" s="24"/>
+      <c r="CE28" s="24"/>
+      <c r="CF28" s="24"/>
+      <c r="CG28" s="24"/>
+      <c r="CH28" s="24"/>
+      <c r="CI28" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="CJ28" s="21"/>
-      <c r="CK28" s="21"/>
-      <c r="CL28" s="21"/>
-      <c r="CM28" s="21"/>
-      <c r="CN28" s="21"/>
+      <c r="CJ28" s="24"/>
+      <c r="CK28" s="24"/>
+      <c r="CL28" s="24"/>
+      <c r="CM28" s="24"/>
+      <c r="CN28" s="24"/>
     </row>
     <row r="29" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A29" s="23">
+      <c r="A29" s="22">
         <f>A27</f>
         <v>10</v>
       </c>
-      <c r="B29" s="23"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="24">
-        <f>'Data package'!$B$21*I27+'Data package'!$B$18</f>
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="23">
+        <f>'Data package'!$B$31*I27+'Data package'!$B$28</f>
         <v>3.3870967741935485</v>
       </c>
-      <c r="J29" s="24"/>
-      <c r="K29" s="24"/>
-      <c r="L29" s="24"/>
-      <c r="M29" s="24"/>
-      <c r="N29" s="21" t="str">
-        <f ca="1">LOOKUP(N27,'Data package'!$D$11:$D$18,'Data package'!$E$11:$E$21)</f>
-        <v>no error</v>
-      </c>
-      <c r="O29" s="21"/>
-      <c r="P29" s="21"/>
+      <c r="J29" s="23"/>
+      <c r="K29" s="23"/>
+      <c r="L29" s="23"/>
+      <c r="M29" s="23"/>
+      <c r="N29" s="24">
+        <f ca="1">LOOKUP(N27,'Data package'!$D$21:$D$24,'Data package'!$E$22:$E$31)</f>
+        <v>0</v>
+      </c>
+      <c r="O29" s="24"/>
+      <c r="P29" s="24"/>
       <c r="Q29" s="25">
         <f>100/(2^3-1)*Q27</f>
         <v>42.857142857142861</v>
@@ -4752,107 +4944,107 @@
       <c r="R29" s="25"/>
       <c r="S29" s="25"/>
       <c r="T29" s="25">
-        <f>'Data package'!$B$30*T27+'Data package'!$B$27</f>
+        <f>'Data package'!$B$40*T27+'Data package'!$B$37</f>
         <v>22.903225806451616</v>
       </c>
-      <c r="U29" s="21"/>
-      <c r="V29" s="21"/>
-      <c r="W29" s="21"/>
-      <c r="X29" s="21"/>
-      <c r="Y29" s="21">
+      <c r="U29" s="24"/>
+      <c r="V29" s="24"/>
+      <c r="W29" s="24"/>
+      <c r="X29" s="24"/>
+      <c r="Y29" s="24">
         <f>Y27</f>
         <v>21</v>
       </c>
-      <c r="Z29" s="21"/>
-      <c r="AA29" s="21"/>
-      <c r="AB29" s="21"/>
-      <c r="AC29" s="21"/>
-      <c r="AD29" s="21">
-        <f>LOOKUP(AD27,'Data package'!$A$67:$A$71,'Data package'!$B$67:$B$71)</f>
-        <v>1</v>
-      </c>
-      <c r="AE29" s="21"/>
-      <c r="AF29" s="21"/>
-      <c r="AG29" s="21" t="s">
+      <c r="Z29" s="24"/>
+      <c r="AA29" s="24"/>
+      <c r="AB29" s="24"/>
+      <c r="AC29" s="24"/>
+      <c r="AD29" s="24">
+        <f>LOOKUP(AD27,'Data package'!$A$77:$A$81,'Data package'!$B$77:$B$81)</f>
+        <v>1</v>
+      </c>
+      <c r="AE29" s="24"/>
+      <c r="AF29" s="24"/>
+      <c r="AG29" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="AH29" s="21"/>
-      <c r="AI29" s="21"/>
-      <c r="AJ29" s="21"/>
-      <c r="AK29" s="21"/>
-      <c r="AL29" s="21"/>
-      <c r="AM29" s="21" t="s">
+      <c r="AH29" s="24"/>
+      <c r="AI29" s="24"/>
+      <c r="AJ29" s="24"/>
+      <c r="AK29" s="24"/>
+      <c r="AL29" s="24"/>
+      <c r="AM29" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="AN29" s="21"/>
-      <c r="AO29" s="21"/>
-      <c r="AP29" s="21"/>
-      <c r="AQ29" s="21"/>
-      <c r="AR29" s="21"/>
-      <c r="AS29" s="21" t="s">
+      <c r="AN29" s="24"/>
+      <c r="AO29" s="24"/>
+      <c r="AP29" s="24"/>
+      <c r="AQ29" s="24"/>
+      <c r="AR29" s="24"/>
+      <c r="AS29" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="AT29" s="21"/>
-      <c r="AU29" s="21"/>
-      <c r="AV29" s="21"/>
-      <c r="AW29" s="21"/>
-      <c r="AX29" s="21"/>
-      <c r="AY29" s="21" t="s">
+      <c r="AT29" s="24"/>
+      <c r="AU29" s="24"/>
+      <c r="AV29" s="24"/>
+      <c r="AW29" s="24"/>
+      <c r="AX29" s="24"/>
+      <c r="AY29" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="AZ29" s="21"/>
-      <c r="BA29" s="21"/>
-      <c r="BB29" s="21"/>
-      <c r="BC29" s="21"/>
-      <c r="BD29" s="21"/>
-      <c r="BE29" s="21" t="s">
+      <c r="AZ29" s="24"/>
+      <c r="BA29" s="24"/>
+      <c r="BB29" s="24"/>
+      <c r="BC29" s="24"/>
+      <c r="BD29" s="24"/>
+      <c r="BE29" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="BF29" s="21"/>
-      <c r="BG29" s="21"/>
-      <c r="BH29" s="21"/>
-      <c r="BI29" s="21"/>
-      <c r="BJ29" s="21"/>
-      <c r="BK29" s="21" t="s">
+      <c r="BF29" s="24"/>
+      <c r="BG29" s="24"/>
+      <c r="BH29" s="24"/>
+      <c r="BI29" s="24"/>
+      <c r="BJ29" s="24"/>
+      <c r="BK29" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="BL29" s="21"/>
-      <c r="BM29" s="21"/>
-      <c r="BN29" s="21"/>
-      <c r="BO29" s="21"/>
-      <c r="BP29" s="21"/>
-      <c r="BQ29" s="21" t="s">
+      <c r="BL29" s="24"/>
+      <c r="BM29" s="24"/>
+      <c r="BN29" s="24"/>
+      <c r="BO29" s="24"/>
+      <c r="BP29" s="24"/>
+      <c r="BQ29" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="BR29" s="21"/>
-      <c r="BS29" s="21"/>
-      <c r="BT29" s="21"/>
-      <c r="BU29" s="21"/>
-      <c r="BV29" s="21"/>
-      <c r="BW29" s="21" t="s">
+      <c r="BR29" s="24"/>
+      <c r="BS29" s="24"/>
+      <c r="BT29" s="24"/>
+      <c r="BU29" s="24"/>
+      <c r="BV29" s="24"/>
+      <c r="BW29" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="BX29" s="21"/>
-      <c r="BY29" s="21"/>
-      <c r="BZ29" s="21"/>
-      <c r="CA29" s="21"/>
-      <c r="CB29" s="21"/>
-      <c r="CC29" s="21" t="s">
+      <c r="BX29" s="24"/>
+      <c r="BY29" s="24"/>
+      <c r="BZ29" s="24"/>
+      <c r="CA29" s="24"/>
+      <c r="CB29" s="24"/>
+      <c r="CC29" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="CD29" s="21"/>
-      <c r="CE29" s="21"/>
-      <c r="CF29" s="21"/>
-      <c r="CG29" s="21"/>
-      <c r="CH29" s="21"/>
-      <c r="CI29" s="21" t="s">
+      <c r="CD29" s="24"/>
+      <c r="CE29" s="24"/>
+      <c r="CF29" s="24"/>
+      <c r="CG29" s="24"/>
+      <c r="CH29" s="24"/>
+      <c r="CI29" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="CJ29" s="21"/>
-      <c r="CK29" s="21"/>
-      <c r="CL29" s="21"/>
-      <c r="CM29" s="21"/>
-      <c r="CN29" s="21"/>
+      <c r="CJ29" s="24"/>
+      <c r="CK29" s="24"/>
+      <c r="CL29" s="24"/>
+      <c r="CM29" s="24"/>
+      <c r="CN29" s="24"/>
     </row>
     <row r="30" spans="1:96" x14ac:dyDescent="0.3">
       <c r="AG30">
@@ -5097,229 +5289,255 @@
       </c>
     </row>
     <row r="31" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="AG31" s="21" t="s">
+      <c r="AG31" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="AH31" s="21"/>
-      <c r="AI31" s="21"/>
-      <c r="AJ31" s="21"/>
-      <c r="AK31" s="21"/>
-      <c r="AL31" s="21"/>
-      <c r="AM31" s="21" t="s">
+      <c r="AH31" s="24"/>
+      <c r="AI31" s="24"/>
+      <c r="AJ31" s="24"/>
+      <c r="AK31" s="24"/>
+      <c r="AL31" s="24"/>
+      <c r="AM31" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="AN31" s="21"/>
-      <c r="AO31" s="21"/>
-      <c r="AP31" s="21"/>
-      <c r="AQ31" s="21"/>
-      <c r="AR31" s="21"/>
-      <c r="AS31" s="21" t="s">
+      <c r="AN31" s="24"/>
+      <c r="AO31" s="24"/>
+      <c r="AP31" s="24"/>
+      <c r="AQ31" s="24"/>
+      <c r="AR31" s="24"/>
+      <c r="AS31" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="AT31" s="21"/>
-      <c r="AU31" s="21"/>
-      <c r="AV31" s="21"/>
-      <c r="AW31" s="21"/>
-      <c r="AX31" s="21"/>
-      <c r="AY31" s="21" t="s">
+      <c r="AT31" s="24"/>
+      <c r="AU31" s="24"/>
+      <c r="AV31" s="24"/>
+      <c r="AW31" s="24"/>
+      <c r="AX31" s="24"/>
+      <c r="AY31" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="AZ31" s="21"/>
-      <c r="BA31" s="21"/>
-      <c r="BB31" s="21"/>
-      <c r="BC31" s="21"/>
-      <c r="BD31" s="21"/>
-      <c r="BE31" s="21" t="s">
+      <c r="AZ31" s="24"/>
+      <c r="BA31" s="24"/>
+      <c r="BB31" s="24"/>
+      <c r="BC31" s="24"/>
+      <c r="BD31" s="24"/>
+      <c r="BE31" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="BF31" s="21"/>
-      <c r="BG31" s="21"/>
-      <c r="BH31" s="21"/>
-      <c r="BI31" s="21"/>
-      <c r="BJ31" s="21"/>
-      <c r="BK31" s="21" t="s">
+      <c r="BF31" s="24"/>
+      <c r="BG31" s="24"/>
+      <c r="BH31" s="24"/>
+      <c r="BI31" s="24"/>
+      <c r="BJ31" s="24"/>
+      <c r="BK31" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="BL31" s="21"/>
-      <c r="BM31" s="21"/>
-      <c r="BN31" s="21"/>
-      <c r="BO31" s="21"/>
-      <c r="BP31" s="21"/>
-      <c r="BQ31" s="21" t="s">
+      <c r="BL31" s="24"/>
+      <c r="BM31" s="24"/>
+      <c r="BN31" s="24"/>
+      <c r="BO31" s="24"/>
+      <c r="BP31" s="24"/>
+      <c r="BQ31" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="BR31" s="21"/>
-      <c r="BS31" s="21"/>
-      <c r="BT31" s="21"/>
-      <c r="BU31" s="21"/>
-      <c r="BV31" s="21"/>
-      <c r="BW31" s="21" t="s">
+      <c r="BR31" s="24"/>
+      <c r="BS31" s="24"/>
+      <c r="BT31" s="24"/>
+      <c r="BU31" s="24"/>
+      <c r="BV31" s="24"/>
+      <c r="BW31" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="BX31" s="21"/>
-      <c r="BY31" s="21"/>
-      <c r="BZ31" s="21"/>
-      <c r="CA31" s="21"/>
-      <c r="CB31" s="21"/>
-      <c r="CC31" s="21" t="s">
+      <c r="BX31" s="24"/>
+      <c r="BY31" s="24"/>
+      <c r="BZ31" s="24"/>
+      <c r="CA31" s="24"/>
+      <c r="CB31" s="24"/>
+      <c r="CC31" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="CD31" s="21"/>
-      <c r="CE31" s="21"/>
-      <c r="CF31" s="21"/>
-      <c r="CG31" s="21"/>
-      <c r="CH31" s="21"/>
-      <c r="CI31" s="21" t="s">
+      <c r="CD31" s="24"/>
+      <c r="CE31" s="24"/>
+      <c r="CF31" s="24"/>
+      <c r="CG31" s="24"/>
+      <c r="CH31" s="24"/>
+      <c r="CI31" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="CJ31" s="21"/>
-      <c r="CK31" s="21"/>
-      <c r="CL31" s="21"/>
-      <c r="CM31" s="21"/>
-      <c r="CN31" s="21"/>
+      <c r="CJ31" s="24"/>
+      <c r="CK31" s="24"/>
+      <c r="CL31" s="24"/>
+      <c r="CM31" s="24"/>
+      <c r="CN31" s="24"/>
     </row>
     <row r="32" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="AG32" s="21">
+      <c r="AG32" s="24">
         <v>25</v>
       </c>
-      <c r="AH32" s="21"/>
-      <c r="AI32" s="21"/>
-      <c r="AJ32" s="21"/>
-      <c r="AK32" s="21"/>
-      <c r="AL32" s="21"/>
-      <c r="AM32" s="21">
+      <c r="AH32" s="24"/>
+      <c r="AI32" s="24"/>
+      <c r="AJ32" s="24"/>
+      <c r="AK32" s="24"/>
+      <c r="AL32" s="24"/>
+      <c r="AM32" s="24">
         <v>25</v>
       </c>
-      <c r="AN32" s="21"/>
-      <c r="AO32" s="21"/>
-      <c r="AP32" s="21"/>
-      <c r="AQ32" s="21"/>
-      <c r="AR32" s="21"/>
-      <c r="AS32" s="21">
+      <c r="AN32" s="24"/>
+      <c r="AO32" s="24"/>
+      <c r="AP32" s="24"/>
+      <c r="AQ32" s="24"/>
+      <c r="AR32" s="24"/>
+      <c r="AS32" s="24">
         <v>25</v>
       </c>
-      <c r="AT32" s="21"/>
-      <c r="AU32" s="21"/>
-      <c r="AV32" s="21"/>
-      <c r="AW32" s="21"/>
-      <c r="AX32" s="21"/>
-      <c r="AY32" s="21">
+      <c r="AT32" s="24"/>
+      <c r="AU32" s="24"/>
+      <c r="AV32" s="24"/>
+      <c r="AW32" s="24"/>
+      <c r="AX32" s="24"/>
+      <c r="AY32" s="24">
         <v>25</v>
       </c>
-      <c r="AZ32" s="21"/>
-      <c r="BA32" s="21"/>
-      <c r="BB32" s="21"/>
-      <c r="BC32" s="21"/>
-      <c r="BD32" s="21"/>
-      <c r="BE32" s="21">
+      <c r="AZ32" s="24"/>
+      <c r="BA32" s="24"/>
+      <c r="BB32" s="24"/>
+      <c r="BC32" s="24"/>
+      <c r="BD32" s="24"/>
+      <c r="BE32" s="24">
         <v>26</v>
       </c>
-      <c r="BF32" s="21"/>
-      <c r="BG32" s="21"/>
-      <c r="BH32" s="21"/>
-      <c r="BI32" s="21"/>
-      <c r="BJ32" s="21"/>
-      <c r="BK32" s="21">
+      <c r="BF32" s="24"/>
+      <c r="BG32" s="24"/>
+      <c r="BH32" s="24"/>
+      <c r="BI32" s="24"/>
+      <c r="BJ32" s="24"/>
+      <c r="BK32" s="24">
         <v>26</v>
       </c>
-      <c r="BL32" s="21"/>
-      <c r="BM32" s="21"/>
-      <c r="BN32" s="21"/>
-      <c r="BO32" s="21"/>
-      <c r="BP32" s="21"/>
-      <c r="BQ32" s="21">
+      <c r="BL32" s="24"/>
+      <c r="BM32" s="24"/>
+      <c r="BN32" s="24"/>
+      <c r="BO32" s="24"/>
+      <c r="BP32" s="24"/>
+      <c r="BQ32" s="24">
         <v>26</v>
       </c>
-      <c r="BR32" s="21"/>
-      <c r="BS32" s="21"/>
-      <c r="BT32" s="21"/>
-      <c r="BU32" s="21"/>
-      <c r="BV32" s="21"/>
-      <c r="BW32" s="21">
+      <c r="BR32" s="24"/>
+      <c r="BS32" s="24"/>
+      <c r="BT32" s="24"/>
+      <c r="BU32" s="24"/>
+      <c r="BV32" s="24"/>
+      <c r="BW32" s="24">
         <v>26</v>
       </c>
-      <c r="BX32" s="21"/>
-      <c r="BY32" s="21"/>
-      <c r="BZ32" s="21"/>
-      <c r="CA32" s="21"/>
-      <c r="CB32" s="21"/>
-      <c r="CC32" s="21">
+      <c r="BX32" s="24"/>
+      <c r="BY32" s="24"/>
+      <c r="BZ32" s="24"/>
+      <c r="CA32" s="24"/>
+      <c r="CB32" s="24"/>
+      <c r="CC32" s="24">
         <v>26</v>
       </c>
-      <c r="CD32" s="21"/>
-      <c r="CE32" s="21"/>
-      <c r="CF32" s="21"/>
-      <c r="CG32" s="21"/>
-      <c r="CH32" s="21"/>
-      <c r="CI32" s="21">
+      <c r="CD32" s="24"/>
+      <c r="CE32" s="24"/>
+      <c r="CF32" s="24"/>
+      <c r="CG32" s="24"/>
+      <c r="CH32" s="24"/>
+      <c r="CI32" s="24">
         <v>26</v>
       </c>
-      <c r="CJ32" s="21"/>
-      <c r="CK32" s="21"/>
-      <c r="CL32" s="21"/>
-      <c r="CM32" s="21"/>
-      <c r="CN32" s="21"/>
+      <c r="CJ32" s="24"/>
+      <c r="CK32" s="24"/>
+      <c r="CL32" s="24"/>
+      <c r="CM32" s="24"/>
+      <c r="CN32" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="166">
-    <mergeCell ref="Y19:AC19"/>
-    <mergeCell ref="AD19:AF19"/>
-    <mergeCell ref="A20:H20"/>
-    <mergeCell ref="I20:M20"/>
-    <mergeCell ref="N20:P20"/>
-    <mergeCell ref="Q20:S20"/>
-    <mergeCell ref="T20:X20"/>
-    <mergeCell ref="Y20:AC20"/>
-    <mergeCell ref="AD20:AF20"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="I19:M19"/>
-    <mergeCell ref="N19:P19"/>
-    <mergeCell ref="Q19:S19"/>
-    <mergeCell ref="T19:X19"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="I15:P15"/>
-    <mergeCell ref="Q15:X15"/>
-    <mergeCell ref="Y15:AF15"/>
-    <mergeCell ref="A14:AF14"/>
-    <mergeCell ref="Y17:AC17"/>
-    <mergeCell ref="AD17:AF17"/>
-    <mergeCell ref="A18:H18"/>
-    <mergeCell ref="I18:M18"/>
-    <mergeCell ref="N18:P18"/>
-    <mergeCell ref="Q18:S18"/>
-    <mergeCell ref="T18:X18"/>
-    <mergeCell ref="Y18:AC18"/>
-    <mergeCell ref="AD18:AF18"/>
-    <mergeCell ref="A17:H17"/>
-    <mergeCell ref="I17:M17"/>
-    <mergeCell ref="N17:P17"/>
-    <mergeCell ref="Q17:S17"/>
-    <mergeCell ref="T17:X17"/>
-    <mergeCell ref="I11:M11"/>
-    <mergeCell ref="A11:H11"/>
-    <mergeCell ref="I10:M10"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="AD10:AF10"/>
-    <mergeCell ref="Y10:AC10"/>
-    <mergeCell ref="T10:X10"/>
-    <mergeCell ref="Q10:S10"/>
-    <mergeCell ref="N10:P10"/>
-    <mergeCell ref="AD11:AF11"/>
-    <mergeCell ref="Y11:AC11"/>
-    <mergeCell ref="T11:X11"/>
-    <mergeCell ref="Q11:S11"/>
-    <mergeCell ref="N11:P11"/>
-    <mergeCell ref="Q6:X6"/>
-    <mergeCell ref="Y6:AF6"/>
-    <mergeCell ref="AD9:AF9"/>
-    <mergeCell ref="AD8:AF8"/>
-    <mergeCell ref="Y9:AC9"/>
-    <mergeCell ref="Y8:AC8"/>
-    <mergeCell ref="N9:P9"/>
-    <mergeCell ref="Q8:S8"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="T8:X8"/>
-    <mergeCell ref="T9:X9"/>
+    <mergeCell ref="BK32:BP32"/>
+    <mergeCell ref="BQ32:BV32"/>
+    <mergeCell ref="BW32:CB32"/>
+    <mergeCell ref="CC32:CH32"/>
+    <mergeCell ref="CI32:CN32"/>
+    <mergeCell ref="AG32:AL32"/>
+    <mergeCell ref="AM32:AR32"/>
+    <mergeCell ref="AS32:AX32"/>
+    <mergeCell ref="AY32:BD32"/>
+    <mergeCell ref="BE32:BJ32"/>
+    <mergeCell ref="BK31:BP31"/>
+    <mergeCell ref="BQ31:BV31"/>
+    <mergeCell ref="BW31:CB31"/>
+    <mergeCell ref="CC31:CH31"/>
+    <mergeCell ref="CI31:CN31"/>
+    <mergeCell ref="AG31:AL31"/>
+    <mergeCell ref="AM31:AR31"/>
+    <mergeCell ref="AS31:AX31"/>
+    <mergeCell ref="AY31:BD31"/>
+    <mergeCell ref="BE31:BJ31"/>
+    <mergeCell ref="BK29:BP29"/>
+    <mergeCell ref="BQ29:BV29"/>
+    <mergeCell ref="BW29:CB29"/>
+    <mergeCell ref="CC29:CH29"/>
+    <mergeCell ref="CI29:CN29"/>
+    <mergeCell ref="AG29:AL29"/>
+    <mergeCell ref="AM29:AR29"/>
+    <mergeCell ref="AS29:AX29"/>
+    <mergeCell ref="AY29:BD29"/>
+    <mergeCell ref="BE29:BJ29"/>
+    <mergeCell ref="BK28:BP28"/>
+    <mergeCell ref="BQ28:BV28"/>
+    <mergeCell ref="BW28:CB28"/>
+    <mergeCell ref="CC28:CH28"/>
+    <mergeCell ref="CI28:CN28"/>
+    <mergeCell ref="AG28:AL28"/>
+    <mergeCell ref="AM28:AR28"/>
+    <mergeCell ref="AS28:AX28"/>
+    <mergeCell ref="AY28:BD28"/>
+    <mergeCell ref="BE28:BJ28"/>
+    <mergeCell ref="BU24:CB24"/>
+    <mergeCell ref="CC24:CJ24"/>
+    <mergeCell ref="CK24:CR24"/>
+    <mergeCell ref="AG26:AN26"/>
+    <mergeCell ref="AO26:AV26"/>
+    <mergeCell ref="AW26:BD26"/>
+    <mergeCell ref="BE26:BL26"/>
+    <mergeCell ref="BM26:BT26"/>
+    <mergeCell ref="BU26:CB26"/>
+    <mergeCell ref="CC26:CJ26"/>
+    <mergeCell ref="CK26:CR26"/>
+    <mergeCell ref="AG24:AN24"/>
+    <mergeCell ref="AO24:AV24"/>
+    <mergeCell ref="AW24:BD24"/>
+    <mergeCell ref="BE24:BL24"/>
+    <mergeCell ref="BM24:BT24"/>
+    <mergeCell ref="Y28:AC28"/>
+    <mergeCell ref="AD28:AF28"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="I29:M29"/>
+    <mergeCell ref="N29:P29"/>
+    <mergeCell ref="Q29:S29"/>
+    <mergeCell ref="T29:X29"/>
+    <mergeCell ref="Y29:AC29"/>
+    <mergeCell ref="AD29:AF29"/>
+    <mergeCell ref="A28:H28"/>
+    <mergeCell ref="I28:M28"/>
+    <mergeCell ref="N28:P28"/>
+    <mergeCell ref="Q28:S28"/>
+    <mergeCell ref="T28:X28"/>
+    <mergeCell ref="Y26:AC26"/>
+    <mergeCell ref="AD26:AF26"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="I27:M27"/>
+    <mergeCell ref="N27:P27"/>
+    <mergeCell ref="Q27:S27"/>
+    <mergeCell ref="T27:X27"/>
+    <mergeCell ref="Y27:AC27"/>
+    <mergeCell ref="AD27:AF27"/>
+    <mergeCell ref="A26:H26"/>
+    <mergeCell ref="I26:M26"/>
+    <mergeCell ref="N26:P26"/>
+    <mergeCell ref="Q26:S26"/>
+    <mergeCell ref="T26:X26"/>
     <mergeCell ref="A23:AF23"/>
     <mergeCell ref="A24:H24"/>
     <mergeCell ref="I24:P24"/>
@@ -5344,90 +5562,64 @@
     <mergeCell ref="I8:M8"/>
     <mergeCell ref="N8:P8"/>
     <mergeCell ref="I9:M9"/>
-    <mergeCell ref="Y26:AC26"/>
-    <mergeCell ref="AD26:AF26"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="I27:M27"/>
-    <mergeCell ref="N27:P27"/>
-    <mergeCell ref="Q27:S27"/>
-    <mergeCell ref="T27:X27"/>
-    <mergeCell ref="Y27:AC27"/>
-    <mergeCell ref="AD27:AF27"/>
-    <mergeCell ref="A26:H26"/>
-    <mergeCell ref="I26:M26"/>
-    <mergeCell ref="N26:P26"/>
-    <mergeCell ref="Q26:S26"/>
-    <mergeCell ref="T26:X26"/>
-    <mergeCell ref="Y28:AC28"/>
-    <mergeCell ref="AD28:AF28"/>
-    <mergeCell ref="A29:H29"/>
-    <mergeCell ref="I29:M29"/>
-    <mergeCell ref="N29:P29"/>
-    <mergeCell ref="Q29:S29"/>
-    <mergeCell ref="T29:X29"/>
-    <mergeCell ref="Y29:AC29"/>
-    <mergeCell ref="AD29:AF29"/>
-    <mergeCell ref="A28:H28"/>
-    <mergeCell ref="I28:M28"/>
-    <mergeCell ref="N28:P28"/>
-    <mergeCell ref="Q28:S28"/>
-    <mergeCell ref="T28:X28"/>
-    <mergeCell ref="BU24:CB24"/>
-    <mergeCell ref="CC24:CJ24"/>
-    <mergeCell ref="CK24:CR24"/>
-    <mergeCell ref="AG26:AN26"/>
-    <mergeCell ref="AO26:AV26"/>
-    <mergeCell ref="AW26:BD26"/>
-    <mergeCell ref="BE26:BL26"/>
-    <mergeCell ref="BM26:BT26"/>
-    <mergeCell ref="BU26:CB26"/>
-    <mergeCell ref="CC26:CJ26"/>
-    <mergeCell ref="CK26:CR26"/>
-    <mergeCell ref="AG24:AN24"/>
-    <mergeCell ref="AO24:AV24"/>
-    <mergeCell ref="AW24:BD24"/>
-    <mergeCell ref="BE24:BL24"/>
-    <mergeCell ref="BM24:BT24"/>
-    <mergeCell ref="BK28:BP28"/>
-    <mergeCell ref="BQ28:BV28"/>
-    <mergeCell ref="BW28:CB28"/>
-    <mergeCell ref="CC28:CH28"/>
-    <mergeCell ref="CI28:CN28"/>
-    <mergeCell ref="AG28:AL28"/>
-    <mergeCell ref="AM28:AR28"/>
-    <mergeCell ref="AS28:AX28"/>
-    <mergeCell ref="AY28:BD28"/>
-    <mergeCell ref="BE28:BJ28"/>
-    <mergeCell ref="BK29:BP29"/>
-    <mergeCell ref="BQ29:BV29"/>
-    <mergeCell ref="BW29:CB29"/>
-    <mergeCell ref="CC29:CH29"/>
-    <mergeCell ref="CI29:CN29"/>
-    <mergeCell ref="AG29:AL29"/>
-    <mergeCell ref="AM29:AR29"/>
-    <mergeCell ref="AS29:AX29"/>
-    <mergeCell ref="AY29:BD29"/>
-    <mergeCell ref="BE29:BJ29"/>
-    <mergeCell ref="BK31:BP31"/>
-    <mergeCell ref="BQ31:BV31"/>
-    <mergeCell ref="BW31:CB31"/>
-    <mergeCell ref="CC31:CH31"/>
-    <mergeCell ref="CI31:CN31"/>
-    <mergeCell ref="AG31:AL31"/>
-    <mergeCell ref="AM31:AR31"/>
-    <mergeCell ref="AS31:AX31"/>
-    <mergeCell ref="AY31:BD31"/>
-    <mergeCell ref="BE31:BJ31"/>
-    <mergeCell ref="BK32:BP32"/>
-    <mergeCell ref="BQ32:BV32"/>
-    <mergeCell ref="BW32:CB32"/>
-    <mergeCell ref="CC32:CH32"/>
-    <mergeCell ref="CI32:CN32"/>
-    <mergeCell ref="AG32:AL32"/>
-    <mergeCell ref="AM32:AR32"/>
-    <mergeCell ref="AS32:AX32"/>
-    <mergeCell ref="AY32:BD32"/>
-    <mergeCell ref="BE32:BJ32"/>
+    <mergeCell ref="Q6:X6"/>
+    <mergeCell ref="Y6:AF6"/>
+    <mergeCell ref="AD9:AF9"/>
+    <mergeCell ref="AD8:AF8"/>
+    <mergeCell ref="Y9:AC9"/>
+    <mergeCell ref="Y8:AC8"/>
+    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="T8:X8"/>
+    <mergeCell ref="T9:X9"/>
+    <mergeCell ref="I11:M11"/>
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="I10:M10"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="AD10:AF10"/>
+    <mergeCell ref="Y10:AC10"/>
+    <mergeCell ref="T10:X10"/>
+    <mergeCell ref="Q10:S10"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="AD11:AF11"/>
+    <mergeCell ref="Y11:AC11"/>
+    <mergeCell ref="T11:X11"/>
+    <mergeCell ref="Q11:S11"/>
+    <mergeCell ref="N11:P11"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="I15:P15"/>
+    <mergeCell ref="Q15:X15"/>
+    <mergeCell ref="Y15:AF15"/>
+    <mergeCell ref="A14:AF14"/>
+    <mergeCell ref="Y17:AC17"/>
+    <mergeCell ref="AD17:AF17"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="I18:M18"/>
+    <mergeCell ref="N18:P18"/>
+    <mergeCell ref="Q18:S18"/>
+    <mergeCell ref="T18:X18"/>
+    <mergeCell ref="Y18:AC18"/>
+    <mergeCell ref="AD18:AF18"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="I17:M17"/>
+    <mergeCell ref="N17:P17"/>
+    <mergeCell ref="Q17:S17"/>
+    <mergeCell ref="T17:X17"/>
+    <mergeCell ref="Y19:AC19"/>
+    <mergeCell ref="AD19:AF19"/>
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="I20:M20"/>
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="Q20:S20"/>
+    <mergeCell ref="T20:X20"/>
+    <mergeCell ref="Y20:AC20"/>
+    <mergeCell ref="AD20:AF20"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="I19:M19"/>
+    <mergeCell ref="N19:P19"/>
+    <mergeCell ref="Q19:S19"/>
+    <mergeCell ref="T19:X19"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -5442,7 +5634,7 @@
       <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.88671875" style="11" customWidth="1"/>
     <col min="2" max="2" width="4.77734375" style="11" customWidth="1"/>
@@ -5456,44 +5648,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
       <c r="E1" s="11">
         <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37" t="s">
+      <c r="C3" s="38"/>
+      <c r="D3" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="K3" s="37" t="s">
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="K3" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37" t="s">
+      <c r="L3" s="38"/>
+      <c r="M3" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="N3" s="37"/>
-      <c r="O3" s="37"/>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="37"/>
-      <c r="R3" s="37"/>
+      <c r="N3" s="38"/>
+      <c r="O3" s="38"/>
+      <c r="P3" s="38"/>
+      <c r="Q3" s="38"/>
+      <c r="R3" s="38"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
       <c r="D4" s="12">
         <v>0.01</v>
       </c>
@@ -5512,8 +5704,8 @@
       <c r="I4" s="12">
         <v>10</v>
       </c>
-      <c r="K4" s="37"/>
-      <c r="L4" s="37"/>
+      <c r="K4" s="38"/>
+      <c r="L4" s="38"/>
       <c r="M4" s="12">
         <v>0.01</v>
       </c>
@@ -5534,7 +5726,7 @@
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="39" t="s">
         <v>41</v>
       </c>
       <c r="C5" s="12">
@@ -5564,7 +5756,7 @@
         <f t="shared" si="0"/>
         <v>1E-3</v>
       </c>
-      <c r="K5" s="38" t="s">
+      <c r="K5" s="39" t="s">
         <v>41</v>
       </c>
       <c r="L5" s="12">
@@ -5596,7 +5788,7 @@
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B6" s="38"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="12">
         <v>0.02</v>
       </c>
@@ -5624,7 +5816,7 @@
         <f t="shared" si="2"/>
         <v>2E-3</v>
       </c>
-      <c r="K6" s="38"/>
+      <c r="K6" s="39"/>
       <c r="L6" s="12">
         <v>0.02</v>
       </c>
@@ -5654,7 +5846,7 @@
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B7" s="38"/>
+      <c r="B7" s="39"/>
       <c r="C7" s="12">
         <v>0.03</v>
       </c>
@@ -5682,7 +5874,7 @@
         <f t="shared" si="2"/>
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="K7" s="38"/>
+      <c r="K7" s="39"/>
       <c r="L7" s="12">
         <v>0.03</v>
       </c>
@@ -5712,7 +5904,7 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B8" s="38"/>
+      <c r="B8" s="39"/>
       <c r="C8" s="12">
         <v>0.05</v>
       </c>
@@ -5740,7 +5932,7 @@
         <f t="shared" si="2"/>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="K8" s="38"/>
+      <c r="K8" s="39"/>
       <c r="L8" s="12">
         <v>0.05</v>
       </c>
@@ -5770,7 +5962,7 @@
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B9" s="38"/>
+      <c r="B9" s="39"/>
       <c r="C9" s="12">
         <v>0.1</v>
       </c>
@@ -5798,7 +5990,7 @@
         <f t="shared" si="2"/>
         <v>0.01</v>
       </c>
-      <c r="K9" s="38"/>
+      <c r="K9" s="39"/>
       <c r="L9" s="12">
         <v>0.1</v>
       </c>
@@ -5828,7 +6020,7 @@
       </c>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B10" s="38"/>
+      <c r="B10" s="39"/>
       <c r="C10" s="12">
         <v>0.2</v>
       </c>
@@ -5856,7 +6048,7 @@
         <f t="shared" si="2"/>
         <v>0.02</v>
       </c>
-      <c r="K10" s="38"/>
+      <c r="K10" s="39"/>
       <c r="L10" s="12">
         <v>0.2</v>
       </c>
@@ -5886,7 +6078,7 @@
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B11" s="38"/>
+      <c r="B11" s="39"/>
       <c r="C11" s="12">
         <v>0.3</v>
       </c>
@@ -5914,7 +6106,7 @@
         <f t="shared" si="2"/>
         <v>0.03</v>
       </c>
-      <c r="K11" s="38"/>
+      <c r="K11" s="39"/>
       <c r="L11" s="12">
         <v>0.3</v>
       </c>
@@ -5944,7 +6136,7 @@
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B12" s="38"/>
+      <c r="B12" s="39"/>
       <c r="C12" s="12">
         <v>0.5</v>
       </c>
@@ -5972,7 +6164,7 @@
         <f t="shared" si="2"/>
         <v>0.05</v>
       </c>
-      <c r="K12" s="38"/>
+      <c r="K12" s="39"/>
       <c r="L12" s="12">
         <v>0.5</v>
       </c>
@@ -6002,7 +6194,7 @@
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B13" s="38"/>
+      <c r="B13" s="39"/>
       <c r="C13" s="12">
         <v>1</v>
       </c>
@@ -6030,7 +6222,7 @@
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="K13" s="38"/>
+      <c r="K13" s="39"/>
       <c r="L13" s="12">
         <v>1</v>
       </c>
@@ -6087,7 +6279,7 @@
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -6204,30 +6396,30 @@
       <selection activeCell="I6" sqref="I6:S11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="19" width="4.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
       <c r="Q1" s="7"/>
       <c r="R1" s="7"/>
       <c r="S1" s="7"/>
@@ -6363,21 +6555,21 @@
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
-      <c r="I6" s="26" t="s">
+      <c r="I6" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="26"/>
-      <c r="M6" s="26"/>
-      <c r="N6" s="26"/>
-      <c r="O6" s="26"/>
-      <c r="P6" s="26"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="27"/>
+      <c r="P6" s="27"/>
       <c r="Q6" s="7"/>
-      <c r="R6" s="23" t="s">
+      <c r="R6" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="S6" s="23"/>
+      <c r="S6" s="22"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
@@ -6415,10 +6607,10 @@
       <c r="Q7" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="R7" s="39" t="s">
+      <c r="R7" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="S7" s="39"/>
+      <c r="S7" s="40"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
@@ -6429,18 +6621,18 @@
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
-      <c r="I8" s="23" t="s">
+      <c r="I8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23" t="s">
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="O8" s="23"/>
-      <c r="P8" s="23"/>
+      <c r="O8" s="22"/>
+      <c r="P8" s="22"/>
       <c r="Q8" s="7"/>
       <c r="R8" s="7"/>
       <c r="S8" s="7"/>
@@ -6454,18 +6646,18 @@
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
-      <c r="I9" s="23">
+      <c r="I9" s="22">
         <v>17</v>
       </c>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23">
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22">
         <v>4</v>
       </c>
-      <c r="O9" s="23"/>
-      <c r="P9" s="23"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="22"/>
       <c r="Q9" s="7"/>
       <c r="R9" s="7"/>
       <c r="S9" s="7"/>
@@ -6484,11 +6676,11 @@
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
-      <c r="N10" s="23" t="s">
+      <c r="N10" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="O10" s="23"/>
-      <c r="P10" s="23"/>
+      <c r="O10" s="22"/>
+      <c r="P10" s="22"/>
       <c r="Q10" s="7"/>
       <c r="R10" s="7"/>
       <c r="S10" s="7"/>
@@ -6507,18 +6699,24 @@
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
-      <c r="N11" s="24">
+      <c r="N11" s="23">
         <f>100/(2^3-1)*N9</f>
         <v>57.142857142857146</v>
       </c>
-      <c r="O11" s="24"/>
-      <c r="P11" s="24"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="23"/>
       <c r="Q11" s="7"/>
       <c r="R11" s="7"/>
       <c r="S11" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="I3:M3"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="I6:P6"/>
     <mergeCell ref="N11:P11"/>
     <mergeCell ref="R7:S7"/>
     <mergeCell ref="I8:M8"/>
@@ -6526,12 +6724,6 @@
     <mergeCell ref="I9:M9"/>
     <mergeCell ref="N9:P9"/>
     <mergeCell ref="N10:P10"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="I3:M3"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="I6:P6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
commit id to sw version table added
</commit_message>
<xml_diff>
--- a/hardware/BikeCounterPro/src/dataPackage/DataPackage.xlsx
+++ b/hardware/BikeCounterPro/src/dataPackage/DataPackage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meier\Documents\repos\lora\hardware\BikeCounterPro\src\dataPackage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8209FCCC-4B59-4353-B97A-78EA8ADF4FC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D74723B-8CD5-43C3-9D0B-D7ECD2544136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41172" yWindow="-108" windowWidth="41496" windowHeight="16896" xr2:uid="{CDF7A0A5-12B1-43F1-AFDE-54CA91221B4B}"/>
+    <workbookView xWindow="44256" yWindow="1200" windowWidth="30960" windowHeight="12264" xr2:uid="{CDF7A0A5-12B1-43F1-AFDE-54CA91221B4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Data package" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="97">
   <si>
     <t>minutes of day</t>
   </si>
@@ -326,6 +326,9 @@
   </si>
   <si>
     <t>Commit:</t>
+  </si>
+  <si>
+    <t>1a98971a35dd68bf7641df746ac4e55f17cc98be [1a98971]</t>
   </si>
 </sst>
 </file>
@@ -583,21 +586,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -626,9 +632,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2089,7 +2092,7 @@
   <dimension ref="A1:S83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2221,6 +2224,9 @@
       <c r="B13" s="4">
         <f>B23-B11</f>
         <v>393</v>
+      </c>
+      <c r="D13" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
@@ -2932,46 +2938,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="28" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="28" t="s">
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="R1" s="29"/>
-      <c r="S1" s="29"/>
-      <c r="T1" s="29"/>
-      <c r="U1" s="29"/>
-      <c r="V1" s="29"/>
-      <c r="W1" s="29"/>
-      <c r="X1" s="30"/>
-      <c r="Y1" s="28" t="s">
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
+      <c r="W1" s="30"/>
+      <c r="X1" s="31"/>
+      <c r="Y1" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="Z1" s="29"/>
-      <c r="AA1" s="29"/>
-      <c r="AB1" s="29"/>
-      <c r="AC1" s="29"/>
-      <c r="AD1" s="29"/>
-      <c r="AE1" s="29"/>
-      <c r="AF1" s="30"/>
+      <c r="Z1" s="30"/>
+      <c r="AA1" s="30"/>
+      <c r="AB1" s="30"/>
+      <c r="AC1" s="30"/>
+      <c r="AD1" s="30"/>
+      <c r="AE1" s="30"/>
+      <c r="AF1" s="31"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
@@ -3072,52 +3078,52 @@
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="34" t="s">
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="34" t="s">
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
+      <c r="M3" s="36"/>
+      <c r="N3" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="O3" s="35"/>
-      <c r="P3" s="36"/>
-      <c r="Q3" s="34" t="s">
+      <c r="O3" s="36"/>
+      <c r="P3" s="37"/>
+      <c r="Q3" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="R3" s="35"/>
-      <c r="S3" s="36"/>
-      <c r="T3" s="31" t="s">
+      <c r="R3" s="36"/>
+      <c r="S3" s="37"/>
+      <c r="T3" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="U3" s="32"/>
-      <c r="V3" s="32"/>
-      <c r="W3" s="32"/>
-      <c r="X3" s="33"/>
-      <c r="Y3" s="31" t="s">
+      <c r="U3" s="33"/>
+      <c r="V3" s="33"/>
+      <c r="W3" s="33"/>
+      <c r="X3" s="34"/>
+      <c r="Y3" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="Z3" s="32"/>
-      <c r="AA3" s="32"/>
-      <c r="AB3" s="32"/>
-      <c r="AC3" s="33"/>
-      <c r="AD3" s="31" t="s">
+      <c r="Z3" s="33"/>
+      <c r="AA3" s="33"/>
+      <c r="AB3" s="33"/>
+      <c r="AC3" s="34"/>
+      <c r="AD3" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="AE3" s="32"/>
-      <c r="AF3" s="33"/>
+      <c r="AE3" s="33"/>
+      <c r="AF3" s="34"/>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" s="11"/>
@@ -3177,46 +3183,46 @@
       <c r="AF5" s="27"/>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26">
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28">
         <v>38</v>
       </c>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="26"/>
-      <c r="M6" s="26"/>
-      <c r="N6" s="26"/>
-      <c r="O6" s="26"/>
-      <c r="P6" s="26"/>
-      <c r="Q6" s="26">
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28"/>
+      <c r="O6" s="28"/>
+      <c r="P6" s="28"/>
+      <c r="Q6" s="28">
         <v>73</v>
       </c>
-      <c r="R6" s="26"/>
-      <c r="S6" s="26"/>
-      <c r="T6" s="26"/>
-      <c r="U6" s="26"/>
-      <c r="V6" s="26"/>
-      <c r="W6" s="26"/>
-      <c r="X6" s="26"/>
-      <c r="Y6" s="26">
+      <c r="R6" s="28"/>
+      <c r="S6" s="28"/>
+      <c r="T6" s="28"/>
+      <c r="U6" s="28"/>
+      <c r="V6" s="28"/>
+      <c r="W6" s="28"/>
+      <c r="X6" s="28"/>
+      <c r="Y6" s="28">
         <v>88</v>
       </c>
-      <c r="Z6" s="26"/>
-      <c r="AA6" s="26"/>
-      <c r="AB6" s="26"/>
-      <c r="AC6" s="26"/>
-      <c r="AD6" s="26"/>
-      <c r="AE6" s="26"/>
-      <c r="AF6" s="26"/>
+      <c r="Z6" s="28"/>
+      <c r="AA6" s="28"/>
+      <c r="AB6" s="28"/>
+      <c r="AC6" s="28"/>
+      <c r="AD6" s="28"/>
+      <c r="AE6" s="28"/>
+      <c r="AF6" s="28"/>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A7" s="16">
@@ -3317,203 +3323,203 @@
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22" t="s">
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="22" t="s">
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="O8" s="22"/>
-      <c r="P8" s="22"/>
-      <c r="Q8" s="22" t="s">
+      <c r="O8" s="24"/>
+      <c r="P8" s="24"/>
+      <c r="Q8" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="R8" s="22"/>
-      <c r="S8" s="22"/>
-      <c r="T8" s="22" t="s">
+      <c r="R8" s="24"/>
+      <c r="S8" s="24"/>
+      <c r="T8" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="U8" s="22"/>
-      <c r="V8" s="22"/>
-      <c r="W8" s="22"/>
-      <c r="X8" s="22"/>
-      <c r="Y8" s="22" t="s">
+      <c r="U8" s="24"/>
+      <c r="V8" s="24"/>
+      <c r="W8" s="24"/>
+      <c r="X8" s="24"/>
+      <c r="Y8" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="Z8" s="22"/>
-      <c r="AA8" s="22"/>
-      <c r="AB8" s="22"/>
-      <c r="AC8" s="22"/>
-      <c r="AD8" s="22" t="s">
+      <c r="Z8" s="24"/>
+      <c r="AA8" s="24"/>
+      <c r="AB8" s="24"/>
+      <c r="AC8" s="24"/>
+      <c r="AD8" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="AE8" s="22"/>
-      <c r="AF8" s="22"/>
+      <c r="AE8" s="24"/>
+      <c r="AF8" s="24"/>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A9" s="22">
+      <c r="A9" s="24">
         <v>10</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22">
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24">
         <v>7</v>
       </c>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="22">
-        <v>0</v>
-      </c>
-      <c r="O9" s="22"/>
-      <c r="P9" s="22"/>
-      <c r="Q9" s="22">
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24">
+        <v>0</v>
+      </c>
+      <c r="O9" s="24"/>
+      <c r="P9" s="24"/>
+      <c r="Q9" s="24">
         <v>3</v>
       </c>
-      <c r="R9" s="22"/>
-      <c r="S9" s="22"/>
-      <c r="T9" s="22">
+      <c r="R9" s="24"/>
+      <c r="S9" s="24"/>
+      <c r="T9" s="24">
         <v>19</v>
       </c>
-      <c r="U9" s="22"/>
-      <c r="V9" s="22"/>
-      <c r="W9" s="22"/>
-      <c r="X9" s="22"/>
-      <c r="Y9" s="22">
+      <c r="U9" s="24"/>
+      <c r="V9" s="24"/>
+      <c r="W9" s="24"/>
+      <c r="X9" s="24"/>
+      <c r="Y9" s="24">
         <v>17</v>
       </c>
-      <c r="Z9" s="22"/>
-      <c r="AA9" s="22"/>
-      <c r="AB9" s="22"/>
-      <c r="AC9" s="22"/>
-      <c r="AD9" s="22">
-        <v>0</v>
-      </c>
-      <c r="AE9" s="22"/>
-      <c r="AF9" s="22"/>
+      <c r="Z9" s="24"/>
+      <c r="AA9" s="24"/>
+      <c r="AB9" s="24"/>
+      <c r="AC9" s="24"/>
+      <c r="AD9" s="24">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="24"/>
+      <c r="AF9" s="24"/>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22" t="s">
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="22" t="s">
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="O10" s="22"/>
-      <c r="P10" s="22"/>
-      <c r="Q10" s="22" t="s">
+      <c r="O10" s="24"/>
+      <c r="P10" s="24"/>
+      <c r="Q10" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="R10" s="22"/>
-      <c r="S10" s="22"/>
-      <c r="T10" s="22" t="s">
+      <c r="R10" s="24"/>
+      <c r="S10" s="24"/>
+      <c r="T10" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="U10" s="22"/>
-      <c r="V10" s="22"/>
-      <c r="W10" s="22"/>
-      <c r="X10" s="22"/>
-      <c r="Y10" s="22" t="s">
+      <c r="U10" s="24"/>
+      <c r="V10" s="24"/>
+      <c r="W10" s="24"/>
+      <c r="X10" s="24"/>
+      <c r="Y10" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="Z10" s="22"/>
-      <c r="AA10" s="22"/>
-      <c r="AB10" s="22"/>
-      <c r="AC10" s="22"/>
-      <c r="AD10" s="22" t="s">
+      <c r="Z10" s="24"/>
+      <c r="AA10" s="24"/>
+      <c r="AB10" s="24"/>
+      <c r="AC10" s="24"/>
+      <c r="AD10" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="AE10" s="22"/>
-      <c r="AF10" s="22"/>
+      <c r="AE10" s="24"/>
+      <c r="AF10" s="24"/>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A11" s="22">
+      <c r="A11" s="24">
         <f>A9</f>
         <v>10</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="23">
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="25">
         <f>'Data package'!$B$31*I9+'Data package'!$B$28</f>
         <v>3.338709677419355</v>
       </c>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="24">
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="22">
         <f ca="1">LOOKUP(N9,'Data package'!$D$21:$D$24,'Data package'!$E$22:$E$31)</f>
         <v>0</v>
       </c>
-      <c r="O11" s="24"/>
-      <c r="P11" s="24"/>
-      <c r="Q11" s="25">
+      <c r="O11" s="22"/>
+      <c r="P11" s="22"/>
+      <c r="Q11" s="26">
         <f>100/(2^3-1)*Q9</f>
         <v>42.857142857142861</v>
       </c>
-      <c r="R11" s="25"/>
-      <c r="S11" s="25"/>
-      <c r="T11" s="25">
+      <c r="R11" s="26"/>
+      <c r="S11" s="26"/>
+      <c r="T11" s="26">
         <f>'Data package'!$B$40*T9+'Data package'!$B$37</f>
         <v>22.903225806451616</v>
       </c>
-      <c r="U11" s="24"/>
-      <c r="V11" s="24"/>
-      <c r="W11" s="24"/>
-      <c r="X11" s="24"/>
-      <c r="Y11" s="24">
+      <c r="U11" s="22"/>
+      <c r="V11" s="22"/>
+      <c r="W11" s="22"/>
+      <c r="X11" s="22"/>
+      <c r="Y11" s="22">
         <f>Y9</f>
         <v>17</v>
       </c>
-      <c r="Z11" s="24"/>
-      <c r="AA11" s="24"/>
-      <c r="AB11" s="24"/>
-      <c r="AC11" s="24"/>
-      <c r="AD11" s="24">
+      <c r="Z11" s="22"/>
+      <c r="AA11" s="22"/>
+      <c r="AB11" s="22"/>
+      <c r="AC11" s="22"/>
+      <c r="AD11" s="22">
         <f>LOOKUP(AD9,'Data package'!$A$77:$A$81,'Data package'!$B$77:$B$81)</f>
         <v>1</v>
       </c>
-      <c r="AE11" s="24"/>
-      <c r="AF11" s="24"/>
+      <c r="AE11" s="22"/>
+      <c r="AF11" s="22"/>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
@@ -3565,46 +3571,46 @@
       <c r="AF14" s="27"/>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26" t="s">
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="J15" s="26"/>
-      <c r="K15" s="26"/>
-      <c r="L15" s="26"/>
-      <c r="M15" s="26"/>
-      <c r="N15" s="26"/>
-      <c r="O15" s="26"/>
-      <c r="P15" s="26"/>
-      <c r="Q15" s="26" t="s">
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="28"/>
+      <c r="P15" s="28"/>
+      <c r="Q15" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="R15" s="26"/>
-      <c r="S15" s="26"/>
-      <c r="T15" s="26"/>
-      <c r="U15" s="26"/>
-      <c r="V15" s="26"/>
-      <c r="W15" s="26"/>
-      <c r="X15" s="26"/>
-      <c r="Y15" s="26" t="s">
+      <c r="R15" s="28"/>
+      <c r="S15" s="28"/>
+      <c r="T15" s="28"/>
+      <c r="U15" s="28"/>
+      <c r="V15" s="28"/>
+      <c r="W15" s="28"/>
+      <c r="X15" s="28"/>
+      <c r="Y15" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="Z15" s="26"/>
-      <c r="AA15" s="26"/>
-      <c r="AB15" s="26"/>
-      <c r="AC15" s="26"/>
-      <c r="AD15" s="26"/>
-      <c r="AE15" s="26"/>
-      <c r="AF15" s="26"/>
+      <c r="Z15" s="28"/>
+      <c r="AA15" s="28"/>
+      <c r="AB15" s="28"/>
+      <c r="AC15" s="28"/>
+      <c r="AD15" s="28"/>
+      <c r="AE15" s="28"/>
+      <c r="AF15" s="28"/>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16" s="16">
@@ -3705,203 +3711,203 @@
       </c>
     </row>
     <row r="17" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22" t="s">
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="J17" s="22"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="22"/>
-      <c r="M17" s="22"/>
-      <c r="N17" s="22" t="s">
+      <c r="J17" s="24"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="24"/>
+      <c r="M17" s="24"/>
+      <c r="N17" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="O17" s="22"/>
-      <c r="P17" s="22"/>
-      <c r="Q17" s="22" t="s">
+      <c r="O17" s="24"/>
+      <c r="P17" s="24"/>
+      <c r="Q17" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="R17" s="22"/>
-      <c r="S17" s="22"/>
-      <c r="T17" s="22" t="s">
+      <c r="R17" s="24"/>
+      <c r="S17" s="24"/>
+      <c r="T17" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="U17" s="22"/>
-      <c r="V17" s="22"/>
-      <c r="W17" s="22"/>
-      <c r="X17" s="22"/>
-      <c r="Y17" s="22" t="s">
+      <c r="U17" s="24"/>
+      <c r="V17" s="24"/>
+      <c r="W17" s="24"/>
+      <c r="X17" s="24"/>
+      <c r="Y17" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="Z17" s="22"/>
-      <c r="AA17" s="22"/>
-      <c r="AB17" s="22"/>
-      <c r="AC17" s="22"/>
-      <c r="AD17" s="22" t="s">
+      <c r="Z17" s="24"/>
+      <c r="AA17" s="24"/>
+      <c r="AB17" s="24"/>
+      <c r="AC17" s="24"/>
+      <c r="AD17" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="AE17" s="22"/>
-      <c r="AF17" s="22"/>
+      <c r="AE17" s="24"/>
+      <c r="AF17" s="24"/>
     </row>
     <row r="18" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A18" s="22">
+      <c r="A18" s="24">
         <v>5</v>
       </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22">
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24">
         <v>8</v>
       </c>
-      <c r="J18" s="22"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="22"/>
-      <c r="N18" s="22">
-        <v>0</v>
-      </c>
-      <c r="O18" s="22"/>
-      <c r="P18" s="22"/>
-      <c r="Q18" s="22">
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="24"/>
+      <c r="N18" s="24">
+        <v>0</v>
+      </c>
+      <c r="O18" s="24"/>
+      <c r="P18" s="24"/>
+      <c r="Q18" s="24">
         <v>3</v>
       </c>
-      <c r="R18" s="22"/>
-      <c r="S18" s="22"/>
-      <c r="T18" s="22">
+      <c r="R18" s="24"/>
+      <c r="S18" s="24"/>
+      <c r="T18" s="24">
         <v>19</v>
       </c>
-      <c r="U18" s="22"/>
-      <c r="V18" s="22"/>
-      <c r="W18" s="22"/>
-      <c r="X18" s="22"/>
-      <c r="Y18" s="22">
+      <c r="U18" s="24"/>
+      <c r="V18" s="24"/>
+      <c r="W18" s="24"/>
+      <c r="X18" s="24"/>
+      <c r="Y18" s="24">
         <v>17</v>
       </c>
-      <c r="Z18" s="22"/>
-      <c r="AA18" s="22"/>
-      <c r="AB18" s="22"/>
-      <c r="AC18" s="22"/>
-      <c r="AD18" s="22">
-        <v>0</v>
-      </c>
-      <c r="AE18" s="22"/>
-      <c r="AF18" s="22"/>
+      <c r="Z18" s="24"/>
+      <c r="AA18" s="24"/>
+      <c r="AB18" s="24"/>
+      <c r="AC18" s="24"/>
+      <c r="AD18" s="24">
+        <v>0</v>
+      </c>
+      <c r="AE18" s="24"/>
+      <c r="AF18" s="24"/>
     </row>
     <row r="19" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22" t="s">
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="J19" s="22"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="22"/>
-      <c r="M19" s="22"/>
-      <c r="N19" s="22" t="s">
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="24"/>
+      <c r="M19" s="24"/>
+      <c r="N19" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="O19" s="22"/>
-      <c r="P19" s="22"/>
-      <c r="Q19" s="22" t="s">
+      <c r="O19" s="24"/>
+      <c r="P19" s="24"/>
+      <c r="Q19" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="R19" s="22"/>
-      <c r="S19" s="22"/>
-      <c r="T19" s="22" t="s">
+      <c r="R19" s="24"/>
+      <c r="S19" s="24"/>
+      <c r="T19" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="U19" s="22"/>
-      <c r="V19" s="22"/>
-      <c r="W19" s="22"/>
-      <c r="X19" s="22"/>
-      <c r="Y19" s="22" t="s">
+      <c r="U19" s="24"/>
+      <c r="V19" s="24"/>
+      <c r="W19" s="24"/>
+      <c r="X19" s="24"/>
+      <c r="Y19" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="Z19" s="22"/>
-      <c r="AA19" s="22"/>
-      <c r="AB19" s="22"/>
-      <c r="AC19" s="22"/>
-      <c r="AD19" s="22" t="s">
+      <c r="Z19" s="24"/>
+      <c r="AA19" s="24"/>
+      <c r="AB19" s="24"/>
+      <c r="AC19" s="24"/>
+      <c r="AD19" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="AE19" s="22"/>
-      <c r="AF19" s="22"/>
+      <c r="AE19" s="24"/>
+      <c r="AF19" s="24"/>
     </row>
     <row r="20" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A20" s="22">
+      <c r="A20" s="24">
         <f>A18</f>
         <v>5</v>
       </c>
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="23">
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="25">
         <f>'Data package'!$B$31*I18+'Data package'!$B$28</f>
         <v>3.3870967741935485</v>
       </c>
-      <c r="J20" s="23"/>
-      <c r="K20" s="23"/>
-      <c r="L20" s="23"/>
-      <c r="M20" s="23"/>
-      <c r="N20" s="24">
+      <c r="J20" s="25"/>
+      <c r="K20" s="25"/>
+      <c r="L20" s="25"/>
+      <c r="M20" s="25"/>
+      <c r="N20" s="22">
         <f ca="1">LOOKUP(N18,'Data package'!$D$21:$D$24,'Data package'!$E$22:$E$31)</f>
         <v>0</v>
       </c>
-      <c r="O20" s="24"/>
-      <c r="P20" s="24"/>
-      <c r="Q20" s="25">
+      <c r="O20" s="22"/>
+      <c r="P20" s="22"/>
+      <c r="Q20" s="26">
         <f>100/(2^3-1)*Q18</f>
         <v>42.857142857142861</v>
       </c>
-      <c r="R20" s="25"/>
-      <c r="S20" s="25"/>
-      <c r="T20" s="25">
+      <c r="R20" s="26"/>
+      <c r="S20" s="26"/>
+      <c r="T20" s="26">
         <f>'Data package'!$B$40*T18+'Data package'!$B$37</f>
         <v>22.903225806451616</v>
       </c>
-      <c r="U20" s="24"/>
-      <c r="V20" s="24"/>
-      <c r="W20" s="24"/>
-      <c r="X20" s="24"/>
-      <c r="Y20" s="24">
+      <c r="U20" s="22"/>
+      <c r="V20" s="22"/>
+      <c r="W20" s="22"/>
+      <c r="X20" s="22"/>
+      <c r="Y20" s="22">
         <f>Y18</f>
         <v>17</v>
       </c>
-      <c r="Z20" s="24"/>
-      <c r="AA20" s="24"/>
-      <c r="AB20" s="24"/>
-      <c r="AC20" s="24"/>
-      <c r="AD20" s="24">
+      <c r="Z20" s="22"/>
+      <c r="AA20" s="22"/>
+      <c r="AB20" s="22"/>
+      <c r="AC20" s="22"/>
+      <c r="AD20" s="22">
         <f>LOOKUP(AD18,'Data package'!$A$77:$A$81,'Data package'!$B$77:$B$81)</f>
         <v>1</v>
       </c>
-      <c r="AE20" s="24"/>
-      <c r="AF20" s="24"/>
+      <c r="AE20" s="22"/>
+      <c r="AF20" s="22"/>
     </row>
     <row r="23" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A23" s="27" t="s">
@@ -3940,126 +3946,126 @@
       <c r="AF23" s="27"/>
     </row>
     <row r="24" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A24" s="26" t="s">
+      <c r="A24" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26" t="s">
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="J24" s="26"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="26"/>
-      <c r="M24" s="26"/>
-      <c r="N24" s="26"/>
-      <c r="O24" s="26"/>
-      <c r="P24" s="26"/>
-      <c r="Q24" s="26" t="s">
+      <c r="J24" s="28"/>
+      <c r="K24" s="28"/>
+      <c r="L24" s="28"/>
+      <c r="M24" s="28"/>
+      <c r="N24" s="28"/>
+      <c r="O24" s="28"/>
+      <c r="P24" s="28"/>
+      <c r="Q24" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="R24" s="26"/>
-      <c r="S24" s="26"/>
-      <c r="T24" s="26"/>
-      <c r="U24" s="26"/>
-      <c r="V24" s="26"/>
-      <c r="W24" s="26"/>
-      <c r="X24" s="26"/>
-      <c r="Y24" s="26" t="s">
+      <c r="R24" s="28"/>
+      <c r="S24" s="28"/>
+      <c r="T24" s="28"/>
+      <c r="U24" s="28"/>
+      <c r="V24" s="28"/>
+      <c r="W24" s="28"/>
+      <c r="X24" s="28"/>
+      <c r="Y24" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="Z24" s="26"/>
-      <c r="AA24" s="26"/>
-      <c r="AB24" s="26"/>
-      <c r="AC24" s="26"/>
-      <c r="AD24" s="26"/>
-      <c r="AE24" s="26"/>
-      <c r="AF24" s="26"/>
-      <c r="AG24" s="37">
+      <c r="Z24" s="28"/>
+      <c r="AA24" s="28"/>
+      <c r="AB24" s="28"/>
+      <c r="AC24" s="28"/>
+      <c r="AD24" s="28"/>
+      <c r="AE24" s="28"/>
+      <c r="AF24" s="28"/>
+      <c r="AG24" s="23">
         <v>59</v>
       </c>
-      <c r="AH24" s="37"/>
-      <c r="AI24" s="37"/>
-      <c r="AJ24" s="37"/>
-      <c r="AK24" s="37"/>
-      <c r="AL24" s="37"/>
-      <c r="AM24" s="37"/>
-      <c r="AN24" s="37"/>
-      <c r="AO24" s="37">
+      <c r="AH24" s="23"/>
+      <c r="AI24" s="23"/>
+      <c r="AJ24" s="23"/>
+      <c r="AK24" s="23"/>
+      <c r="AL24" s="23"/>
+      <c r="AM24" s="23"/>
+      <c r="AN24" s="23"/>
+      <c r="AO24" s="23">
         <v>96</v>
       </c>
-      <c r="AP24" s="37"/>
-      <c r="AQ24" s="37"/>
-      <c r="AR24" s="37"/>
-      <c r="AS24" s="37"/>
-      <c r="AT24" s="37"/>
-      <c r="AU24" s="37"/>
-      <c r="AV24" s="37"/>
-      <c r="AW24" s="37">
+      <c r="AP24" s="23"/>
+      <c r="AQ24" s="23"/>
+      <c r="AR24" s="23"/>
+      <c r="AS24" s="23"/>
+      <c r="AT24" s="23"/>
+      <c r="AU24" s="23"/>
+      <c r="AV24" s="23"/>
+      <c r="AW24" s="23">
         <v>65</v>
       </c>
-      <c r="AX24" s="37"/>
-      <c r="AY24" s="37"/>
-      <c r="AZ24" s="37"/>
-      <c r="BA24" s="37"/>
-      <c r="BB24" s="37"/>
-      <c r="BC24" s="37"/>
-      <c r="BD24" s="37"/>
-      <c r="BE24" s="37" t="s">
+      <c r="AX24" s="23"/>
+      <c r="AY24" s="23"/>
+      <c r="AZ24" s="23"/>
+      <c r="BA24" s="23"/>
+      <c r="BB24" s="23"/>
+      <c r="BC24" s="23"/>
+      <c r="BD24" s="23"/>
+      <c r="BE24" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="BF24" s="37"/>
-      <c r="BG24" s="37"/>
-      <c r="BH24" s="37"/>
-      <c r="BI24" s="37"/>
-      <c r="BJ24" s="37"/>
-      <c r="BK24" s="37"/>
-      <c r="BL24" s="37"/>
-      <c r="BM24" s="37" t="s">
+      <c r="BF24" s="23"/>
+      <c r="BG24" s="23"/>
+      <c r="BH24" s="23"/>
+      <c r="BI24" s="23"/>
+      <c r="BJ24" s="23"/>
+      <c r="BK24" s="23"/>
+      <c r="BL24" s="23"/>
+      <c r="BM24" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="BN24" s="37"/>
-      <c r="BO24" s="37"/>
-      <c r="BP24" s="37"/>
-      <c r="BQ24" s="37"/>
-      <c r="BR24" s="37"/>
-      <c r="BS24" s="37"/>
-      <c r="BT24" s="37"/>
-      <c r="BU24" s="37">
+      <c r="BN24" s="23"/>
+      <c r="BO24" s="23"/>
+      <c r="BP24" s="23"/>
+      <c r="BQ24" s="23"/>
+      <c r="BR24" s="23"/>
+      <c r="BS24" s="23"/>
+      <c r="BT24" s="23"/>
+      <c r="BU24" s="23">
         <v>69</v>
       </c>
-      <c r="BV24" s="37"/>
-      <c r="BW24" s="37"/>
-      <c r="BX24" s="37"/>
-      <c r="BY24" s="37"/>
-      <c r="BZ24" s="37"/>
-      <c r="CA24" s="37"/>
-      <c r="CB24" s="37"/>
-      <c r="CC24" s="37" t="s">
+      <c r="BV24" s="23"/>
+      <c r="BW24" s="23"/>
+      <c r="BX24" s="23"/>
+      <c r="BY24" s="23"/>
+      <c r="BZ24" s="23"/>
+      <c r="CA24" s="23"/>
+      <c r="CB24" s="23"/>
+      <c r="CC24" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="CD24" s="37"/>
-      <c r="CE24" s="37"/>
-      <c r="CF24" s="37"/>
-      <c r="CG24" s="37"/>
-      <c r="CH24" s="37"/>
-      <c r="CI24" s="37"/>
-      <c r="CJ24" s="37"/>
-      <c r="CK24" s="37" t="s">
+      <c r="CD24" s="23"/>
+      <c r="CE24" s="23"/>
+      <c r="CF24" s="23"/>
+      <c r="CG24" s="23"/>
+      <c r="CH24" s="23"/>
+      <c r="CI24" s="23"/>
+      <c r="CJ24" s="23"/>
+      <c r="CK24" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="CL24" s="37"/>
-      <c r="CM24" s="37"/>
-      <c r="CN24" s="37"/>
-      <c r="CO24" s="37"/>
-      <c r="CP24" s="37"/>
-      <c r="CQ24" s="37"/>
-      <c r="CR24" s="37"/>
+      <c r="CL24" s="23"/>
+      <c r="CM24" s="23"/>
+      <c r="CN24" s="23"/>
+      <c r="CO24" s="23"/>
+      <c r="CP24" s="23"/>
+      <c r="CQ24" s="23"/>
+      <c r="CR24" s="23"/>
     </row>
     <row r="25" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A25" s="18">
@@ -4352,180 +4358,180 @@
       </c>
     </row>
     <row r="26" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22" t="s">
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="J26" s="22"/>
-      <c r="K26" s="22"/>
-      <c r="L26" s="22"/>
-      <c r="M26" s="22"/>
-      <c r="N26" s="22" t="s">
+      <c r="J26" s="24"/>
+      <c r="K26" s="24"/>
+      <c r="L26" s="24"/>
+      <c r="M26" s="24"/>
+      <c r="N26" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="O26" s="22"/>
-      <c r="P26" s="22"/>
-      <c r="Q26" s="22" t="s">
+      <c r="O26" s="24"/>
+      <c r="P26" s="24"/>
+      <c r="Q26" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="R26" s="22"/>
-      <c r="S26" s="22"/>
-      <c r="T26" s="22" t="s">
+      <c r="R26" s="24"/>
+      <c r="S26" s="24"/>
+      <c r="T26" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="U26" s="22"/>
-      <c r="V26" s="22"/>
-      <c r="W26" s="22"/>
-      <c r="X26" s="22"/>
-      <c r="Y26" s="22" t="s">
+      <c r="U26" s="24"/>
+      <c r="V26" s="24"/>
+      <c r="W26" s="24"/>
+      <c r="X26" s="24"/>
+      <c r="Y26" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="Z26" s="22"/>
-      <c r="AA26" s="22"/>
-      <c r="AB26" s="22"/>
-      <c r="AC26" s="22"/>
-      <c r="AD26" s="22" t="s">
+      <c r="Z26" s="24"/>
+      <c r="AA26" s="24"/>
+      <c r="AB26" s="24"/>
+      <c r="AC26" s="24"/>
+      <c r="AD26" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="AE26" s="22"/>
-      <c r="AF26" s="22"/>
-      <c r="AG26" s="24" t="s">
+      <c r="AE26" s="24"/>
+      <c r="AF26" s="24"/>
+      <c r="AG26" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="AH26" s="24"/>
-      <c r="AI26" s="24"/>
-      <c r="AJ26" s="24"/>
-      <c r="AK26" s="24"/>
-      <c r="AL26" s="24"/>
-      <c r="AM26" s="24"/>
-      <c r="AN26" s="24"/>
-      <c r="AO26" s="24" t="s">
+      <c r="AH26" s="22"/>
+      <c r="AI26" s="22"/>
+      <c r="AJ26" s="22"/>
+      <c r="AK26" s="22"/>
+      <c r="AL26" s="22"/>
+      <c r="AM26" s="22"/>
+      <c r="AN26" s="22"/>
+      <c r="AO26" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="AP26" s="24"/>
-      <c r="AQ26" s="24"/>
-      <c r="AR26" s="24"/>
-      <c r="AS26" s="24"/>
-      <c r="AT26" s="24"/>
-      <c r="AU26" s="24"/>
-      <c r="AV26" s="24"/>
-      <c r="AW26" s="24" t="s">
+      <c r="AP26" s="22"/>
+      <c r="AQ26" s="22"/>
+      <c r="AR26" s="22"/>
+      <c r="AS26" s="22"/>
+      <c r="AT26" s="22"/>
+      <c r="AU26" s="22"/>
+      <c r="AV26" s="22"/>
+      <c r="AW26" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="AX26" s="24"/>
-      <c r="AY26" s="24"/>
-      <c r="AZ26" s="24"/>
-      <c r="BA26" s="24"/>
-      <c r="BB26" s="24"/>
-      <c r="BC26" s="24"/>
-      <c r="BD26" s="24"/>
-      <c r="BE26" s="24" t="s">
+      <c r="AX26" s="22"/>
+      <c r="AY26" s="22"/>
+      <c r="AZ26" s="22"/>
+      <c r="BA26" s="22"/>
+      <c r="BB26" s="22"/>
+      <c r="BC26" s="22"/>
+      <c r="BD26" s="22"/>
+      <c r="BE26" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="BF26" s="24"/>
-      <c r="BG26" s="24"/>
-      <c r="BH26" s="24"/>
-      <c r="BI26" s="24"/>
-      <c r="BJ26" s="24"/>
-      <c r="BK26" s="24"/>
-      <c r="BL26" s="24"/>
-      <c r="BM26" s="24" t="s">
+      <c r="BF26" s="22"/>
+      <c r="BG26" s="22"/>
+      <c r="BH26" s="22"/>
+      <c r="BI26" s="22"/>
+      <c r="BJ26" s="22"/>
+      <c r="BK26" s="22"/>
+      <c r="BL26" s="22"/>
+      <c r="BM26" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="BN26" s="24"/>
-      <c r="BO26" s="24"/>
-      <c r="BP26" s="24"/>
-      <c r="BQ26" s="24"/>
-      <c r="BR26" s="24"/>
-      <c r="BS26" s="24"/>
-      <c r="BT26" s="24"/>
-      <c r="BU26" s="24" t="s">
+      <c r="BN26" s="22"/>
+      <c r="BO26" s="22"/>
+      <c r="BP26" s="22"/>
+      <c r="BQ26" s="22"/>
+      <c r="BR26" s="22"/>
+      <c r="BS26" s="22"/>
+      <c r="BT26" s="22"/>
+      <c r="BU26" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="BV26" s="24"/>
-      <c r="BW26" s="24"/>
-      <c r="BX26" s="24"/>
-      <c r="BY26" s="24"/>
-      <c r="BZ26" s="24"/>
-      <c r="CA26" s="24"/>
-      <c r="CB26" s="24"/>
-      <c r="CC26" s="24" t="s">
+      <c r="BV26" s="22"/>
+      <c r="BW26" s="22"/>
+      <c r="BX26" s="22"/>
+      <c r="BY26" s="22"/>
+      <c r="BZ26" s="22"/>
+      <c r="CA26" s="22"/>
+      <c r="CB26" s="22"/>
+      <c r="CC26" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="CD26" s="24"/>
-      <c r="CE26" s="24"/>
-      <c r="CF26" s="24"/>
-      <c r="CG26" s="24"/>
-      <c r="CH26" s="24"/>
-      <c r="CI26" s="24"/>
-      <c r="CJ26" s="24"/>
-      <c r="CK26" s="24" t="s">
+      <c r="CD26" s="22"/>
+      <c r="CE26" s="22"/>
+      <c r="CF26" s="22"/>
+      <c r="CG26" s="22"/>
+      <c r="CH26" s="22"/>
+      <c r="CI26" s="22"/>
+      <c r="CJ26" s="22"/>
+      <c r="CK26" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="CL26" s="24"/>
-      <c r="CM26" s="24"/>
-      <c r="CN26" s="24"/>
-      <c r="CO26" s="24"/>
-      <c r="CP26" s="24"/>
-      <c r="CQ26" s="24"/>
-      <c r="CR26" s="24"/>
+      <c r="CL26" s="22"/>
+      <c r="CM26" s="22"/>
+      <c r="CN26" s="22"/>
+      <c r="CO26" s="22"/>
+      <c r="CP26" s="22"/>
+      <c r="CQ26" s="22"/>
+      <c r="CR26" s="22"/>
     </row>
     <row r="27" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A27" s="22">
+      <c r="A27" s="24">
         <v>10</v>
       </c>
-      <c r="B27" s="22"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22">
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24">
         <v>8</v>
       </c>
-      <c r="J27" s="22"/>
-      <c r="K27" s="22"/>
-      <c r="L27" s="22"/>
-      <c r="M27" s="22"/>
-      <c r="N27" s="22">
-        <v>0</v>
-      </c>
-      <c r="O27" s="22"/>
-      <c r="P27" s="22"/>
-      <c r="Q27" s="22">
+      <c r="J27" s="24"/>
+      <c r="K27" s="24"/>
+      <c r="L27" s="24"/>
+      <c r="M27" s="24"/>
+      <c r="N27" s="24">
+        <v>0</v>
+      </c>
+      <c r="O27" s="24"/>
+      <c r="P27" s="24"/>
+      <c r="Q27" s="24">
         <v>3</v>
       </c>
-      <c r="R27" s="22"/>
-      <c r="S27" s="22"/>
-      <c r="T27" s="22">
+      <c r="R27" s="24"/>
+      <c r="S27" s="24"/>
+      <c r="T27" s="24">
         <v>19</v>
       </c>
-      <c r="U27" s="22"/>
-      <c r="V27" s="22"/>
-      <c r="W27" s="22"/>
-      <c r="X27" s="22"/>
-      <c r="Y27" s="22">
+      <c r="U27" s="24"/>
+      <c r="V27" s="24"/>
+      <c r="W27" s="24"/>
+      <c r="X27" s="24"/>
+      <c r="Y27" s="24">
         <v>21</v>
       </c>
-      <c r="Z27" s="22"/>
-      <c r="AA27" s="22"/>
-      <c r="AB27" s="22"/>
-      <c r="AC27" s="22"/>
-      <c r="AD27" s="22">
-        <v>0</v>
-      </c>
-      <c r="AE27" s="22"/>
-      <c r="AF27" s="22"/>
+      <c r="Z27" s="24"/>
+      <c r="AA27" s="24"/>
+      <c r="AB27" s="24"/>
+      <c r="AC27" s="24"/>
+      <c r="AD27" s="24">
+        <v>0</v>
+      </c>
+      <c r="AE27" s="24"/>
+      <c r="AF27" s="24"/>
       <c r="AG27">
         <f>AN25</f>
         <v>1</v>
@@ -4784,267 +4790,267 @@
       </c>
     </row>
     <row r="28" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A28" s="22" t="s">
+      <c r="A28" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22" t="s">
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="J28" s="22"/>
-      <c r="K28" s="22"/>
-      <c r="L28" s="22"/>
-      <c r="M28" s="22"/>
-      <c r="N28" s="22" t="s">
+      <c r="J28" s="24"/>
+      <c r="K28" s="24"/>
+      <c r="L28" s="24"/>
+      <c r="M28" s="24"/>
+      <c r="N28" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="O28" s="22"/>
-      <c r="P28" s="22"/>
-      <c r="Q28" s="22" t="s">
+      <c r="O28" s="24"/>
+      <c r="P28" s="24"/>
+      <c r="Q28" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="R28" s="22"/>
-      <c r="S28" s="22"/>
-      <c r="T28" s="22" t="s">
+      <c r="R28" s="24"/>
+      <c r="S28" s="24"/>
+      <c r="T28" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="U28" s="22"/>
-      <c r="V28" s="22"/>
-      <c r="W28" s="22"/>
-      <c r="X28" s="22"/>
-      <c r="Y28" s="22" t="s">
+      <c r="U28" s="24"/>
+      <c r="V28" s="24"/>
+      <c r="W28" s="24"/>
+      <c r="X28" s="24"/>
+      <c r="Y28" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="Z28" s="22"/>
-      <c r="AA28" s="22"/>
-      <c r="AB28" s="22"/>
-      <c r="AC28" s="22"/>
-      <c r="AD28" s="22" t="s">
+      <c r="Z28" s="24"/>
+      <c r="AA28" s="24"/>
+      <c r="AB28" s="24"/>
+      <c r="AC28" s="24"/>
+      <c r="AD28" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="AE28" s="22"/>
-      <c r="AF28" s="22"/>
-      <c r="AG28" s="24" t="s">
+      <c r="AE28" s="24"/>
+      <c r="AF28" s="24"/>
+      <c r="AG28" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="AH28" s="24"/>
-      <c r="AI28" s="24"/>
-      <c r="AJ28" s="24"/>
-      <c r="AK28" s="24"/>
-      <c r="AL28" s="24"/>
-      <c r="AM28" s="24" t="s">
+      <c r="AH28" s="22"/>
+      <c r="AI28" s="22"/>
+      <c r="AJ28" s="22"/>
+      <c r="AK28" s="22"/>
+      <c r="AL28" s="22"/>
+      <c r="AM28" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="AN28" s="24"/>
-      <c r="AO28" s="24"/>
-      <c r="AP28" s="24"/>
-      <c r="AQ28" s="24"/>
-      <c r="AR28" s="24"/>
-      <c r="AS28" s="24" t="s">
+      <c r="AN28" s="22"/>
+      <c r="AO28" s="22"/>
+      <c r="AP28" s="22"/>
+      <c r="AQ28" s="22"/>
+      <c r="AR28" s="22"/>
+      <c r="AS28" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="AT28" s="24"/>
-      <c r="AU28" s="24"/>
-      <c r="AV28" s="24"/>
-      <c r="AW28" s="24"/>
-      <c r="AX28" s="24"/>
-      <c r="AY28" s="24" t="s">
+      <c r="AT28" s="22"/>
+      <c r="AU28" s="22"/>
+      <c r="AV28" s="22"/>
+      <c r="AW28" s="22"/>
+      <c r="AX28" s="22"/>
+      <c r="AY28" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="AZ28" s="24"/>
-      <c r="BA28" s="24"/>
-      <c r="BB28" s="24"/>
-      <c r="BC28" s="24"/>
-      <c r="BD28" s="24"/>
-      <c r="BE28" s="24" t="s">
+      <c r="AZ28" s="22"/>
+      <c r="BA28" s="22"/>
+      <c r="BB28" s="22"/>
+      <c r="BC28" s="22"/>
+      <c r="BD28" s="22"/>
+      <c r="BE28" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="BF28" s="24"/>
-      <c r="BG28" s="24"/>
-      <c r="BH28" s="24"/>
-      <c r="BI28" s="24"/>
-      <c r="BJ28" s="24"/>
-      <c r="BK28" s="24" t="s">
+      <c r="BF28" s="22"/>
+      <c r="BG28" s="22"/>
+      <c r="BH28" s="22"/>
+      <c r="BI28" s="22"/>
+      <c r="BJ28" s="22"/>
+      <c r="BK28" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="BL28" s="24"/>
-      <c r="BM28" s="24"/>
-      <c r="BN28" s="24"/>
-      <c r="BO28" s="24"/>
-      <c r="BP28" s="24"/>
-      <c r="BQ28" s="24" t="s">
+      <c r="BL28" s="22"/>
+      <c r="BM28" s="22"/>
+      <c r="BN28" s="22"/>
+      <c r="BO28" s="22"/>
+      <c r="BP28" s="22"/>
+      <c r="BQ28" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="BR28" s="24"/>
-      <c r="BS28" s="24"/>
-      <c r="BT28" s="24"/>
-      <c r="BU28" s="24"/>
-      <c r="BV28" s="24"/>
-      <c r="BW28" s="24" t="s">
+      <c r="BR28" s="22"/>
+      <c r="BS28" s="22"/>
+      <c r="BT28" s="22"/>
+      <c r="BU28" s="22"/>
+      <c r="BV28" s="22"/>
+      <c r="BW28" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="BX28" s="24"/>
-      <c r="BY28" s="24"/>
-      <c r="BZ28" s="24"/>
-      <c r="CA28" s="24"/>
-      <c r="CB28" s="24"/>
-      <c r="CC28" s="24" t="s">
+      <c r="BX28" s="22"/>
+      <c r="BY28" s="22"/>
+      <c r="BZ28" s="22"/>
+      <c r="CA28" s="22"/>
+      <c r="CB28" s="22"/>
+      <c r="CC28" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="CD28" s="24"/>
-      <c r="CE28" s="24"/>
-      <c r="CF28" s="24"/>
-      <c r="CG28" s="24"/>
-      <c r="CH28" s="24"/>
-      <c r="CI28" s="24" t="s">
+      <c r="CD28" s="22"/>
+      <c r="CE28" s="22"/>
+      <c r="CF28" s="22"/>
+      <c r="CG28" s="22"/>
+      <c r="CH28" s="22"/>
+      <c r="CI28" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="CJ28" s="24"/>
-      <c r="CK28" s="24"/>
-      <c r="CL28" s="24"/>
-      <c r="CM28" s="24"/>
-      <c r="CN28" s="24"/>
+      <c r="CJ28" s="22"/>
+      <c r="CK28" s="22"/>
+      <c r="CL28" s="22"/>
+      <c r="CM28" s="22"/>
+      <c r="CN28" s="22"/>
     </row>
     <row r="29" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A29" s="22">
+      <c r="A29" s="24">
         <f>A27</f>
         <v>10</v>
       </c>
-      <c r="B29" s="22"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="23">
+      <c r="B29" s="24"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="24"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="25">
         <f>'Data package'!$B$31*I27+'Data package'!$B$28</f>
         <v>3.3870967741935485</v>
       </c>
-      <c r="J29" s="23"/>
-      <c r="K29" s="23"/>
-      <c r="L29" s="23"/>
-      <c r="M29" s="23"/>
-      <c r="N29" s="24">
+      <c r="J29" s="25"/>
+      <c r="K29" s="25"/>
+      <c r="L29" s="25"/>
+      <c r="M29" s="25"/>
+      <c r="N29" s="22">
         <f ca="1">LOOKUP(N27,'Data package'!$D$21:$D$24,'Data package'!$E$22:$E$31)</f>
         <v>0</v>
       </c>
-      <c r="O29" s="24"/>
-      <c r="P29" s="24"/>
-      <c r="Q29" s="25">
+      <c r="O29" s="22"/>
+      <c r="P29" s="22"/>
+      <c r="Q29" s="26">
         <f>100/(2^3-1)*Q27</f>
         <v>42.857142857142861</v>
       </c>
-      <c r="R29" s="25"/>
-      <c r="S29" s="25"/>
-      <c r="T29" s="25">
+      <c r="R29" s="26"/>
+      <c r="S29" s="26"/>
+      <c r="T29" s="26">
         <f>'Data package'!$B$40*T27+'Data package'!$B$37</f>
         <v>22.903225806451616</v>
       </c>
-      <c r="U29" s="24"/>
-      <c r="V29" s="24"/>
-      <c r="W29" s="24"/>
-      <c r="X29" s="24"/>
-      <c r="Y29" s="24">
+      <c r="U29" s="22"/>
+      <c r="V29" s="22"/>
+      <c r="W29" s="22"/>
+      <c r="X29" s="22"/>
+      <c r="Y29" s="22">
         <f>Y27</f>
         <v>21</v>
       </c>
-      <c r="Z29" s="24"/>
-      <c r="AA29" s="24"/>
-      <c r="AB29" s="24"/>
-      <c r="AC29" s="24"/>
-      <c r="AD29" s="24">
+      <c r="Z29" s="22"/>
+      <c r="AA29" s="22"/>
+      <c r="AB29" s="22"/>
+      <c r="AC29" s="22"/>
+      <c r="AD29" s="22">
         <f>LOOKUP(AD27,'Data package'!$A$77:$A$81,'Data package'!$B$77:$B$81)</f>
         <v>1</v>
       </c>
-      <c r="AE29" s="24"/>
-      <c r="AF29" s="24"/>
-      <c r="AG29" s="24" t="s">
+      <c r="AE29" s="22"/>
+      <c r="AF29" s="22"/>
+      <c r="AG29" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="AH29" s="24"/>
-      <c r="AI29" s="24"/>
-      <c r="AJ29" s="24"/>
-      <c r="AK29" s="24"/>
-      <c r="AL29" s="24"/>
-      <c r="AM29" s="24" t="s">
+      <c r="AH29" s="22"/>
+      <c r="AI29" s="22"/>
+      <c r="AJ29" s="22"/>
+      <c r="AK29" s="22"/>
+      <c r="AL29" s="22"/>
+      <c r="AM29" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="AN29" s="24"/>
-      <c r="AO29" s="24"/>
-      <c r="AP29" s="24"/>
-      <c r="AQ29" s="24"/>
-      <c r="AR29" s="24"/>
-      <c r="AS29" s="24" t="s">
+      <c r="AN29" s="22"/>
+      <c r="AO29" s="22"/>
+      <c r="AP29" s="22"/>
+      <c r="AQ29" s="22"/>
+      <c r="AR29" s="22"/>
+      <c r="AS29" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="AT29" s="24"/>
-      <c r="AU29" s="24"/>
-      <c r="AV29" s="24"/>
-      <c r="AW29" s="24"/>
-      <c r="AX29" s="24"/>
-      <c r="AY29" s="24" t="s">
+      <c r="AT29" s="22"/>
+      <c r="AU29" s="22"/>
+      <c r="AV29" s="22"/>
+      <c r="AW29" s="22"/>
+      <c r="AX29" s="22"/>
+      <c r="AY29" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="AZ29" s="24"/>
-      <c r="BA29" s="24"/>
-      <c r="BB29" s="24"/>
-      <c r="BC29" s="24"/>
-      <c r="BD29" s="24"/>
-      <c r="BE29" s="24" t="s">
+      <c r="AZ29" s="22"/>
+      <c r="BA29" s="22"/>
+      <c r="BB29" s="22"/>
+      <c r="BC29" s="22"/>
+      <c r="BD29" s="22"/>
+      <c r="BE29" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="BF29" s="24"/>
-      <c r="BG29" s="24"/>
-      <c r="BH29" s="24"/>
-      <c r="BI29" s="24"/>
-      <c r="BJ29" s="24"/>
-      <c r="BK29" s="24" t="s">
+      <c r="BF29" s="22"/>
+      <c r="BG29" s="22"/>
+      <c r="BH29" s="22"/>
+      <c r="BI29" s="22"/>
+      <c r="BJ29" s="22"/>
+      <c r="BK29" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="BL29" s="24"/>
-      <c r="BM29" s="24"/>
-      <c r="BN29" s="24"/>
-      <c r="BO29" s="24"/>
-      <c r="BP29" s="24"/>
-      <c r="BQ29" s="24" t="s">
+      <c r="BL29" s="22"/>
+      <c r="BM29" s="22"/>
+      <c r="BN29" s="22"/>
+      <c r="BO29" s="22"/>
+      <c r="BP29" s="22"/>
+      <c r="BQ29" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="BR29" s="24"/>
-      <c r="BS29" s="24"/>
-      <c r="BT29" s="24"/>
-      <c r="BU29" s="24"/>
-      <c r="BV29" s="24"/>
-      <c r="BW29" s="24" t="s">
+      <c r="BR29" s="22"/>
+      <c r="BS29" s="22"/>
+      <c r="BT29" s="22"/>
+      <c r="BU29" s="22"/>
+      <c r="BV29" s="22"/>
+      <c r="BW29" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="BX29" s="24"/>
-      <c r="BY29" s="24"/>
-      <c r="BZ29" s="24"/>
-      <c r="CA29" s="24"/>
-      <c r="CB29" s="24"/>
-      <c r="CC29" s="24" t="s">
+      <c r="BX29" s="22"/>
+      <c r="BY29" s="22"/>
+      <c r="BZ29" s="22"/>
+      <c r="CA29" s="22"/>
+      <c r="CB29" s="22"/>
+      <c r="CC29" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="CD29" s="24"/>
-      <c r="CE29" s="24"/>
-      <c r="CF29" s="24"/>
-      <c r="CG29" s="24"/>
-      <c r="CH29" s="24"/>
-      <c r="CI29" s="24" t="s">
+      <c r="CD29" s="22"/>
+      <c r="CE29" s="22"/>
+      <c r="CF29" s="22"/>
+      <c r="CG29" s="22"/>
+      <c r="CH29" s="22"/>
+      <c r="CI29" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="CJ29" s="24"/>
-      <c r="CK29" s="24"/>
-      <c r="CL29" s="24"/>
-      <c r="CM29" s="24"/>
-      <c r="CN29" s="24"/>
+      <c r="CJ29" s="22"/>
+      <c r="CK29" s="22"/>
+      <c r="CL29" s="22"/>
+      <c r="CM29" s="22"/>
+      <c r="CN29" s="22"/>
     </row>
     <row r="30" spans="1:96" x14ac:dyDescent="0.3">
       <c r="AG30">
@@ -5289,255 +5295,229 @@
       </c>
     </row>
     <row r="31" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="AG31" s="24" t="s">
+      <c r="AG31" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="AH31" s="24"/>
-      <c r="AI31" s="24"/>
-      <c r="AJ31" s="24"/>
-      <c r="AK31" s="24"/>
-      <c r="AL31" s="24"/>
-      <c r="AM31" s="24" t="s">
+      <c r="AH31" s="22"/>
+      <c r="AI31" s="22"/>
+      <c r="AJ31" s="22"/>
+      <c r="AK31" s="22"/>
+      <c r="AL31" s="22"/>
+      <c r="AM31" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="AN31" s="24"/>
-      <c r="AO31" s="24"/>
-      <c r="AP31" s="24"/>
-      <c r="AQ31" s="24"/>
-      <c r="AR31" s="24"/>
-      <c r="AS31" s="24" t="s">
+      <c r="AN31" s="22"/>
+      <c r="AO31" s="22"/>
+      <c r="AP31" s="22"/>
+      <c r="AQ31" s="22"/>
+      <c r="AR31" s="22"/>
+      <c r="AS31" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="AT31" s="24"/>
-      <c r="AU31" s="24"/>
-      <c r="AV31" s="24"/>
-      <c r="AW31" s="24"/>
-      <c r="AX31" s="24"/>
-      <c r="AY31" s="24" t="s">
+      <c r="AT31" s="22"/>
+      <c r="AU31" s="22"/>
+      <c r="AV31" s="22"/>
+      <c r="AW31" s="22"/>
+      <c r="AX31" s="22"/>
+      <c r="AY31" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="AZ31" s="24"/>
-      <c r="BA31" s="24"/>
-      <c r="BB31" s="24"/>
-      <c r="BC31" s="24"/>
-      <c r="BD31" s="24"/>
-      <c r="BE31" s="24" t="s">
+      <c r="AZ31" s="22"/>
+      <c r="BA31" s="22"/>
+      <c r="BB31" s="22"/>
+      <c r="BC31" s="22"/>
+      <c r="BD31" s="22"/>
+      <c r="BE31" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="BF31" s="24"/>
-      <c r="BG31" s="24"/>
-      <c r="BH31" s="24"/>
-      <c r="BI31" s="24"/>
-      <c r="BJ31" s="24"/>
-      <c r="BK31" s="24" t="s">
+      <c r="BF31" s="22"/>
+      <c r="BG31" s="22"/>
+      <c r="BH31" s="22"/>
+      <c r="BI31" s="22"/>
+      <c r="BJ31" s="22"/>
+      <c r="BK31" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="BL31" s="24"/>
-      <c r="BM31" s="24"/>
-      <c r="BN31" s="24"/>
-      <c r="BO31" s="24"/>
-      <c r="BP31" s="24"/>
-      <c r="BQ31" s="24" t="s">
+      <c r="BL31" s="22"/>
+      <c r="BM31" s="22"/>
+      <c r="BN31" s="22"/>
+      <c r="BO31" s="22"/>
+      <c r="BP31" s="22"/>
+      <c r="BQ31" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="BR31" s="24"/>
-      <c r="BS31" s="24"/>
-      <c r="BT31" s="24"/>
-      <c r="BU31" s="24"/>
-      <c r="BV31" s="24"/>
-      <c r="BW31" s="24" t="s">
+      <c r="BR31" s="22"/>
+      <c r="BS31" s="22"/>
+      <c r="BT31" s="22"/>
+      <c r="BU31" s="22"/>
+      <c r="BV31" s="22"/>
+      <c r="BW31" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="BX31" s="24"/>
-      <c r="BY31" s="24"/>
-      <c r="BZ31" s="24"/>
-      <c r="CA31" s="24"/>
-      <c r="CB31" s="24"/>
-      <c r="CC31" s="24" t="s">
+      <c r="BX31" s="22"/>
+      <c r="BY31" s="22"/>
+      <c r="BZ31" s="22"/>
+      <c r="CA31" s="22"/>
+      <c r="CB31" s="22"/>
+      <c r="CC31" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="CD31" s="24"/>
-      <c r="CE31" s="24"/>
-      <c r="CF31" s="24"/>
-      <c r="CG31" s="24"/>
-      <c r="CH31" s="24"/>
-      <c r="CI31" s="24" t="s">
+      <c r="CD31" s="22"/>
+      <c r="CE31" s="22"/>
+      <c r="CF31" s="22"/>
+      <c r="CG31" s="22"/>
+      <c r="CH31" s="22"/>
+      <c r="CI31" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="CJ31" s="24"/>
-      <c r="CK31" s="24"/>
-      <c r="CL31" s="24"/>
-      <c r="CM31" s="24"/>
-      <c r="CN31" s="24"/>
+      <c r="CJ31" s="22"/>
+      <c r="CK31" s="22"/>
+      <c r="CL31" s="22"/>
+      <c r="CM31" s="22"/>
+      <c r="CN31" s="22"/>
     </row>
     <row r="32" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="AG32" s="24">
+      <c r="AG32" s="22">
         <v>25</v>
       </c>
-      <c r="AH32" s="24"/>
-      <c r="AI32" s="24"/>
-      <c r="AJ32" s="24"/>
-      <c r="AK32" s="24"/>
-      <c r="AL32" s="24"/>
-      <c r="AM32" s="24">
+      <c r="AH32" s="22"/>
+      <c r="AI32" s="22"/>
+      <c r="AJ32" s="22"/>
+      <c r="AK32" s="22"/>
+      <c r="AL32" s="22"/>
+      <c r="AM32" s="22">
         <v>25</v>
       </c>
-      <c r="AN32" s="24"/>
-      <c r="AO32" s="24"/>
-      <c r="AP32" s="24"/>
-      <c r="AQ32" s="24"/>
-      <c r="AR32" s="24"/>
-      <c r="AS32" s="24">
+      <c r="AN32" s="22"/>
+      <c r="AO32" s="22"/>
+      <c r="AP32" s="22"/>
+      <c r="AQ32" s="22"/>
+      <c r="AR32" s="22"/>
+      <c r="AS32" s="22">
         <v>25</v>
       </c>
-      <c r="AT32" s="24"/>
-      <c r="AU32" s="24"/>
-      <c r="AV32" s="24"/>
-      <c r="AW32" s="24"/>
-      <c r="AX32" s="24"/>
-      <c r="AY32" s="24">
+      <c r="AT32" s="22"/>
+      <c r="AU32" s="22"/>
+      <c r="AV32" s="22"/>
+      <c r="AW32" s="22"/>
+      <c r="AX32" s="22"/>
+      <c r="AY32" s="22">
         <v>25</v>
       </c>
-      <c r="AZ32" s="24"/>
-      <c r="BA32" s="24"/>
-      <c r="BB32" s="24"/>
-      <c r="BC32" s="24"/>
-      <c r="BD32" s="24"/>
-      <c r="BE32" s="24">
+      <c r="AZ32" s="22"/>
+      <c r="BA32" s="22"/>
+      <c r="BB32" s="22"/>
+      <c r="BC32" s="22"/>
+      <c r="BD32" s="22"/>
+      <c r="BE32" s="22">
         <v>26</v>
       </c>
-      <c r="BF32" s="24"/>
-      <c r="BG32" s="24"/>
-      <c r="BH32" s="24"/>
-      <c r="BI32" s="24"/>
-      <c r="BJ32" s="24"/>
-      <c r="BK32" s="24">
+      <c r="BF32" s="22"/>
+      <c r="BG32" s="22"/>
+      <c r="BH32" s="22"/>
+      <c r="BI32" s="22"/>
+      <c r="BJ32" s="22"/>
+      <c r="BK32" s="22">
         <v>26</v>
       </c>
-      <c r="BL32" s="24"/>
-      <c r="BM32" s="24"/>
-      <c r="BN32" s="24"/>
-      <c r="BO32" s="24"/>
-      <c r="BP32" s="24"/>
-      <c r="BQ32" s="24">
+      <c r="BL32" s="22"/>
+      <c r="BM32" s="22"/>
+      <c r="BN32" s="22"/>
+      <c r="BO32" s="22"/>
+      <c r="BP32" s="22"/>
+      <c r="BQ32" s="22">
         <v>26</v>
       </c>
-      <c r="BR32" s="24"/>
-      <c r="BS32" s="24"/>
-      <c r="BT32" s="24"/>
-      <c r="BU32" s="24"/>
-      <c r="BV32" s="24"/>
-      <c r="BW32" s="24">
+      <c r="BR32" s="22"/>
+      <c r="BS32" s="22"/>
+      <c r="BT32" s="22"/>
+      <c r="BU32" s="22"/>
+      <c r="BV32" s="22"/>
+      <c r="BW32" s="22">
         <v>26</v>
       </c>
-      <c r="BX32" s="24"/>
-      <c r="BY32" s="24"/>
-      <c r="BZ32" s="24"/>
-      <c r="CA32" s="24"/>
-      <c r="CB32" s="24"/>
-      <c r="CC32" s="24">
+      <c r="BX32" s="22"/>
+      <c r="BY32" s="22"/>
+      <c r="BZ32" s="22"/>
+      <c r="CA32" s="22"/>
+      <c r="CB32" s="22"/>
+      <c r="CC32" s="22">
         <v>26</v>
       </c>
-      <c r="CD32" s="24"/>
-      <c r="CE32" s="24"/>
-      <c r="CF32" s="24"/>
-      <c r="CG32" s="24"/>
-      <c r="CH32" s="24"/>
-      <c r="CI32" s="24">
+      <c r="CD32" s="22"/>
+      <c r="CE32" s="22"/>
+      <c r="CF32" s="22"/>
+      <c r="CG32" s="22"/>
+      <c r="CH32" s="22"/>
+      <c r="CI32" s="22">
         <v>26</v>
       </c>
-      <c r="CJ32" s="24"/>
-      <c r="CK32" s="24"/>
-      <c r="CL32" s="24"/>
-      <c r="CM32" s="24"/>
-      <c r="CN32" s="24"/>
+      <c r="CJ32" s="22"/>
+      <c r="CK32" s="22"/>
+      <c r="CL32" s="22"/>
+      <c r="CM32" s="22"/>
+      <c r="CN32" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="166">
-    <mergeCell ref="BK32:BP32"/>
-    <mergeCell ref="BQ32:BV32"/>
-    <mergeCell ref="BW32:CB32"/>
-    <mergeCell ref="CC32:CH32"/>
-    <mergeCell ref="CI32:CN32"/>
-    <mergeCell ref="AG32:AL32"/>
-    <mergeCell ref="AM32:AR32"/>
-    <mergeCell ref="AS32:AX32"/>
-    <mergeCell ref="AY32:BD32"/>
-    <mergeCell ref="BE32:BJ32"/>
-    <mergeCell ref="BK31:BP31"/>
-    <mergeCell ref="BQ31:BV31"/>
-    <mergeCell ref="BW31:CB31"/>
-    <mergeCell ref="CC31:CH31"/>
-    <mergeCell ref="CI31:CN31"/>
-    <mergeCell ref="AG31:AL31"/>
-    <mergeCell ref="AM31:AR31"/>
-    <mergeCell ref="AS31:AX31"/>
-    <mergeCell ref="AY31:BD31"/>
-    <mergeCell ref="BE31:BJ31"/>
-    <mergeCell ref="BK29:BP29"/>
-    <mergeCell ref="BQ29:BV29"/>
-    <mergeCell ref="BW29:CB29"/>
-    <mergeCell ref="CC29:CH29"/>
-    <mergeCell ref="CI29:CN29"/>
-    <mergeCell ref="AG29:AL29"/>
-    <mergeCell ref="AM29:AR29"/>
-    <mergeCell ref="AS29:AX29"/>
-    <mergeCell ref="AY29:BD29"/>
-    <mergeCell ref="BE29:BJ29"/>
-    <mergeCell ref="BK28:BP28"/>
-    <mergeCell ref="BQ28:BV28"/>
-    <mergeCell ref="BW28:CB28"/>
-    <mergeCell ref="CC28:CH28"/>
-    <mergeCell ref="CI28:CN28"/>
-    <mergeCell ref="AG28:AL28"/>
-    <mergeCell ref="AM28:AR28"/>
-    <mergeCell ref="AS28:AX28"/>
-    <mergeCell ref="AY28:BD28"/>
-    <mergeCell ref="BE28:BJ28"/>
-    <mergeCell ref="BU24:CB24"/>
-    <mergeCell ref="CC24:CJ24"/>
-    <mergeCell ref="CK24:CR24"/>
-    <mergeCell ref="AG26:AN26"/>
-    <mergeCell ref="AO26:AV26"/>
-    <mergeCell ref="AW26:BD26"/>
-    <mergeCell ref="BE26:BL26"/>
-    <mergeCell ref="BM26:BT26"/>
-    <mergeCell ref="BU26:CB26"/>
-    <mergeCell ref="CC26:CJ26"/>
-    <mergeCell ref="CK26:CR26"/>
-    <mergeCell ref="AG24:AN24"/>
-    <mergeCell ref="AO24:AV24"/>
-    <mergeCell ref="AW24:BD24"/>
-    <mergeCell ref="BE24:BL24"/>
-    <mergeCell ref="BM24:BT24"/>
-    <mergeCell ref="Y28:AC28"/>
-    <mergeCell ref="AD28:AF28"/>
-    <mergeCell ref="A29:H29"/>
-    <mergeCell ref="I29:M29"/>
-    <mergeCell ref="N29:P29"/>
-    <mergeCell ref="Q29:S29"/>
-    <mergeCell ref="T29:X29"/>
-    <mergeCell ref="Y29:AC29"/>
-    <mergeCell ref="AD29:AF29"/>
-    <mergeCell ref="A28:H28"/>
-    <mergeCell ref="I28:M28"/>
-    <mergeCell ref="N28:P28"/>
-    <mergeCell ref="Q28:S28"/>
-    <mergeCell ref="T28:X28"/>
-    <mergeCell ref="Y26:AC26"/>
-    <mergeCell ref="AD26:AF26"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="I27:M27"/>
-    <mergeCell ref="N27:P27"/>
-    <mergeCell ref="Q27:S27"/>
-    <mergeCell ref="T27:X27"/>
-    <mergeCell ref="Y27:AC27"/>
-    <mergeCell ref="AD27:AF27"/>
-    <mergeCell ref="A26:H26"/>
-    <mergeCell ref="I26:M26"/>
-    <mergeCell ref="N26:P26"/>
-    <mergeCell ref="Q26:S26"/>
-    <mergeCell ref="T26:X26"/>
+    <mergeCell ref="Y19:AC19"/>
+    <mergeCell ref="AD19:AF19"/>
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="I20:M20"/>
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="Q20:S20"/>
+    <mergeCell ref="T20:X20"/>
+    <mergeCell ref="Y20:AC20"/>
+    <mergeCell ref="AD20:AF20"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="I19:M19"/>
+    <mergeCell ref="N19:P19"/>
+    <mergeCell ref="Q19:S19"/>
+    <mergeCell ref="T19:X19"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="I15:P15"/>
+    <mergeCell ref="Q15:X15"/>
+    <mergeCell ref="Y15:AF15"/>
+    <mergeCell ref="A14:AF14"/>
+    <mergeCell ref="Y17:AC17"/>
+    <mergeCell ref="AD17:AF17"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="I18:M18"/>
+    <mergeCell ref="N18:P18"/>
+    <mergeCell ref="Q18:S18"/>
+    <mergeCell ref="T18:X18"/>
+    <mergeCell ref="Y18:AC18"/>
+    <mergeCell ref="AD18:AF18"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="I17:M17"/>
+    <mergeCell ref="N17:P17"/>
+    <mergeCell ref="Q17:S17"/>
+    <mergeCell ref="T17:X17"/>
+    <mergeCell ref="I11:M11"/>
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="I10:M10"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="AD10:AF10"/>
+    <mergeCell ref="Y10:AC10"/>
+    <mergeCell ref="T10:X10"/>
+    <mergeCell ref="Q10:S10"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="AD11:AF11"/>
+    <mergeCell ref="Y11:AC11"/>
+    <mergeCell ref="T11:X11"/>
+    <mergeCell ref="Q11:S11"/>
+    <mergeCell ref="N11:P11"/>
+    <mergeCell ref="Q6:X6"/>
+    <mergeCell ref="Y6:AF6"/>
+    <mergeCell ref="AD9:AF9"/>
+    <mergeCell ref="AD8:AF8"/>
+    <mergeCell ref="Y9:AC9"/>
+    <mergeCell ref="Y8:AC8"/>
+    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="T8:X8"/>
+    <mergeCell ref="T9:X9"/>
     <mergeCell ref="A23:AF23"/>
     <mergeCell ref="A24:H24"/>
     <mergeCell ref="I24:P24"/>
@@ -5562,64 +5542,90 @@
     <mergeCell ref="I8:M8"/>
     <mergeCell ref="N8:P8"/>
     <mergeCell ref="I9:M9"/>
-    <mergeCell ref="Q6:X6"/>
-    <mergeCell ref="Y6:AF6"/>
-    <mergeCell ref="AD9:AF9"/>
-    <mergeCell ref="AD8:AF8"/>
-    <mergeCell ref="Y9:AC9"/>
-    <mergeCell ref="Y8:AC8"/>
-    <mergeCell ref="N9:P9"/>
-    <mergeCell ref="Q8:S8"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="T8:X8"/>
-    <mergeCell ref="T9:X9"/>
-    <mergeCell ref="I11:M11"/>
-    <mergeCell ref="A11:H11"/>
-    <mergeCell ref="I10:M10"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="AD10:AF10"/>
-    <mergeCell ref="Y10:AC10"/>
-    <mergeCell ref="T10:X10"/>
-    <mergeCell ref="Q10:S10"/>
-    <mergeCell ref="N10:P10"/>
-    <mergeCell ref="AD11:AF11"/>
-    <mergeCell ref="Y11:AC11"/>
-    <mergeCell ref="T11:X11"/>
-    <mergeCell ref="Q11:S11"/>
-    <mergeCell ref="N11:P11"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="I15:P15"/>
-    <mergeCell ref="Q15:X15"/>
-    <mergeCell ref="Y15:AF15"/>
-    <mergeCell ref="A14:AF14"/>
-    <mergeCell ref="Y17:AC17"/>
-    <mergeCell ref="AD17:AF17"/>
-    <mergeCell ref="A18:H18"/>
-    <mergeCell ref="I18:M18"/>
-    <mergeCell ref="N18:P18"/>
-    <mergeCell ref="Q18:S18"/>
-    <mergeCell ref="T18:X18"/>
-    <mergeCell ref="Y18:AC18"/>
-    <mergeCell ref="AD18:AF18"/>
-    <mergeCell ref="A17:H17"/>
-    <mergeCell ref="I17:M17"/>
-    <mergeCell ref="N17:P17"/>
-    <mergeCell ref="Q17:S17"/>
-    <mergeCell ref="T17:X17"/>
-    <mergeCell ref="Y19:AC19"/>
-    <mergeCell ref="AD19:AF19"/>
-    <mergeCell ref="A20:H20"/>
-    <mergeCell ref="I20:M20"/>
-    <mergeCell ref="N20:P20"/>
-    <mergeCell ref="Q20:S20"/>
-    <mergeCell ref="T20:X20"/>
-    <mergeCell ref="Y20:AC20"/>
-    <mergeCell ref="AD20:AF20"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="I19:M19"/>
-    <mergeCell ref="N19:P19"/>
-    <mergeCell ref="Q19:S19"/>
-    <mergeCell ref="T19:X19"/>
+    <mergeCell ref="Y26:AC26"/>
+    <mergeCell ref="AD26:AF26"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="I27:M27"/>
+    <mergeCell ref="N27:P27"/>
+    <mergeCell ref="Q27:S27"/>
+    <mergeCell ref="T27:X27"/>
+    <mergeCell ref="Y27:AC27"/>
+    <mergeCell ref="AD27:AF27"/>
+    <mergeCell ref="A26:H26"/>
+    <mergeCell ref="I26:M26"/>
+    <mergeCell ref="N26:P26"/>
+    <mergeCell ref="Q26:S26"/>
+    <mergeCell ref="T26:X26"/>
+    <mergeCell ref="Y28:AC28"/>
+    <mergeCell ref="AD28:AF28"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="I29:M29"/>
+    <mergeCell ref="N29:P29"/>
+    <mergeCell ref="Q29:S29"/>
+    <mergeCell ref="T29:X29"/>
+    <mergeCell ref="Y29:AC29"/>
+    <mergeCell ref="AD29:AF29"/>
+    <mergeCell ref="A28:H28"/>
+    <mergeCell ref="I28:M28"/>
+    <mergeCell ref="N28:P28"/>
+    <mergeCell ref="Q28:S28"/>
+    <mergeCell ref="T28:X28"/>
+    <mergeCell ref="BU24:CB24"/>
+    <mergeCell ref="CC24:CJ24"/>
+    <mergeCell ref="CK24:CR24"/>
+    <mergeCell ref="AG26:AN26"/>
+    <mergeCell ref="AO26:AV26"/>
+    <mergeCell ref="AW26:BD26"/>
+    <mergeCell ref="BE26:BL26"/>
+    <mergeCell ref="BM26:BT26"/>
+    <mergeCell ref="BU26:CB26"/>
+    <mergeCell ref="CC26:CJ26"/>
+    <mergeCell ref="CK26:CR26"/>
+    <mergeCell ref="AG24:AN24"/>
+    <mergeCell ref="AO24:AV24"/>
+    <mergeCell ref="AW24:BD24"/>
+    <mergeCell ref="BE24:BL24"/>
+    <mergeCell ref="BM24:BT24"/>
+    <mergeCell ref="BK28:BP28"/>
+    <mergeCell ref="BQ28:BV28"/>
+    <mergeCell ref="BW28:CB28"/>
+    <mergeCell ref="CC28:CH28"/>
+    <mergeCell ref="CI28:CN28"/>
+    <mergeCell ref="AG28:AL28"/>
+    <mergeCell ref="AM28:AR28"/>
+    <mergeCell ref="AS28:AX28"/>
+    <mergeCell ref="AY28:BD28"/>
+    <mergeCell ref="BE28:BJ28"/>
+    <mergeCell ref="BK29:BP29"/>
+    <mergeCell ref="BQ29:BV29"/>
+    <mergeCell ref="BW29:CB29"/>
+    <mergeCell ref="CC29:CH29"/>
+    <mergeCell ref="CI29:CN29"/>
+    <mergeCell ref="AG29:AL29"/>
+    <mergeCell ref="AM29:AR29"/>
+    <mergeCell ref="AS29:AX29"/>
+    <mergeCell ref="AY29:BD29"/>
+    <mergeCell ref="BE29:BJ29"/>
+    <mergeCell ref="BK31:BP31"/>
+    <mergeCell ref="BQ31:BV31"/>
+    <mergeCell ref="BW31:CB31"/>
+    <mergeCell ref="CC31:CH31"/>
+    <mergeCell ref="CI31:CN31"/>
+    <mergeCell ref="AG31:AL31"/>
+    <mergeCell ref="AM31:AR31"/>
+    <mergeCell ref="AS31:AX31"/>
+    <mergeCell ref="AY31:BD31"/>
+    <mergeCell ref="BE31:BJ31"/>
+    <mergeCell ref="BK32:BP32"/>
+    <mergeCell ref="BQ32:BV32"/>
+    <mergeCell ref="BW32:CB32"/>
+    <mergeCell ref="CC32:CH32"/>
+    <mergeCell ref="CI32:CN32"/>
+    <mergeCell ref="AG32:AL32"/>
+    <mergeCell ref="AM32:AR32"/>
+    <mergeCell ref="AS32:AX32"/>
+    <mergeCell ref="AY32:BD32"/>
+    <mergeCell ref="BE32:BJ32"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -5648,11 +5654,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
       <c r="E1" s="11">
         <v>0.5</v>
       </c>
@@ -6478,28 +6484,28 @@
       <c r="S2" s="7"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="34" t="s">
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="34" t="s">
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
+      <c r="M3" s="36"/>
+      <c r="N3" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="O3" s="35"/>
-      <c r="P3" s="36"/>
+      <c r="O3" s="36"/>
+      <c r="P3" s="37"/>
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
       <c r="S3" s="7"/>
@@ -6566,10 +6572,10 @@
       <c r="O6" s="27"/>
       <c r="P6" s="27"/>
       <c r="Q6" s="7"/>
-      <c r="R6" s="22" t="s">
+      <c r="R6" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="S6" s="22"/>
+      <c r="S6" s="24"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
@@ -6621,18 +6627,18 @@
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
-      <c r="I8" s="22" t="s">
+      <c r="I8" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="22" t="s">
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="O8" s="22"/>
-      <c r="P8" s="22"/>
+      <c r="O8" s="24"/>
+      <c r="P8" s="24"/>
       <c r="Q8" s="7"/>
       <c r="R8" s="7"/>
       <c r="S8" s="7"/>
@@ -6646,18 +6652,18 @@
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
-      <c r="I9" s="22">
+      <c r="I9" s="24">
         <v>17</v>
       </c>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="22">
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24">
         <v>4</v>
       </c>
-      <c r="O9" s="22"/>
-      <c r="P9" s="22"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="24"/>
       <c r="Q9" s="7"/>
       <c r="R9" s="7"/>
       <c r="S9" s="7"/>
@@ -6676,11 +6682,11 @@
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
-      <c r="N10" s="22" t="s">
+      <c r="N10" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="O10" s="22"/>
-      <c r="P10" s="22"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="24"/>
       <c r="Q10" s="7"/>
       <c r="R10" s="7"/>
       <c r="S10" s="7"/>
@@ -6699,24 +6705,18 @@
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
-      <c r="N11" s="23">
+      <c r="N11" s="25">
         <f>100/(2^3-1)*N9</f>
         <v>57.142857142857146</v>
       </c>
-      <c r="O11" s="23"/>
-      <c r="P11" s="23"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="25"/>
       <c r="Q11" s="7"/>
       <c r="R11" s="7"/>
       <c r="S11" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="I3:M3"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="I6:P6"/>
     <mergeCell ref="N11:P11"/>
     <mergeCell ref="R7:S7"/>
     <mergeCell ref="I8:M8"/>
@@ -6724,6 +6724,12 @@
     <mergeCell ref="I9:M9"/>
     <mergeCell ref="N9:P9"/>
     <mergeCell ref="N10:P10"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="I3:M3"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="I6:P6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
time synchronization properties to payload formatter added
</commit_message>
<xml_diff>
--- a/hardware/BikeCounterPro/src/dataPackage/DataPackage.xlsx
+++ b/hardware/BikeCounterPro/src/dataPackage/DataPackage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meier\Documents\repos\lora\hardware\BikeCounterPro\src\dataPackage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF0735F2-D222-43E9-812A-B2EB377BA5B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1029DD3A-FE16-4E2B-95EB-35D4C9543096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5130" yWindow="3517" windowWidth="15390" windowHeight="9443" xr2:uid="{CDF7A0A5-12B1-43F1-AFDE-54CA91221B4B}"/>
+    <workbookView xWindow="41172" yWindow="-108" windowWidth="41496" windowHeight="16896" xr2:uid="{CDF7A0A5-12B1-43F1-AFDE-54CA91221B4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Data package" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="116">
   <si>
     <t>minutes of day</t>
   </si>
@@ -383,6 +383,9 @@
   </si>
   <si>
     <t>Epoch [s]</t>
+  </si>
+  <si>
+    <t>sync call</t>
   </si>
 </sst>
 </file>
@@ -639,7 +642,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -648,16 +659,13 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -687,9 +695,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -699,8 +704,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
@@ -2151,19 +2154,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{088FF0E6-8FE4-49E3-812F-B76B934E1ACD}">
   <dimension ref="A1:S90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C24" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.86328125" customWidth="1"/>
-    <col min="5" max="5" width="12.1328125" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -2171,7 +2174,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -2180,12 +2183,12 @@
         <v>408</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -2193,7 +2196,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -2201,7 +2204,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -2210,7 +2213,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>88</v>
       </c>
@@ -2266,7 +2269,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -2278,7 +2281,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -2290,7 +2293,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>89</v>
       </c>
@@ -2346,7 +2349,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -2361,7 +2364,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -2376,7 +2379,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D19" t="s">
         <v>91</v>
       </c>
@@ -2384,7 +2387,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -2416,7 +2419,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -2427,8 +2430,11 @@
       <c r="D22" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="K22" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -2437,12 +2443,12 @@
         <v>397</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>11</v>
       </c>
@@ -2465,7 +2471,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>83</v>
       </c>
@@ -2478,7 +2484,7 @@
       <c r="E28" t="s">
         <v>97</v>
       </c>
-      <c r="F28" s="37">
+      <c r="F28" s="17">
         <v>1640995200</v>
       </c>
       <c r="G28">
@@ -2494,7 +2500,7 @@
         <v>2734992</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>84</v>
       </c>
@@ -2502,7 +2508,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>85</v>
       </c>
@@ -2532,7 +2538,7 @@
         <v>3155760</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>12</v>
       </c>
@@ -2553,7 +2559,7 @@
         <v>420768</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -2574,7 +2580,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D33" t="s">
         <v>109</v>
       </c>
@@ -2584,7 +2590,7 @@
       <c r="F33">
         <v>2208988800</v>
       </c>
-      <c r="G33" s="38">
+      <c r="G33" s="18">
         <f>F33/60</f>
         <v>36816480</v>
       </c>
@@ -2597,11 +2603,11 @@
         <v>3681648</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F34" t="s">
         <v>104</v>
       </c>
-      <c r="G34" s="38">
+      <c r="G34" s="18">
         <f>G33-G28</f>
         <v>9466560</v>
       </c>
@@ -2614,14 +2620,14 @@
         <v>946656</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>37</v>
       </c>
       <c r="F35" t="s">
         <v>105</v>
       </c>
-      <c r="G35" s="38">
+      <c r="G35" s="18">
         <f>_xlfn.CEILING.MATH(LOG10(G34)/LOG(2))</f>
         <v>24</v>
       </c>
@@ -2634,7 +2640,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -2642,7 +2648,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>33</v>
       </c>
@@ -2650,7 +2656,7 @@
         <v>-20</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>34</v>
       </c>
@@ -2658,7 +2664,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>35</v>
       </c>
@@ -2667,7 +2673,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>36</v>
       </c>
@@ -2677,7 +2683,7 @@
       </c>
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>18</v>
       </c>
@@ -2686,12 +2692,12 @@
         <v>379</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>11</v>
       </c>
@@ -2699,7 +2705,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>12</v>
       </c>
@@ -2708,7 +2714,7 @@
         <v>14.285714285714286</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>18</v>
       </c>
@@ -2717,12 +2723,12 @@
         <v>376</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>11</v>
       </c>
@@ -2733,7 +2739,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>111</v>
       </c>
@@ -2748,7 +2754,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>112</v>
       </c>
@@ -2764,7 +2770,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>18</v>
       </c>
@@ -2773,12 +2779,12 @@
         <v>352</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>11</v>
       </c>
@@ -2786,7 +2792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>18</v>
       </c>
@@ -2795,22 +2801,22 @@
         <v>352</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A63" s="17" t="s">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B63" s="17"/>
-      <c r="C63" s="17"/>
-      <c r="D63" s="17"/>
-      <c r="E63" s="17"/>
-      <c r="F63" s="17"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B63" s="19"/>
+      <c r="C63" s="19"/>
+      <c r="D63" s="19"/>
+      <c r="E63" s="19"/>
+      <c r="F63" s="19"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>1</v>
       </c>
@@ -2825,7 +2831,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>2</v>
       </c>
@@ -2840,7 +2846,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B68">
         <f>2^B67</f>
         <v>2048</v>
@@ -2853,17 +2859,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A71" s="17" t="s">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B71" s="17"/>
-      <c r="C71" s="17"/>
-      <c r="D71" s="17"/>
-      <c r="E71" s="17"/>
-      <c r="F71" s="17"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B71" s="19"/>
+      <c r="C71" s="19"/>
+      <c r="D71" s="19"/>
+      <c r="E71" s="19"/>
+      <c r="F71" s="19"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -2871,7 +2877,7 @@
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="7" t="s">
         <v>51</v>
       </c>
@@ -2881,7 +2887,7 @@
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="7" t="s">
         <v>11</v>
       </c>
@@ -2893,7 +2899,7 @@
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="7" t="s">
         <v>18</v>
       </c>
@@ -2906,13 +2912,13 @@
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>16</v>
       </c>
@@ -2922,7 +2928,7 @@
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>11</v>
       </c>
@@ -2934,7 +2940,7 @@
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>17</v>
       </c>
@@ -2947,7 +2953,7 @@
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -2955,7 +2961,7 @@
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>18</v>
       </c>
@@ -2973,13 +2979,13 @@
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="D82" s="1"/>
       <c r="F82" s="1"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>52</v>
       </c>
@@ -3005,7 +3011,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>0</v>
       </c>
@@ -3036,7 +3042,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>1</v>
       </c>
@@ -3067,7 +3073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>2</v>
       </c>
@@ -3098,7 +3104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>3</v>
       </c>
@@ -3129,7 +3135,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>4</v>
       </c>
@@ -3160,10 +3166,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E89" s="3"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E90" s="3"/>
     </row>
   </sheetData>
@@ -3184,55 +3190,55 @@
       <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="32" width="4.19921875" customWidth="1"/>
-    <col min="33" max="150" width="3.1328125" customWidth="1"/>
+    <col min="1" max="32" width="4.21875" customWidth="1"/>
+    <col min="33" max="150" width="3.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.45">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A1" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="24" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="24" t="s">
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
-      <c r="X1" s="26"/>
-      <c r="Y1" s="24" t="s">
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="29"/>
+      <c r="Y1" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="Z1" s="25"/>
-      <c r="AA1" s="25"/>
-      <c r="AB1" s="25"/>
-      <c r="AC1" s="25"/>
-      <c r="AD1" s="25"/>
-      <c r="AE1" s="25"/>
-      <c r="AF1" s="26"/>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="Z1" s="28"/>
+      <c r="AA1" s="28"/>
+      <c r="AB1" s="28"/>
+      <c r="AC1" s="28"/>
+      <c r="AD1" s="28"/>
+      <c r="AE1" s="28"/>
+      <c r="AF1" s="29"/>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>7</v>
       </c>
@@ -3330,55 +3336,55 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.45">
-      <c r="A3" s="30" t="s">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A3" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="30" t="s">
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="J3" s="31"/>
-      <c r="K3" s="31"/>
-      <c r="L3" s="31"/>
-      <c r="M3" s="31"/>
-      <c r="N3" s="30" t="s">
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="O3" s="31"/>
-      <c r="P3" s="32"/>
-      <c r="Q3" s="30" t="s">
+      <c r="O3" s="34"/>
+      <c r="P3" s="35"/>
+      <c r="Q3" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="R3" s="31"/>
-      <c r="S3" s="32"/>
-      <c r="T3" s="27" t="s">
+      <c r="R3" s="34"/>
+      <c r="S3" s="35"/>
+      <c r="T3" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="U3" s="28"/>
-      <c r="V3" s="28"/>
-      <c r="W3" s="28"/>
-      <c r="X3" s="29"/>
-      <c r="Y3" s="27" t="s">
+      <c r="U3" s="31"/>
+      <c r="V3" s="31"/>
+      <c r="W3" s="31"/>
+      <c r="X3" s="32"/>
+      <c r="Y3" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="Z3" s="28"/>
-      <c r="AA3" s="28"/>
-      <c r="AB3" s="28"/>
-      <c r="AC3" s="29"/>
-      <c r="AD3" s="27" t="s">
+      <c r="Z3" s="31"/>
+      <c r="AA3" s="31"/>
+      <c r="AB3" s="31"/>
+      <c r="AC3" s="32"/>
+      <c r="AD3" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="AE3" s="28"/>
-      <c r="AF3" s="29"/>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="AE3" s="31"/>
+      <c r="AF3" s="32"/>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -3399,85 +3405,85 @@
       <c r="R4" s="7"/>
       <c r="S4" s="7"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.45">
-      <c r="A5" s="23" t="s">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A5" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="23"/>
-      <c r="P5" s="23"/>
-      <c r="Q5" s="23"/>
-      <c r="R5" s="23"/>
-      <c r="S5" s="23"/>
-      <c r="T5" s="23"/>
-      <c r="U5" s="23"/>
-      <c r="V5" s="23"/>
-      <c r="W5" s="23"/>
-      <c r="X5" s="23"/>
-      <c r="Y5" s="23"/>
-      <c r="Z5" s="23"/>
-      <c r="AA5" s="23"/>
-      <c r="AB5" s="23"/>
-      <c r="AC5" s="23"/>
-      <c r="AD5" s="23"/>
-      <c r="AE5" s="23"/>
-      <c r="AF5" s="23"/>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.45">
-      <c r="A6" s="22" t="s">
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="25"/>
+      <c r="O5" s="25"/>
+      <c r="P5" s="25"/>
+      <c r="Q5" s="25"/>
+      <c r="R5" s="25"/>
+      <c r="S5" s="25"/>
+      <c r="T5" s="25"/>
+      <c r="U5" s="25"/>
+      <c r="V5" s="25"/>
+      <c r="W5" s="25"/>
+      <c r="X5" s="25"/>
+      <c r="Y5" s="25"/>
+      <c r="Z5" s="25"/>
+      <c r="AA5" s="25"/>
+      <c r="AB5" s="25"/>
+      <c r="AC5" s="25"/>
+      <c r="AD5" s="25"/>
+      <c r="AE5" s="25"/>
+      <c r="AF5" s="25"/>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A6" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22">
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26">
         <v>38</v>
       </c>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="22"/>
-      <c r="N6" s="22"/>
-      <c r="O6" s="22"/>
-      <c r="P6" s="22"/>
-      <c r="Q6" s="22">
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="26"/>
+      <c r="Q6" s="26">
         <v>73</v>
       </c>
-      <c r="R6" s="22"/>
-      <c r="S6" s="22"/>
-      <c r="T6" s="22"/>
-      <c r="U6" s="22"/>
-      <c r="V6" s="22"/>
-      <c r="W6" s="22"/>
-      <c r="X6" s="22"/>
-      <c r="Y6" s="22">
+      <c r="R6" s="26"/>
+      <c r="S6" s="26"/>
+      <c r="T6" s="26"/>
+      <c r="U6" s="26"/>
+      <c r="V6" s="26"/>
+      <c r="W6" s="26"/>
+      <c r="X6" s="26"/>
+      <c r="Y6" s="26">
         <v>88</v>
       </c>
-      <c r="Z6" s="22"/>
-      <c r="AA6" s="22"/>
-      <c r="AB6" s="22"/>
-      <c r="AC6" s="22"/>
-      <c r="AD6" s="22"/>
-      <c r="AE6" s="22"/>
-      <c r="AF6" s="22"/>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="Z6" s="26"/>
+      <c r="AA6" s="26"/>
+      <c r="AB6" s="26"/>
+      <c r="AC6" s="26"/>
+      <c r="AD6" s="26"/>
+      <c r="AE6" s="26"/>
+      <c r="AF6" s="26"/>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>0</v>
       </c>
@@ -3575,183 +3581,183 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.45">
-      <c r="A8" s="18" t="s">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18" t="s">
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18" t="s">
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="O8" s="18"/>
-      <c r="P8" s="18"/>
-      <c r="Q8" s="18" t="s">
+      <c r="O8" s="22"/>
+      <c r="P8" s="22"/>
+      <c r="Q8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="R8" s="18"/>
-      <c r="S8" s="18"/>
-      <c r="T8" s="18" t="s">
+      <c r="R8" s="22"/>
+      <c r="S8" s="22"/>
+      <c r="T8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="U8" s="18"/>
-      <c r="V8" s="18"/>
-      <c r="W8" s="18"/>
-      <c r="X8" s="18"/>
-      <c r="Y8" s="18" t="s">
+      <c r="U8" s="22"/>
+      <c r="V8" s="22"/>
+      <c r="W8" s="22"/>
+      <c r="X8" s="22"/>
+      <c r="Y8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="Z8" s="18"/>
-      <c r="AA8" s="18"/>
-      <c r="AB8" s="18"/>
-      <c r="AC8" s="18"/>
-      <c r="AD8" s="18" t="s">
+      <c r="Z8" s="22"/>
+      <c r="AA8" s="22"/>
+      <c r="AB8" s="22"/>
+      <c r="AC8" s="22"/>
+      <c r="AD8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="AE8" s="18"/>
-      <c r="AF8" s="18"/>
-    </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.45">
-      <c r="A9" s="18">
+      <c r="AE8" s="22"/>
+      <c r="AF8" s="22"/>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A9" s="22">
         <v>10</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18">
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22">
         <v>7</v>
       </c>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="18">
-        <v>0</v>
-      </c>
-      <c r="O9" s="18"/>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="18">
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22">
+        <v>0</v>
+      </c>
+      <c r="O9" s="22"/>
+      <c r="P9" s="22"/>
+      <c r="Q9" s="22">
         <v>3</v>
       </c>
-      <c r="R9" s="18"/>
-      <c r="S9" s="18"/>
-      <c r="T9" s="18">
+      <c r="R9" s="22"/>
+      <c r="S9" s="22"/>
+      <c r="T9" s="22">
         <v>19</v>
       </c>
-      <c r="U9" s="18"/>
-      <c r="V9" s="18"/>
-      <c r="W9" s="18"/>
-      <c r="X9" s="18"/>
-      <c r="Y9" s="18">
+      <c r="U9" s="22"/>
+      <c r="V9" s="22"/>
+      <c r="W9" s="22"/>
+      <c r="X9" s="22"/>
+      <c r="Y9" s="22">
         <v>17</v>
       </c>
-      <c r="Z9" s="18"/>
-      <c r="AA9" s="18"/>
-      <c r="AB9" s="18"/>
-      <c r="AC9" s="18"/>
-      <c r="AD9" s="18">
-        <v>0</v>
-      </c>
-      <c r="AE9" s="18"/>
-      <c r="AF9" s="18"/>
-    </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.45">
-      <c r="A10" s="18" t="s">
+      <c r="Z9" s="22"/>
+      <c r="AA9" s="22"/>
+      <c r="AB9" s="22"/>
+      <c r="AC9" s="22"/>
+      <c r="AD9" s="22">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="22"/>
+      <c r="AF9" s="22"/>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A10" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18" t="s">
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="18" t="s">
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="O10" s="18"/>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="18" t="s">
+      <c r="O10" s="22"/>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="R10" s="18"/>
-      <c r="S10" s="18"/>
-      <c r="T10" s="18" t="s">
+      <c r="R10" s="22"/>
+      <c r="S10" s="22"/>
+      <c r="T10" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="U10" s="18"/>
-      <c r="V10" s="18"/>
-      <c r="W10" s="18"/>
-      <c r="X10" s="18"/>
-      <c r="Y10" s="18" t="s">
+      <c r="U10" s="22"/>
+      <c r="V10" s="22"/>
+      <c r="W10" s="22"/>
+      <c r="X10" s="22"/>
+      <c r="Y10" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="Z10" s="18"/>
-      <c r="AA10" s="18"/>
-      <c r="AB10" s="18"/>
-      <c r="AC10" s="18"/>
-      <c r="AD10" s="18" t="s">
+      <c r="Z10" s="22"/>
+      <c r="AA10" s="22"/>
+      <c r="AB10" s="22"/>
+      <c r="AC10" s="22"/>
+      <c r="AD10" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="AE10" s="18"/>
-      <c r="AF10" s="18"/>
-    </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.45">
-      <c r="A11" s="18">
+      <c r="AE10" s="22"/>
+      <c r="AF10" s="22"/>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A11" s="22">
         <f>A9</f>
         <v>10</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="19">
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="23">
         <f>'Data package'!$B$31*I9+'Data package'!$B$28</f>
         <v>3.338709677419355</v>
       </c>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="19"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
       <c r="N11" s="20">
         <f ca="1">LOOKUP(N9,'Data package'!$D$21:$D$24,'Data package'!$E$22:$E$35)</f>
         <v>0</v>
       </c>
       <c r="O11" s="20"/>
       <c r="P11" s="20"/>
-      <c r="Q11" s="21">
+      <c r="Q11" s="24">
         <f>100/(2^3-1)*Q9</f>
         <v>42.857142857142861</v>
       </c>
-      <c r="R11" s="21"/>
-      <c r="S11" s="21"/>
-      <c r="T11" s="21">
+      <c r="R11" s="24"/>
+      <c r="S11" s="24"/>
+      <c r="T11" s="24">
         <f>'Data package'!$B$40*T9+'Data package'!$B$37</f>
         <v>22.903225806451616</v>
       </c>
@@ -3774,7 +3780,7 @@
       <c r="AE11" s="20"/>
       <c r="AF11" s="20"/>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -3787,85 +3793,85 @@
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.45">
-      <c r="A14" s="23" t="s">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A14" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="23"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="23"/>
-      <c r="L14" s="23"/>
-      <c r="M14" s="23"/>
-      <c r="N14" s="23"/>
-      <c r="O14" s="23"/>
-      <c r="P14" s="23"/>
-      <c r="Q14" s="23"/>
-      <c r="R14" s="23"/>
-      <c r="S14" s="23"/>
-      <c r="T14" s="23"/>
-      <c r="U14" s="23"/>
-      <c r="V14" s="23"/>
-      <c r="W14" s="23"/>
-      <c r="X14" s="23"/>
-      <c r="Y14" s="23"/>
-      <c r="Z14" s="23"/>
-      <c r="AA14" s="23"/>
-      <c r="AB14" s="23"/>
-      <c r="AC14" s="23"/>
-      <c r="AD14" s="23"/>
-      <c r="AE14" s="23"/>
-      <c r="AF14" s="23"/>
-    </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.45">
-      <c r="A15" s="22" t="s">
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="25"/>
+      <c r="M14" s="25"/>
+      <c r="N14" s="25"/>
+      <c r="O14" s="25"/>
+      <c r="P14" s="25"/>
+      <c r="Q14" s="25"/>
+      <c r="R14" s="25"/>
+      <c r="S14" s="25"/>
+      <c r="T14" s="25"/>
+      <c r="U14" s="25"/>
+      <c r="V14" s="25"/>
+      <c r="W14" s="25"/>
+      <c r="X14" s="25"/>
+      <c r="Y14" s="25"/>
+      <c r="Z14" s="25"/>
+      <c r="AA14" s="25"/>
+      <c r="AB14" s="25"/>
+      <c r="AC14" s="25"/>
+      <c r="AD14" s="25"/>
+      <c r="AE14" s="25"/>
+      <c r="AF14" s="25"/>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A15" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22" t="s">
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="J15" s="22"/>
-      <c r="K15" s="22"/>
-      <c r="L15" s="22"/>
-      <c r="M15" s="22"/>
-      <c r="N15" s="22"/>
-      <c r="O15" s="22"/>
-      <c r="P15" s="22"/>
-      <c r="Q15" s="22" t="s">
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="26"/>
+      <c r="O15" s="26"/>
+      <c r="P15" s="26"/>
+      <c r="Q15" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="R15" s="22"/>
-      <c r="S15" s="22"/>
-      <c r="T15" s="22"/>
-      <c r="U15" s="22"/>
-      <c r="V15" s="22"/>
-      <c r="W15" s="22"/>
-      <c r="X15" s="22"/>
-      <c r="Y15" s="22" t="s">
+      <c r="R15" s="26"/>
+      <c r="S15" s="26"/>
+      <c r="T15" s="26"/>
+      <c r="U15" s="26"/>
+      <c r="V15" s="26"/>
+      <c r="W15" s="26"/>
+      <c r="X15" s="26"/>
+      <c r="Y15" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="Z15" s="22"/>
-      <c r="AA15" s="22"/>
-      <c r="AB15" s="22"/>
-      <c r="AC15" s="22"/>
-      <c r="AD15" s="22"/>
-      <c r="AE15" s="22"/>
-      <c r="AF15" s="22"/>
-    </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="Z15" s="26"/>
+      <c r="AA15" s="26"/>
+      <c r="AB15" s="26"/>
+      <c r="AC15" s="26"/>
+      <c r="AD15" s="26"/>
+      <c r="AE15" s="26"/>
+      <c r="AF15" s="26"/>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
         <v>0</v>
       </c>
@@ -3963,183 +3969,183 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:96" x14ac:dyDescent="0.45">
-      <c r="A17" s="18" t="s">
+    <row r="17" spans="1:96" x14ac:dyDescent="0.3">
+      <c r="A17" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18" t="s">
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18"/>
-      <c r="N17" s="18" t="s">
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22"/>
+      <c r="N17" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="O17" s="18"/>
-      <c r="P17" s="18"/>
-      <c r="Q17" s="18" t="s">
+      <c r="O17" s="22"/>
+      <c r="P17" s="22"/>
+      <c r="Q17" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="R17" s="18"/>
-      <c r="S17" s="18"/>
-      <c r="T17" s="18" t="s">
+      <c r="R17" s="22"/>
+      <c r="S17" s="22"/>
+      <c r="T17" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="U17" s="18"/>
-      <c r="V17" s="18"/>
-      <c r="W17" s="18"/>
-      <c r="X17" s="18"/>
-      <c r="Y17" s="18" t="s">
+      <c r="U17" s="22"/>
+      <c r="V17" s="22"/>
+      <c r="W17" s="22"/>
+      <c r="X17" s="22"/>
+      <c r="Y17" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="Z17" s="18"/>
-      <c r="AA17" s="18"/>
-      <c r="AB17" s="18"/>
-      <c r="AC17" s="18"/>
-      <c r="AD17" s="18" t="s">
+      <c r="Z17" s="22"/>
+      <c r="AA17" s="22"/>
+      <c r="AB17" s="22"/>
+      <c r="AC17" s="22"/>
+      <c r="AD17" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="AE17" s="18"/>
-      <c r="AF17" s="18"/>
-    </row>
-    <row r="18" spans="1:96" x14ac:dyDescent="0.45">
-      <c r="A18" s="18">
+      <c r="AE17" s="22"/>
+      <c r="AF17" s="22"/>
+    </row>
+    <row r="18" spans="1:96" x14ac:dyDescent="0.3">
+      <c r="A18" s="22">
         <v>5</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18">
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22">
         <v>8</v>
       </c>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="18"/>
-      <c r="M18" s="18"/>
-      <c r="N18" s="18">
-        <v>0</v>
-      </c>
-      <c r="O18" s="18"/>
-      <c r="P18" s="18"/>
-      <c r="Q18" s="18">
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="22"/>
+      <c r="N18" s="22">
+        <v>0</v>
+      </c>
+      <c r="O18" s="22"/>
+      <c r="P18" s="22"/>
+      <c r="Q18" s="22">
         <v>3</v>
       </c>
-      <c r="R18" s="18"/>
-      <c r="S18" s="18"/>
-      <c r="T18" s="18">
+      <c r="R18" s="22"/>
+      <c r="S18" s="22"/>
+      <c r="T18" s="22">
         <v>19</v>
       </c>
-      <c r="U18" s="18"/>
-      <c r="V18" s="18"/>
-      <c r="W18" s="18"/>
-      <c r="X18" s="18"/>
-      <c r="Y18" s="18">
+      <c r="U18" s="22"/>
+      <c r="V18" s="22"/>
+      <c r="W18" s="22"/>
+      <c r="X18" s="22"/>
+      <c r="Y18" s="22">
         <v>17</v>
       </c>
-      <c r="Z18" s="18"/>
-      <c r="AA18" s="18"/>
-      <c r="AB18" s="18"/>
-      <c r="AC18" s="18"/>
-      <c r="AD18" s="18">
-        <v>0</v>
-      </c>
-      <c r="AE18" s="18"/>
-      <c r="AF18" s="18"/>
-    </row>
-    <row r="19" spans="1:96" x14ac:dyDescent="0.45">
-      <c r="A19" s="18" t="s">
+      <c r="Z18" s="22"/>
+      <c r="AA18" s="22"/>
+      <c r="AB18" s="22"/>
+      <c r="AC18" s="22"/>
+      <c r="AD18" s="22">
+        <v>0</v>
+      </c>
+      <c r="AE18" s="22"/>
+      <c r="AF18" s="22"/>
+    </row>
+    <row r="19" spans="1:96" x14ac:dyDescent="0.3">
+      <c r="A19" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18" t="s">
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
-      <c r="M19" s="18"/>
-      <c r="N19" s="18" t="s">
+      <c r="J19" s="22"/>
+      <c r="K19" s="22"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="22"/>
+      <c r="N19" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="O19" s="18"/>
-      <c r="P19" s="18"/>
-      <c r="Q19" s="18" t="s">
+      <c r="O19" s="22"/>
+      <c r="P19" s="22"/>
+      <c r="Q19" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="R19" s="18"/>
-      <c r="S19" s="18"/>
-      <c r="T19" s="18" t="s">
+      <c r="R19" s="22"/>
+      <c r="S19" s="22"/>
+      <c r="T19" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="U19" s="18"/>
-      <c r="V19" s="18"/>
-      <c r="W19" s="18"/>
-      <c r="X19" s="18"/>
-      <c r="Y19" s="18" t="s">
+      <c r="U19" s="22"/>
+      <c r="V19" s="22"/>
+      <c r="W19" s="22"/>
+      <c r="X19" s="22"/>
+      <c r="Y19" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="Z19" s="18"/>
-      <c r="AA19" s="18"/>
-      <c r="AB19" s="18"/>
-      <c r="AC19" s="18"/>
-      <c r="AD19" s="18" t="s">
+      <c r="Z19" s="22"/>
+      <c r="AA19" s="22"/>
+      <c r="AB19" s="22"/>
+      <c r="AC19" s="22"/>
+      <c r="AD19" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="AE19" s="18"/>
-      <c r="AF19" s="18"/>
-    </row>
-    <row r="20" spans="1:96" x14ac:dyDescent="0.45">
-      <c r="A20" s="18">
+      <c r="AE19" s="22"/>
+      <c r="AF19" s="22"/>
+    </row>
+    <row r="20" spans="1:96" x14ac:dyDescent="0.3">
+      <c r="A20" s="22">
         <f>A18</f>
         <v>5</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="19">
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="23">
         <f>'Data package'!$B$31*I18+'Data package'!$B$28</f>
         <v>3.3870967741935485</v>
       </c>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="19"/>
-      <c r="M20" s="19"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="23"/>
       <c r="N20" s="20">
         <f ca="1">LOOKUP(N18,'Data package'!$D$21:$D$24,'Data package'!$E$22:$E$35)</f>
         <v>0</v>
       </c>
       <c r="O20" s="20"/>
       <c r="P20" s="20"/>
-      <c r="Q20" s="21">
+      <c r="Q20" s="24">
         <f>100/(2^3-1)*Q18</f>
         <v>42.857142857142861</v>
       </c>
-      <c r="R20" s="21"/>
-      <c r="S20" s="21"/>
-      <c r="T20" s="21">
+      <c r="R20" s="24"/>
+      <c r="S20" s="24"/>
+      <c r="T20" s="24">
         <f>'Data package'!$B$40*T18+'Data package'!$B$37</f>
         <v>22.903225806451616</v>
       </c>
@@ -4162,165 +4168,165 @@
       <c r="AE20" s="20"/>
       <c r="AF20" s="20"/>
     </row>
-    <row r="23" spans="1:96" x14ac:dyDescent="0.45">
-      <c r="A23" s="23" t="s">
+    <row r="23" spans="1:96" x14ac:dyDescent="0.3">
+      <c r="A23" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="23"/>
-      <c r="M23" s="23"/>
-      <c r="N23" s="23"/>
-      <c r="O23" s="23"/>
-      <c r="P23" s="23"/>
-      <c r="Q23" s="23"/>
-      <c r="R23" s="23"/>
-      <c r="S23" s="23"/>
-      <c r="T23" s="23"/>
-      <c r="U23" s="23"/>
-      <c r="V23" s="23"/>
-      <c r="W23" s="23"/>
-      <c r="X23" s="23"/>
-      <c r="Y23" s="23"/>
-      <c r="Z23" s="23"/>
-      <c r="AA23" s="23"/>
-      <c r="AB23" s="23"/>
-      <c r="AC23" s="23"/>
-      <c r="AD23" s="23"/>
-      <c r="AE23" s="23"/>
-      <c r="AF23" s="23"/>
-    </row>
-    <row r="24" spans="1:96" x14ac:dyDescent="0.45">
-      <c r="A24" s="22" t="s">
+      <c r="B23" s="25"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="25"/>
+      <c r="K23" s="25"/>
+      <c r="L23" s="25"/>
+      <c r="M23" s="25"/>
+      <c r="N23" s="25"/>
+      <c r="O23" s="25"/>
+      <c r="P23" s="25"/>
+      <c r="Q23" s="25"/>
+      <c r="R23" s="25"/>
+      <c r="S23" s="25"/>
+      <c r="T23" s="25"/>
+      <c r="U23" s="25"/>
+      <c r="V23" s="25"/>
+      <c r="W23" s="25"/>
+      <c r="X23" s="25"/>
+      <c r="Y23" s="25"/>
+      <c r="Z23" s="25"/>
+      <c r="AA23" s="25"/>
+      <c r="AB23" s="25"/>
+      <c r="AC23" s="25"/>
+      <c r="AD23" s="25"/>
+      <c r="AE23" s="25"/>
+      <c r="AF23" s="25"/>
+    </row>
+    <row r="24" spans="1:96" x14ac:dyDescent="0.3">
+      <c r="A24" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="22"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="22" t="s">
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="J24" s="22"/>
-      <c r="K24" s="22"/>
-      <c r="L24" s="22"/>
-      <c r="M24" s="22"/>
-      <c r="N24" s="22"/>
-      <c r="O24" s="22"/>
-      <c r="P24" s="22"/>
-      <c r="Q24" s="22" t="s">
+      <c r="J24" s="26"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="26"/>
+      <c r="M24" s="26"/>
+      <c r="N24" s="26"/>
+      <c r="O24" s="26"/>
+      <c r="P24" s="26"/>
+      <c r="Q24" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="R24" s="22"/>
-      <c r="S24" s="22"/>
-      <c r="T24" s="22"/>
-      <c r="U24" s="22"/>
-      <c r="V24" s="22"/>
-      <c r="W24" s="22"/>
-      <c r="X24" s="22"/>
-      <c r="Y24" s="22" t="s">
+      <c r="R24" s="26"/>
+      <c r="S24" s="26"/>
+      <c r="T24" s="26"/>
+      <c r="U24" s="26"/>
+      <c r="V24" s="26"/>
+      <c r="W24" s="26"/>
+      <c r="X24" s="26"/>
+      <c r="Y24" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="Z24" s="22"/>
-      <c r="AA24" s="22"/>
-      <c r="AB24" s="22"/>
-      <c r="AC24" s="22"/>
-      <c r="AD24" s="22"/>
-      <c r="AE24" s="22"/>
-      <c r="AF24" s="22"/>
-      <c r="AG24" s="33">
+      <c r="Z24" s="26"/>
+      <c r="AA24" s="26"/>
+      <c r="AB24" s="26"/>
+      <c r="AC24" s="26"/>
+      <c r="AD24" s="26"/>
+      <c r="AE24" s="26"/>
+      <c r="AF24" s="26"/>
+      <c r="AG24" s="21">
         <v>59</v>
       </c>
-      <c r="AH24" s="33"/>
-      <c r="AI24" s="33"/>
-      <c r="AJ24" s="33"/>
-      <c r="AK24" s="33"/>
-      <c r="AL24" s="33"/>
-      <c r="AM24" s="33"/>
-      <c r="AN24" s="33"/>
-      <c r="AO24" s="33">
+      <c r="AH24" s="21"/>
+      <c r="AI24" s="21"/>
+      <c r="AJ24" s="21"/>
+      <c r="AK24" s="21"/>
+      <c r="AL24" s="21"/>
+      <c r="AM24" s="21"/>
+      <c r="AN24" s="21"/>
+      <c r="AO24" s="21">
         <v>96</v>
       </c>
-      <c r="AP24" s="33"/>
-      <c r="AQ24" s="33"/>
-      <c r="AR24" s="33"/>
-      <c r="AS24" s="33"/>
-      <c r="AT24" s="33"/>
-      <c r="AU24" s="33"/>
-      <c r="AV24" s="33"/>
-      <c r="AW24" s="33">
+      <c r="AP24" s="21"/>
+      <c r="AQ24" s="21"/>
+      <c r="AR24" s="21"/>
+      <c r="AS24" s="21"/>
+      <c r="AT24" s="21"/>
+      <c r="AU24" s="21"/>
+      <c r="AV24" s="21"/>
+      <c r="AW24" s="21">
         <v>65</v>
       </c>
-      <c r="AX24" s="33"/>
-      <c r="AY24" s="33"/>
-      <c r="AZ24" s="33"/>
-      <c r="BA24" s="33"/>
-      <c r="BB24" s="33"/>
-      <c r="BC24" s="33"/>
-      <c r="BD24" s="33"/>
-      <c r="BE24" s="33" t="s">
+      <c r="AX24" s="21"/>
+      <c r="AY24" s="21"/>
+      <c r="AZ24" s="21"/>
+      <c r="BA24" s="21"/>
+      <c r="BB24" s="21"/>
+      <c r="BC24" s="21"/>
+      <c r="BD24" s="21"/>
+      <c r="BE24" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="BF24" s="33"/>
-      <c r="BG24" s="33"/>
-      <c r="BH24" s="33"/>
-      <c r="BI24" s="33"/>
-      <c r="BJ24" s="33"/>
-      <c r="BK24" s="33"/>
-      <c r="BL24" s="33"/>
-      <c r="BM24" s="33" t="s">
+      <c r="BF24" s="21"/>
+      <c r="BG24" s="21"/>
+      <c r="BH24" s="21"/>
+      <c r="BI24" s="21"/>
+      <c r="BJ24" s="21"/>
+      <c r="BK24" s="21"/>
+      <c r="BL24" s="21"/>
+      <c r="BM24" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="BN24" s="33"/>
-      <c r="BO24" s="33"/>
-      <c r="BP24" s="33"/>
-      <c r="BQ24" s="33"/>
-      <c r="BR24" s="33"/>
-      <c r="BS24" s="33"/>
-      <c r="BT24" s="33"/>
-      <c r="BU24" s="33">
+      <c r="BN24" s="21"/>
+      <c r="BO24" s="21"/>
+      <c r="BP24" s="21"/>
+      <c r="BQ24" s="21"/>
+      <c r="BR24" s="21"/>
+      <c r="BS24" s="21"/>
+      <c r="BT24" s="21"/>
+      <c r="BU24" s="21">
         <v>69</v>
       </c>
-      <c r="BV24" s="33"/>
-      <c r="BW24" s="33"/>
-      <c r="BX24" s="33"/>
-      <c r="BY24" s="33"/>
-      <c r="BZ24" s="33"/>
-      <c r="CA24" s="33"/>
-      <c r="CB24" s="33"/>
-      <c r="CC24" s="33" t="s">
+      <c r="BV24" s="21"/>
+      <c r="BW24" s="21"/>
+      <c r="BX24" s="21"/>
+      <c r="BY24" s="21"/>
+      <c r="BZ24" s="21"/>
+      <c r="CA24" s="21"/>
+      <c r="CB24" s="21"/>
+      <c r="CC24" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="CD24" s="33"/>
-      <c r="CE24" s="33"/>
-      <c r="CF24" s="33"/>
-      <c r="CG24" s="33"/>
-      <c r="CH24" s="33"/>
-      <c r="CI24" s="33"/>
-      <c r="CJ24" s="33"/>
-      <c r="CK24" s="33" t="s">
+      <c r="CD24" s="21"/>
+      <c r="CE24" s="21"/>
+      <c r="CF24" s="21"/>
+      <c r="CG24" s="21"/>
+      <c r="CH24" s="21"/>
+      <c r="CI24" s="21"/>
+      <c r="CJ24" s="21"/>
+      <c r="CK24" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="CL24" s="33"/>
-      <c r="CM24" s="33"/>
-      <c r="CN24" s="33"/>
-      <c r="CO24" s="33"/>
-      <c r="CP24" s="33"/>
-      <c r="CQ24" s="33"/>
-      <c r="CR24" s="33"/>
-    </row>
-    <row r="25" spans="1:96" x14ac:dyDescent="0.45">
+      <c r="CL24" s="21"/>
+      <c r="CM24" s="21"/>
+      <c r="CN24" s="21"/>
+      <c r="CO24" s="21"/>
+      <c r="CP24" s="21"/>
+      <c r="CQ24" s="21"/>
+      <c r="CR24" s="21"/>
+    </row>
+    <row r="25" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A25" s="7">
         <v>0</v>
       </c>
@@ -4610,53 +4616,53 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:96" x14ac:dyDescent="0.45">
-      <c r="A26" s="18" t="s">
+    <row r="26" spans="1:96" x14ac:dyDescent="0.3">
+      <c r="A26" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="18" t="s">
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="J26" s="18"/>
-      <c r="K26" s="18"/>
-      <c r="L26" s="18"/>
-      <c r="M26" s="18"/>
-      <c r="N26" s="18" t="s">
+      <c r="J26" s="22"/>
+      <c r="K26" s="22"/>
+      <c r="L26" s="22"/>
+      <c r="M26" s="22"/>
+      <c r="N26" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="O26" s="18"/>
-      <c r="P26" s="18"/>
-      <c r="Q26" s="18" t="s">
+      <c r="O26" s="22"/>
+      <c r="P26" s="22"/>
+      <c r="Q26" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="R26" s="18"/>
-      <c r="S26" s="18"/>
-      <c r="T26" s="18" t="s">
+      <c r="R26" s="22"/>
+      <c r="S26" s="22"/>
+      <c r="T26" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="U26" s="18"/>
-      <c r="V26" s="18"/>
-      <c r="W26" s="18"/>
-      <c r="X26" s="18"/>
-      <c r="Y26" s="18" t="s">
+      <c r="U26" s="22"/>
+      <c r="V26" s="22"/>
+      <c r="W26" s="22"/>
+      <c r="X26" s="22"/>
+      <c r="Y26" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="Z26" s="18"/>
-      <c r="AA26" s="18"/>
-      <c r="AB26" s="18"/>
-      <c r="AC26" s="18"/>
-      <c r="AD26" s="18" t="s">
+      <c r="Z26" s="22"/>
+      <c r="AA26" s="22"/>
+      <c r="AB26" s="22"/>
+      <c r="AC26" s="22"/>
+      <c r="AD26" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="AE26" s="18"/>
-      <c r="AF26" s="18"/>
+      <c r="AE26" s="22"/>
+      <c r="AF26" s="22"/>
       <c r="AG26" s="20" t="s">
         <v>70</v>
       </c>
@@ -4738,53 +4744,53 @@
       <c r="CQ26" s="20"/>
       <c r="CR26" s="20"/>
     </row>
-    <row r="27" spans="1:96" x14ac:dyDescent="0.45">
-      <c r="A27" s="18">
+    <row r="27" spans="1:96" x14ac:dyDescent="0.3">
+      <c r="A27" s="22">
         <v>10</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18">
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22">
         <v>8</v>
       </c>
-      <c r="J27" s="18"/>
-      <c r="K27" s="18"/>
-      <c r="L27" s="18"/>
-      <c r="M27" s="18"/>
-      <c r="N27" s="18">
-        <v>0</v>
-      </c>
-      <c r="O27" s="18"/>
-      <c r="P27" s="18"/>
-      <c r="Q27" s="18">
+      <c r="J27" s="22"/>
+      <c r="K27" s="22"/>
+      <c r="L27" s="22"/>
+      <c r="M27" s="22"/>
+      <c r="N27" s="22">
+        <v>0</v>
+      </c>
+      <c r="O27" s="22"/>
+      <c r="P27" s="22"/>
+      <c r="Q27" s="22">
         <v>3</v>
       </c>
-      <c r="R27" s="18"/>
-      <c r="S27" s="18"/>
-      <c r="T27" s="18">
+      <c r="R27" s="22"/>
+      <c r="S27" s="22"/>
+      <c r="T27" s="22">
         <v>19</v>
       </c>
-      <c r="U27" s="18"/>
-      <c r="V27" s="18"/>
-      <c r="W27" s="18"/>
-      <c r="X27" s="18"/>
-      <c r="Y27" s="18">
+      <c r="U27" s="22"/>
+      <c r="V27" s="22"/>
+      <c r="W27" s="22"/>
+      <c r="X27" s="22"/>
+      <c r="Y27" s="22">
         <v>21</v>
       </c>
-      <c r="Z27" s="18"/>
-      <c r="AA27" s="18"/>
-      <c r="AB27" s="18"/>
-      <c r="AC27" s="18"/>
-      <c r="AD27" s="18">
-        <v>0</v>
-      </c>
-      <c r="AE27" s="18"/>
-      <c r="AF27" s="18"/>
+      <c r="Z27" s="22"/>
+      <c r="AA27" s="22"/>
+      <c r="AB27" s="22"/>
+      <c r="AC27" s="22"/>
+      <c r="AD27" s="22">
+        <v>0</v>
+      </c>
+      <c r="AE27" s="22"/>
+      <c r="AF27" s="22"/>
       <c r="AG27">
         <f>AN25</f>
         <v>1</v>
@@ -5042,53 +5048,53 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:96" x14ac:dyDescent="0.45">
-      <c r="A28" s="18" t="s">
+    <row r="28" spans="1:96" x14ac:dyDescent="0.3">
+      <c r="A28" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="18" t="s">
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="J28" s="18"/>
-      <c r="K28" s="18"/>
-      <c r="L28" s="18"/>
-      <c r="M28" s="18"/>
-      <c r="N28" s="18" t="s">
+      <c r="J28" s="22"/>
+      <c r="K28" s="22"/>
+      <c r="L28" s="22"/>
+      <c r="M28" s="22"/>
+      <c r="N28" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="O28" s="18"/>
-      <c r="P28" s="18"/>
-      <c r="Q28" s="18" t="s">
+      <c r="O28" s="22"/>
+      <c r="P28" s="22"/>
+      <c r="Q28" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="R28" s="18"/>
-      <c r="S28" s="18"/>
-      <c r="T28" s="18" t="s">
+      <c r="R28" s="22"/>
+      <c r="S28" s="22"/>
+      <c r="T28" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="U28" s="18"/>
-      <c r="V28" s="18"/>
-      <c r="W28" s="18"/>
-      <c r="X28" s="18"/>
-      <c r="Y28" s="18" t="s">
+      <c r="U28" s="22"/>
+      <c r="V28" s="22"/>
+      <c r="W28" s="22"/>
+      <c r="X28" s="22"/>
+      <c r="Y28" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="Z28" s="18"/>
-      <c r="AA28" s="18"/>
-      <c r="AB28" s="18"/>
-      <c r="AC28" s="18"/>
-      <c r="AD28" s="18" t="s">
+      <c r="Z28" s="22"/>
+      <c r="AA28" s="22"/>
+      <c r="AB28" s="22"/>
+      <c r="AC28" s="22"/>
+      <c r="AD28" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="AE28" s="18"/>
-      <c r="AF28" s="18"/>
+      <c r="AE28" s="22"/>
+      <c r="AF28" s="22"/>
       <c r="AG28" s="20" t="s">
         <v>71</v>
       </c>
@@ -5170,39 +5176,39 @@
       <c r="CM28" s="20"/>
       <c r="CN28" s="20"/>
     </row>
-    <row r="29" spans="1:96" x14ac:dyDescent="0.45">
-      <c r="A29" s="18">
+    <row r="29" spans="1:96" x14ac:dyDescent="0.3">
+      <c r="A29" s="22">
         <f>A27</f>
         <v>10</v>
       </c>
-      <c r="B29" s="18"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="18"/>
-      <c r="I29" s="19">
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="23">
         <f>'Data package'!$B$31*I27+'Data package'!$B$28</f>
         <v>3.3870967741935485</v>
       </c>
-      <c r="J29" s="19"/>
-      <c r="K29" s="19"/>
-      <c r="L29" s="19"/>
-      <c r="M29" s="19"/>
+      <c r="J29" s="23"/>
+      <c r="K29" s="23"/>
+      <c r="L29" s="23"/>
+      <c r="M29" s="23"/>
       <c r="N29" s="20">
         <f ca="1">LOOKUP(N27,'Data package'!$D$21:$D$24,'Data package'!$E$22:$E$35)</f>
         <v>0</v>
       </c>
       <c r="O29" s="20"/>
       <c r="P29" s="20"/>
-      <c r="Q29" s="21">
+      <c r="Q29" s="24">
         <f>100/(2^3-1)*Q27</f>
         <v>42.857142857142861</v>
       </c>
-      <c r="R29" s="21"/>
-      <c r="S29" s="21"/>
-      <c r="T29" s="21">
+      <c r="R29" s="24"/>
+      <c r="S29" s="24"/>
+      <c r="T29" s="24">
         <f>'Data package'!$B$40*T27+'Data package'!$B$37</f>
         <v>22.903225806451616</v>
       </c>
@@ -5305,7 +5311,7 @@
       <c r="CM29" s="20"/>
       <c r="CN29" s="20"/>
     </row>
-    <row r="30" spans="1:96" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:96" x14ac:dyDescent="0.3">
       <c r="AG30">
         <f>AL27</f>
         <v>0</v>
@@ -5547,7 +5553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:96" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:96" x14ac:dyDescent="0.3">
       <c r="AG31" s="20" t="s">
         <v>81</v>
       </c>
@@ -5629,7 +5635,7 @@
       <c r="CM31" s="20"/>
       <c r="CN31" s="20"/>
     </row>
-    <row r="32" spans="1:96" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:96" x14ac:dyDescent="0.3">
       <c r="AG32" s="20">
         <v>25</v>
       </c>
@@ -5713,90 +5719,64 @@
     </row>
   </sheetData>
   <mergeCells count="166">
-    <mergeCell ref="BK32:BP32"/>
-    <mergeCell ref="BQ32:BV32"/>
-    <mergeCell ref="BW32:CB32"/>
-    <mergeCell ref="CC32:CH32"/>
-    <mergeCell ref="CI32:CN32"/>
-    <mergeCell ref="AG32:AL32"/>
-    <mergeCell ref="AM32:AR32"/>
-    <mergeCell ref="AS32:AX32"/>
-    <mergeCell ref="AY32:BD32"/>
-    <mergeCell ref="BE32:BJ32"/>
-    <mergeCell ref="BK31:BP31"/>
-    <mergeCell ref="BQ31:BV31"/>
-    <mergeCell ref="BW31:CB31"/>
-    <mergeCell ref="CC31:CH31"/>
-    <mergeCell ref="CI31:CN31"/>
-    <mergeCell ref="AG31:AL31"/>
-    <mergeCell ref="AM31:AR31"/>
-    <mergeCell ref="AS31:AX31"/>
-    <mergeCell ref="AY31:BD31"/>
-    <mergeCell ref="BE31:BJ31"/>
-    <mergeCell ref="BK29:BP29"/>
-    <mergeCell ref="BQ29:BV29"/>
-    <mergeCell ref="BW29:CB29"/>
-    <mergeCell ref="CC29:CH29"/>
-    <mergeCell ref="CI29:CN29"/>
-    <mergeCell ref="AG29:AL29"/>
-    <mergeCell ref="AM29:AR29"/>
-    <mergeCell ref="AS29:AX29"/>
-    <mergeCell ref="AY29:BD29"/>
-    <mergeCell ref="BE29:BJ29"/>
-    <mergeCell ref="BK28:BP28"/>
-    <mergeCell ref="BQ28:BV28"/>
-    <mergeCell ref="BW28:CB28"/>
-    <mergeCell ref="CC28:CH28"/>
-    <mergeCell ref="CI28:CN28"/>
-    <mergeCell ref="AG28:AL28"/>
-    <mergeCell ref="AM28:AR28"/>
-    <mergeCell ref="AS28:AX28"/>
-    <mergeCell ref="AY28:BD28"/>
-    <mergeCell ref="BE28:BJ28"/>
-    <mergeCell ref="BU24:CB24"/>
-    <mergeCell ref="CC24:CJ24"/>
-    <mergeCell ref="CK24:CR24"/>
-    <mergeCell ref="AG26:AN26"/>
-    <mergeCell ref="AO26:AV26"/>
-    <mergeCell ref="AW26:BD26"/>
-    <mergeCell ref="BE26:BL26"/>
-    <mergeCell ref="BM26:BT26"/>
-    <mergeCell ref="BU26:CB26"/>
-    <mergeCell ref="CC26:CJ26"/>
-    <mergeCell ref="CK26:CR26"/>
-    <mergeCell ref="AG24:AN24"/>
-    <mergeCell ref="AO24:AV24"/>
-    <mergeCell ref="AW24:BD24"/>
-    <mergeCell ref="BE24:BL24"/>
-    <mergeCell ref="BM24:BT24"/>
-    <mergeCell ref="Y28:AC28"/>
-    <mergeCell ref="AD28:AF28"/>
-    <mergeCell ref="A29:H29"/>
-    <mergeCell ref="I29:M29"/>
-    <mergeCell ref="N29:P29"/>
-    <mergeCell ref="Q29:S29"/>
-    <mergeCell ref="T29:X29"/>
-    <mergeCell ref="Y29:AC29"/>
-    <mergeCell ref="AD29:AF29"/>
-    <mergeCell ref="A28:H28"/>
-    <mergeCell ref="I28:M28"/>
-    <mergeCell ref="N28:P28"/>
-    <mergeCell ref="Q28:S28"/>
-    <mergeCell ref="T28:X28"/>
-    <mergeCell ref="Y26:AC26"/>
-    <mergeCell ref="AD26:AF26"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="I27:M27"/>
-    <mergeCell ref="N27:P27"/>
-    <mergeCell ref="Q27:S27"/>
-    <mergeCell ref="T27:X27"/>
-    <mergeCell ref="Y27:AC27"/>
-    <mergeCell ref="AD27:AF27"/>
-    <mergeCell ref="A26:H26"/>
-    <mergeCell ref="I26:M26"/>
-    <mergeCell ref="N26:P26"/>
-    <mergeCell ref="Q26:S26"/>
-    <mergeCell ref="T26:X26"/>
+    <mergeCell ref="Y19:AC19"/>
+    <mergeCell ref="AD19:AF19"/>
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="I20:M20"/>
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="Q20:S20"/>
+    <mergeCell ref="T20:X20"/>
+    <mergeCell ref="Y20:AC20"/>
+    <mergeCell ref="AD20:AF20"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="I19:M19"/>
+    <mergeCell ref="N19:P19"/>
+    <mergeCell ref="Q19:S19"/>
+    <mergeCell ref="T19:X19"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="I15:P15"/>
+    <mergeCell ref="Q15:X15"/>
+    <mergeCell ref="Y15:AF15"/>
+    <mergeCell ref="A14:AF14"/>
+    <mergeCell ref="Y17:AC17"/>
+    <mergeCell ref="AD17:AF17"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="I18:M18"/>
+    <mergeCell ref="N18:P18"/>
+    <mergeCell ref="Q18:S18"/>
+    <mergeCell ref="T18:X18"/>
+    <mergeCell ref="Y18:AC18"/>
+    <mergeCell ref="AD18:AF18"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="I17:M17"/>
+    <mergeCell ref="N17:P17"/>
+    <mergeCell ref="Q17:S17"/>
+    <mergeCell ref="T17:X17"/>
+    <mergeCell ref="I11:M11"/>
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="I10:M10"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="AD10:AF10"/>
+    <mergeCell ref="Y10:AC10"/>
+    <mergeCell ref="T10:X10"/>
+    <mergeCell ref="Q10:S10"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="AD11:AF11"/>
+    <mergeCell ref="Y11:AC11"/>
+    <mergeCell ref="T11:X11"/>
+    <mergeCell ref="Q11:S11"/>
+    <mergeCell ref="N11:P11"/>
+    <mergeCell ref="Q6:X6"/>
+    <mergeCell ref="Y6:AF6"/>
+    <mergeCell ref="AD9:AF9"/>
+    <mergeCell ref="AD8:AF8"/>
+    <mergeCell ref="Y9:AC9"/>
+    <mergeCell ref="Y8:AC8"/>
+    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="T8:X8"/>
+    <mergeCell ref="T9:X9"/>
     <mergeCell ref="A23:AF23"/>
     <mergeCell ref="A24:H24"/>
     <mergeCell ref="I24:P24"/>
@@ -5821,64 +5801,90 @@
     <mergeCell ref="I8:M8"/>
     <mergeCell ref="N8:P8"/>
     <mergeCell ref="I9:M9"/>
-    <mergeCell ref="Q6:X6"/>
-    <mergeCell ref="Y6:AF6"/>
-    <mergeCell ref="AD9:AF9"/>
-    <mergeCell ref="AD8:AF8"/>
-    <mergeCell ref="Y9:AC9"/>
-    <mergeCell ref="Y8:AC8"/>
-    <mergeCell ref="N9:P9"/>
-    <mergeCell ref="Q8:S8"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="T8:X8"/>
-    <mergeCell ref="T9:X9"/>
-    <mergeCell ref="I11:M11"/>
-    <mergeCell ref="A11:H11"/>
-    <mergeCell ref="I10:M10"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="AD10:AF10"/>
-    <mergeCell ref="Y10:AC10"/>
-    <mergeCell ref="T10:X10"/>
-    <mergeCell ref="Q10:S10"/>
-    <mergeCell ref="N10:P10"/>
-    <mergeCell ref="AD11:AF11"/>
-    <mergeCell ref="Y11:AC11"/>
-    <mergeCell ref="T11:X11"/>
-    <mergeCell ref="Q11:S11"/>
-    <mergeCell ref="N11:P11"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="I15:P15"/>
-    <mergeCell ref="Q15:X15"/>
-    <mergeCell ref="Y15:AF15"/>
-    <mergeCell ref="A14:AF14"/>
-    <mergeCell ref="Y17:AC17"/>
-    <mergeCell ref="AD17:AF17"/>
-    <mergeCell ref="A18:H18"/>
-    <mergeCell ref="I18:M18"/>
-    <mergeCell ref="N18:P18"/>
-    <mergeCell ref="Q18:S18"/>
-    <mergeCell ref="T18:X18"/>
-    <mergeCell ref="Y18:AC18"/>
-    <mergeCell ref="AD18:AF18"/>
-    <mergeCell ref="A17:H17"/>
-    <mergeCell ref="I17:M17"/>
-    <mergeCell ref="N17:P17"/>
-    <mergeCell ref="Q17:S17"/>
-    <mergeCell ref="T17:X17"/>
-    <mergeCell ref="Y19:AC19"/>
-    <mergeCell ref="AD19:AF19"/>
-    <mergeCell ref="A20:H20"/>
-    <mergeCell ref="I20:M20"/>
-    <mergeCell ref="N20:P20"/>
-    <mergeCell ref="Q20:S20"/>
-    <mergeCell ref="T20:X20"/>
-    <mergeCell ref="Y20:AC20"/>
-    <mergeCell ref="AD20:AF20"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="I19:M19"/>
-    <mergeCell ref="N19:P19"/>
-    <mergeCell ref="Q19:S19"/>
-    <mergeCell ref="T19:X19"/>
+    <mergeCell ref="Y26:AC26"/>
+    <mergeCell ref="AD26:AF26"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="I27:M27"/>
+    <mergeCell ref="N27:P27"/>
+    <mergeCell ref="Q27:S27"/>
+    <mergeCell ref="T27:X27"/>
+    <mergeCell ref="Y27:AC27"/>
+    <mergeCell ref="AD27:AF27"/>
+    <mergeCell ref="A26:H26"/>
+    <mergeCell ref="I26:M26"/>
+    <mergeCell ref="N26:P26"/>
+    <mergeCell ref="Q26:S26"/>
+    <mergeCell ref="T26:X26"/>
+    <mergeCell ref="Y28:AC28"/>
+    <mergeCell ref="AD28:AF28"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="I29:M29"/>
+    <mergeCell ref="N29:P29"/>
+    <mergeCell ref="Q29:S29"/>
+    <mergeCell ref="T29:X29"/>
+    <mergeCell ref="Y29:AC29"/>
+    <mergeCell ref="AD29:AF29"/>
+    <mergeCell ref="A28:H28"/>
+    <mergeCell ref="I28:M28"/>
+    <mergeCell ref="N28:P28"/>
+    <mergeCell ref="Q28:S28"/>
+    <mergeCell ref="T28:X28"/>
+    <mergeCell ref="BU24:CB24"/>
+    <mergeCell ref="CC24:CJ24"/>
+    <mergeCell ref="CK24:CR24"/>
+    <mergeCell ref="AG26:AN26"/>
+    <mergeCell ref="AO26:AV26"/>
+    <mergeCell ref="AW26:BD26"/>
+    <mergeCell ref="BE26:BL26"/>
+    <mergeCell ref="BM26:BT26"/>
+    <mergeCell ref="BU26:CB26"/>
+    <mergeCell ref="CC26:CJ26"/>
+    <mergeCell ref="CK26:CR26"/>
+    <mergeCell ref="AG24:AN24"/>
+    <mergeCell ref="AO24:AV24"/>
+    <mergeCell ref="AW24:BD24"/>
+    <mergeCell ref="BE24:BL24"/>
+    <mergeCell ref="BM24:BT24"/>
+    <mergeCell ref="BK28:BP28"/>
+    <mergeCell ref="BQ28:BV28"/>
+    <mergeCell ref="BW28:CB28"/>
+    <mergeCell ref="CC28:CH28"/>
+    <mergeCell ref="CI28:CN28"/>
+    <mergeCell ref="AG28:AL28"/>
+    <mergeCell ref="AM28:AR28"/>
+    <mergeCell ref="AS28:AX28"/>
+    <mergeCell ref="AY28:BD28"/>
+    <mergeCell ref="BE28:BJ28"/>
+    <mergeCell ref="BK29:BP29"/>
+    <mergeCell ref="BQ29:BV29"/>
+    <mergeCell ref="BW29:CB29"/>
+    <mergeCell ref="CC29:CH29"/>
+    <mergeCell ref="CI29:CN29"/>
+    <mergeCell ref="AG29:AL29"/>
+    <mergeCell ref="AM29:AR29"/>
+    <mergeCell ref="AS29:AX29"/>
+    <mergeCell ref="AY29:BD29"/>
+    <mergeCell ref="BE29:BJ29"/>
+    <mergeCell ref="BK31:BP31"/>
+    <mergeCell ref="BQ31:BV31"/>
+    <mergeCell ref="BW31:CB31"/>
+    <mergeCell ref="CC31:CH31"/>
+    <mergeCell ref="CI31:CN31"/>
+    <mergeCell ref="AG31:AL31"/>
+    <mergeCell ref="AM31:AR31"/>
+    <mergeCell ref="AS31:AX31"/>
+    <mergeCell ref="AY31:BD31"/>
+    <mergeCell ref="BE31:BJ31"/>
+    <mergeCell ref="BK32:BP32"/>
+    <mergeCell ref="BQ32:BV32"/>
+    <mergeCell ref="BW32:CB32"/>
+    <mergeCell ref="CC32:CH32"/>
+    <mergeCell ref="CI32:CN32"/>
+    <mergeCell ref="AG32:AL32"/>
+    <mergeCell ref="AM32:AR32"/>
+    <mergeCell ref="AS32:AX32"/>
+    <mergeCell ref="AY32:BD32"/>
+    <mergeCell ref="BE32:BJ32"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -5893,58 +5899,58 @@
       <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.86328125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="4.796875" style="7" customWidth="1"/>
-    <col min="3" max="3" width="8.46484375" style="7" customWidth="1"/>
-    <col min="4" max="9" width="5.53125" style="7" customWidth="1"/>
-    <col min="10" max="10" width="11.53125" style="7"/>
-    <col min="11" max="11" width="4.796875" style="7" customWidth="1"/>
-    <col min="12" max="12" width="8.46484375" style="7" customWidth="1"/>
-    <col min="13" max="18" width="5.53125" style="7" customWidth="1"/>
-    <col min="19" max="16384" width="11.53125" style="7"/>
+    <col min="1" max="1" width="5.88671875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="4.77734375" style="7" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" style="7" customWidth="1"/>
+    <col min="4" max="9" width="5.5546875" style="7" customWidth="1"/>
+    <col min="10" max="10" width="11.5546875" style="7"/>
+    <col min="11" max="11" width="4.77734375" style="7" customWidth="1"/>
+    <col min="12" max="12" width="8.44140625" style="7" customWidth="1"/>
+    <col min="13" max="18" width="5.5546875" style="7" customWidth="1"/>
+    <col min="19" max="16384" width="11.5546875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" x14ac:dyDescent="0.45">
-      <c r="B1" s="18" t="s">
+    <row r="1" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B1" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
       <c r="E1" s="7">
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.45">
-      <c r="B3" s="34" t="s">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B3" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34" t="s">
+      <c r="C3" s="36"/>
+      <c r="D3" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
-      <c r="K3" s="34" t="s">
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="K3" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="L3" s="34"/>
-      <c r="M3" s="34" t="s">
+      <c r="L3" s="36"/>
+      <c r="M3" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="N3" s="34"/>
-      <c r="O3" s="34"/>
-      <c r="P3" s="34"/>
-      <c r="Q3" s="34"/>
-      <c r="R3" s="34"/>
-    </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.45">
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
+      <c r="N3" s="36"/>
+      <c r="O3" s="36"/>
+      <c r="P3" s="36"/>
+      <c r="Q3" s="36"/>
+      <c r="R3" s="36"/>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
       <c r="D4" s="11">
         <v>0.01</v>
       </c>
@@ -5963,8 +5969,8 @@
       <c r="I4" s="11">
         <v>10</v>
       </c>
-      <c r="K4" s="34"/>
-      <c r="L4" s="34"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
       <c r="M4" s="11">
         <v>0.01</v>
       </c>
@@ -5984,8 +5990,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.45">
-      <c r="B5" s="35" t="s">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B5" s="37" t="s">
         <v>41</v>
       </c>
       <c r="C5" s="11">
@@ -6015,7 +6021,7 @@
         <f t="shared" si="0"/>
         <v>1E-3</v>
       </c>
-      <c r="K5" s="35" t="s">
+      <c r="K5" s="37" t="s">
         <v>41</v>
       </c>
       <c r="L5" s="11">
@@ -6046,8 +6052,8 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.45">
-      <c r="B6" s="35"/>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B6" s="37"/>
       <c r="C6" s="11">
         <v>0.02</v>
       </c>
@@ -6075,7 +6081,7 @@
         <f t="shared" si="2"/>
         <v>2E-3</v>
       </c>
-      <c r="K6" s="35"/>
+      <c r="K6" s="37"/>
       <c r="L6" s="11">
         <v>0.02</v>
       </c>
@@ -6104,8 +6110,8 @@
         <v>4.0000000000000003E-5</v>
       </c>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.45">
-      <c r="B7" s="35"/>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B7" s="37"/>
       <c r="C7" s="11">
         <v>0.03</v>
       </c>
@@ -6133,7 +6139,7 @@
         <f t="shared" si="2"/>
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="K7" s="35"/>
+      <c r="K7" s="37"/>
       <c r="L7" s="11">
         <v>0.03</v>
       </c>
@@ -6162,8 +6168,8 @@
         <v>8.9999999999999992E-5</v>
       </c>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.45">
-      <c r="B8" s="35"/>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B8" s="37"/>
       <c r="C8" s="11">
         <v>0.05</v>
       </c>
@@ -6191,7 +6197,7 @@
         <f t="shared" si="2"/>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="K8" s="35"/>
+      <c r="K8" s="37"/>
       <c r="L8" s="11">
         <v>0.05</v>
       </c>
@@ -6220,8 +6226,8 @@
         <v>2.5000000000000001E-4</v>
       </c>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.45">
-      <c r="B9" s="35"/>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B9" s="37"/>
       <c r="C9" s="11">
         <v>0.1</v>
       </c>
@@ -6249,7 +6255,7 @@
         <f t="shared" si="2"/>
         <v>0.01</v>
       </c>
-      <c r="K9" s="35"/>
+      <c r="K9" s="37"/>
       <c r="L9" s="11">
         <v>0.1</v>
       </c>
@@ -6278,8 +6284,8 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.45">
-      <c r="B10" s="35"/>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B10" s="37"/>
       <c r="C10" s="11">
         <v>0.2</v>
       </c>
@@ -6307,7 +6313,7 @@
         <f t="shared" si="2"/>
         <v>0.02</v>
       </c>
-      <c r="K10" s="35"/>
+      <c r="K10" s="37"/>
       <c r="L10" s="11">
         <v>0.2</v>
       </c>
@@ -6336,8 +6342,8 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.45">
-      <c r="B11" s="35"/>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B11" s="37"/>
       <c r="C11" s="11">
         <v>0.3</v>
       </c>
@@ -6365,7 +6371,7 @@
         <f t="shared" si="2"/>
         <v>0.03</v>
       </c>
-      <c r="K11" s="35"/>
+      <c r="K11" s="37"/>
       <c r="L11" s="11">
         <v>0.3</v>
       </c>
@@ -6394,8 +6400,8 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.45">
-      <c r="B12" s="35"/>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B12" s="37"/>
       <c r="C12" s="11">
         <v>0.5</v>
       </c>
@@ -6423,7 +6429,7 @@
         <f t="shared" si="2"/>
         <v>0.05</v>
       </c>
-      <c r="K12" s="35"/>
+      <c r="K12" s="37"/>
       <c r="L12" s="11">
         <v>0.5</v>
       </c>
@@ -6452,8 +6458,8 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.45">
-      <c r="B13" s="35"/>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B13" s="37"/>
       <c r="C13" s="11">
         <v>1</v>
       </c>
@@ -6481,7 +6487,7 @@
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="K13" s="35"/>
+      <c r="K13" s="37"/>
       <c r="L13" s="11">
         <v>1</v>
       </c>
@@ -6538,14 +6544,14 @@
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>4.2</v>
       </c>
@@ -6553,7 +6559,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>4.0999999999999996</v>
       </c>
@@ -6561,7 +6567,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
@@ -6569,7 +6575,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3.9</v>
       </c>
@@ -6577,7 +6583,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3.8</v>
       </c>
@@ -6585,7 +6591,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>3.7</v>
       </c>
@@ -6593,7 +6599,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>3.6</v>
       </c>
@@ -6601,7 +6607,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>3.5</v>
       </c>
@@ -6609,7 +6615,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>3.4</v>
       </c>
@@ -6617,7 +6623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>3.3</v>
       </c>
@@ -6625,7 +6631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>3.19999999999999</v>
       </c>
@@ -6633,7 +6639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>3.0999999999999899</v>
       </c>
@@ -6655,35 +6661,35 @@
       <selection activeCell="I6" sqref="I6:S11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="19" width="4.19921875" customWidth="1"/>
+    <col min="1" max="19" width="4.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
       <c r="Q1" s="7"/>
       <c r="R1" s="7"/>
       <c r="S1" s="7"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>7</v>
       </c>
@@ -6736,34 +6742,34 @@
       <c r="R2" s="7"/>
       <c r="S2" s="7"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A3" s="30" t="s">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="30" t="s">
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="31"/>
-      <c r="K3" s="31"/>
-      <c r="L3" s="31"/>
-      <c r="M3" s="31"/>
-      <c r="N3" s="30" t="s">
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="O3" s="31"/>
-      <c r="P3" s="32"/>
+      <c r="O3" s="34"/>
+      <c r="P3" s="35"/>
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
       <c r="S3" s="7"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -6784,7 +6790,7 @@
       <c r="R4" s="7"/>
       <c r="S4" s="7"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -6805,7 +6811,7 @@
       <c r="R5" s="7"/>
       <c r="S5" s="7"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -6814,23 +6820,23 @@
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
-      <c r="I6" s="23" t="s">
+      <c r="I6" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="25"/>
+      <c r="P6" s="25"/>
       <c r="Q6" s="7"/>
-      <c r="R6" s="18" t="s">
+      <c r="R6" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="S6" s="18"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="S6" s="22"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -6866,12 +6872,12 @@
       <c r="Q7" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="R7" s="36" t="s">
+      <c r="R7" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="S7" s="36"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="S7" s="38"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -6880,23 +6886,23 @@
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
-      <c r="I8" s="18" t="s">
+      <c r="I8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18" t="s">
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="O8" s="18"/>
-      <c r="P8" s="18"/>
+      <c r="O8" s="22"/>
+      <c r="P8" s="22"/>
       <c r="Q8" s="7"/>
       <c r="R8" s="7"/>
       <c r="S8" s="7"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -6905,23 +6911,23 @@
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
-      <c r="I9" s="18">
+      <c r="I9" s="22">
         <v>17</v>
       </c>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="18">
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22">
         <v>4</v>
       </c>
-      <c r="O9" s="18"/>
-      <c r="P9" s="18"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="22"/>
       <c r="Q9" s="7"/>
       <c r="R9" s="7"/>
       <c r="S9" s="7"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -6935,16 +6941,16 @@
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
-      <c r="N10" s="18" t="s">
+      <c r="N10" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="O10" s="18"/>
-      <c r="P10" s="18"/>
+      <c r="O10" s="22"/>
+      <c r="P10" s="22"/>
       <c r="Q10" s="7"/>
       <c r="R10" s="7"/>
       <c r="S10" s="7"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -6958,24 +6964,18 @@
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
-      <c r="N11" s="19">
+      <c r="N11" s="23">
         <f>100/(2^3-1)*N9</f>
         <v>57.142857142857146</v>
       </c>
-      <c r="O11" s="19"/>
-      <c r="P11" s="19"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="23"/>
       <c r="Q11" s="7"/>
       <c r="R11" s="7"/>
       <c r="S11" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="I3:M3"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="I6:P6"/>
     <mergeCell ref="N11:P11"/>
     <mergeCell ref="R7:S7"/>
     <mergeCell ref="I8:M8"/>
@@ -6983,6 +6983,12 @@
     <mergeCell ref="I9:M9"/>
     <mergeCell ref="N9:P9"/>
     <mergeCell ref="N10:P10"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="I3:M3"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="I6:P6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
time sync bug fixed and downlink post request example script created
</commit_message>
<xml_diff>
--- a/hardware/BikeCounterPro/src/dataPackage/DataPackage.xlsx
+++ b/hardware/BikeCounterPro/src/dataPackage/DataPackage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meier\Documents\repos\lora\hardware\BikeCounterPro\src\dataPackage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1029DD3A-FE16-4E2B-95EB-35D4C9543096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B8C60FE-EBC7-424D-8F24-3A881E03F713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="41172" yWindow="-108" windowWidth="41496" windowHeight="16896" xr2:uid="{CDF7A0A5-12B1-43F1-AFDE-54CA91221B4B}"/>
   </bookViews>
@@ -648,24 +648,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -694,6 +691,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2154,8 +2154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{088FF0E6-8FE4-49E3-812F-B76B934E1ACD}">
   <dimension ref="A1:S90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2546,6 +2546,10 @@
         <f>B30/(2^B27-1)</f>
         <v>4.8387096774193547E-2</v>
       </c>
+      <c r="F31">
+        <f>F30-F28</f>
+        <v>252460800</v>
+      </c>
       <c r="G31">
         <f>G30-G28</f>
         <v>4207680</v>
@@ -2567,6 +2571,10 @@
         <f>B18-B27</f>
         <v>384</v>
       </c>
+      <c r="F32">
+        <f>_xlfn.CEILING.MATH(LOG10(F31)/LOG(2))</f>
+        <v>28</v>
+      </c>
       <c r="G32">
         <f>_xlfn.CEILING.MATH(LOG10(G31)/LOG(2))</f>
         <v>23</v>
@@ -2604,8 +2612,12 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F34" t="s">
+      <c r="E34" t="s">
         <v>104</v>
+      </c>
+      <c r="F34">
+        <f>F33-F28</f>
+        <v>567993600</v>
       </c>
       <c r="G34" s="18">
         <f>G33-G28</f>
@@ -2624,8 +2636,12 @@
       <c r="A35" t="s">
         <v>37</v>
       </c>
-      <c r="F35" t="s">
+      <c r="E35" t="s">
         <v>105</v>
+      </c>
+      <c r="F35">
+        <f>_xlfn.CEILING.MATH(LOG10(F34)/LOG(2))</f>
+        <v>30</v>
       </c>
       <c r="G35" s="18">
         <f>_xlfn.CEILING.MATH(LOG10(G34)/LOG(2))</f>
@@ -3197,46 +3213,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="27" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="27" t="s">
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
-      <c r="X1" s="29"/>
-      <c r="Y1" s="27" t="s">
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
+      <c r="T1" s="27"/>
+      <c r="U1" s="27"/>
+      <c r="V1" s="27"/>
+      <c r="W1" s="27"/>
+      <c r="X1" s="28"/>
+      <c r="Y1" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="Z1" s="28"/>
-      <c r="AA1" s="28"/>
-      <c r="AB1" s="28"/>
-      <c r="AC1" s="28"/>
-      <c r="AD1" s="28"/>
-      <c r="AE1" s="28"/>
-      <c r="AF1" s="29"/>
+      <c r="Z1" s="27"/>
+      <c r="AA1" s="27"/>
+      <c r="AB1" s="27"/>
+      <c r="AC1" s="27"/>
+      <c r="AD1" s="27"/>
+      <c r="AE1" s="27"/>
+      <c r="AF1" s="28"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
@@ -3337,52 +3353,52 @@
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="33" t="s">
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="34"/>
-      <c r="N3" s="33" t="s">
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="O3" s="34"/>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="33" t="s">
+      <c r="O3" s="33"/>
+      <c r="P3" s="34"/>
+      <c r="Q3" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="R3" s="34"/>
-      <c r="S3" s="35"/>
-      <c r="T3" s="30" t="s">
+      <c r="R3" s="33"/>
+      <c r="S3" s="34"/>
+      <c r="T3" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="U3" s="31"/>
-      <c r="V3" s="31"/>
-      <c r="W3" s="31"/>
-      <c r="X3" s="32"/>
-      <c r="Y3" s="30" t="s">
+      <c r="U3" s="30"/>
+      <c r="V3" s="30"/>
+      <c r="W3" s="30"/>
+      <c r="X3" s="31"/>
+      <c r="Y3" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="Z3" s="31"/>
-      <c r="AA3" s="31"/>
-      <c r="AB3" s="31"/>
-      <c r="AC3" s="32"/>
-      <c r="AD3" s="30" t="s">
+      <c r="Z3" s="30"/>
+      <c r="AA3" s="30"/>
+      <c r="AB3" s="30"/>
+      <c r="AC3" s="31"/>
+      <c r="AD3" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="AE3" s="31"/>
-      <c r="AF3" s="32"/>
+      <c r="AE3" s="30"/>
+      <c r="AF3" s="31"/>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
@@ -3442,46 +3458,46 @@
       <c r="AF5" s="25"/>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26">
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24">
         <v>38</v>
       </c>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="26"/>
-      <c r="M6" s="26"/>
-      <c r="N6" s="26"/>
-      <c r="O6" s="26"/>
-      <c r="P6" s="26"/>
-      <c r="Q6" s="26">
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="24"/>
+      <c r="N6" s="24"/>
+      <c r="O6" s="24"/>
+      <c r="P6" s="24"/>
+      <c r="Q6" s="24">
         <v>73</v>
       </c>
-      <c r="R6" s="26"/>
-      <c r="S6" s="26"/>
-      <c r="T6" s="26"/>
-      <c r="U6" s="26"/>
-      <c r="V6" s="26"/>
-      <c r="W6" s="26"/>
-      <c r="X6" s="26"/>
-      <c r="Y6" s="26">
+      <c r="R6" s="24"/>
+      <c r="S6" s="24"/>
+      <c r="T6" s="24"/>
+      <c r="U6" s="24"/>
+      <c r="V6" s="24"/>
+      <c r="W6" s="24"/>
+      <c r="X6" s="24"/>
+      <c r="Y6" s="24">
         <v>88</v>
       </c>
-      <c r="Z6" s="26"/>
-      <c r="AA6" s="26"/>
-      <c r="AB6" s="26"/>
-      <c r="AC6" s="26"/>
-      <c r="AD6" s="26"/>
-      <c r="AE6" s="26"/>
-      <c r="AF6" s="26"/>
+      <c r="Z6" s="24"/>
+      <c r="AA6" s="24"/>
+      <c r="AB6" s="24"/>
+      <c r="AC6" s="24"/>
+      <c r="AD6" s="24"/>
+      <c r="AE6" s="24"/>
+      <c r="AF6" s="24"/>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
@@ -3582,203 +3598,203 @@
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22" t="s">
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="22" t="s">
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="O8" s="22"/>
-      <c r="P8" s="22"/>
-      <c r="Q8" s="22" t="s">
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="R8" s="22"/>
-      <c r="S8" s="22"/>
-      <c r="T8" s="22" t="s">
+      <c r="R8" s="20"/>
+      <c r="S8" s="20"/>
+      <c r="T8" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="U8" s="22"/>
-      <c r="V8" s="22"/>
-      <c r="W8" s="22"/>
-      <c r="X8" s="22"/>
-      <c r="Y8" s="22" t="s">
+      <c r="U8" s="20"/>
+      <c r="V8" s="20"/>
+      <c r="W8" s="20"/>
+      <c r="X8" s="20"/>
+      <c r="Y8" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z8" s="22"/>
-      <c r="AA8" s="22"/>
-      <c r="AB8" s="22"/>
-      <c r="AC8" s="22"/>
-      <c r="AD8" s="22" t="s">
+      <c r="Z8" s="20"/>
+      <c r="AA8" s="20"/>
+      <c r="AB8" s="20"/>
+      <c r="AC8" s="20"/>
+      <c r="AD8" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="AE8" s="22"/>
-      <c r="AF8" s="22"/>
+      <c r="AE8" s="20"/>
+      <c r="AF8" s="20"/>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A9" s="22">
+      <c r="A9" s="20">
         <v>10</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22">
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20">
         <v>7</v>
       </c>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="22">
-        <v>0</v>
-      </c>
-      <c r="O9" s="22"/>
-      <c r="P9" s="22"/>
-      <c r="Q9" s="22">
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20">
+        <v>0</v>
+      </c>
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="20">
         <v>3</v>
       </c>
-      <c r="R9" s="22"/>
-      <c r="S9" s="22"/>
-      <c r="T9" s="22">
+      <c r="R9" s="20"/>
+      <c r="S9" s="20"/>
+      <c r="T9" s="20">
         <v>19</v>
       </c>
-      <c r="U9" s="22"/>
-      <c r="V9" s="22"/>
-      <c r="W9" s="22"/>
-      <c r="X9" s="22"/>
-      <c r="Y9" s="22">
+      <c r="U9" s="20"/>
+      <c r="V9" s="20"/>
+      <c r="W9" s="20"/>
+      <c r="X9" s="20"/>
+      <c r="Y9" s="20">
         <v>17</v>
       </c>
-      <c r="Z9" s="22"/>
-      <c r="AA9" s="22"/>
-      <c r="AB9" s="22"/>
-      <c r="AC9" s="22"/>
-      <c r="AD9" s="22">
-        <v>0</v>
-      </c>
-      <c r="AE9" s="22"/>
-      <c r="AF9" s="22"/>
+      <c r="Z9" s="20"/>
+      <c r="AA9" s="20"/>
+      <c r="AB9" s="20"/>
+      <c r="AC9" s="20"/>
+      <c r="AD9" s="20">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="20"/>
+      <c r="AF9" s="20"/>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22" t="s">
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="22" t="s">
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="O10" s="22"/>
-      <c r="P10" s="22"/>
-      <c r="Q10" s="22" t="s">
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="R10" s="22"/>
-      <c r="S10" s="22"/>
-      <c r="T10" s="22" t="s">
+      <c r="R10" s="20"/>
+      <c r="S10" s="20"/>
+      <c r="T10" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="U10" s="22"/>
-      <c r="V10" s="22"/>
-      <c r="W10" s="22"/>
-      <c r="X10" s="22"/>
-      <c r="Y10" s="22" t="s">
+      <c r="U10" s="20"/>
+      <c r="V10" s="20"/>
+      <c r="W10" s="20"/>
+      <c r="X10" s="20"/>
+      <c r="Y10" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="Z10" s="22"/>
-      <c r="AA10" s="22"/>
-      <c r="AB10" s="22"/>
-      <c r="AC10" s="22"/>
-      <c r="AD10" s="22" t="s">
+      <c r="Z10" s="20"/>
+      <c r="AA10" s="20"/>
+      <c r="AB10" s="20"/>
+      <c r="AC10" s="20"/>
+      <c r="AD10" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="AE10" s="22"/>
-      <c r="AF10" s="22"/>
+      <c r="AE10" s="20"/>
+      <c r="AF10" s="20"/>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A11" s="22">
+      <c r="A11" s="20">
         <f>A9</f>
         <v>10</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="23">
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="21">
         <f>'Data package'!$B$31*I9+'Data package'!$B$28</f>
         <v>3.338709677419355</v>
       </c>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="20">
+      <c r="J11" s="21"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="22">
         <f ca="1">LOOKUP(N9,'Data package'!$D$21:$D$24,'Data package'!$E$22:$E$35)</f>
         <v>0</v>
       </c>
-      <c r="O11" s="20"/>
-      <c r="P11" s="20"/>
-      <c r="Q11" s="24">
+      <c r="O11" s="22"/>
+      <c r="P11" s="22"/>
+      <c r="Q11" s="23">
         <f>100/(2^3-1)*Q9</f>
         <v>42.857142857142861</v>
       </c>
-      <c r="R11" s="24"/>
-      <c r="S11" s="24"/>
-      <c r="T11" s="24">
+      <c r="R11" s="23"/>
+      <c r="S11" s="23"/>
+      <c r="T11" s="23">
         <f>'Data package'!$B$40*T9+'Data package'!$B$37</f>
         <v>22.903225806451616</v>
       </c>
-      <c r="U11" s="20"/>
-      <c r="V11" s="20"/>
-      <c r="W11" s="20"/>
-      <c r="X11" s="20"/>
-      <c r="Y11" s="20">
+      <c r="U11" s="22"/>
+      <c r="V11" s="22"/>
+      <c r="W11" s="22"/>
+      <c r="X11" s="22"/>
+      <c r="Y11" s="22">
         <f>Y9</f>
         <v>17</v>
       </c>
-      <c r="Z11" s="20"/>
-      <c r="AA11" s="20"/>
-      <c r="AB11" s="20"/>
-      <c r="AC11" s="20"/>
-      <c r="AD11" s="20">
+      <c r="Z11" s="22"/>
+      <c r="AA11" s="22"/>
+      <c r="AB11" s="22"/>
+      <c r="AC11" s="22"/>
+      <c r="AD11" s="22">
         <f>LOOKUP(AD9,'Data package'!$A$84:$A$88,'Data package'!$B$84:$B$88)</f>
         <v>1</v>
       </c>
-      <c r="AE11" s="20"/>
-      <c r="AF11" s="20"/>
+      <c r="AE11" s="22"/>
+      <c r="AF11" s="22"/>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
@@ -3830,46 +3846,46 @@
       <c r="AF14" s="25"/>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26" t="s">
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="J15" s="26"/>
-      <c r="K15" s="26"/>
-      <c r="L15" s="26"/>
-      <c r="M15" s="26"/>
-      <c r="N15" s="26"/>
-      <c r="O15" s="26"/>
-      <c r="P15" s="26"/>
-      <c r="Q15" s="26" t="s">
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="24"/>
+      <c r="N15" s="24"/>
+      <c r="O15" s="24"/>
+      <c r="P15" s="24"/>
+      <c r="Q15" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="R15" s="26"/>
-      <c r="S15" s="26"/>
-      <c r="T15" s="26"/>
-      <c r="U15" s="26"/>
-      <c r="V15" s="26"/>
-      <c r="W15" s="26"/>
-      <c r="X15" s="26"/>
-      <c r="Y15" s="26" t="s">
+      <c r="R15" s="24"/>
+      <c r="S15" s="24"/>
+      <c r="T15" s="24"/>
+      <c r="U15" s="24"/>
+      <c r="V15" s="24"/>
+      <c r="W15" s="24"/>
+      <c r="X15" s="24"/>
+      <c r="Y15" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="Z15" s="26"/>
-      <c r="AA15" s="26"/>
-      <c r="AB15" s="26"/>
-      <c r="AC15" s="26"/>
-      <c r="AD15" s="26"/>
-      <c r="AE15" s="26"/>
-      <c r="AF15" s="26"/>
+      <c r="Z15" s="24"/>
+      <c r="AA15" s="24"/>
+      <c r="AB15" s="24"/>
+      <c r="AC15" s="24"/>
+      <c r="AD15" s="24"/>
+      <c r="AE15" s="24"/>
+      <c r="AF15" s="24"/>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
@@ -3970,203 +3986,203 @@
       </c>
     </row>
     <row r="17" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22" t="s">
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="J17" s="22"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="22"/>
-      <c r="M17" s="22"/>
-      <c r="N17" s="22" t="s">
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="20"/>
+      <c r="N17" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="O17" s="22"/>
-      <c r="P17" s="22"/>
-      <c r="Q17" s="22" t="s">
+      <c r="O17" s="20"/>
+      <c r="P17" s="20"/>
+      <c r="Q17" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="R17" s="22"/>
-      <c r="S17" s="22"/>
-      <c r="T17" s="22" t="s">
+      <c r="R17" s="20"/>
+      <c r="S17" s="20"/>
+      <c r="T17" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="U17" s="22"/>
-      <c r="V17" s="22"/>
-      <c r="W17" s="22"/>
-      <c r="X17" s="22"/>
-      <c r="Y17" s="22" t="s">
+      <c r="U17" s="20"/>
+      <c r="V17" s="20"/>
+      <c r="W17" s="20"/>
+      <c r="X17" s="20"/>
+      <c r="Y17" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z17" s="22"/>
-      <c r="AA17" s="22"/>
-      <c r="AB17" s="22"/>
-      <c r="AC17" s="22"/>
-      <c r="AD17" s="22" t="s">
+      <c r="Z17" s="20"/>
+      <c r="AA17" s="20"/>
+      <c r="AB17" s="20"/>
+      <c r="AC17" s="20"/>
+      <c r="AD17" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="AE17" s="22"/>
-      <c r="AF17" s="22"/>
+      <c r="AE17" s="20"/>
+      <c r="AF17" s="20"/>
     </row>
     <row r="18" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A18" s="22">
+      <c r="A18" s="20">
         <v>5</v>
       </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22">
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20">
         <v>8</v>
       </c>
-      <c r="J18" s="22"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="22"/>
-      <c r="N18" s="22">
-        <v>0</v>
-      </c>
-      <c r="O18" s="22"/>
-      <c r="P18" s="22"/>
-      <c r="Q18" s="22">
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="20">
+        <v>0</v>
+      </c>
+      <c r="O18" s="20"/>
+      <c r="P18" s="20"/>
+      <c r="Q18" s="20">
         <v>3</v>
       </c>
-      <c r="R18" s="22"/>
-      <c r="S18" s="22"/>
-      <c r="T18" s="22">
+      <c r="R18" s="20"/>
+      <c r="S18" s="20"/>
+      <c r="T18" s="20">
         <v>19</v>
       </c>
-      <c r="U18" s="22"/>
-      <c r="V18" s="22"/>
-      <c r="W18" s="22"/>
-      <c r="X18" s="22"/>
-      <c r="Y18" s="22">
+      <c r="U18" s="20"/>
+      <c r="V18" s="20"/>
+      <c r="W18" s="20"/>
+      <c r="X18" s="20"/>
+      <c r="Y18" s="20">
         <v>17</v>
       </c>
-      <c r="Z18" s="22"/>
-      <c r="AA18" s="22"/>
-      <c r="AB18" s="22"/>
-      <c r="AC18" s="22"/>
-      <c r="AD18" s="22">
-        <v>0</v>
-      </c>
-      <c r="AE18" s="22"/>
-      <c r="AF18" s="22"/>
+      <c r="Z18" s="20"/>
+      <c r="AA18" s="20"/>
+      <c r="AB18" s="20"/>
+      <c r="AC18" s="20"/>
+      <c r="AD18" s="20">
+        <v>0</v>
+      </c>
+      <c r="AE18" s="20"/>
+      <c r="AF18" s="20"/>
     </row>
     <row r="19" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22" t="s">
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="J19" s="22"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="22"/>
-      <c r="M19" s="22"/>
-      <c r="N19" s="22" t="s">
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="20"/>
+      <c r="N19" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="O19" s="22"/>
-      <c r="P19" s="22"/>
-      <c r="Q19" s="22" t="s">
+      <c r="O19" s="20"/>
+      <c r="P19" s="20"/>
+      <c r="Q19" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="R19" s="22"/>
-      <c r="S19" s="22"/>
-      <c r="T19" s="22" t="s">
+      <c r="R19" s="20"/>
+      <c r="S19" s="20"/>
+      <c r="T19" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="U19" s="22"/>
-      <c r="V19" s="22"/>
-      <c r="W19" s="22"/>
-      <c r="X19" s="22"/>
-      <c r="Y19" s="22" t="s">
+      <c r="U19" s="20"/>
+      <c r="V19" s="20"/>
+      <c r="W19" s="20"/>
+      <c r="X19" s="20"/>
+      <c r="Y19" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="Z19" s="22"/>
-      <c r="AA19" s="22"/>
-      <c r="AB19" s="22"/>
-      <c r="AC19" s="22"/>
-      <c r="AD19" s="22" t="s">
+      <c r="Z19" s="20"/>
+      <c r="AA19" s="20"/>
+      <c r="AB19" s="20"/>
+      <c r="AC19" s="20"/>
+      <c r="AD19" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="AE19" s="22"/>
-      <c r="AF19" s="22"/>
+      <c r="AE19" s="20"/>
+      <c r="AF19" s="20"/>
     </row>
     <row r="20" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A20" s="22">
+      <c r="A20" s="20">
         <f>A18</f>
         <v>5</v>
       </c>
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="23">
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="21">
         <f>'Data package'!$B$31*I18+'Data package'!$B$28</f>
         <v>3.3870967741935485</v>
       </c>
-      <c r="J20" s="23"/>
-      <c r="K20" s="23"/>
-      <c r="L20" s="23"/>
-      <c r="M20" s="23"/>
-      <c r="N20" s="20">
+      <c r="J20" s="21"/>
+      <c r="K20" s="21"/>
+      <c r="L20" s="21"/>
+      <c r="M20" s="21"/>
+      <c r="N20" s="22">
         <f ca="1">LOOKUP(N18,'Data package'!$D$21:$D$24,'Data package'!$E$22:$E$35)</f>
         <v>0</v>
       </c>
-      <c r="O20" s="20"/>
-      <c r="P20" s="20"/>
-      <c r="Q20" s="24">
+      <c r="O20" s="22"/>
+      <c r="P20" s="22"/>
+      <c r="Q20" s="23">
         <f>100/(2^3-1)*Q18</f>
         <v>42.857142857142861</v>
       </c>
-      <c r="R20" s="24"/>
-      <c r="S20" s="24"/>
-      <c r="T20" s="24">
+      <c r="R20" s="23"/>
+      <c r="S20" s="23"/>
+      <c r="T20" s="23">
         <f>'Data package'!$B$40*T18+'Data package'!$B$37</f>
         <v>22.903225806451616</v>
       </c>
-      <c r="U20" s="20"/>
-      <c r="V20" s="20"/>
-      <c r="W20" s="20"/>
-      <c r="X20" s="20"/>
-      <c r="Y20" s="20">
+      <c r="U20" s="22"/>
+      <c r="V20" s="22"/>
+      <c r="W20" s="22"/>
+      <c r="X20" s="22"/>
+      <c r="Y20" s="22">
         <f>Y18</f>
         <v>17</v>
       </c>
-      <c r="Z20" s="20"/>
-      <c r="AA20" s="20"/>
-      <c r="AB20" s="20"/>
-      <c r="AC20" s="20"/>
-      <c r="AD20" s="20">
+      <c r="Z20" s="22"/>
+      <c r="AA20" s="22"/>
+      <c r="AB20" s="22"/>
+      <c r="AC20" s="22"/>
+      <c r="AD20" s="22">
         <f>LOOKUP(AD18,'Data package'!$A$84:$A$88,'Data package'!$B$84:$B$88)</f>
         <v>1</v>
       </c>
-      <c r="AE20" s="20"/>
-      <c r="AF20" s="20"/>
+      <c r="AE20" s="22"/>
+      <c r="AF20" s="22"/>
     </row>
     <row r="23" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A23" s="25" t="s">
@@ -4205,126 +4221,126 @@
       <c r="AF23" s="25"/>
     </row>
     <row r="24" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A24" s="26" t="s">
+      <c r="A24" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26" t="s">
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="J24" s="26"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="26"/>
-      <c r="M24" s="26"/>
-      <c r="N24" s="26"/>
-      <c r="O24" s="26"/>
-      <c r="P24" s="26"/>
-      <c r="Q24" s="26" t="s">
+      <c r="J24" s="24"/>
+      <c r="K24" s="24"/>
+      <c r="L24" s="24"/>
+      <c r="M24" s="24"/>
+      <c r="N24" s="24"/>
+      <c r="O24" s="24"/>
+      <c r="P24" s="24"/>
+      <c r="Q24" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="R24" s="26"/>
-      <c r="S24" s="26"/>
-      <c r="T24" s="26"/>
-      <c r="U24" s="26"/>
-      <c r="V24" s="26"/>
-      <c r="W24" s="26"/>
-      <c r="X24" s="26"/>
-      <c r="Y24" s="26" t="s">
+      <c r="R24" s="24"/>
+      <c r="S24" s="24"/>
+      <c r="T24" s="24"/>
+      <c r="U24" s="24"/>
+      <c r="V24" s="24"/>
+      <c r="W24" s="24"/>
+      <c r="X24" s="24"/>
+      <c r="Y24" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="Z24" s="26"/>
-      <c r="AA24" s="26"/>
-      <c r="AB24" s="26"/>
-      <c r="AC24" s="26"/>
-      <c r="AD24" s="26"/>
-      <c r="AE24" s="26"/>
-      <c r="AF24" s="26"/>
-      <c r="AG24" s="21">
+      <c r="Z24" s="24"/>
+      <c r="AA24" s="24"/>
+      <c r="AB24" s="24"/>
+      <c r="AC24" s="24"/>
+      <c r="AD24" s="24"/>
+      <c r="AE24" s="24"/>
+      <c r="AF24" s="24"/>
+      <c r="AG24" s="35">
         <v>59</v>
       </c>
-      <c r="AH24" s="21"/>
-      <c r="AI24" s="21"/>
-      <c r="AJ24" s="21"/>
-      <c r="AK24" s="21"/>
-      <c r="AL24" s="21"/>
-      <c r="AM24" s="21"/>
-      <c r="AN24" s="21"/>
-      <c r="AO24" s="21">
+      <c r="AH24" s="35"/>
+      <c r="AI24" s="35"/>
+      <c r="AJ24" s="35"/>
+      <c r="AK24" s="35"/>
+      <c r="AL24" s="35"/>
+      <c r="AM24" s="35"/>
+      <c r="AN24" s="35"/>
+      <c r="AO24" s="35">
         <v>96</v>
       </c>
-      <c r="AP24" s="21"/>
-      <c r="AQ24" s="21"/>
-      <c r="AR24" s="21"/>
-      <c r="AS24" s="21"/>
-      <c r="AT24" s="21"/>
-      <c r="AU24" s="21"/>
-      <c r="AV24" s="21"/>
-      <c r="AW24" s="21">
+      <c r="AP24" s="35"/>
+      <c r="AQ24" s="35"/>
+      <c r="AR24" s="35"/>
+      <c r="AS24" s="35"/>
+      <c r="AT24" s="35"/>
+      <c r="AU24" s="35"/>
+      <c r="AV24" s="35"/>
+      <c r="AW24" s="35">
         <v>65</v>
       </c>
-      <c r="AX24" s="21"/>
-      <c r="AY24" s="21"/>
-      <c r="AZ24" s="21"/>
-      <c r="BA24" s="21"/>
-      <c r="BB24" s="21"/>
-      <c r="BC24" s="21"/>
-      <c r="BD24" s="21"/>
-      <c r="BE24" s="21" t="s">
+      <c r="AX24" s="35"/>
+      <c r="AY24" s="35"/>
+      <c r="AZ24" s="35"/>
+      <c r="BA24" s="35"/>
+      <c r="BB24" s="35"/>
+      <c r="BC24" s="35"/>
+      <c r="BD24" s="35"/>
+      <c r="BE24" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="BF24" s="21"/>
-      <c r="BG24" s="21"/>
-      <c r="BH24" s="21"/>
-      <c r="BI24" s="21"/>
-      <c r="BJ24" s="21"/>
-      <c r="BK24" s="21"/>
-      <c r="BL24" s="21"/>
-      <c r="BM24" s="21" t="s">
+      <c r="BF24" s="35"/>
+      <c r="BG24" s="35"/>
+      <c r="BH24" s="35"/>
+      <c r="BI24" s="35"/>
+      <c r="BJ24" s="35"/>
+      <c r="BK24" s="35"/>
+      <c r="BL24" s="35"/>
+      <c r="BM24" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="BN24" s="21"/>
-      <c r="BO24" s="21"/>
-      <c r="BP24" s="21"/>
-      <c r="BQ24" s="21"/>
-      <c r="BR24" s="21"/>
-      <c r="BS24" s="21"/>
-      <c r="BT24" s="21"/>
-      <c r="BU24" s="21">
+      <c r="BN24" s="35"/>
+      <c r="BO24" s="35"/>
+      <c r="BP24" s="35"/>
+      <c r="BQ24" s="35"/>
+      <c r="BR24" s="35"/>
+      <c r="BS24" s="35"/>
+      <c r="BT24" s="35"/>
+      <c r="BU24" s="35">
         <v>69</v>
       </c>
-      <c r="BV24" s="21"/>
-      <c r="BW24" s="21"/>
-      <c r="BX24" s="21"/>
-      <c r="BY24" s="21"/>
-      <c r="BZ24" s="21"/>
-      <c r="CA24" s="21"/>
-      <c r="CB24" s="21"/>
-      <c r="CC24" s="21" t="s">
+      <c r="BV24" s="35"/>
+      <c r="BW24" s="35"/>
+      <c r="BX24" s="35"/>
+      <c r="BY24" s="35"/>
+      <c r="BZ24" s="35"/>
+      <c r="CA24" s="35"/>
+      <c r="CB24" s="35"/>
+      <c r="CC24" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="CD24" s="21"/>
-      <c r="CE24" s="21"/>
-      <c r="CF24" s="21"/>
-      <c r="CG24" s="21"/>
-      <c r="CH24" s="21"/>
-      <c r="CI24" s="21"/>
-      <c r="CJ24" s="21"/>
-      <c r="CK24" s="21" t="s">
+      <c r="CD24" s="35"/>
+      <c r="CE24" s="35"/>
+      <c r="CF24" s="35"/>
+      <c r="CG24" s="35"/>
+      <c r="CH24" s="35"/>
+      <c r="CI24" s="35"/>
+      <c r="CJ24" s="35"/>
+      <c r="CK24" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="CL24" s="21"/>
-      <c r="CM24" s="21"/>
-      <c r="CN24" s="21"/>
-      <c r="CO24" s="21"/>
-      <c r="CP24" s="21"/>
-      <c r="CQ24" s="21"/>
-      <c r="CR24" s="21"/>
+      <c r="CL24" s="35"/>
+      <c r="CM24" s="35"/>
+      <c r="CN24" s="35"/>
+      <c r="CO24" s="35"/>
+      <c r="CP24" s="35"/>
+      <c r="CQ24" s="35"/>
+      <c r="CR24" s="35"/>
     </row>
     <row r="25" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A25" s="7">
@@ -4617,180 +4633,180 @@
       </c>
     </row>
     <row r="26" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22" t="s">
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="J26" s="22"/>
-      <c r="K26" s="22"/>
-      <c r="L26" s="22"/>
-      <c r="M26" s="22"/>
-      <c r="N26" s="22" t="s">
+      <c r="J26" s="20"/>
+      <c r="K26" s="20"/>
+      <c r="L26" s="20"/>
+      <c r="M26" s="20"/>
+      <c r="N26" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="O26" s="22"/>
-      <c r="P26" s="22"/>
-      <c r="Q26" s="22" t="s">
+      <c r="O26" s="20"/>
+      <c r="P26" s="20"/>
+      <c r="Q26" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="R26" s="22"/>
-      <c r="S26" s="22"/>
-      <c r="T26" s="22" t="s">
+      <c r="R26" s="20"/>
+      <c r="S26" s="20"/>
+      <c r="T26" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="U26" s="22"/>
-      <c r="V26" s="22"/>
-      <c r="W26" s="22"/>
-      <c r="X26" s="22"/>
-      <c r="Y26" s="22" t="s">
+      <c r="U26" s="20"/>
+      <c r="V26" s="20"/>
+      <c r="W26" s="20"/>
+      <c r="X26" s="20"/>
+      <c r="Y26" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z26" s="22"/>
-      <c r="AA26" s="22"/>
-      <c r="AB26" s="22"/>
-      <c r="AC26" s="22"/>
-      <c r="AD26" s="22" t="s">
+      <c r="Z26" s="20"/>
+      <c r="AA26" s="20"/>
+      <c r="AB26" s="20"/>
+      <c r="AC26" s="20"/>
+      <c r="AD26" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="AE26" s="22"/>
-      <c r="AF26" s="22"/>
-      <c r="AG26" s="20" t="s">
+      <c r="AE26" s="20"/>
+      <c r="AF26" s="20"/>
+      <c r="AG26" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="AH26" s="20"/>
-      <c r="AI26" s="20"/>
-      <c r="AJ26" s="20"/>
-      <c r="AK26" s="20"/>
-      <c r="AL26" s="20"/>
-      <c r="AM26" s="20"/>
-      <c r="AN26" s="20"/>
-      <c r="AO26" s="20" t="s">
+      <c r="AH26" s="22"/>
+      <c r="AI26" s="22"/>
+      <c r="AJ26" s="22"/>
+      <c r="AK26" s="22"/>
+      <c r="AL26" s="22"/>
+      <c r="AM26" s="22"/>
+      <c r="AN26" s="22"/>
+      <c r="AO26" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="AP26" s="20"/>
-      <c r="AQ26" s="20"/>
-      <c r="AR26" s="20"/>
-      <c r="AS26" s="20"/>
-      <c r="AT26" s="20"/>
-      <c r="AU26" s="20"/>
-      <c r="AV26" s="20"/>
-      <c r="AW26" s="20" t="s">
+      <c r="AP26" s="22"/>
+      <c r="AQ26" s="22"/>
+      <c r="AR26" s="22"/>
+      <c r="AS26" s="22"/>
+      <c r="AT26" s="22"/>
+      <c r="AU26" s="22"/>
+      <c r="AV26" s="22"/>
+      <c r="AW26" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="AX26" s="20"/>
-      <c r="AY26" s="20"/>
-      <c r="AZ26" s="20"/>
-      <c r="BA26" s="20"/>
-      <c r="BB26" s="20"/>
-      <c r="BC26" s="20"/>
-      <c r="BD26" s="20"/>
-      <c r="BE26" s="20" t="s">
+      <c r="AX26" s="22"/>
+      <c r="AY26" s="22"/>
+      <c r="AZ26" s="22"/>
+      <c r="BA26" s="22"/>
+      <c r="BB26" s="22"/>
+      <c r="BC26" s="22"/>
+      <c r="BD26" s="22"/>
+      <c r="BE26" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="BF26" s="20"/>
-      <c r="BG26" s="20"/>
-      <c r="BH26" s="20"/>
-      <c r="BI26" s="20"/>
-      <c r="BJ26" s="20"/>
-      <c r="BK26" s="20"/>
-      <c r="BL26" s="20"/>
-      <c r="BM26" s="20" t="s">
+      <c r="BF26" s="22"/>
+      <c r="BG26" s="22"/>
+      <c r="BH26" s="22"/>
+      <c r="BI26" s="22"/>
+      <c r="BJ26" s="22"/>
+      <c r="BK26" s="22"/>
+      <c r="BL26" s="22"/>
+      <c r="BM26" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="BN26" s="20"/>
-      <c r="BO26" s="20"/>
-      <c r="BP26" s="20"/>
-      <c r="BQ26" s="20"/>
-      <c r="BR26" s="20"/>
-      <c r="BS26" s="20"/>
-      <c r="BT26" s="20"/>
-      <c r="BU26" s="20" t="s">
+      <c r="BN26" s="22"/>
+      <c r="BO26" s="22"/>
+      <c r="BP26" s="22"/>
+      <c r="BQ26" s="22"/>
+      <c r="BR26" s="22"/>
+      <c r="BS26" s="22"/>
+      <c r="BT26" s="22"/>
+      <c r="BU26" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="BV26" s="20"/>
-      <c r="BW26" s="20"/>
-      <c r="BX26" s="20"/>
-      <c r="BY26" s="20"/>
-      <c r="BZ26" s="20"/>
-      <c r="CA26" s="20"/>
-      <c r="CB26" s="20"/>
-      <c r="CC26" s="20" t="s">
+      <c r="BV26" s="22"/>
+      <c r="BW26" s="22"/>
+      <c r="BX26" s="22"/>
+      <c r="BY26" s="22"/>
+      <c r="BZ26" s="22"/>
+      <c r="CA26" s="22"/>
+      <c r="CB26" s="22"/>
+      <c r="CC26" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="CD26" s="20"/>
-      <c r="CE26" s="20"/>
-      <c r="CF26" s="20"/>
-      <c r="CG26" s="20"/>
-      <c r="CH26" s="20"/>
-      <c r="CI26" s="20"/>
-      <c r="CJ26" s="20"/>
-      <c r="CK26" s="20" t="s">
+      <c r="CD26" s="22"/>
+      <c r="CE26" s="22"/>
+      <c r="CF26" s="22"/>
+      <c r="CG26" s="22"/>
+      <c r="CH26" s="22"/>
+      <c r="CI26" s="22"/>
+      <c r="CJ26" s="22"/>
+      <c r="CK26" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="CL26" s="20"/>
-      <c r="CM26" s="20"/>
-      <c r="CN26" s="20"/>
-      <c r="CO26" s="20"/>
-      <c r="CP26" s="20"/>
-      <c r="CQ26" s="20"/>
-      <c r="CR26" s="20"/>
+      <c r="CL26" s="22"/>
+      <c r="CM26" s="22"/>
+      <c r="CN26" s="22"/>
+      <c r="CO26" s="22"/>
+      <c r="CP26" s="22"/>
+      <c r="CQ26" s="22"/>
+      <c r="CR26" s="22"/>
     </row>
     <row r="27" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A27" s="22">
+      <c r="A27" s="20">
         <v>10</v>
       </c>
-      <c r="B27" s="22"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22">
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20">
         <v>8</v>
       </c>
-      <c r="J27" s="22"/>
-      <c r="K27" s="22"/>
-      <c r="L27" s="22"/>
-      <c r="M27" s="22"/>
-      <c r="N27" s="22">
-        <v>0</v>
-      </c>
-      <c r="O27" s="22"/>
-      <c r="P27" s="22"/>
-      <c r="Q27" s="22">
+      <c r="J27" s="20"/>
+      <c r="K27" s="20"/>
+      <c r="L27" s="20"/>
+      <c r="M27" s="20"/>
+      <c r="N27" s="20">
+        <v>0</v>
+      </c>
+      <c r="O27" s="20"/>
+      <c r="P27" s="20"/>
+      <c r="Q27" s="20">
         <v>3</v>
       </c>
-      <c r="R27" s="22"/>
-      <c r="S27" s="22"/>
-      <c r="T27" s="22">
+      <c r="R27" s="20"/>
+      <c r="S27" s="20"/>
+      <c r="T27" s="20">
         <v>19</v>
       </c>
-      <c r="U27" s="22"/>
-      <c r="V27" s="22"/>
-      <c r="W27" s="22"/>
-      <c r="X27" s="22"/>
-      <c r="Y27" s="22">
+      <c r="U27" s="20"/>
+      <c r="V27" s="20"/>
+      <c r="W27" s="20"/>
+      <c r="X27" s="20"/>
+      <c r="Y27" s="20">
         <v>21</v>
       </c>
-      <c r="Z27" s="22"/>
-      <c r="AA27" s="22"/>
-      <c r="AB27" s="22"/>
-      <c r="AC27" s="22"/>
-      <c r="AD27" s="22">
-        <v>0</v>
-      </c>
-      <c r="AE27" s="22"/>
-      <c r="AF27" s="22"/>
+      <c r="Z27" s="20"/>
+      <c r="AA27" s="20"/>
+      <c r="AB27" s="20"/>
+      <c r="AC27" s="20"/>
+      <c r="AD27" s="20">
+        <v>0</v>
+      </c>
+      <c r="AE27" s="20"/>
+      <c r="AF27" s="20"/>
       <c r="AG27">
         <f>AN25</f>
         <v>1</v>
@@ -5049,267 +5065,267 @@
       </c>
     </row>
     <row r="28" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A28" s="22" t="s">
+      <c r="A28" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22" t="s">
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="J28" s="22"/>
-      <c r="K28" s="22"/>
-      <c r="L28" s="22"/>
-      <c r="M28" s="22"/>
-      <c r="N28" s="22" t="s">
+      <c r="J28" s="20"/>
+      <c r="K28" s="20"/>
+      <c r="L28" s="20"/>
+      <c r="M28" s="20"/>
+      <c r="N28" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="O28" s="22"/>
-      <c r="P28" s="22"/>
-      <c r="Q28" s="22" t="s">
+      <c r="O28" s="20"/>
+      <c r="P28" s="20"/>
+      <c r="Q28" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="R28" s="22"/>
-      <c r="S28" s="22"/>
-      <c r="T28" s="22" t="s">
+      <c r="R28" s="20"/>
+      <c r="S28" s="20"/>
+      <c r="T28" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="U28" s="22"/>
-      <c r="V28" s="22"/>
-      <c r="W28" s="22"/>
-      <c r="X28" s="22"/>
-      <c r="Y28" s="22" t="s">
+      <c r="U28" s="20"/>
+      <c r="V28" s="20"/>
+      <c r="W28" s="20"/>
+      <c r="X28" s="20"/>
+      <c r="Y28" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="Z28" s="22"/>
-      <c r="AA28" s="22"/>
-      <c r="AB28" s="22"/>
-      <c r="AC28" s="22"/>
-      <c r="AD28" s="22" t="s">
+      <c r="Z28" s="20"/>
+      <c r="AA28" s="20"/>
+      <c r="AB28" s="20"/>
+      <c r="AC28" s="20"/>
+      <c r="AD28" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="AE28" s="22"/>
-      <c r="AF28" s="22"/>
-      <c r="AG28" s="20" t="s">
+      <c r="AE28" s="20"/>
+      <c r="AF28" s="20"/>
+      <c r="AG28" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="AH28" s="20"/>
-      <c r="AI28" s="20"/>
-      <c r="AJ28" s="20"/>
-      <c r="AK28" s="20"/>
-      <c r="AL28" s="20"/>
-      <c r="AM28" s="20" t="s">
+      <c r="AH28" s="22"/>
+      <c r="AI28" s="22"/>
+      <c r="AJ28" s="22"/>
+      <c r="AK28" s="22"/>
+      <c r="AL28" s="22"/>
+      <c r="AM28" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="AN28" s="20"/>
-      <c r="AO28" s="20"/>
-      <c r="AP28" s="20"/>
-      <c r="AQ28" s="20"/>
-      <c r="AR28" s="20"/>
-      <c r="AS28" s="20" t="s">
+      <c r="AN28" s="22"/>
+      <c r="AO28" s="22"/>
+      <c r="AP28" s="22"/>
+      <c r="AQ28" s="22"/>
+      <c r="AR28" s="22"/>
+      <c r="AS28" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="AT28" s="20"/>
-      <c r="AU28" s="20"/>
-      <c r="AV28" s="20"/>
-      <c r="AW28" s="20"/>
-      <c r="AX28" s="20"/>
-      <c r="AY28" s="20" t="s">
+      <c r="AT28" s="22"/>
+      <c r="AU28" s="22"/>
+      <c r="AV28" s="22"/>
+      <c r="AW28" s="22"/>
+      <c r="AX28" s="22"/>
+      <c r="AY28" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="AZ28" s="20"/>
-      <c r="BA28" s="20"/>
-      <c r="BB28" s="20"/>
-      <c r="BC28" s="20"/>
-      <c r="BD28" s="20"/>
-      <c r="BE28" s="20" t="s">
+      <c r="AZ28" s="22"/>
+      <c r="BA28" s="22"/>
+      <c r="BB28" s="22"/>
+      <c r="BC28" s="22"/>
+      <c r="BD28" s="22"/>
+      <c r="BE28" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="BF28" s="20"/>
-      <c r="BG28" s="20"/>
-      <c r="BH28" s="20"/>
-      <c r="BI28" s="20"/>
-      <c r="BJ28" s="20"/>
-      <c r="BK28" s="20" t="s">
+      <c r="BF28" s="22"/>
+      <c r="BG28" s="22"/>
+      <c r="BH28" s="22"/>
+      <c r="BI28" s="22"/>
+      <c r="BJ28" s="22"/>
+      <c r="BK28" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="BL28" s="20"/>
-      <c r="BM28" s="20"/>
-      <c r="BN28" s="20"/>
-      <c r="BO28" s="20"/>
-      <c r="BP28" s="20"/>
-      <c r="BQ28" s="20" t="s">
+      <c r="BL28" s="22"/>
+      <c r="BM28" s="22"/>
+      <c r="BN28" s="22"/>
+      <c r="BO28" s="22"/>
+      <c r="BP28" s="22"/>
+      <c r="BQ28" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="BR28" s="20"/>
-      <c r="BS28" s="20"/>
-      <c r="BT28" s="20"/>
-      <c r="BU28" s="20"/>
-      <c r="BV28" s="20"/>
-      <c r="BW28" s="20" t="s">
+      <c r="BR28" s="22"/>
+      <c r="BS28" s="22"/>
+      <c r="BT28" s="22"/>
+      <c r="BU28" s="22"/>
+      <c r="BV28" s="22"/>
+      <c r="BW28" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="BX28" s="20"/>
-      <c r="BY28" s="20"/>
-      <c r="BZ28" s="20"/>
-      <c r="CA28" s="20"/>
-      <c r="CB28" s="20"/>
-      <c r="CC28" s="20" t="s">
+      <c r="BX28" s="22"/>
+      <c r="BY28" s="22"/>
+      <c r="BZ28" s="22"/>
+      <c r="CA28" s="22"/>
+      <c r="CB28" s="22"/>
+      <c r="CC28" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="CD28" s="20"/>
-      <c r="CE28" s="20"/>
-      <c r="CF28" s="20"/>
-      <c r="CG28" s="20"/>
-      <c r="CH28" s="20"/>
-      <c r="CI28" s="20" t="s">
+      <c r="CD28" s="22"/>
+      <c r="CE28" s="22"/>
+      <c r="CF28" s="22"/>
+      <c r="CG28" s="22"/>
+      <c r="CH28" s="22"/>
+      <c r="CI28" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="CJ28" s="20"/>
-      <c r="CK28" s="20"/>
-      <c r="CL28" s="20"/>
-      <c r="CM28" s="20"/>
-      <c r="CN28" s="20"/>
+      <c r="CJ28" s="22"/>
+      <c r="CK28" s="22"/>
+      <c r="CL28" s="22"/>
+      <c r="CM28" s="22"/>
+      <c r="CN28" s="22"/>
     </row>
     <row r="29" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A29" s="22">
+      <c r="A29" s="20">
         <f>A27</f>
         <v>10</v>
       </c>
-      <c r="B29" s="22"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="23">
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="21">
         <f>'Data package'!$B$31*I27+'Data package'!$B$28</f>
         <v>3.3870967741935485</v>
       </c>
-      <c r="J29" s="23"/>
-      <c r="K29" s="23"/>
-      <c r="L29" s="23"/>
-      <c r="M29" s="23"/>
-      <c r="N29" s="20">
+      <c r="J29" s="21"/>
+      <c r="K29" s="21"/>
+      <c r="L29" s="21"/>
+      <c r="M29" s="21"/>
+      <c r="N29" s="22">
         <f ca="1">LOOKUP(N27,'Data package'!$D$21:$D$24,'Data package'!$E$22:$E$35)</f>
         <v>0</v>
       </c>
-      <c r="O29" s="20"/>
-      <c r="P29" s="20"/>
-      <c r="Q29" s="24">
+      <c r="O29" s="22"/>
+      <c r="P29" s="22"/>
+      <c r="Q29" s="23">
         <f>100/(2^3-1)*Q27</f>
         <v>42.857142857142861</v>
       </c>
-      <c r="R29" s="24"/>
-      <c r="S29" s="24"/>
-      <c r="T29" s="24">
+      <c r="R29" s="23"/>
+      <c r="S29" s="23"/>
+      <c r="T29" s="23">
         <f>'Data package'!$B$40*T27+'Data package'!$B$37</f>
         <v>22.903225806451616</v>
       </c>
-      <c r="U29" s="20"/>
-      <c r="V29" s="20"/>
-      <c r="W29" s="20"/>
-      <c r="X29" s="20"/>
-      <c r="Y29" s="20">
+      <c r="U29" s="22"/>
+      <c r="V29" s="22"/>
+      <c r="W29" s="22"/>
+      <c r="X29" s="22"/>
+      <c r="Y29" s="22">
         <f>Y27</f>
         <v>21</v>
       </c>
-      <c r="Z29" s="20"/>
-      <c r="AA29" s="20"/>
-      <c r="AB29" s="20"/>
-      <c r="AC29" s="20"/>
-      <c r="AD29" s="20">
+      <c r="Z29" s="22"/>
+      <c r="AA29" s="22"/>
+      <c r="AB29" s="22"/>
+      <c r="AC29" s="22"/>
+      <c r="AD29" s="22">
         <f>LOOKUP(AD27,'Data package'!$A$84:$A$88,'Data package'!$B$84:$B$88)</f>
         <v>1</v>
       </c>
-      <c r="AE29" s="20"/>
-      <c r="AF29" s="20"/>
-      <c r="AG29" s="20" t="s">
+      <c r="AE29" s="22"/>
+      <c r="AF29" s="22"/>
+      <c r="AG29" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="AH29" s="20"/>
-      <c r="AI29" s="20"/>
-      <c r="AJ29" s="20"/>
-      <c r="AK29" s="20"/>
-      <c r="AL29" s="20"/>
-      <c r="AM29" s="20" t="s">
+      <c r="AH29" s="22"/>
+      <c r="AI29" s="22"/>
+      <c r="AJ29" s="22"/>
+      <c r="AK29" s="22"/>
+      <c r="AL29" s="22"/>
+      <c r="AM29" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="AN29" s="20"/>
-      <c r="AO29" s="20"/>
-      <c r="AP29" s="20"/>
-      <c r="AQ29" s="20"/>
-      <c r="AR29" s="20"/>
-      <c r="AS29" s="20" t="s">
+      <c r="AN29" s="22"/>
+      <c r="AO29" s="22"/>
+      <c r="AP29" s="22"/>
+      <c r="AQ29" s="22"/>
+      <c r="AR29" s="22"/>
+      <c r="AS29" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="AT29" s="20"/>
-      <c r="AU29" s="20"/>
-      <c r="AV29" s="20"/>
-      <c r="AW29" s="20"/>
-      <c r="AX29" s="20"/>
-      <c r="AY29" s="20" t="s">
+      <c r="AT29" s="22"/>
+      <c r="AU29" s="22"/>
+      <c r="AV29" s="22"/>
+      <c r="AW29" s="22"/>
+      <c r="AX29" s="22"/>
+      <c r="AY29" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="AZ29" s="20"/>
-      <c r="BA29" s="20"/>
-      <c r="BB29" s="20"/>
-      <c r="BC29" s="20"/>
-      <c r="BD29" s="20"/>
-      <c r="BE29" s="20" t="s">
+      <c r="AZ29" s="22"/>
+      <c r="BA29" s="22"/>
+      <c r="BB29" s="22"/>
+      <c r="BC29" s="22"/>
+      <c r="BD29" s="22"/>
+      <c r="BE29" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="BF29" s="20"/>
-      <c r="BG29" s="20"/>
-      <c r="BH29" s="20"/>
-      <c r="BI29" s="20"/>
-      <c r="BJ29" s="20"/>
-      <c r="BK29" s="20" t="s">
+      <c r="BF29" s="22"/>
+      <c r="BG29" s="22"/>
+      <c r="BH29" s="22"/>
+      <c r="BI29" s="22"/>
+      <c r="BJ29" s="22"/>
+      <c r="BK29" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="BL29" s="20"/>
-      <c r="BM29" s="20"/>
-      <c r="BN29" s="20"/>
-      <c r="BO29" s="20"/>
-      <c r="BP29" s="20"/>
-      <c r="BQ29" s="20" t="s">
+      <c r="BL29" s="22"/>
+      <c r="BM29" s="22"/>
+      <c r="BN29" s="22"/>
+      <c r="BO29" s="22"/>
+      <c r="BP29" s="22"/>
+      <c r="BQ29" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="BR29" s="20"/>
-      <c r="BS29" s="20"/>
-      <c r="BT29" s="20"/>
-      <c r="BU29" s="20"/>
-      <c r="BV29" s="20"/>
-      <c r="BW29" s="20" t="s">
+      <c r="BR29" s="22"/>
+      <c r="BS29" s="22"/>
+      <c r="BT29" s="22"/>
+      <c r="BU29" s="22"/>
+      <c r="BV29" s="22"/>
+      <c r="BW29" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="BX29" s="20"/>
-      <c r="BY29" s="20"/>
-      <c r="BZ29" s="20"/>
-      <c r="CA29" s="20"/>
-      <c r="CB29" s="20"/>
-      <c r="CC29" s="20" t="s">
+      <c r="BX29" s="22"/>
+      <c r="BY29" s="22"/>
+      <c r="BZ29" s="22"/>
+      <c r="CA29" s="22"/>
+      <c r="CB29" s="22"/>
+      <c r="CC29" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="CD29" s="20"/>
-      <c r="CE29" s="20"/>
-      <c r="CF29" s="20"/>
-      <c r="CG29" s="20"/>
-      <c r="CH29" s="20"/>
-      <c r="CI29" s="20" t="s">
+      <c r="CD29" s="22"/>
+      <c r="CE29" s="22"/>
+      <c r="CF29" s="22"/>
+      <c r="CG29" s="22"/>
+      <c r="CH29" s="22"/>
+      <c r="CI29" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="CJ29" s="20"/>
-      <c r="CK29" s="20"/>
-      <c r="CL29" s="20"/>
-      <c r="CM29" s="20"/>
-      <c r="CN29" s="20"/>
+      <c r="CJ29" s="22"/>
+      <c r="CK29" s="22"/>
+      <c r="CL29" s="22"/>
+      <c r="CM29" s="22"/>
+      <c r="CN29" s="22"/>
     </row>
     <row r="30" spans="1:96" x14ac:dyDescent="0.3">
       <c r="AG30">
@@ -5554,229 +5570,255 @@
       </c>
     </row>
     <row r="31" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="AG31" s="20" t="s">
+      <c r="AG31" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="AH31" s="20"/>
-      <c r="AI31" s="20"/>
-      <c r="AJ31" s="20"/>
-      <c r="AK31" s="20"/>
-      <c r="AL31" s="20"/>
-      <c r="AM31" s="20" t="s">
+      <c r="AH31" s="22"/>
+      <c r="AI31" s="22"/>
+      <c r="AJ31" s="22"/>
+      <c r="AK31" s="22"/>
+      <c r="AL31" s="22"/>
+      <c r="AM31" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="AN31" s="20"/>
-      <c r="AO31" s="20"/>
-      <c r="AP31" s="20"/>
-      <c r="AQ31" s="20"/>
-      <c r="AR31" s="20"/>
-      <c r="AS31" s="20" t="s">
+      <c r="AN31" s="22"/>
+      <c r="AO31" s="22"/>
+      <c r="AP31" s="22"/>
+      <c r="AQ31" s="22"/>
+      <c r="AR31" s="22"/>
+      <c r="AS31" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="AT31" s="20"/>
-      <c r="AU31" s="20"/>
-      <c r="AV31" s="20"/>
-      <c r="AW31" s="20"/>
-      <c r="AX31" s="20"/>
-      <c r="AY31" s="20" t="s">
+      <c r="AT31" s="22"/>
+      <c r="AU31" s="22"/>
+      <c r="AV31" s="22"/>
+      <c r="AW31" s="22"/>
+      <c r="AX31" s="22"/>
+      <c r="AY31" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="AZ31" s="20"/>
-      <c r="BA31" s="20"/>
-      <c r="BB31" s="20"/>
-      <c r="BC31" s="20"/>
-      <c r="BD31" s="20"/>
-      <c r="BE31" s="20" t="s">
+      <c r="AZ31" s="22"/>
+      <c r="BA31" s="22"/>
+      <c r="BB31" s="22"/>
+      <c r="BC31" s="22"/>
+      <c r="BD31" s="22"/>
+      <c r="BE31" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="BF31" s="20"/>
-      <c r="BG31" s="20"/>
-      <c r="BH31" s="20"/>
-      <c r="BI31" s="20"/>
-      <c r="BJ31" s="20"/>
-      <c r="BK31" s="20" t="s">
+      <c r="BF31" s="22"/>
+      <c r="BG31" s="22"/>
+      <c r="BH31" s="22"/>
+      <c r="BI31" s="22"/>
+      <c r="BJ31" s="22"/>
+      <c r="BK31" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="BL31" s="20"/>
-      <c r="BM31" s="20"/>
-      <c r="BN31" s="20"/>
-      <c r="BO31" s="20"/>
-      <c r="BP31" s="20"/>
-      <c r="BQ31" s="20" t="s">
+      <c r="BL31" s="22"/>
+      <c r="BM31" s="22"/>
+      <c r="BN31" s="22"/>
+      <c r="BO31" s="22"/>
+      <c r="BP31" s="22"/>
+      <c r="BQ31" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="BR31" s="20"/>
-      <c r="BS31" s="20"/>
-      <c r="BT31" s="20"/>
-      <c r="BU31" s="20"/>
-      <c r="BV31" s="20"/>
-      <c r="BW31" s="20" t="s">
+      <c r="BR31" s="22"/>
+      <c r="BS31" s="22"/>
+      <c r="BT31" s="22"/>
+      <c r="BU31" s="22"/>
+      <c r="BV31" s="22"/>
+      <c r="BW31" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="BX31" s="20"/>
-      <c r="BY31" s="20"/>
-      <c r="BZ31" s="20"/>
-      <c r="CA31" s="20"/>
-      <c r="CB31" s="20"/>
-      <c r="CC31" s="20" t="s">
+      <c r="BX31" s="22"/>
+      <c r="BY31" s="22"/>
+      <c r="BZ31" s="22"/>
+      <c r="CA31" s="22"/>
+      <c r="CB31" s="22"/>
+      <c r="CC31" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="CD31" s="20"/>
-      <c r="CE31" s="20"/>
-      <c r="CF31" s="20"/>
-      <c r="CG31" s="20"/>
-      <c r="CH31" s="20"/>
-      <c r="CI31" s="20" t="s">
+      <c r="CD31" s="22"/>
+      <c r="CE31" s="22"/>
+      <c r="CF31" s="22"/>
+      <c r="CG31" s="22"/>
+      <c r="CH31" s="22"/>
+      <c r="CI31" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="CJ31" s="20"/>
-      <c r="CK31" s="20"/>
-      <c r="CL31" s="20"/>
-      <c r="CM31" s="20"/>
-      <c r="CN31" s="20"/>
+      <c r="CJ31" s="22"/>
+      <c r="CK31" s="22"/>
+      <c r="CL31" s="22"/>
+      <c r="CM31" s="22"/>
+      <c r="CN31" s="22"/>
     </row>
     <row r="32" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="AG32" s="20">
+      <c r="AG32" s="22">
         <v>25</v>
       </c>
-      <c r="AH32" s="20"/>
-      <c r="AI32" s="20"/>
-      <c r="AJ32" s="20"/>
-      <c r="AK32" s="20"/>
-      <c r="AL32" s="20"/>
-      <c r="AM32" s="20">
+      <c r="AH32" s="22"/>
+      <c r="AI32" s="22"/>
+      <c r="AJ32" s="22"/>
+      <c r="AK32" s="22"/>
+      <c r="AL32" s="22"/>
+      <c r="AM32" s="22">
         <v>25</v>
       </c>
-      <c r="AN32" s="20"/>
-      <c r="AO32" s="20"/>
-      <c r="AP32" s="20"/>
-      <c r="AQ32" s="20"/>
-      <c r="AR32" s="20"/>
-      <c r="AS32" s="20">
+      <c r="AN32" s="22"/>
+      <c r="AO32" s="22"/>
+      <c r="AP32" s="22"/>
+      <c r="AQ32" s="22"/>
+      <c r="AR32" s="22"/>
+      <c r="AS32" s="22">
         <v>25</v>
       </c>
-      <c r="AT32" s="20"/>
-      <c r="AU32" s="20"/>
-      <c r="AV32" s="20"/>
-      <c r="AW32" s="20"/>
-      <c r="AX32" s="20"/>
-      <c r="AY32" s="20">
+      <c r="AT32" s="22"/>
+      <c r="AU32" s="22"/>
+      <c r="AV32" s="22"/>
+      <c r="AW32" s="22"/>
+      <c r="AX32" s="22"/>
+      <c r="AY32" s="22">
         <v>25</v>
       </c>
-      <c r="AZ32" s="20"/>
-      <c r="BA32" s="20"/>
-      <c r="BB32" s="20"/>
-      <c r="BC32" s="20"/>
-      <c r="BD32" s="20"/>
-      <c r="BE32" s="20">
+      <c r="AZ32" s="22"/>
+      <c r="BA32" s="22"/>
+      <c r="BB32" s="22"/>
+      <c r="BC32" s="22"/>
+      <c r="BD32" s="22"/>
+      <c r="BE32" s="22">
         <v>26</v>
       </c>
-      <c r="BF32" s="20"/>
-      <c r="BG32" s="20"/>
-      <c r="BH32" s="20"/>
-      <c r="BI32" s="20"/>
-      <c r="BJ32" s="20"/>
-      <c r="BK32" s="20">
+      <c r="BF32" s="22"/>
+      <c r="BG32" s="22"/>
+      <c r="BH32" s="22"/>
+      <c r="BI32" s="22"/>
+      <c r="BJ32" s="22"/>
+      <c r="BK32" s="22">
         <v>26</v>
       </c>
-      <c r="BL32" s="20"/>
-      <c r="BM32" s="20"/>
-      <c r="BN32" s="20"/>
-      <c r="BO32" s="20"/>
-      <c r="BP32" s="20"/>
-      <c r="BQ32" s="20">
+      <c r="BL32" s="22"/>
+      <c r="BM32" s="22"/>
+      <c r="BN32" s="22"/>
+      <c r="BO32" s="22"/>
+      <c r="BP32" s="22"/>
+      <c r="BQ32" s="22">
         <v>26</v>
       </c>
-      <c r="BR32" s="20"/>
-      <c r="BS32" s="20"/>
-      <c r="BT32" s="20"/>
-      <c r="BU32" s="20"/>
-      <c r="BV32" s="20"/>
-      <c r="BW32" s="20">
+      <c r="BR32" s="22"/>
+      <c r="BS32" s="22"/>
+      <c r="BT32" s="22"/>
+      <c r="BU32" s="22"/>
+      <c r="BV32" s="22"/>
+      <c r="BW32" s="22">
         <v>26</v>
       </c>
-      <c r="BX32" s="20"/>
-      <c r="BY32" s="20"/>
-      <c r="BZ32" s="20"/>
-      <c r="CA32" s="20"/>
-      <c r="CB32" s="20"/>
-      <c r="CC32" s="20">
+      <c r="BX32" s="22"/>
+      <c r="BY32" s="22"/>
+      <c r="BZ32" s="22"/>
+      <c r="CA32" s="22"/>
+      <c r="CB32" s="22"/>
+      <c r="CC32" s="22">
         <v>26</v>
       </c>
-      <c r="CD32" s="20"/>
-      <c r="CE32" s="20"/>
-      <c r="CF32" s="20"/>
-      <c r="CG32" s="20"/>
-      <c r="CH32" s="20"/>
-      <c r="CI32" s="20">
+      <c r="CD32" s="22"/>
+      <c r="CE32" s="22"/>
+      <c r="CF32" s="22"/>
+      <c r="CG32" s="22"/>
+      <c r="CH32" s="22"/>
+      <c r="CI32" s="22">
         <v>26</v>
       </c>
-      <c r="CJ32" s="20"/>
-      <c r="CK32" s="20"/>
-      <c r="CL32" s="20"/>
-      <c r="CM32" s="20"/>
-      <c r="CN32" s="20"/>
+      <c r="CJ32" s="22"/>
+      <c r="CK32" s="22"/>
+      <c r="CL32" s="22"/>
+      <c r="CM32" s="22"/>
+      <c r="CN32" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="166">
-    <mergeCell ref="Y19:AC19"/>
-    <mergeCell ref="AD19:AF19"/>
-    <mergeCell ref="A20:H20"/>
-    <mergeCell ref="I20:M20"/>
-    <mergeCell ref="N20:P20"/>
-    <mergeCell ref="Q20:S20"/>
-    <mergeCell ref="T20:X20"/>
-    <mergeCell ref="Y20:AC20"/>
-    <mergeCell ref="AD20:AF20"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="I19:M19"/>
-    <mergeCell ref="N19:P19"/>
-    <mergeCell ref="Q19:S19"/>
-    <mergeCell ref="T19:X19"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="I15:P15"/>
-    <mergeCell ref="Q15:X15"/>
-    <mergeCell ref="Y15:AF15"/>
-    <mergeCell ref="A14:AF14"/>
-    <mergeCell ref="Y17:AC17"/>
-    <mergeCell ref="AD17:AF17"/>
-    <mergeCell ref="A18:H18"/>
-    <mergeCell ref="I18:M18"/>
-    <mergeCell ref="N18:P18"/>
-    <mergeCell ref="Q18:S18"/>
-    <mergeCell ref="T18:X18"/>
-    <mergeCell ref="Y18:AC18"/>
-    <mergeCell ref="AD18:AF18"/>
-    <mergeCell ref="A17:H17"/>
-    <mergeCell ref="I17:M17"/>
-    <mergeCell ref="N17:P17"/>
-    <mergeCell ref="Q17:S17"/>
-    <mergeCell ref="T17:X17"/>
-    <mergeCell ref="I11:M11"/>
-    <mergeCell ref="A11:H11"/>
-    <mergeCell ref="I10:M10"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="AD10:AF10"/>
-    <mergeCell ref="Y10:AC10"/>
-    <mergeCell ref="T10:X10"/>
-    <mergeCell ref="Q10:S10"/>
-    <mergeCell ref="N10:P10"/>
-    <mergeCell ref="AD11:AF11"/>
-    <mergeCell ref="Y11:AC11"/>
-    <mergeCell ref="T11:X11"/>
-    <mergeCell ref="Q11:S11"/>
-    <mergeCell ref="N11:P11"/>
-    <mergeCell ref="Q6:X6"/>
-    <mergeCell ref="Y6:AF6"/>
-    <mergeCell ref="AD9:AF9"/>
-    <mergeCell ref="AD8:AF8"/>
-    <mergeCell ref="Y9:AC9"/>
-    <mergeCell ref="Y8:AC8"/>
-    <mergeCell ref="N9:P9"/>
-    <mergeCell ref="Q8:S8"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="T8:X8"/>
-    <mergeCell ref="T9:X9"/>
+    <mergeCell ref="BK32:BP32"/>
+    <mergeCell ref="BQ32:BV32"/>
+    <mergeCell ref="BW32:CB32"/>
+    <mergeCell ref="CC32:CH32"/>
+    <mergeCell ref="CI32:CN32"/>
+    <mergeCell ref="AG32:AL32"/>
+    <mergeCell ref="AM32:AR32"/>
+    <mergeCell ref="AS32:AX32"/>
+    <mergeCell ref="AY32:BD32"/>
+    <mergeCell ref="BE32:BJ32"/>
+    <mergeCell ref="BK31:BP31"/>
+    <mergeCell ref="BQ31:BV31"/>
+    <mergeCell ref="BW31:CB31"/>
+    <mergeCell ref="CC31:CH31"/>
+    <mergeCell ref="CI31:CN31"/>
+    <mergeCell ref="AG31:AL31"/>
+    <mergeCell ref="AM31:AR31"/>
+    <mergeCell ref="AS31:AX31"/>
+    <mergeCell ref="AY31:BD31"/>
+    <mergeCell ref="BE31:BJ31"/>
+    <mergeCell ref="BK29:BP29"/>
+    <mergeCell ref="BQ29:BV29"/>
+    <mergeCell ref="BW29:CB29"/>
+    <mergeCell ref="CC29:CH29"/>
+    <mergeCell ref="CI29:CN29"/>
+    <mergeCell ref="AG29:AL29"/>
+    <mergeCell ref="AM29:AR29"/>
+    <mergeCell ref="AS29:AX29"/>
+    <mergeCell ref="AY29:BD29"/>
+    <mergeCell ref="BE29:BJ29"/>
+    <mergeCell ref="BK28:BP28"/>
+    <mergeCell ref="BQ28:BV28"/>
+    <mergeCell ref="BW28:CB28"/>
+    <mergeCell ref="CC28:CH28"/>
+    <mergeCell ref="CI28:CN28"/>
+    <mergeCell ref="AG28:AL28"/>
+    <mergeCell ref="AM28:AR28"/>
+    <mergeCell ref="AS28:AX28"/>
+    <mergeCell ref="AY28:BD28"/>
+    <mergeCell ref="BE28:BJ28"/>
+    <mergeCell ref="BU24:CB24"/>
+    <mergeCell ref="CC24:CJ24"/>
+    <mergeCell ref="CK24:CR24"/>
+    <mergeCell ref="AG26:AN26"/>
+    <mergeCell ref="AO26:AV26"/>
+    <mergeCell ref="AW26:BD26"/>
+    <mergeCell ref="BE26:BL26"/>
+    <mergeCell ref="BM26:BT26"/>
+    <mergeCell ref="BU26:CB26"/>
+    <mergeCell ref="CC26:CJ26"/>
+    <mergeCell ref="CK26:CR26"/>
+    <mergeCell ref="AG24:AN24"/>
+    <mergeCell ref="AO24:AV24"/>
+    <mergeCell ref="AW24:BD24"/>
+    <mergeCell ref="BE24:BL24"/>
+    <mergeCell ref="BM24:BT24"/>
+    <mergeCell ref="Y28:AC28"/>
+    <mergeCell ref="AD28:AF28"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="I29:M29"/>
+    <mergeCell ref="N29:P29"/>
+    <mergeCell ref="Q29:S29"/>
+    <mergeCell ref="T29:X29"/>
+    <mergeCell ref="Y29:AC29"/>
+    <mergeCell ref="AD29:AF29"/>
+    <mergeCell ref="A28:H28"/>
+    <mergeCell ref="I28:M28"/>
+    <mergeCell ref="N28:P28"/>
+    <mergeCell ref="Q28:S28"/>
+    <mergeCell ref="T28:X28"/>
+    <mergeCell ref="Y26:AC26"/>
+    <mergeCell ref="AD26:AF26"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="I27:M27"/>
+    <mergeCell ref="N27:P27"/>
+    <mergeCell ref="Q27:S27"/>
+    <mergeCell ref="T27:X27"/>
+    <mergeCell ref="Y27:AC27"/>
+    <mergeCell ref="AD27:AF27"/>
+    <mergeCell ref="A26:H26"/>
+    <mergeCell ref="I26:M26"/>
+    <mergeCell ref="N26:P26"/>
+    <mergeCell ref="Q26:S26"/>
+    <mergeCell ref="T26:X26"/>
     <mergeCell ref="A23:AF23"/>
     <mergeCell ref="A24:H24"/>
     <mergeCell ref="I24:P24"/>
@@ -5801,90 +5843,64 @@
     <mergeCell ref="I8:M8"/>
     <mergeCell ref="N8:P8"/>
     <mergeCell ref="I9:M9"/>
-    <mergeCell ref="Y26:AC26"/>
-    <mergeCell ref="AD26:AF26"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="I27:M27"/>
-    <mergeCell ref="N27:P27"/>
-    <mergeCell ref="Q27:S27"/>
-    <mergeCell ref="T27:X27"/>
-    <mergeCell ref="Y27:AC27"/>
-    <mergeCell ref="AD27:AF27"/>
-    <mergeCell ref="A26:H26"/>
-    <mergeCell ref="I26:M26"/>
-    <mergeCell ref="N26:P26"/>
-    <mergeCell ref="Q26:S26"/>
-    <mergeCell ref="T26:X26"/>
-    <mergeCell ref="Y28:AC28"/>
-    <mergeCell ref="AD28:AF28"/>
-    <mergeCell ref="A29:H29"/>
-    <mergeCell ref="I29:M29"/>
-    <mergeCell ref="N29:P29"/>
-    <mergeCell ref="Q29:S29"/>
-    <mergeCell ref="T29:X29"/>
-    <mergeCell ref="Y29:AC29"/>
-    <mergeCell ref="AD29:AF29"/>
-    <mergeCell ref="A28:H28"/>
-    <mergeCell ref="I28:M28"/>
-    <mergeCell ref="N28:P28"/>
-    <mergeCell ref="Q28:S28"/>
-    <mergeCell ref="T28:X28"/>
-    <mergeCell ref="BU24:CB24"/>
-    <mergeCell ref="CC24:CJ24"/>
-    <mergeCell ref="CK24:CR24"/>
-    <mergeCell ref="AG26:AN26"/>
-    <mergeCell ref="AO26:AV26"/>
-    <mergeCell ref="AW26:BD26"/>
-    <mergeCell ref="BE26:BL26"/>
-    <mergeCell ref="BM26:BT26"/>
-    <mergeCell ref="BU26:CB26"/>
-    <mergeCell ref="CC26:CJ26"/>
-    <mergeCell ref="CK26:CR26"/>
-    <mergeCell ref="AG24:AN24"/>
-    <mergeCell ref="AO24:AV24"/>
-    <mergeCell ref="AW24:BD24"/>
-    <mergeCell ref="BE24:BL24"/>
-    <mergeCell ref="BM24:BT24"/>
-    <mergeCell ref="BK28:BP28"/>
-    <mergeCell ref="BQ28:BV28"/>
-    <mergeCell ref="BW28:CB28"/>
-    <mergeCell ref="CC28:CH28"/>
-    <mergeCell ref="CI28:CN28"/>
-    <mergeCell ref="AG28:AL28"/>
-    <mergeCell ref="AM28:AR28"/>
-    <mergeCell ref="AS28:AX28"/>
-    <mergeCell ref="AY28:BD28"/>
-    <mergeCell ref="BE28:BJ28"/>
-    <mergeCell ref="BK29:BP29"/>
-    <mergeCell ref="BQ29:BV29"/>
-    <mergeCell ref="BW29:CB29"/>
-    <mergeCell ref="CC29:CH29"/>
-    <mergeCell ref="CI29:CN29"/>
-    <mergeCell ref="AG29:AL29"/>
-    <mergeCell ref="AM29:AR29"/>
-    <mergeCell ref="AS29:AX29"/>
-    <mergeCell ref="AY29:BD29"/>
-    <mergeCell ref="BE29:BJ29"/>
-    <mergeCell ref="BK31:BP31"/>
-    <mergeCell ref="BQ31:BV31"/>
-    <mergeCell ref="BW31:CB31"/>
-    <mergeCell ref="CC31:CH31"/>
-    <mergeCell ref="CI31:CN31"/>
-    <mergeCell ref="AG31:AL31"/>
-    <mergeCell ref="AM31:AR31"/>
-    <mergeCell ref="AS31:AX31"/>
-    <mergeCell ref="AY31:BD31"/>
-    <mergeCell ref="BE31:BJ31"/>
-    <mergeCell ref="BK32:BP32"/>
-    <mergeCell ref="BQ32:BV32"/>
-    <mergeCell ref="BW32:CB32"/>
-    <mergeCell ref="CC32:CH32"/>
-    <mergeCell ref="CI32:CN32"/>
-    <mergeCell ref="AG32:AL32"/>
-    <mergeCell ref="AM32:AR32"/>
-    <mergeCell ref="AS32:AX32"/>
-    <mergeCell ref="AY32:BD32"/>
-    <mergeCell ref="BE32:BJ32"/>
+    <mergeCell ref="Q6:X6"/>
+    <mergeCell ref="Y6:AF6"/>
+    <mergeCell ref="AD9:AF9"/>
+    <mergeCell ref="AD8:AF8"/>
+    <mergeCell ref="Y9:AC9"/>
+    <mergeCell ref="Y8:AC8"/>
+    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="T8:X8"/>
+    <mergeCell ref="T9:X9"/>
+    <mergeCell ref="I11:M11"/>
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="I10:M10"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="AD10:AF10"/>
+    <mergeCell ref="Y10:AC10"/>
+    <mergeCell ref="T10:X10"/>
+    <mergeCell ref="Q10:S10"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="AD11:AF11"/>
+    <mergeCell ref="Y11:AC11"/>
+    <mergeCell ref="T11:X11"/>
+    <mergeCell ref="Q11:S11"/>
+    <mergeCell ref="N11:P11"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="I15:P15"/>
+    <mergeCell ref="Q15:X15"/>
+    <mergeCell ref="Y15:AF15"/>
+    <mergeCell ref="A14:AF14"/>
+    <mergeCell ref="Y17:AC17"/>
+    <mergeCell ref="AD17:AF17"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="I18:M18"/>
+    <mergeCell ref="N18:P18"/>
+    <mergeCell ref="Q18:S18"/>
+    <mergeCell ref="T18:X18"/>
+    <mergeCell ref="Y18:AC18"/>
+    <mergeCell ref="AD18:AF18"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="I17:M17"/>
+    <mergeCell ref="N17:P17"/>
+    <mergeCell ref="Q17:S17"/>
+    <mergeCell ref="T17:X17"/>
+    <mergeCell ref="Y19:AC19"/>
+    <mergeCell ref="AD19:AF19"/>
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="I20:M20"/>
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="Q20:S20"/>
+    <mergeCell ref="T20:X20"/>
+    <mergeCell ref="Y20:AC20"/>
+    <mergeCell ref="AD20:AF20"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="I19:M19"/>
+    <mergeCell ref="N19:P19"/>
+    <mergeCell ref="Q19:S19"/>
+    <mergeCell ref="T19:X19"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -5913,11 +5929,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
       <c r="E1" s="7">
         <v>0.5</v>
       </c>
@@ -6743,28 +6759,28 @@
       <c r="S2" s="7"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="33" t="s">
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="34"/>
-      <c r="N3" s="33" t="s">
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="O3" s="34"/>
-      <c r="P3" s="35"/>
+      <c r="O3" s="33"/>
+      <c r="P3" s="34"/>
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
       <c r="S3" s="7"/>
@@ -6831,10 +6847,10 @@
       <c r="O6" s="25"/>
       <c r="P6" s="25"/>
       <c r="Q6" s="7"/>
-      <c r="R6" s="22" t="s">
+      <c r="R6" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="S6" s="22"/>
+      <c r="S6" s="20"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
@@ -6886,18 +6902,18 @@
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
-      <c r="I8" s="22" t="s">
+      <c r="I8" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="22" t="s">
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="O8" s="22"/>
-      <c r="P8" s="22"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
       <c r="Q8" s="7"/>
       <c r="R8" s="7"/>
       <c r="S8" s="7"/>
@@ -6911,18 +6927,18 @@
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
-      <c r="I9" s="22">
+      <c r="I9" s="20">
         <v>17</v>
       </c>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="22">
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20">
         <v>4</v>
       </c>
-      <c r="O9" s="22"/>
-      <c r="P9" s="22"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
       <c r="Q9" s="7"/>
       <c r="R9" s="7"/>
       <c r="S9" s="7"/>
@@ -6941,11 +6957,11 @@
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
-      <c r="N10" s="22" t="s">
+      <c r="N10" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="O10" s="22"/>
-      <c r="P10" s="22"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
       <c r="Q10" s="7"/>
       <c r="R10" s="7"/>
       <c r="S10" s="7"/>
@@ -6964,18 +6980,24 @@
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
-      <c r="N11" s="23">
+      <c r="N11" s="21">
         <f>100/(2^3-1)*N9</f>
         <v>57.142857142857146</v>
       </c>
-      <c r="O11" s="23"/>
-      <c r="P11" s="23"/>
+      <c r="O11" s="21"/>
+      <c r="P11" s="21"/>
       <c r="Q11" s="7"/>
       <c r="R11" s="7"/>
       <c r="S11" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="I3:M3"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="I6:P6"/>
     <mergeCell ref="N11:P11"/>
     <mergeCell ref="R7:S7"/>
     <mergeCell ref="I8:M8"/>
@@ -6983,12 +7005,6 @@
     <mergeCell ref="I9:M9"/>
     <mergeCell ref="N9:P9"/>
     <mergeCell ref="N10:P10"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="I3:M3"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="I6:P6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
rtc initialization bug fixed and payload formatter updated
</commit_message>
<xml_diff>
--- a/hardware/BikeCounterPro/src/dataPackage/DataPackage.xlsx
+++ b/hardware/BikeCounterPro/src/dataPackage/DataPackage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meier\Documents\repos\lora\hardware\BikeCounterPro\src\dataPackage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meier\Documents\repos\bikecounter\hardware\BikeCounterPro\src\dataPackage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B8C60FE-EBC7-424D-8F24-3A881E03F713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A0AA74-FFA5-4FCD-83F6-2FA4116196A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41172" yWindow="-108" windowWidth="41496" windowHeight="16896" xr2:uid="{CDF7A0A5-12B1-43F1-AFDE-54CA91221B4B}"/>
+    <workbookView xWindow="50592" yWindow="3180" windowWidth="31968" windowHeight="13500" xr2:uid="{CDF7A0A5-12B1-43F1-AFDE-54CA91221B4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Data package" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="118">
   <si>
     <t>minutes of day</t>
   </si>
@@ -386,6 +386,12 @@
   </si>
   <si>
     <t>sync call</t>
+  </si>
+  <si>
+    <t>board v0.1 ohne RTC</t>
+  </si>
+  <si>
+    <t>753649f6cd0a613f381e185e22c4f90cc98fa9b9 [753649f]</t>
   </si>
 </sst>
 </file>
@@ -648,21 +654,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -691,9 +700,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2154,8 +2160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{088FF0E6-8FE4-49E3-812F-B76B934E1ACD}">
   <dimension ref="A1:S90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2292,6 +2298,9 @@
       <c r="D13" t="s">
         <v>96</v>
       </c>
+      <c r="E13" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -2363,6 +2372,9 @@
       <c r="E17" t="s">
         <v>90</v>
       </c>
+      <c r="F17" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
@@ -2378,6 +2390,9 @@
       <c r="E18" t="s">
         <v>93</v>
       </c>
+      <c r="F18" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D19" t="s">
@@ -2385,6 +2400,9 @@
       </c>
       <c r="E19" t="s">
         <v>94</v>
+      </c>
+      <c r="F19" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -3213,46 +3231,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="26" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="26" t="s">
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="26" t="s">
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="29"/>
+      <c r="Y1" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="27"/>
-      <c r="AB1" s="27"/>
-      <c r="AC1" s="27"/>
-      <c r="AD1" s="27"/>
-      <c r="AE1" s="27"/>
-      <c r="AF1" s="28"/>
+      <c r="Z1" s="28"/>
+      <c r="AA1" s="28"/>
+      <c r="AB1" s="28"/>
+      <c r="AC1" s="28"/>
+      <c r="AD1" s="28"/>
+      <c r="AE1" s="28"/>
+      <c r="AF1" s="29"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
@@ -3353,52 +3371,52 @@
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="32" t="s">
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="32" t="s">
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="O3" s="33"/>
-      <c r="P3" s="34"/>
-      <c r="Q3" s="32" t="s">
+      <c r="O3" s="34"/>
+      <c r="P3" s="35"/>
+      <c r="Q3" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="R3" s="33"/>
-      <c r="S3" s="34"/>
-      <c r="T3" s="29" t="s">
+      <c r="R3" s="34"/>
+      <c r="S3" s="35"/>
+      <c r="T3" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="U3" s="30"/>
-      <c r="V3" s="30"/>
-      <c r="W3" s="30"/>
-      <c r="X3" s="31"/>
-      <c r="Y3" s="29" t="s">
+      <c r="U3" s="31"/>
+      <c r="V3" s="31"/>
+      <c r="W3" s="31"/>
+      <c r="X3" s="32"/>
+      <c r="Y3" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="Z3" s="30"/>
-      <c r="AA3" s="30"/>
-      <c r="AB3" s="30"/>
-      <c r="AC3" s="31"/>
-      <c r="AD3" s="29" t="s">
+      <c r="Z3" s="31"/>
+      <c r="AA3" s="31"/>
+      <c r="AB3" s="31"/>
+      <c r="AC3" s="32"/>
+      <c r="AD3" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="AE3" s="30"/>
-      <c r="AF3" s="31"/>
+      <c r="AE3" s="31"/>
+      <c r="AF3" s="32"/>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
@@ -3458,46 +3476,46 @@
       <c r="AF5" s="25"/>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24">
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26">
         <v>38</v>
       </c>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="24"/>
-      <c r="O6" s="24"/>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="24">
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="26"/>
+      <c r="Q6" s="26">
         <v>73</v>
       </c>
-      <c r="R6" s="24"/>
-      <c r="S6" s="24"/>
-      <c r="T6" s="24"/>
-      <c r="U6" s="24"/>
-      <c r="V6" s="24"/>
-      <c r="W6" s="24"/>
-      <c r="X6" s="24"/>
-      <c r="Y6" s="24">
+      <c r="R6" s="26"/>
+      <c r="S6" s="26"/>
+      <c r="T6" s="26"/>
+      <c r="U6" s="26"/>
+      <c r="V6" s="26"/>
+      <c r="W6" s="26"/>
+      <c r="X6" s="26"/>
+      <c r="Y6" s="26">
         <v>88</v>
       </c>
-      <c r="Z6" s="24"/>
-      <c r="AA6" s="24"/>
-      <c r="AB6" s="24"/>
-      <c r="AC6" s="24"/>
-      <c r="AD6" s="24"/>
-      <c r="AE6" s="24"/>
-      <c r="AF6" s="24"/>
+      <c r="Z6" s="26"/>
+      <c r="AA6" s="26"/>
+      <c r="AB6" s="26"/>
+      <c r="AC6" s="26"/>
+      <c r="AD6" s="26"/>
+      <c r="AE6" s="26"/>
+      <c r="AF6" s="26"/>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
@@ -3598,203 +3616,203 @@
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20" t="s">
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="20" t="s">
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="O8" s="20"/>
-      <c r="P8" s="20"/>
-      <c r="Q8" s="20" t="s">
+      <c r="O8" s="22"/>
+      <c r="P8" s="22"/>
+      <c r="Q8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="R8" s="20"/>
-      <c r="S8" s="20"/>
-      <c r="T8" s="20" t="s">
+      <c r="R8" s="22"/>
+      <c r="S8" s="22"/>
+      <c r="T8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="U8" s="20"/>
-      <c r="V8" s="20"/>
-      <c r="W8" s="20"/>
-      <c r="X8" s="20"/>
-      <c r="Y8" s="20" t="s">
+      <c r="U8" s="22"/>
+      <c r="V8" s="22"/>
+      <c r="W8" s="22"/>
+      <c r="X8" s="22"/>
+      <c r="Y8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="Z8" s="20"/>
-      <c r="AA8" s="20"/>
-      <c r="AB8" s="20"/>
-      <c r="AC8" s="20"/>
-      <c r="AD8" s="20" t="s">
+      <c r="Z8" s="22"/>
+      <c r="AA8" s="22"/>
+      <c r="AB8" s="22"/>
+      <c r="AC8" s="22"/>
+      <c r="AD8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="AE8" s="20"/>
-      <c r="AF8" s="20"/>
+      <c r="AE8" s="22"/>
+      <c r="AF8" s="22"/>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A9" s="20">
+      <c r="A9" s="22">
         <v>10</v>
       </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20">
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22">
         <v>7</v>
       </c>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="20">
-        <v>0</v>
-      </c>
-      <c r="O9" s="20"/>
-      <c r="P9" s="20"/>
-      <c r="Q9" s="20">
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22">
+        <v>0</v>
+      </c>
+      <c r="O9" s="22"/>
+      <c r="P9" s="22"/>
+      <c r="Q9" s="22">
         <v>3</v>
       </c>
-      <c r="R9" s="20"/>
-      <c r="S9" s="20"/>
-      <c r="T9" s="20">
+      <c r="R9" s="22"/>
+      <c r="S9" s="22"/>
+      <c r="T9" s="22">
         <v>19</v>
       </c>
-      <c r="U9" s="20"/>
-      <c r="V9" s="20"/>
-      <c r="W9" s="20"/>
-      <c r="X9" s="20"/>
-      <c r="Y9" s="20">
+      <c r="U9" s="22"/>
+      <c r="V9" s="22"/>
+      <c r="W9" s="22"/>
+      <c r="X9" s="22"/>
+      <c r="Y9" s="22">
         <v>17</v>
       </c>
-      <c r="Z9" s="20"/>
-      <c r="AA9" s="20"/>
-      <c r="AB9" s="20"/>
-      <c r="AC9" s="20"/>
-      <c r="AD9" s="20">
-        <v>0</v>
-      </c>
-      <c r="AE9" s="20"/>
-      <c r="AF9" s="20"/>
+      <c r="Z9" s="22"/>
+      <c r="AA9" s="22"/>
+      <c r="AB9" s="22"/>
+      <c r="AC9" s="22"/>
+      <c r="AD9" s="22">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="22"/>
+      <c r="AF9" s="22"/>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20" t="s">
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="20" t="s">
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="O10" s="20"/>
-      <c r="P10" s="20"/>
-      <c r="Q10" s="20" t="s">
+      <c r="O10" s="22"/>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="R10" s="20"/>
-      <c r="S10" s="20"/>
-      <c r="T10" s="20" t="s">
+      <c r="R10" s="22"/>
+      <c r="S10" s="22"/>
+      <c r="T10" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="U10" s="20"/>
-      <c r="V10" s="20"/>
-      <c r="W10" s="20"/>
-      <c r="X10" s="20"/>
-      <c r="Y10" s="20" t="s">
+      <c r="U10" s="22"/>
+      <c r="V10" s="22"/>
+      <c r="W10" s="22"/>
+      <c r="X10" s="22"/>
+      <c r="Y10" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="Z10" s="20"/>
-      <c r="AA10" s="20"/>
-      <c r="AB10" s="20"/>
-      <c r="AC10" s="20"/>
-      <c r="AD10" s="20" t="s">
+      <c r="Z10" s="22"/>
+      <c r="AA10" s="22"/>
+      <c r="AB10" s="22"/>
+      <c r="AC10" s="22"/>
+      <c r="AD10" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="AE10" s="20"/>
-      <c r="AF10" s="20"/>
+      <c r="AE10" s="22"/>
+      <c r="AF10" s="22"/>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A11" s="20">
+      <c r="A11" s="22">
         <f>A9</f>
         <v>10</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="21">
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="23">
         <f>'Data package'!$B$31*I9+'Data package'!$B$28</f>
         <v>3.338709677419355</v>
       </c>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="21"/>
-      <c r="M11" s="21"/>
-      <c r="N11" s="22">
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="20">
         <f ca="1">LOOKUP(N9,'Data package'!$D$21:$D$24,'Data package'!$E$22:$E$35)</f>
         <v>0</v>
       </c>
-      <c r="O11" s="22"/>
-      <c r="P11" s="22"/>
-      <c r="Q11" s="23">
+      <c r="O11" s="20"/>
+      <c r="P11" s="20"/>
+      <c r="Q11" s="24">
         <f>100/(2^3-1)*Q9</f>
         <v>42.857142857142861</v>
       </c>
-      <c r="R11" s="23"/>
-      <c r="S11" s="23"/>
-      <c r="T11" s="23">
+      <c r="R11" s="24"/>
+      <c r="S11" s="24"/>
+      <c r="T11" s="24">
         <f>'Data package'!$B$40*T9+'Data package'!$B$37</f>
         <v>22.903225806451616</v>
       </c>
-      <c r="U11" s="22"/>
-      <c r="V11" s="22"/>
-      <c r="W11" s="22"/>
-      <c r="X11" s="22"/>
-      <c r="Y11" s="22">
+      <c r="U11" s="20"/>
+      <c r="V11" s="20"/>
+      <c r="W11" s="20"/>
+      <c r="X11" s="20"/>
+      <c r="Y11" s="20">
         <f>Y9</f>
         <v>17</v>
       </c>
-      <c r="Z11" s="22"/>
-      <c r="AA11" s="22"/>
-      <c r="AB11" s="22"/>
-      <c r="AC11" s="22"/>
-      <c r="AD11" s="22">
+      <c r="Z11" s="20"/>
+      <c r="AA11" s="20"/>
+      <c r="AB11" s="20"/>
+      <c r="AC11" s="20"/>
+      <c r="AD11" s="20">
         <f>LOOKUP(AD9,'Data package'!$A$84:$A$88,'Data package'!$B$84:$B$88)</f>
         <v>1</v>
       </c>
-      <c r="AE11" s="22"/>
-      <c r="AF11" s="22"/>
+      <c r="AE11" s="20"/>
+      <c r="AF11" s="20"/>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
@@ -3846,46 +3864,46 @@
       <c r="AF14" s="25"/>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24" t="s">
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="J15" s="24"/>
-      <c r="K15" s="24"/>
-      <c r="L15" s="24"/>
-      <c r="M15" s="24"/>
-      <c r="N15" s="24"/>
-      <c r="O15" s="24"/>
-      <c r="P15" s="24"/>
-      <c r="Q15" s="24" t="s">
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="26"/>
+      <c r="O15" s="26"/>
+      <c r="P15" s="26"/>
+      <c r="Q15" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="R15" s="24"/>
-      <c r="S15" s="24"/>
-      <c r="T15" s="24"/>
-      <c r="U15" s="24"/>
-      <c r="V15" s="24"/>
-      <c r="W15" s="24"/>
-      <c r="X15" s="24"/>
-      <c r="Y15" s="24" t="s">
+      <c r="R15" s="26"/>
+      <c r="S15" s="26"/>
+      <c r="T15" s="26"/>
+      <c r="U15" s="26"/>
+      <c r="V15" s="26"/>
+      <c r="W15" s="26"/>
+      <c r="X15" s="26"/>
+      <c r="Y15" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="Z15" s="24"/>
-      <c r="AA15" s="24"/>
-      <c r="AB15" s="24"/>
-      <c r="AC15" s="24"/>
-      <c r="AD15" s="24"/>
-      <c r="AE15" s="24"/>
-      <c r="AF15" s="24"/>
+      <c r="Z15" s="26"/>
+      <c r="AA15" s="26"/>
+      <c r="AB15" s="26"/>
+      <c r="AC15" s="26"/>
+      <c r="AD15" s="26"/>
+      <c r="AE15" s="26"/>
+      <c r="AF15" s="26"/>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
@@ -3986,203 +4004,203 @@
       </c>
     </row>
     <row r="17" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20" t="s">
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="20"/>
-      <c r="M17" s="20"/>
-      <c r="N17" s="20" t="s">
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22"/>
+      <c r="N17" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="O17" s="20"/>
-      <c r="P17" s="20"/>
-      <c r="Q17" s="20" t="s">
+      <c r="O17" s="22"/>
+      <c r="P17" s="22"/>
+      <c r="Q17" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="R17" s="20"/>
-      <c r="S17" s="20"/>
-      <c r="T17" s="20" t="s">
+      <c r="R17" s="22"/>
+      <c r="S17" s="22"/>
+      <c r="T17" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="U17" s="20"/>
-      <c r="V17" s="20"/>
-      <c r="W17" s="20"/>
-      <c r="X17" s="20"/>
-      <c r="Y17" s="20" t="s">
+      <c r="U17" s="22"/>
+      <c r="V17" s="22"/>
+      <c r="W17" s="22"/>
+      <c r="X17" s="22"/>
+      <c r="Y17" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="Z17" s="20"/>
-      <c r="AA17" s="20"/>
-      <c r="AB17" s="20"/>
-      <c r="AC17" s="20"/>
-      <c r="AD17" s="20" t="s">
+      <c r="Z17" s="22"/>
+      <c r="AA17" s="22"/>
+      <c r="AB17" s="22"/>
+      <c r="AC17" s="22"/>
+      <c r="AD17" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="AE17" s="20"/>
-      <c r="AF17" s="20"/>
+      <c r="AE17" s="22"/>
+      <c r="AF17" s="22"/>
     </row>
     <row r="18" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A18" s="20">
+      <c r="A18" s="22">
         <v>5</v>
       </c>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20">
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22">
         <v>8</v>
       </c>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="20"/>
-      <c r="M18" s="20"/>
-      <c r="N18" s="20">
-        <v>0</v>
-      </c>
-      <c r="O18" s="20"/>
-      <c r="P18" s="20"/>
-      <c r="Q18" s="20">
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="22"/>
+      <c r="N18" s="22">
+        <v>0</v>
+      </c>
+      <c r="O18" s="22"/>
+      <c r="P18" s="22"/>
+      <c r="Q18" s="22">
         <v>3</v>
       </c>
-      <c r="R18" s="20"/>
-      <c r="S18" s="20"/>
-      <c r="T18" s="20">
+      <c r="R18" s="22"/>
+      <c r="S18" s="22"/>
+      <c r="T18" s="22">
         <v>19</v>
       </c>
-      <c r="U18" s="20"/>
-      <c r="V18" s="20"/>
-      <c r="W18" s="20"/>
-      <c r="X18" s="20"/>
-      <c r="Y18" s="20">
+      <c r="U18" s="22"/>
+      <c r="V18" s="22"/>
+      <c r="W18" s="22"/>
+      <c r="X18" s="22"/>
+      <c r="Y18" s="22">
         <v>17</v>
       </c>
-      <c r="Z18" s="20"/>
-      <c r="AA18" s="20"/>
-      <c r="AB18" s="20"/>
-      <c r="AC18" s="20"/>
-      <c r="AD18" s="20">
-        <v>0</v>
-      </c>
-      <c r="AE18" s="20"/>
-      <c r="AF18" s="20"/>
+      <c r="Z18" s="22"/>
+      <c r="AA18" s="22"/>
+      <c r="AB18" s="22"/>
+      <c r="AC18" s="22"/>
+      <c r="AD18" s="22">
+        <v>0</v>
+      </c>
+      <c r="AE18" s="22"/>
+      <c r="AF18" s="22"/>
     </row>
     <row r="19" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A19" s="20" t="s">
+      <c r="A19" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20" t="s">
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
-      <c r="M19" s="20"/>
-      <c r="N19" s="20" t="s">
+      <c r="J19" s="22"/>
+      <c r="K19" s="22"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="22"/>
+      <c r="N19" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="O19" s="20"/>
-      <c r="P19" s="20"/>
-      <c r="Q19" s="20" t="s">
+      <c r="O19" s="22"/>
+      <c r="P19" s="22"/>
+      <c r="Q19" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="R19" s="20"/>
-      <c r="S19" s="20"/>
-      <c r="T19" s="20" t="s">
+      <c r="R19" s="22"/>
+      <c r="S19" s="22"/>
+      <c r="T19" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="U19" s="20"/>
-      <c r="V19" s="20"/>
-      <c r="W19" s="20"/>
-      <c r="X19" s="20"/>
-      <c r="Y19" s="20" t="s">
+      <c r="U19" s="22"/>
+      <c r="V19" s="22"/>
+      <c r="W19" s="22"/>
+      <c r="X19" s="22"/>
+      <c r="Y19" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="Z19" s="20"/>
-      <c r="AA19" s="20"/>
-      <c r="AB19" s="20"/>
-      <c r="AC19" s="20"/>
-      <c r="AD19" s="20" t="s">
+      <c r="Z19" s="22"/>
+      <c r="AA19" s="22"/>
+      <c r="AB19" s="22"/>
+      <c r="AC19" s="22"/>
+      <c r="AD19" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="AE19" s="20"/>
-      <c r="AF19" s="20"/>
+      <c r="AE19" s="22"/>
+      <c r="AF19" s="22"/>
     </row>
     <row r="20" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A20" s="20">
+      <c r="A20" s="22">
         <f>A18</f>
         <v>5</v>
       </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="21">
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="23">
         <f>'Data package'!$B$31*I18+'Data package'!$B$28</f>
         <v>3.3870967741935485</v>
       </c>
-      <c r="J20" s="21"/>
-      <c r="K20" s="21"/>
-      <c r="L20" s="21"/>
-      <c r="M20" s="21"/>
-      <c r="N20" s="22">
+      <c r="J20" s="23"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="23"/>
+      <c r="N20" s="20">
         <f ca="1">LOOKUP(N18,'Data package'!$D$21:$D$24,'Data package'!$E$22:$E$35)</f>
         <v>0</v>
       </c>
-      <c r="O20" s="22"/>
-      <c r="P20" s="22"/>
-      <c r="Q20" s="23">
+      <c r="O20" s="20"/>
+      <c r="P20" s="20"/>
+      <c r="Q20" s="24">
         <f>100/(2^3-1)*Q18</f>
         <v>42.857142857142861</v>
       </c>
-      <c r="R20" s="23"/>
-      <c r="S20" s="23"/>
-      <c r="T20" s="23">
+      <c r="R20" s="24"/>
+      <c r="S20" s="24"/>
+      <c r="T20" s="24">
         <f>'Data package'!$B$40*T18+'Data package'!$B$37</f>
         <v>22.903225806451616</v>
       </c>
-      <c r="U20" s="22"/>
-      <c r="V20" s="22"/>
-      <c r="W20" s="22"/>
-      <c r="X20" s="22"/>
-      <c r="Y20" s="22">
+      <c r="U20" s="20"/>
+      <c r="V20" s="20"/>
+      <c r="W20" s="20"/>
+      <c r="X20" s="20"/>
+      <c r="Y20" s="20">
         <f>Y18</f>
         <v>17</v>
       </c>
-      <c r="Z20" s="22"/>
-      <c r="AA20" s="22"/>
-      <c r="AB20" s="22"/>
-      <c r="AC20" s="22"/>
-      <c r="AD20" s="22">
+      <c r="Z20" s="20"/>
+      <c r="AA20" s="20"/>
+      <c r="AB20" s="20"/>
+      <c r="AC20" s="20"/>
+      <c r="AD20" s="20">
         <f>LOOKUP(AD18,'Data package'!$A$84:$A$88,'Data package'!$B$84:$B$88)</f>
         <v>1</v>
       </c>
-      <c r="AE20" s="22"/>
-      <c r="AF20" s="22"/>
+      <c r="AE20" s="20"/>
+      <c r="AF20" s="20"/>
     </row>
     <row r="23" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A23" s="25" t="s">
@@ -4221,126 +4239,126 @@
       <c r="AF23" s="25"/>
     </row>
     <row r="24" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="24"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="24" t="s">
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="J24" s="24"/>
-      <c r="K24" s="24"/>
-      <c r="L24" s="24"/>
-      <c r="M24" s="24"/>
-      <c r="N24" s="24"/>
-      <c r="O24" s="24"/>
-      <c r="P24" s="24"/>
-      <c r="Q24" s="24" t="s">
+      <c r="J24" s="26"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="26"/>
+      <c r="M24" s="26"/>
+      <c r="N24" s="26"/>
+      <c r="O24" s="26"/>
+      <c r="P24" s="26"/>
+      <c r="Q24" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="R24" s="24"/>
-      <c r="S24" s="24"/>
-      <c r="T24" s="24"/>
-      <c r="U24" s="24"/>
-      <c r="V24" s="24"/>
-      <c r="W24" s="24"/>
-      <c r="X24" s="24"/>
-      <c r="Y24" s="24" t="s">
+      <c r="R24" s="26"/>
+      <c r="S24" s="26"/>
+      <c r="T24" s="26"/>
+      <c r="U24" s="26"/>
+      <c r="V24" s="26"/>
+      <c r="W24" s="26"/>
+      <c r="X24" s="26"/>
+      <c r="Y24" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="Z24" s="24"/>
-      <c r="AA24" s="24"/>
-      <c r="AB24" s="24"/>
-      <c r="AC24" s="24"/>
-      <c r="AD24" s="24"/>
-      <c r="AE24" s="24"/>
-      <c r="AF24" s="24"/>
-      <c r="AG24" s="35">
+      <c r="Z24" s="26"/>
+      <c r="AA24" s="26"/>
+      <c r="AB24" s="26"/>
+      <c r="AC24" s="26"/>
+      <c r="AD24" s="26"/>
+      <c r="AE24" s="26"/>
+      <c r="AF24" s="26"/>
+      <c r="AG24" s="21">
         <v>59</v>
       </c>
-      <c r="AH24" s="35"/>
-      <c r="AI24" s="35"/>
-      <c r="AJ24" s="35"/>
-      <c r="AK24" s="35"/>
-      <c r="AL24" s="35"/>
-      <c r="AM24" s="35"/>
-      <c r="AN24" s="35"/>
-      <c r="AO24" s="35">
+      <c r="AH24" s="21"/>
+      <c r="AI24" s="21"/>
+      <c r="AJ24" s="21"/>
+      <c r="AK24" s="21"/>
+      <c r="AL24" s="21"/>
+      <c r="AM24" s="21"/>
+      <c r="AN24" s="21"/>
+      <c r="AO24" s="21">
         <v>96</v>
       </c>
-      <c r="AP24" s="35"/>
-      <c r="AQ24" s="35"/>
-      <c r="AR24" s="35"/>
-      <c r="AS24" s="35"/>
-      <c r="AT24" s="35"/>
-      <c r="AU24" s="35"/>
-      <c r="AV24" s="35"/>
-      <c r="AW24" s="35">
+      <c r="AP24" s="21"/>
+      <c r="AQ24" s="21"/>
+      <c r="AR24" s="21"/>
+      <c r="AS24" s="21"/>
+      <c r="AT24" s="21"/>
+      <c r="AU24" s="21"/>
+      <c r="AV24" s="21"/>
+      <c r="AW24" s="21">
         <v>65</v>
       </c>
-      <c r="AX24" s="35"/>
-      <c r="AY24" s="35"/>
-      <c r="AZ24" s="35"/>
-      <c r="BA24" s="35"/>
-      <c r="BB24" s="35"/>
-      <c r="BC24" s="35"/>
-      <c r="BD24" s="35"/>
-      <c r="BE24" s="35" t="s">
+      <c r="AX24" s="21"/>
+      <c r="AY24" s="21"/>
+      <c r="AZ24" s="21"/>
+      <c r="BA24" s="21"/>
+      <c r="BB24" s="21"/>
+      <c r="BC24" s="21"/>
+      <c r="BD24" s="21"/>
+      <c r="BE24" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="BF24" s="35"/>
-      <c r="BG24" s="35"/>
-      <c r="BH24" s="35"/>
-      <c r="BI24" s="35"/>
-      <c r="BJ24" s="35"/>
-      <c r="BK24" s="35"/>
-      <c r="BL24" s="35"/>
-      <c r="BM24" s="35" t="s">
+      <c r="BF24" s="21"/>
+      <c r="BG24" s="21"/>
+      <c r="BH24" s="21"/>
+      <c r="BI24" s="21"/>
+      <c r="BJ24" s="21"/>
+      <c r="BK24" s="21"/>
+      <c r="BL24" s="21"/>
+      <c r="BM24" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="BN24" s="35"/>
-      <c r="BO24" s="35"/>
-      <c r="BP24" s="35"/>
-      <c r="BQ24" s="35"/>
-      <c r="BR24" s="35"/>
-      <c r="BS24" s="35"/>
-      <c r="BT24" s="35"/>
-      <c r="BU24" s="35">
+      <c r="BN24" s="21"/>
+      <c r="BO24" s="21"/>
+      <c r="BP24" s="21"/>
+      <c r="BQ24" s="21"/>
+      <c r="BR24" s="21"/>
+      <c r="BS24" s="21"/>
+      <c r="BT24" s="21"/>
+      <c r="BU24" s="21">
         <v>69</v>
       </c>
-      <c r="BV24" s="35"/>
-      <c r="BW24" s="35"/>
-      <c r="BX24" s="35"/>
-      <c r="BY24" s="35"/>
-      <c r="BZ24" s="35"/>
-      <c r="CA24" s="35"/>
-      <c r="CB24" s="35"/>
-      <c r="CC24" s="35" t="s">
+      <c r="BV24" s="21"/>
+      <c r="BW24" s="21"/>
+      <c r="BX24" s="21"/>
+      <c r="BY24" s="21"/>
+      <c r="BZ24" s="21"/>
+      <c r="CA24" s="21"/>
+      <c r="CB24" s="21"/>
+      <c r="CC24" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="CD24" s="35"/>
-      <c r="CE24" s="35"/>
-      <c r="CF24" s="35"/>
-      <c r="CG24" s="35"/>
-      <c r="CH24" s="35"/>
-      <c r="CI24" s="35"/>
-      <c r="CJ24" s="35"/>
-      <c r="CK24" s="35" t="s">
+      <c r="CD24" s="21"/>
+      <c r="CE24" s="21"/>
+      <c r="CF24" s="21"/>
+      <c r="CG24" s="21"/>
+      <c r="CH24" s="21"/>
+      <c r="CI24" s="21"/>
+      <c r="CJ24" s="21"/>
+      <c r="CK24" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="CL24" s="35"/>
-      <c r="CM24" s="35"/>
-      <c r="CN24" s="35"/>
-      <c r="CO24" s="35"/>
-      <c r="CP24" s="35"/>
-      <c r="CQ24" s="35"/>
-      <c r="CR24" s="35"/>
+      <c r="CL24" s="21"/>
+      <c r="CM24" s="21"/>
+      <c r="CN24" s="21"/>
+      <c r="CO24" s="21"/>
+      <c r="CP24" s="21"/>
+      <c r="CQ24" s="21"/>
+      <c r="CR24" s="21"/>
     </row>
     <row r="25" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A25" s="7">
@@ -4633,180 +4651,180 @@
       </c>
     </row>
     <row r="26" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A26" s="20" t="s">
+      <c r="A26" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20" t="s">
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="J26" s="20"/>
-      <c r="K26" s="20"/>
-      <c r="L26" s="20"/>
-      <c r="M26" s="20"/>
-      <c r="N26" s="20" t="s">
+      <c r="J26" s="22"/>
+      <c r="K26" s="22"/>
+      <c r="L26" s="22"/>
+      <c r="M26" s="22"/>
+      <c r="N26" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="O26" s="20"/>
-      <c r="P26" s="20"/>
-      <c r="Q26" s="20" t="s">
+      <c r="O26" s="22"/>
+      <c r="P26" s="22"/>
+      <c r="Q26" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="R26" s="20"/>
-      <c r="S26" s="20"/>
-      <c r="T26" s="20" t="s">
+      <c r="R26" s="22"/>
+      <c r="S26" s="22"/>
+      <c r="T26" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="U26" s="20"/>
-      <c r="V26" s="20"/>
-      <c r="W26" s="20"/>
-      <c r="X26" s="20"/>
-      <c r="Y26" s="20" t="s">
+      <c r="U26" s="22"/>
+      <c r="V26" s="22"/>
+      <c r="W26" s="22"/>
+      <c r="X26" s="22"/>
+      <c r="Y26" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="Z26" s="20"/>
-      <c r="AA26" s="20"/>
-      <c r="AB26" s="20"/>
-      <c r="AC26" s="20"/>
-      <c r="AD26" s="20" t="s">
+      <c r="Z26" s="22"/>
+      <c r="AA26" s="22"/>
+      <c r="AB26" s="22"/>
+      <c r="AC26" s="22"/>
+      <c r="AD26" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="AE26" s="20"/>
-      <c r="AF26" s="20"/>
-      <c r="AG26" s="22" t="s">
+      <c r="AE26" s="22"/>
+      <c r="AF26" s="22"/>
+      <c r="AG26" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="AH26" s="22"/>
-      <c r="AI26" s="22"/>
-      <c r="AJ26" s="22"/>
-      <c r="AK26" s="22"/>
-      <c r="AL26" s="22"/>
-      <c r="AM26" s="22"/>
-      <c r="AN26" s="22"/>
-      <c r="AO26" s="22" t="s">
+      <c r="AH26" s="20"/>
+      <c r="AI26" s="20"/>
+      <c r="AJ26" s="20"/>
+      <c r="AK26" s="20"/>
+      <c r="AL26" s="20"/>
+      <c r="AM26" s="20"/>
+      <c r="AN26" s="20"/>
+      <c r="AO26" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="AP26" s="22"/>
-      <c r="AQ26" s="22"/>
-      <c r="AR26" s="22"/>
-      <c r="AS26" s="22"/>
-      <c r="AT26" s="22"/>
-      <c r="AU26" s="22"/>
-      <c r="AV26" s="22"/>
-      <c r="AW26" s="22" t="s">
+      <c r="AP26" s="20"/>
+      <c r="AQ26" s="20"/>
+      <c r="AR26" s="20"/>
+      <c r="AS26" s="20"/>
+      <c r="AT26" s="20"/>
+      <c r="AU26" s="20"/>
+      <c r="AV26" s="20"/>
+      <c r="AW26" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="AX26" s="22"/>
-      <c r="AY26" s="22"/>
-      <c r="AZ26" s="22"/>
-      <c r="BA26" s="22"/>
-      <c r="BB26" s="22"/>
-      <c r="BC26" s="22"/>
-      <c r="BD26" s="22"/>
-      <c r="BE26" s="22" t="s">
+      <c r="AX26" s="20"/>
+      <c r="AY26" s="20"/>
+      <c r="AZ26" s="20"/>
+      <c r="BA26" s="20"/>
+      <c r="BB26" s="20"/>
+      <c r="BC26" s="20"/>
+      <c r="BD26" s="20"/>
+      <c r="BE26" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="BF26" s="22"/>
-      <c r="BG26" s="22"/>
-      <c r="BH26" s="22"/>
-      <c r="BI26" s="22"/>
-      <c r="BJ26" s="22"/>
-      <c r="BK26" s="22"/>
-      <c r="BL26" s="22"/>
-      <c r="BM26" s="22" t="s">
+      <c r="BF26" s="20"/>
+      <c r="BG26" s="20"/>
+      <c r="BH26" s="20"/>
+      <c r="BI26" s="20"/>
+      <c r="BJ26" s="20"/>
+      <c r="BK26" s="20"/>
+      <c r="BL26" s="20"/>
+      <c r="BM26" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="BN26" s="22"/>
-      <c r="BO26" s="22"/>
-      <c r="BP26" s="22"/>
-      <c r="BQ26" s="22"/>
-      <c r="BR26" s="22"/>
-      <c r="BS26" s="22"/>
-      <c r="BT26" s="22"/>
-      <c r="BU26" s="22" t="s">
+      <c r="BN26" s="20"/>
+      <c r="BO26" s="20"/>
+      <c r="BP26" s="20"/>
+      <c r="BQ26" s="20"/>
+      <c r="BR26" s="20"/>
+      <c r="BS26" s="20"/>
+      <c r="BT26" s="20"/>
+      <c r="BU26" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="BV26" s="22"/>
-      <c r="BW26" s="22"/>
-      <c r="BX26" s="22"/>
-      <c r="BY26" s="22"/>
-      <c r="BZ26" s="22"/>
-      <c r="CA26" s="22"/>
-      <c r="CB26" s="22"/>
-      <c r="CC26" s="22" t="s">
+      <c r="BV26" s="20"/>
+      <c r="BW26" s="20"/>
+      <c r="BX26" s="20"/>
+      <c r="BY26" s="20"/>
+      <c r="BZ26" s="20"/>
+      <c r="CA26" s="20"/>
+      <c r="CB26" s="20"/>
+      <c r="CC26" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="CD26" s="22"/>
-      <c r="CE26" s="22"/>
-      <c r="CF26" s="22"/>
-      <c r="CG26" s="22"/>
-      <c r="CH26" s="22"/>
-      <c r="CI26" s="22"/>
-      <c r="CJ26" s="22"/>
-      <c r="CK26" s="22" t="s">
+      <c r="CD26" s="20"/>
+      <c r="CE26" s="20"/>
+      <c r="CF26" s="20"/>
+      <c r="CG26" s="20"/>
+      <c r="CH26" s="20"/>
+      <c r="CI26" s="20"/>
+      <c r="CJ26" s="20"/>
+      <c r="CK26" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="CL26" s="22"/>
-      <c r="CM26" s="22"/>
-      <c r="CN26" s="22"/>
-      <c r="CO26" s="22"/>
-      <c r="CP26" s="22"/>
-      <c r="CQ26" s="22"/>
-      <c r="CR26" s="22"/>
+      <c r="CL26" s="20"/>
+      <c r="CM26" s="20"/>
+      <c r="CN26" s="20"/>
+      <c r="CO26" s="20"/>
+      <c r="CP26" s="20"/>
+      <c r="CQ26" s="20"/>
+      <c r="CR26" s="20"/>
     </row>
     <row r="27" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A27" s="20">
+      <c r="A27" s="22">
         <v>10</v>
       </c>
-      <c r="B27" s="20"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="20">
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22">
         <v>8</v>
       </c>
-      <c r="J27" s="20"/>
-      <c r="K27" s="20"/>
-      <c r="L27" s="20"/>
-      <c r="M27" s="20"/>
-      <c r="N27" s="20">
-        <v>0</v>
-      </c>
-      <c r="O27" s="20"/>
-      <c r="P27" s="20"/>
-      <c r="Q27" s="20">
+      <c r="J27" s="22"/>
+      <c r="K27" s="22"/>
+      <c r="L27" s="22"/>
+      <c r="M27" s="22"/>
+      <c r="N27" s="22">
+        <v>0</v>
+      </c>
+      <c r="O27" s="22"/>
+      <c r="P27" s="22"/>
+      <c r="Q27" s="22">
         <v>3</v>
       </c>
-      <c r="R27" s="20"/>
-      <c r="S27" s="20"/>
-      <c r="T27" s="20">
+      <c r="R27" s="22"/>
+      <c r="S27" s="22"/>
+      <c r="T27" s="22">
         <v>19</v>
       </c>
-      <c r="U27" s="20"/>
-      <c r="V27" s="20"/>
-      <c r="W27" s="20"/>
-      <c r="X27" s="20"/>
-      <c r="Y27" s="20">
+      <c r="U27" s="22"/>
+      <c r="V27" s="22"/>
+      <c r="W27" s="22"/>
+      <c r="X27" s="22"/>
+      <c r="Y27" s="22">
         <v>21</v>
       </c>
-      <c r="Z27" s="20"/>
-      <c r="AA27" s="20"/>
-      <c r="AB27" s="20"/>
-      <c r="AC27" s="20"/>
-      <c r="AD27" s="20">
-        <v>0</v>
-      </c>
-      <c r="AE27" s="20"/>
-      <c r="AF27" s="20"/>
+      <c r="Z27" s="22"/>
+      <c r="AA27" s="22"/>
+      <c r="AB27" s="22"/>
+      <c r="AC27" s="22"/>
+      <c r="AD27" s="22">
+        <v>0</v>
+      </c>
+      <c r="AE27" s="22"/>
+      <c r="AF27" s="22"/>
       <c r="AG27">
         <f>AN25</f>
         <v>1</v>
@@ -5065,267 +5083,267 @@
       </c>
     </row>
     <row r="28" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A28" s="20" t="s">
+      <c r="A28" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="20"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
-      <c r="I28" s="20" t="s">
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="J28" s="20"/>
-      <c r="K28" s="20"/>
-      <c r="L28" s="20"/>
-      <c r="M28" s="20"/>
-      <c r="N28" s="20" t="s">
+      <c r="J28" s="22"/>
+      <c r="K28" s="22"/>
+      <c r="L28" s="22"/>
+      <c r="M28" s="22"/>
+      <c r="N28" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="O28" s="20"/>
-      <c r="P28" s="20"/>
-      <c r="Q28" s="20" t="s">
+      <c r="O28" s="22"/>
+      <c r="P28" s="22"/>
+      <c r="Q28" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="R28" s="20"/>
-      <c r="S28" s="20"/>
-      <c r="T28" s="20" t="s">
+      <c r="R28" s="22"/>
+      <c r="S28" s="22"/>
+      <c r="T28" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="U28" s="20"/>
-      <c r="V28" s="20"/>
-      <c r="W28" s="20"/>
-      <c r="X28" s="20"/>
-      <c r="Y28" s="20" t="s">
+      <c r="U28" s="22"/>
+      <c r="V28" s="22"/>
+      <c r="W28" s="22"/>
+      <c r="X28" s="22"/>
+      <c r="Y28" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="Z28" s="20"/>
-      <c r="AA28" s="20"/>
-      <c r="AB28" s="20"/>
-      <c r="AC28" s="20"/>
-      <c r="AD28" s="20" t="s">
+      <c r="Z28" s="22"/>
+      <c r="AA28" s="22"/>
+      <c r="AB28" s="22"/>
+      <c r="AC28" s="22"/>
+      <c r="AD28" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="AE28" s="20"/>
-      <c r="AF28" s="20"/>
-      <c r="AG28" s="22" t="s">
+      <c r="AE28" s="22"/>
+      <c r="AF28" s="22"/>
+      <c r="AG28" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="AH28" s="22"/>
-      <c r="AI28" s="22"/>
-      <c r="AJ28" s="22"/>
-      <c r="AK28" s="22"/>
-      <c r="AL28" s="22"/>
-      <c r="AM28" s="22" t="s">
+      <c r="AH28" s="20"/>
+      <c r="AI28" s="20"/>
+      <c r="AJ28" s="20"/>
+      <c r="AK28" s="20"/>
+      <c r="AL28" s="20"/>
+      <c r="AM28" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="AN28" s="22"/>
-      <c r="AO28" s="22"/>
-      <c r="AP28" s="22"/>
-      <c r="AQ28" s="22"/>
-      <c r="AR28" s="22"/>
-      <c r="AS28" s="22" t="s">
+      <c r="AN28" s="20"/>
+      <c r="AO28" s="20"/>
+      <c r="AP28" s="20"/>
+      <c r="AQ28" s="20"/>
+      <c r="AR28" s="20"/>
+      <c r="AS28" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="AT28" s="22"/>
-      <c r="AU28" s="22"/>
-      <c r="AV28" s="22"/>
-      <c r="AW28" s="22"/>
-      <c r="AX28" s="22"/>
-      <c r="AY28" s="22" t="s">
+      <c r="AT28" s="20"/>
+      <c r="AU28" s="20"/>
+      <c r="AV28" s="20"/>
+      <c r="AW28" s="20"/>
+      <c r="AX28" s="20"/>
+      <c r="AY28" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="AZ28" s="22"/>
-      <c r="BA28" s="22"/>
-      <c r="BB28" s="22"/>
-      <c r="BC28" s="22"/>
-      <c r="BD28" s="22"/>
-      <c r="BE28" s="22" t="s">
+      <c r="AZ28" s="20"/>
+      <c r="BA28" s="20"/>
+      <c r="BB28" s="20"/>
+      <c r="BC28" s="20"/>
+      <c r="BD28" s="20"/>
+      <c r="BE28" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="BF28" s="22"/>
-      <c r="BG28" s="22"/>
-      <c r="BH28" s="22"/>
-      <c r="BI28" s="22"/>
-      <c r="BJ28" s="22"/>
-      <c r="BK28" s="22" t="s">
+      <c r="BF28" s="20"/>
+      <c r="BG28" s="20"/>
+      <c r="BH28" s="20"/>
+      <c r="BI28" s="20"/>
+      <c r="BJ28" s="20"/>
+      <c r="BK28" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="BL28" s="22"/>
-      <c r="BM28" s="22"/>
-      <c r="BN28" s="22"/>
-      <c r="BO28" s="22"/>
-      <c r="BP28" s="22"/>
-      <c r="BQ28" s="22" t="s">
+      <c r="BL28" s="20"/>
+      <c r="BM28" s="20"/>
+      <c r="BN28" s="20"/>
+      <c r="BO28" s="20"/>
+      <c r="BP28" s="20"/>
+      <c r="BQ28" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="BR28" s="22"/>
-      <c r="BS28" s="22"/>
-      <c r="BT28" s="22"/>
-      <c r="BU28" s="22"/>
-      <c r="BV28" s="22"/>
-      <c r="BW28" s="22" t="s">
+      <c r="BR28" s="20"/>
+      <c r="BS28" s="20"/>
+      <c r="BT28" s="20"/>
+      <c r="BU28" s="20"/>
+      <c r="BV28" s="20"/>
+      <c r="BW28" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="BX28" s="22"/>
-      <c r="BY28" s="22"/>
-      <c r="BZ28" s="22"/>
-      <c r="CA28" s="22"/>
-      <c r="CB28" s="22"/>
-      <c r="CC28" s="22" t="s">
+      <c r="BX28" s="20"/>
+      <c r="BY28" s="20"/>
+      <c r="BZ28" s="20"/>
+      <c r="CA28" s="20"/>
+      <c r="CB28" s="20"/>
+      <c r="CC28" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="CD28" s="22"/>
-      <c r="CE28" s="22"/>
-      <c r="CF28" s="22"/>
-      <c r="CG28" s="22"/>
-      <c r="CH28" s="22"/>
-      <c r="CI28" s="22" t="s">
+      <c r="CD28" s="20"/>
+      <c r="CE28" s="20"/>
+      <c r="CF28" s="20"/>
+      <c r="CG28" s="20"/>
+      <c r="CH28" s="20"/>
+      <c r="CI28" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="CJ28" s="22"/>
-      <c r="CK28" s="22"/>
-      <c r="CL28" s="22"/>
-      <c r="CM28" s="22"/>
-      <c r="CN28" s="22"/>
+      <c r="CJ28" s="20"/>
+      <c r="CK28" s="20"/>
+      <c r="CL28" s="20"/>
+      <c r="CM28" s="20"/>
+      <c r="CN28" s="20"/>
     </row>
     <row r="29" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A29" s="20">
+      <c r="A29" s="22">
         <f>A27</f>
         <v>10</v>
       </c>
-      <c r="B29" s="20"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
-      <c r="I29" s="21">
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="23">
         <f>'Data package'!$B$31*I27+'Data package'!$B$28</f>
         <v>3.3870967741935485</v>
       </c>
-      <c r="J29" s="21"/>
-      <c r="K29" s="21"/>
-      <c r="L29" s="21"/>
-      <c r="M29" s="21"/>
-      <c r="N29" s="22">
+      <c r="J29" s="23"/>
+      <c r="K29" s="23"/>
+      <c r="L29" s="23"/>
+      <c r="M29" s="23"/>
+      <c r="N29" s="20">
         <f ca="1">LOOKUP(N27,'Data package'!$D$21:$D$24,'Data package'!$E$22:$E$35)</f>
         <v>0</v>
       </c>
-      <c r="O29" s="22"/>
-      <c r="P29" s="22"/>
-      <c r="Q29" s="23">
+      <c r="O29" s="20"/>
+      <c r="P29" s="20"/>
+      <c r="Q29" s="24">
         <f>100/(2^3-1)*Q27</f>
         <v>42.857142857142861</v>
       </c>
-      <c r="R29" s="23"/>
-      <c r="S29" s="23"/>
-      <c r="T29" s="23">
+      <c r="R29" s="24"/>
+      <c r="S29" s="24"/>
+      <c r="T29" s="24">
         <f>'Data package'!$B$40*T27+'Data package'!$B$37</f>
         <v>22.903225806451616</v>
       </c>
-      <c r="U29" s="22"/>
-      <c r="V29" s="22"/>
-      <c r="W29" s="22"/>
-      <c r="X29" s="22"/>
-      <c r="Y29" s="22">
+      <c r="U29" s="20"/>
+      <c r="V29" s="20"/>
+      <c r="W29" s="20"/>
+      <c r="X29" s="20"/>
+      <c r="Y29" s="20">
         <f>Y27</f>
         <v>21</v>
       </c>
-      <c r="Z29" s="22"/>
-      <c r="AA29" s="22"/>
-      <c r="AB29" s="22"/>
-      <c r="AC29" s="22"/>
-      <c r="AD29" s="22">
+      <c r="Z29" s="20"/>
+      <c r="AA29" s="20"/>
+      <c r="AB29" s="20"/>
+      <c r="AC29" s="20"/>
+      <c r="AD29" s="20">
         <f>LOOKUP(AD27,'Data package'!$A$84:$A$88,'Data package'!$B$84:$B$88)</f>
         <v>1</v>
       </c>
-      <c r="AE29" s="22"/>
-      <c r="AF29" s="22"/>
-      <c r="AG29" s="22" t="s">
+      <c r="AE29" s="20"/>
+      <c r="AF29" s="20"/>
+      <c r="AG29" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="AH29" s="22"/>
-      <c r="AI29" s="22"/>
-      <c r="AJ29" s="22"/>
-      <c r="AK29" s="22"/>
-      <c r="AL29" s="22"/>
-      <c r="AM29" s="22" t="s">
+      <c r="AH29" s="20"/>
+      <c r="AI29" s="20"/>
+      <c r="AJ29" s="20"/>
+      <c r="AK29" s="20"/>
+      <c r="AL29" s="20"/>
+      <c r="AM29" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="AN29" s="22"/>
-      <c r="AO29" s="22"/>
-      <c r="AP29" s="22"/>
-      <c r="AQ29" s="22"/>
-      <c r="AR29" s="22"/>
-      <c r="AS29" s="22" t="s">
+      <c r="AN29" s="20"/>
+      <c r="AO29" s="20"/>
+      <c r="AP29" s="20"/>
+      <c r="AQ29" s="20"/>
+      <c r="AR29" s="20"/>
+      <c r="AS29" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="AT29" s="22"/>
-      <c r="AU29" s="22"/>
-      <c r="AV29" s="22"/>
-      <c r="AW29" s="22"/>
-      <c r="AX29" s="22"/>
-      <c r="AY29" s="22" t="s">
+      <c r="AT29" s="20"/>
+      <c r="AU29" s="20"/>
+      <c r="AV29" s="20"/>
+      <c r="AW29" s="20"/>
+      <c r="AX29" s="20"/>
+      <c r="AY29" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="AZ29" s="22"/>
-      <c r="BA29" s="22"/>
-      <c r="BB29" s="22"/>
-      <c r="BC29" s="22"/>
-      <c r="BD29" s="22"/>
-      <c r="BE29" s="22" t="s">
+      <c r="AZ29" s="20"/>
+      <c r="BA29" s="20"/>
+      <c r="BB29" s="20"/>
+      <c r="BC29" s="20"/>
+      <c r="BD29" s="20"/>
+      <c r="BE29" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="BF29" s="22"/>
-      <c r="BG29" s="22"/>
-      <c r="BH29" s="22"/>
-      <c r="BI29" s="22"/>
-      <c r="BJ29" s="22"/>
-      <c r="BK29" s="22" t="s">
+      <c r="BF29" s="20"/>
+      <c r="BG29" s="20"/>
+      <c r="BH29" s="20"/>
+      <c r="BI29" s="20"/>
+      <c r="BJ29" s="20"/>
+      <c r="BK29" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="BL29" s="22"/>
-      <c r="BM29" s="22"/>
-      <c r="BN29" s="22"/>
-      <c r="BO29" s="22"/>
-      <c r="BP29" s="22"/>
-      <c r="BQ29" s="22" t="s">
+      <c r="BL29" s="20"/>
+      <c r="BM29" s="20"/>
+      <c r="BN29" s="20"/>
+      <c r="BO29" s="20"/>
+      <c r="BP29" s="20"/>
+      <c r="BQ29" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="BR29" s="22"/>
-      <c r="BS29" s="22"/>
-      <c r="BT29" s="22"/>
-      <c r="BU29" s="22"/>
-      <c r="BV29" s="22"/>
-      <c r="BW29" s="22" t="s">
+      <c r="BR29" s="20"/>
+      <c r="BS29" s="20"/>
+      <c r="BT29" s="20"/>
+      <c r="BU29" s="20"/>
+      <c r="BV29" s="20"/>
+      <c r="BW29" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="BX29" s="22"/>
-      <c r="BY29" s="22"/>
-      <c r="BZ29" s="22"/>
-      <c r="CA29" s="22"/>
-      <c r="CB29" s="22"/>
-      <c r="CC29" s="22" t="s">
+      <c r="BX29" s="20"/>
+      <c r="BY29" s="20"/>
+      <c r="BZ29" s="20"/>
+      <c r="CA29" s="20"/>
+      <c r="CB29" s="20"/>
+      <c r="CC29" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="CD29" s="22"/>
-      <c r="CE29" s="22"/>
-      <c r="CF29" s="22"/>
-      <c r="CG29" s="22"/>
-      <c r="CH29" s="22"/>
-      <c r="CI29" s="22" t="s">
+      <c r="CD29" s="20"/>
+      <c r="CE29" s="20"/>
+      <c r="CF29" s="20"/>
+      <c r="CG29" s="20"/>
+      <c r="CH29" s="20"/>
+      <c r="CI29" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="CJ29" s="22"/>
-      <c r="CK29" s="22"/>
-      <c r="CL29" s="22"/>
-      <c r="CM29" s="22"/>
-      <c r="CN29" s="22"/>
+      <c r="CJ29" s="20"/>
+      <c r="CK29" s="20"/>
+      <c r="CL29" s="20"/>
+      <c r="CM29" s="20"/>
+      <c r="CN29" s="20"/>
     </row>
     <row r="30" spans="1:96" x14ac:dyDescent="0.3">
       <c r="AG30">
@@ -5570,255 +5588,229 @@
       </c>
     </row>
     <row r="31" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="AG31" s="22" t="s">
+      <c r="AG31" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="AH31" s="22"/>
-      <c r="AI31" s="22"/>
-      <c r="AJ31" s="22"/>
-      <c r="AK31" s="22"/>
-      <c r="AL31" s="22"/>
-      <c r="AM31" s="22" t="s">
+      <c r="AH31" s="20"/>
+      <c r="AI31" s="20"/>
+      <c r="AJ31" s="20"/>
+      <c r="AK31" s="20"/>
+      <c r="AL31" s="20"/>
+      <c r="AM31" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="AN31" s="22"/>
-      <c r="AO31" s="22"/>
-      <c r="AP31" s="22"/>
-      <c r="AQ31" s="22"/>
-      <c r="AR31" s="22"/>
-      <c r="AS31" s="22" t="s">
+      <c r="AN31" s="20"/>
+      <c r="AO31" s="20"/>
+      <c r="AP31" s="20"/>
+      <c r="AQ31" s="20"/>
+      <c r="AR31" s="20"/>
+      <c r="AS31" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="AT31" s="22"/>
-      <c r="AU31" s="22"/>
-      <c r="AV31" s="22"/>
-      <c r="AW31" s="22"/>
-      <c r="AX31" s="22"/>
-      <c r="AY31" s="22" t="s">
+      <c r="AT31" s="20"/>
+      <c r="AU31" s="20"/>
+      <c r="AV31" s="20"/>
+      <c r="AW31" s="20"/>
+      <c r="AX31" s="20"/>
+      <c r="AY31" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="AZ31" s="22"/>
-      <c r="BA31" s="22"/>
-      <c r="BB31" s="22"/>
-      <c r="BC31" s="22"/>
-      <c r="BD31" s="22"/>
-      <c r="BE31" s="22" t="s">
+      <c r="AZ31" s="20"/>
+      <c r="BA31" s="20"/>
+      <c r="BB31" s="20"/>
+      <c r="BC31" s="20"/>
+      <c r="BD31" s="20"/>
+      <c r="BE31" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="BF31" s="22"/>
-      <c r="BG31" s="22"/>
-      <c r="BH31" s="22"/>
-      <c r="BI31" s="22"/>
-      <c r="BJ31" s="22"/>
-      <c r="BK31" s="22" t="s">
+      <c r="BF31" s="20"/>
+      <c r="BG31" s="20"/>
+      <c r="BH31" s="20"/>
+      <c r="BI31" s="20"/>
+      <c r="BJ31" s="20"/>
+      <c r="BK31" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="BL31" s="22"/>
-      <c r="BM31" s="22"/>
-      <c r="BN31" s="22"/>
-      <c r="BO31" s="22"/>
-      <c r="BP31" s="22"/>
-      <c r="BQ31" s="22" t="s">
+      <c r="BL31" s="20"/>
+      <c r="BM31" s="20"/>
+      <c r="BN31" s="20"/>
+      <c r="BO31" s="20"/>
+      <c r="BP31" s="20"/>
+      <c r="BQ31" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="BR31" s="22"/>
-      <c r="BS31" s="22"/>
-      <c r="BT31" s="22"/>
-      <c r="BU31" s="22"/>
-      <c r="BV31" s="22"/>
-      <c r="BW31" s="22" t="s">
+      <c r="BR31" s="20"/>
+      <c r="BS31" s="20"/>
+      <c r="BT31" s="20"/>
+      <c r="BU31" s="20"/>
+      <c r="BV31" s="20"/>
+      <c r="BW31" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="BX31" s="22"/>
-      <c r="BY31" s="22"/>
-      <c r="BZ31" s="22"/>
-      <c r="CA31" s="22"/>
-      <c r="CB31" s="22"/>
-      <c r="CC31" s="22" t="s">
+      <c r="BX31" s="20"/>
+      <c r="BY31" s="20"/>
+      <c r="BZ31" s="20"/>
+      <c r="CA31" s="20"/>
+      <c r="CB31" s="20"/>
+      <c r="CC31" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="CD31" s="22"/>
-      <c r="CE31" s="22"/>
-      <c r="CF31" s="22"/>
-      <c r="CG31" s="22"/>
-      <c r="CH31" s="22"/>
-      <c r="CI31" s="22" t="s">
+      <c r="CD31" s="20"/>
+      <c r="CE31" s="20"/>
+      <c r="CF31" s="20"/>
+      <c r="CG31" s="20"/>
+      <c r="CH31" s="20"/>
+      <c r="CI31" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="CJ31" s="22"/>
-      <c r="CK31" s="22"/>
-      <c r="CL31" s="22"/>
-      <c r="CM31" s="22"/>
-      <c r="CN31" s="22"/>
+      <c r="CJ31" s="20"/>
+      <c r="CK31" s="20"/>
+      <c r="CL31" s="20"/>
+      <c r="CM31" s="20"/>
+      <c r="CN31" s="20"/>
     </row>
     <row r="32" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="AG32" s="22">
+      <c r="AG32" s="20">
         <v>25</v>
       </c>
-      <c r="AH32" s="22"/>
-      <c r="AI32" s="22"/>
-      <c r="AJ32" s="22"/>
-      <c r="AK32" s="22"/>
-      <c r="AL32" s="22"/>
-      <c r="AM32" s="22">
+      <c r="AH32" s="20"/>
+      <c r="AI32" s="20"/>
+      <c r="AJ32" s="20"/>
+      <c r="AK32" s="20"/>
+      <c r="AL32" s="20"/>
+      <c r="AM32" s="20">
         <v>25</v>
       </c>
-      <c r="AN32" s="22"/>
-      <c r="AO32" s="22"/>
-      <c r="AP32" s="22"/>
-      <c r="AQ32" s="22"/>
-      <c r="AR32" s="22"/>
-      <c r="AS32" s="22">
+      <c r="AN32" s="20"/>
+      <c r="AO32" s="20"/>
+      <c r="AP32" s="20"/>
+      <c r="AQ32" s="20"/>
+      <c r="AR32" s="20"/>
+      <c r="AS32" s="20">
         <v>25</v>
       </c>
-      <c r="AT32" s="22"/>
-      <c r="AU32" s="22"/>
-      <c r="AV32" s="22"/>
-      <c r="AW32" s="22"/>
-      <c r="AX32" s="22"/>
-      <c r="AY32" s="22">
+      <c r="AT32" s="20"/>
+      <c r="AU32" s="20"/>
+      <c r="AV32" s="20"/>
+      <c r="AW32" s="20"/>
+      <c r="AX32" s="20"/>
+      <c r="AY32" s="20">
         <v>25</v>
       </c>
-      <c r="AZ32" s="22"/>
-      <c r="BA32" s="22"/>
-      <c r="BB32" s="22"/>
-      <c r="BC32" s="22"/>
-      <c r="BD32" s="22"/>
-      <c r="BE32" s="22">
+      <c r="AZ32" s="20"/>
+      <c r="BA32" s="20"/>
+      <c r="BB32" s="20"/>
+      <c r="BC32" s="20"/>
+      <c r="BD32" s="20"/>
+      <c r="BE32" s="20">
         <v>26</v>
       </c>
-      <c r="BF32" s="22"/>
-      <c r="BG32" s="22"/>
-      <c r="BH32" s="22"/>
-      <c r="BI32" s="22"/>
-      <c r="BJ32" s="22"/>
-      <c r="BK32" s="22">
+      <c r="BF32" s="20"/>
+      <c r="BG32" s="20"/>
+      <c r="BH32" s="20"/>
+      <c r="BI32" s="20"/>
+      <c r="BJ32" s="20"/>
+      <c r="BK32" s="20">
         <v>26</v>
       </c>
-      <c r="BL32" s="22"/>
-      <c r="BM32" s="22"/>
-      <c r="BN32" s="22"/>
-      <c r="BO32" s="22"/>
-      <c r="BP32" s="22"/>
-      <c r="BQ32" s="22">
+      <c r="BL32" s="20"/>
+      <c r="BM32" s="20"/>
+      <c r="BN32" s="20"/>
+      <c r="BO32" s="20"/>
+      <c r="BP32" s="20"/>
+      <c r="BQ32" s="20">
         <v>26</v>
       </c>
-      <c r="BR32" s="22"/>
-      <c r="BS32" s="22"/>
-      <c r="BT32" s="22"/>
-      <c r="BU32" s="22"/>
-      <c r="BV32" s="22"/>
-      <c r="BW32" s="22">
+      <c r="BR32" s="20"/>
+      <c r="BS32" s="20"/>
+      <c r="BT32" s="20"/>
+      <c r="BU32" s="20"/>
+      <c r="BV32" s="20"/>
+      <c r="BW32" s="20">
         <v>26</v>
       </c>
-      <c r="BX32" s="22"/>
-      <c r="BY32" s="22"/>
-      <c r="BZ32" s="22"/>
-      <c r="CA32" s="22"/>
-      <c r="CB32" s="22"/>
-      <c r="CC32" s="22">
+      <c r="BX32" s="20"/>
+      <c r="BY32" s="20"/>
+      <c r="BZ32" s="20"/>
+      <c r="CA32" s="20"/>
+      <c r="CB32" s="20"/>
+      <c r="CC32" s="20">
         <v>26</v>
       </c>
-      <c r="CD32" s="22"/>
-      <c r="CE32" s="22"/>
-      <c r="CF32" s="22"/>
-      <c r="CG32" s="22"/>
-      <c r="CH32" s="22"/>
-      <c r="CI32" s="22">
+      <c r="CD32" s="20"/>
+      <c r="CE32" s="20"/>
+      <c r="CF32" s="20"/>
+      <c r="CG32" s="20"/>
+      <c r="CH32" s="20"/>
+      <c r="CI32" s="20">
         <v>26</v>
       </c>
-      <c r="CJ32" s="22"/>
-      <c r="CK32" s="22"/>
-      <c r="CL32" s="22"/>
-      <c r="CM32" s="22"/>
-      <c r="CN32" s="22"/>
+      <c r="CJ32" s="20"/>
+      <c r="CK32" s="20"/>
+      <c r="CL32" s="20"/>
+      <c r="CM32" s="20"/>
+      <c r="CN32" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="166">
-    <mergeCell ref="BK32:BP32"/>
-    <mergeCell ref="BQ32:BV32"/>
-    <mergeCell ref="BW32:CB32"/>
-    <mergeCell ref="CC32:CH32"/>
-    <mergeCell ref="CI32:CN32"/>
-    <mergeCell ref="AG32:AL32"/>
-    <mergeCell ref="AM32:AR32"/>
-    <mergeCell ref="AS32:AX32"/>
-    <mergeCell ref="AY32:BD32"/>
-    <mergeCell ref="BE32:BJ32"/>
-    <mergeCell ref="BK31:BP31"/>
-    <mergeCell ref="BQ31:BV31"/>
-    <mergeCell ref="BW31:CB31"/>
-    <mergeCell ref="CC31:CH31"/>
-    <mergeCell ref="CI31:CN31"/>
-    <mergeCell ref="AG31:AL31"/>
-    <mergeCell ref="AM31:AR31"/>
-    <mergeCell ref="AS31:AX31"/>
-    <mergeCell ref="AY31:BD31"/>
-    <mergeCell ref="BE31:BJ31"/>
-    <mergeCell ref="BK29:BP29"/>
-    <mergeCell ref="BQ29:BV29"/>
-    <mergeCell ref="BW29:CB29"/>
-    <mergeCell ref="CC29:CH29"/>
-    <mergeCell ref="CI29:CN29"/>
-    <mergeCell ref="AG29:AL29"/>
-    <mergeCell ref="AM29:AR29"/>
-    <mergeCell ref="AS29:AX29"/>
-    <mergeCell ref="AY29:BD29"/>
-    <mergeCell ref="BE29:BJ29"/>
-    <mergeCell ref="BK28:BP28"/>
-    <mergeCell ref="BQ28:BV28"/>
-    <mergeCell ref="BW28:CB28"/>
-    <mergeCell ref="CC28:CH28"/>
-    <mergeCell ref="CI28:CN28"/>
-    <mergeCell ref="AG28:AL28"/>
-    <mergeCell ref="AM28:AR28"/>
-    <mergeCell ref="AS28:AX28"/>
-    <mergeCell ref="AY28:BD28"/>
-    <mergeCell ref="BE28:BJ28"/>
-    <mergeCell ref="BU24:CB24"/>
-    <mergeCell ref="CC24:CJ24"/>
-    <mergeCell ref="CK24:CR24"/>
-    <mergeCell ref="AG26:AN26"/>
-    <mergeCell ref="AO26:AV26"/>
-    <mergeCell ref="AW26:BD26"/>
-    <mergeCell ref="BE26:BL26"/>
-    <mergeCell ref="BM26:BT26"/>
-    <mergeCell ref="BU26:CB26"/>
-    <mergeCell ref="CC26:CJ26"/>
-    <mergeCell ref="CK26:CR26"/>
-    <mergeCell ref="AG24:AN24"/>
-    <mergeCell ref="AO24:AV24"/>
-    <mergeCell ref="AW24:BD24"/>
-    <mergeCell ref="BE24:BL24"/>
-    <mergeCell ref="BM24:BT24"/>
-    <mergeCell ref="Y28:AC28"/>
-    <mergeCell ref="AD28:AF28"/>
-    <mergeCell ref="A29:H29"/>
-    <mergeCell ref="I29:M29"/>
-    <mergeCell ref="N29:P29"/>
-    <mergeCell ref="Q29:S29"/>
-    <mergeCell ref="T29:X29"/>
-    <mergeCell ref="Y29:AC29"/>
-    <mergeCell ref="AD29:AF29"/>
-    <mergeCell ref="A28:H28"/>
-    <mergeCell ref="I28:M28"/>
-    <mergeCell ref="N28:P28"/>
-    <mergeCell ref="Q28:S28"/>
-    <mergeCell ref="T28:X28"/>
-    <mergeCell ref="Y26:AC26"/>
-    <mergeCell ref="AD26:AF26"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="I27:M27"/>
-    <mergeCell ref="N27:P27"/>
-    <mergeCell ref="Q27:S27"/>
-    <mergeCell ref="T27:X27"/>
-    <mergeCell ref="Y27:AC27"/>
-    <mergeCell ref="AD27:AF27"/>
-    <mergeCell ref="A26:H26"/>
-    <mergeCell ref="I26:M26"/>
-    <mergeCell ref="N26:P26"/>
-    <mergeCell ref="Q26:S26"/>
-    <mergeCell ref="T26:X26"/>
+    <mergeCell ref="Y19:AC19"/>
+    <mergeCell ref="AD19:AF19"/>
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="I20:M20"/>
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="Q20:S20"/>
+    <mergeCell ref="T20:X20"/>
+    <mergeCell ref="Y20:AC20"/>
+    <mergeCell ref="AD20:AF20"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="I19:M19"/>
+    <mergeCell ref="N19:P19"/>
+    <mergeCell ref="Q19:S19"/>
+    <mergeCell ref="T19:X19"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="I15:P15"/>
+    <mergeCell ref="Q15:X15"/>
+    <mergeCell ref="Y15:AF15"/>
+    <mergeCell ref="A14:AF14"/>
+    <mergeCell ref="Y17:AC17"/>
+    <mergeCell ref="AD17:AF17"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="I18:M18"/>
+    <mergeCell ref="N18:P18"/>
+    <mergeCell ref="Q18:S18"/>
+    <mergeCell ref="T18:X18"/>
+    <mergeCell ref="Y18:AC18"/>
+    <mergeCell ref="AD18:AF18"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="I17:M17"/>
+    <mergeCell ref="N17:P17"/>
+    <mergeCell ref="Q17:S17"/>
+    <mergeCell ref="T17:X17"/>
+    <mergeCell ref="I11:M11"/>
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="I10:M10"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="AD10:AF10"/>
+    <mergeCell ref="Y10:AC10"/>
+    <mergeCell ref="T10:X10"/>
+    <mergeCell ref="Q10:S10"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="AD11:AF11"/>
+    <mergeCell ref="Y11:AC11"/>
+    <mergeCell ref="T11:X11"/>
+    <mergeCell ref="Q11:S11"/>
+    <mergeCell ref="N11:P11"/>
+    <mergeCell ref="Q6:X6"/>
+    <mergeCell ref="Y6:AF6"/>
+    <mergeCell ref="AD9:AF9"/>
+    <mergeCell ref="AD8:AF8"/>
+    <mergeCell ref="Y9:AC9"/>
+    <mergeCell ref="Y8:AC8"/>
+    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="T8:X8"/>
+    <mergeCell ref="T9:X9"/>
     <mergeCell ref="A23:AF23"/>
     <mergeCell ref="A24:H24"/>
     <mergeCell ref="I24:P24"/>
@@ -5843,64 +5835,90 @@
     <mergeCell ref="I8:M8"/>
     <mergeCell ref="N8:P8"/>
     <mergeCell ref="I9:M9"/>
-    <mergeCell ref="Q6:X6"/>
-    <mergeCell ref="Y6:AF6"/>
-    <mergeCell ref="AD9:AF9"/>
-    <mergeCell ref="AD8:AF8"/>
-    <mergeCell ref="Y9:AC9"/>
-    <mergeCell ref="Y8:AC8"/>
-    <mergeCell ref="N9:P9"/>
-    <mergeCell ref="Q8:S8"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="T8:X8"/>
-    <mergeCell ref="T9:X9"/>
-    <mergeCell ref="I11:M11"/>
-    <mergeCell ref="A11:H11"/>
-    <mergeCell ref="I10:M10"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="AD10:AF10"/>
-    <mergeCell ref="Y10:AC10"/>
-    <mergeCell ref="T10:X10"/>
-    <mergeCell ref="Q10:S10"/>
-    <mergeCell ref="N10:P10"/>
-    <mergeCell ref="AD11:AF11"/>
-    <mergeCell ref="Y11:AC11"/>
-    <mergeCell ref="T11:X11"/>
-    <mergeCell ref="Q11:S11"/>
-    <mergeCell ref="N11:P11"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="I15:P15"/>
-    <mergeCell ref="Q15:X15"/>
-    <mergeCell ref="Y15:AF15"/>
-    <mergeCell ref="A14:AF14"/>
-    <mergeCell ref="Y17:AC17"/>
-    <mergeCell ref="AD17:AF17"/>
-    <mergeCell ref="A18:H18"/>
-    <mergeCell ref="I18:M18"/>
-    <mergeCell ref="N18:P18"/>
-    <mergeCell ref="Q18:S18"/>
-    <mergeCell ref="T18:X18"/>
-    <mergeCell ref="Y18:AC18"/>
-    <mergeCell ref="AD18:AF18"/>
-    <mergeCell ref="A17:H17"/>
-    <mergeCell ref="I17:M17"/>
-    <mergeCell ref="N17:P17"/>
-    <mergeCell ref="Q17:S17"/>
-    <mergeCell ref="T17:X17"/>
-    <mergeCell ref="Y19:AC19"/>
-    <mergeCell ref="AD19:AF19"/>
-    <mergeCell ref="A20:H20"/>
-    <mergeCell ref="I20:M20"/>
-    <mergeCell ref="N20:P20"/>
-    <mergeCell ref="Q20:S20"/>
-    <mergeCell ref="T20:X20"/>
-    <mergeCell ref="Y20:AC20"/>
-    <mergeCell ref="AD20:AF20"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="I19:M19"/>
-    <mergeCell ref="N19:P19"/>
-    <mergeCell ref="Q19:S19"/>
-    <mergeCell ref="T19:X19"/>
+    <mergeCell ref="Y26:AC26"/>
+    <mergeCell ref="AD26:AF26"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="I27:M27"/>
+    <mergeCell ref="N27:P27"/>
+    <mergeCell ref="Q27:S27"/>
+    <mergeCell ref="T27:X27"/>
+    <mergeCell ref="Y27:AC27"/>
+    <mergeCell ref="AD27:AF27"/>
+    <mergeCell ref="A26:H26"/>
+    <mergeCell ref="I26:M26"/>
+    <mergeCell ref="N26:P26"/>
+    <mergeCell ref="Q26:S26"/>
+    <mergeCell ref="T26:X26"/>
+    <mergeCell ref="Y28:AC28"/>
+    <mergeCell ref="AD28:AF28"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="I29:M29"/>
+    <mergeCell ref="N29:P29"/>
+    <mergeCell ref="Q29:S29"/>
+    <mergeCell ref="T29:X29"/>
+    <mergeCell ref="Y29:AC29"/>
+    <mergeCell ref="AD29:AF29"/>
+    <mergeCell ref="A28:H28"/>
+    <mergeCell ref="I28:M28"/>
+    <mergeCell ref="N28:P28"/>
+    <mergeCell ref="Q28:S28"/>
+    <mergeCell ref="T28:X28"/>
+    <mergeCell ref="BU24:CB24"/>
+    <mergeCell ref="CC24:CJ24"/>
+    <mergeCell ref="CK24:CR24"/>
+    <mergeCell ref="AG26:AN26"/>
+    <mergeCell ref="AO26:AV26"/>
+    <mergeCell ref="AW26:BD26"/>
+    <mergeCell ref="BE26:BL26"/>
+    <mergeCell ref="BM26:BT26"/>
+    <mergeCell ref="BU26:CB26"/>
+    <mergeCell ref="CC26:CJ26"/>
+    <mergeCell ref="CK26:CR26"/>
+    <mergeCell ref="AG24:AN24"/>
+    <mergeCell ref="AO24:AV24"/>
+    <mergeCell ref="AW24:BD24"/>
+    <mergeCell ref="BE24:BL24"/>
+    <mergeCell ref="BM24:BT24"/>
+    <mergeCell ref="BK28:BP28"/>
+    <mergeCell ref="BQ28:BV28"/>
+    <mergeCell ref="BW28:CB28"/>
+    <mergeCell ref="CC28:CH28"/>
+    <mergeCell ref="CI28:CN28"/>
+    <mergeCell ref="AG28:AL28"/>
+    <mergeCell ref="AM28:AR28"/>
+    <mergeCell ref="AS28:AX28"/>
+    <mergeCell ref="AY28:BD28"/>
+    <mergeCell ref="BE28:BJ28"/>
+    <mergeCell ref="BK29:BP29"/>
+    <mergeCell ref="BQ29:BV29"/>
+    <mergeCell ref="BW29:CB29"/>
+    <mergeCell ref="CC29:CH29"/>
+    <mergeCell ref="CI29:CN29"/>
+    <mergeCell ref="AG29:AL29"/>
+    <mergeCell ref="AM29:AR29"/>
+    <mergeCell ref="AS29:AX29"/>
+    <mergeCell ref="AY29:BD29"/>
+    <mergeCell ref="BE29:BJ29"/>
+    <mergeCell ref="BK31:BP31"/>
+    <mergeCell ref="BQ31:BV31"/>
+    <mergeCell ref="BW31:CB31"/>
+    <mergeCell ref="CC31:CH31"/>
+    <mergeCell ref="CI31:CN31"/>
+    <mergeCell ref="AG31:AL31"/>
+    <mergeCell ref="AM31:AR31"/>
+    <mergeCell ref="AS31:AX31"/>
+    <mergeCell ref="AY31:BD31"/>
+    <mergeCell ref="BE31:BJ31"/>
+    <mergeCell ref="BK32:BP32"/>
+    <mergeCell ref="BQ32:BV32"/>
+    <mergeCell ref="BW32:CB32"/>
+    <mergeCell ref="CC32:CH32"/>
+    <mergeCell ref="CI32:CN32"/>
+    <mergeCell ref="AG32:AL32"/>
+    <mergeCell ref="AM32:AR32"/>
+    <mergeCell ref="AS32:AX32"/>
+    <mergeCell ref="AY32:BD32"/>
+    <mergeCell ref="BE32:BJ32"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -5929,11 +5947,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
       <c r="E1" s="7">
         <v>0.5</v>
       </c>
@@ -6759,28 +6777,28 @@
       <c r="S2" s="7"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="32" t="s">
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="32" t="s">
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="O3" s="33"/>
-      <c r="P3" s="34"/>
+      <c r="O3" s="34"/>
+      <c r="P3" s="35"/>
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
       <c r="S3" s="7"/>
@@ -6847,10 +6865,10 @@
       <c r="O6" s="25"/>
       <c r="P6" s="25"/>
       <c r="Q6" s="7"/>
-      <c r="R6" s="20" t="s">
+      <c r="R6" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="S6" s="20"/>
+      <c r="S6" s="22"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
@@ -6902,18 +6920,18 @@
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
-      <c r="I8" s="20" t="s">
+      <c r="I8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="20" t="s">
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="O8" s="20"/>
-      <c r="P8" s="20"/>
+      <c r="O8" s="22"/>
+      <c r="P8" s="22"/>
       <c r="Q8" s="7"/>
       <c r="R8" s="7"/>
       <c r="S8" s="7"/>
@@ -6927,18 +6945,18 @@
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
-      <c r="I9" s="20">
+      <c r="I9" s="22">
         <v>17</v>
       </c>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="20">
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22">
         <v>4</v>
       </c>
-      <c r="O9" s="20"/>
-      <c r="P9" s="20"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="22"/>
       <c r="Q9" s="7"/>
       <c r="R9" s="7"/>
       <c r="S9" s="7"/>
@@ -6957,11 +6975,11 @@
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
-      <c r="N10" s="20" t="s">
+      <c r="N10" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="O10" s="20"/>
-      <c r="P10" s="20"/>
+      <c r="O10" s="22"/>
+      <c r="P10" s="22"/>
       <c r="Q10" s="7"/>
       <c r="R10" s="7"/>
       <c r="S10" s="7"/>
@@ -6980,24 +6998,18 @@
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
-      <c r="N11" s="21">
+      <c r="N11" s="23">
         <f>100/(2^3-1)*N9</f>
         <v>57.142857142857146</v>
       </c>
-      <c r="O11" s="21"/>
-      <c r="P11" s="21"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="23"/>
       <c r="Q11" s="7"/>
       <c r="R11" s="7"/>
       <c r="S11" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="I3:M3"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="I6:P6"/>
     <mergeCell ref="N11:P11"/>
     <mergeCell ref="R7:S7"/>
     <mergeCell ref="I8:M8"/>
@@ -7005,6 +7017,12 @@
     <mergeCell ref="I9:M9"/>
     <mergeCell ref="N9:P9"/>
     <mergeCell ref="N10:P10"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="I3:M3"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="I6:P6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
software version commit tag in DataPackage.xlsx updated
</commit_message>
<xml_diff>
--- a/hardware/BikeCounterPro/src/dataPackage/DataPackage.xlsx
+++ b/hardware/BikeCounterPro/src/dataPackage/DataPackage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meier\Documents\repos\bikecounter\hardware\BikeCounterPro\src\dataPackage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A0AA74-FFA5-4FCD-83F6-2FA4116196A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CEA4BA4-A91E-4B05-98FD-EB6F6FE6D292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="50592" yWindow="3180" windowWidth="31968" windowHeight="13500" xr2:uid="{CDF7A0A5-12B1-43F1-AFDE-54CA91221B4B}"/>
+    <workbookView xWindow="9312" yWindow="3180" windowWidth="31968" windowHeight="13500" xr2:uid="{CDF7A0A5-12B1-43F1-AFDE-54CA91221B4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Data package" sheetId="1" r:id="rId1"/>
@@ -391,7 +391,7 @@
     <t>board v0.1 ohne RTC</t>
   </si>
   <si>
-    <t>753649f6cd0a613f381e185e22c4f90cc98fa9b9 [753649f]</t>
+    <t>d11abf00db12795104943221308b7b15bbd1c374 [d11abf0]</t>
   </si>
 </sst>
 </file>
@@ -654,24 +654,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -700,6 +697,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2161,7 +2161,7 @@
   <dimension ref="A1:S90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3231,46 +3231,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="27" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="27" t="s">
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
-      <c r="X1" s="29"/>
-      <c r="Y1" s="27" t="s">
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
+      <c r="T1" s="27"/>
+      <c r="U1" s="27"/>
+      <c r="V1" s="27"/>
+      <c r="W1" s="27"/>
+      <c r="X1" s="28"/>
+      <c r="Y1" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="Z1" s="28"/>
-      <c r="AA1" s="28"/>
-      <c r="AB1" s="28"/>
-      <c r="AC1" s="28"/>
-      <c r="AD1" s="28"/>
-      <c r="AE1" s="28"/>
-      <c r="AF1" s="29"/>
+      <c r="Z1" s="27"/>
+      <c r="AA1" s="27"/>
+      <c r="AB1" s="27"/>
+      <c r="AC1" s="27"/>
+      <c r="AD1" s="27"/>
+      <c r="AE1" s="27"/>
+      <c r="AF1" s="28"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
@@ -3371,52 +3371,52 @@
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="33" t="s">
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="34"/>
-      <c r="N3" s="33" t="s">
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="O3" s="34"/>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="33" t="s">
+      <c r="O3" s="33"/>
+      <c r="P3" s="34"/>
+      <c r="Q3" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="R3" s="34"/>
-      <c r="S3" s="35"/>
-      <c r="T3" s="30" t="s">
+      <c r="R3" s="33"/>
+      <c r="S3" s="34"/>
+      <c r="T3" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="U3" s="31"/>
-      <c r="V3" s="31"/>
-      <c r="W3" s="31"/>
-      <c r="X3" s="32"/>
-      <c r="Y3" s="30" t="s">
+      <c r="U3" s="30"/>
+      <c r="V3" s="30"/>
+      <c r="W3" s="30"/>
+      <c r="X3" s="31"/>
+      <c r="Y3" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="Z3" s="31"/>
-      <c r="AA3" s="31"/>
-      <c r="AB3" s="31"/>
-      <c r="AC3" s="32"/>
-      <c r="AD3" s="30" t="s">
+      <c r="Z3" s="30"/>
+      <c r="AA3" s="30"/>
+      <c r="AB3" s="30"/>
+      <c r="AC3" s="31"/>
+      <c r="AD3" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="AE3" s="31"/>
-      <c r="AF3" s="32"/>
+      <c r="AE3" s="30"/>
+      <c r="AF3" s="31"/>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
@@ -3476,46 +3476,46 @@
       <c r="AF5" s="25"/>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26">
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24">
         <v>38</v>
       </c>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="26"/>
-      <c r="M6" s="26"/>
-      <c r="N6" s="26"/>
-      <c r="O6" s="26"/>
-      <c r="P6" s="26"/>
-      <c r="Q6" s="26">
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="24"/>
+      <c r="N6" s="24"/>
+      <c r="O6" s="24"/>
+      <c r="P6" s="24"/>
+      <c r="Q6" s="24">
         <v>73</v>
       </c>
-      <c r="R6" s="26"/>
-      <c r="S6" s="26"/>
-      <c r="T6" s="26"/>
-      <c r="U6" s="26"/>
-      <c r="V6" s="26"/>
-      <c r="W6" s="26"/>
-      <c r="X6" s="26"/>
-      <c r="Y6" s="26">
+      <c r="R6" s="24"/>
+      <c r="S6" s="24"/>
+      <c r="T6" s="24"/>
+      <c r="U6" s="24"/>
+      <c r="V6" s="24"/>
+      <c r="W6" s="24"/>
+      <c r="X6" s="24"/>
+      <c r="Y6" s="24">
         <v>88</v>
       </c>
-      <c r="Z6" s="26"/>
-      <c r="AA6" s="26"/>
-      <c r="AB6" s="26"/>
-      <c r="AC6" s="26"/>
-      <c r="AD6" s="26"/>
-      <c r="AE6" s="26"/>
-      <c r="AF6" s="26"/>
+      <c r="Z6" s="24"/>
+      <c r="AA6" s="24"/>
+      <c r="AB6" s="24"/>
+      <c r="AC6" s="24"/>
+      <c r="AD6" s="24"/>
+      <c r="AE6" s="24"/>
+      <c r="AF6" s="24"/>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
@@ -3616,203 +3616,203 @@
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22" t="s">
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="22" t="s">
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="O8" s="22"/>
-      <c r="P8" s="22"/>
-      <c r="Q8" s="22" t="s">
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="R8" s="22"/>
-      <c r="S8" s="22"/>
-      <c r="T8" s="22" t="s">
+      <c r="R8" s="20"/>
+      <c r="S8" s="20"/>
+      <c r="T8" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="U8" s="22"/>
-      <c r="V8" s="22"/>
-      <c r="W8" s="22"/>
-      <c r="X8" s="22"/>
-      <c r="Y8" s="22" t="s">
+      <c r="U8" s="20"/>
+      <c r="V8" s="20"/>
+      <c r="W8" s="20"/>
+      <c r="X8" s="20"/>
+      <c r="Y8" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z8" s="22"/>
-      <c r="AA8" s="22"/>
-      <c r="AB8" s="22"/>
-      <c r="AC8" s="22"/>
-      <c r="AD8" s="22" t="s">
+      <c r="Z8" s="20"/>
+      <c r="AA8" s="20"/>
+      <c r="AB8" s="20"/>
+      <c r="AC8" s="20"/>
+      <c r="AD8" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="AE8" s="22"/>
-      <c r="AF8" s="22"/>
+      <c r="AE8" s="20"/>
+      <c r="AF8" s="20"/>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A9" s="22">
+      <c r="A9" s="20">
         <v>10</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22">
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20">
         <v>7</v>
       </c>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="22">
-        <v>0</v>
-      </c>
-      <c r="O9" s="22"/>
-      <c r="P9" s="22"/>
-      <c r="Q9" s="22">
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20">
+        <v>0</v>
+      </c>
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="20">
         <v>3</v>
       </c>
-      <c r="R9" s="22"/>
-      <c r="S9" s="22"/>
-      <c r="T9" s="22">
+      <c r="R9" s="20"/>
+      <c r="S9" s="20"/>
+      <c r="T9" s="20">
         <v>19</v>
       </c>
-      <c r="U9" s="22"/>
-      <c r="V9" s="22"/>
-      <c r="W9" s="22"/>
-      <c r="X9" s="22"/>
-      <c r="Y9" s="22">
+      <c r="U9" s="20"/>
+      <c r="V9" s="20"/>
+      <c r="W9" s="20"/>
+      <c r="X9" s="20"/>
+      <c r="Y9" s="20">
         <v>17</v>
       </c>
-      <c r="Z9" s="22"/>
-      <c r="AA9" s="22"/>
-      <c r="AB9" s="22"/>
-      <c r="AC9" s="22"/>
-      <c r="AD9" s="22">
-        <v>0</v>
-      </c>
-      <c r="AE9" s="22"/>
-      <c r="AF9" s="22"/>
+      <c r="Z9" s="20"/>
+      <c r="AA9" s="20"/>
+      <c r="AB9" s="20"/>
+      <c r="AC9" s="20"/>
+      <c r="AD9" s="20">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="20"/>
+      <c r="AF9" s="20"/>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22" t="s">
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="22" t="s">
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="O10" s="22"/>
-      <c r="P10" s="22"/>
-      <c r="Q10" s="22" t="s">
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="R10" s="22"/>
-      <c r="S10" s="22"/>
-      <c r="T10" s="22" t="s">
+      <c r="R10" s="20"/>
+      <c r="S10" s="20"/>
+      <c r="T10" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="U10" s="22"/>
-      <c r="V10" s="22"/>
-      <c r="W10" s="22"/>
-      <c r="X10" s="22"/>
-      <c r="Y10" s="22" t="s">
+      <c r="U10" s="20"/>
+      <c r="V10" s="20"/>
+      <c r="W10" s="20"/>
+      <c r="X10" s="20"/>
+      <c r="Y10" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="Z10" s="22"/>
-      <c r="AA10" s="22"/>
-      <c r="AB10" s="22"/>
-      <c r="AC10" s="22"/>
-      <c r="AD10" s="22" t="s">
+      <c r="Z10" s="20"/>
+      <c r="AA10" s="20"/>
+      <c r="AB10" s="20"/>
+      <c r="AC10" s="20"/>
+      <c r="AD10" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="AE10" s="22"/>
-      <c r="AF10" s="22"/>
+      <c r="AE10" s="20"/>
+      <c r="AF10" s="20"/>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A11" s="22">
+      <c r="A11" s="20">
         <f>A9</f>
         <v>10</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="23">
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="21">
         <f>'Data package'!$B$31*I9+'Data package'!$B$28</f>
         <v>3.338709677419355</v>
       </c>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="20">
+      <c r="J11" s="21"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="22">
         <f ca="1">LOOKUP(N9,'Data package'!$D$21:$D$24,'Data package'!$E$22:$E$35)</f>
         <v>0</v>
       </c>
-      <c r="O11" s="20"/>
-      <c r="P11" s="20"/>
-      <c r="Q11" s="24">
+      <c r="O11" s="22"/>
+      <c r="P11" s="22"/>
+      <c r="Q11" s="23">
         <f>100/(2^3-1)*Q9</f>
         <v>42.857142857142861</v>
       </c>
-      <c r="R11" s="24"/>
-      <c r="S11" s="24"/>
-      <c r="T11" s="24">
+      <c r="R11" s="23"/>
+      <c r="S11" s="23"/>
+      <c r="T11" s="23">
         <f>'Data package'!$B$40*T9+'Data package'!$B$37</f>
         <v>22.903225806451616</v>
       </c>
-      <c r="U11" s="20"/>
-      <c r="V11" s="20"/>
-      <c r="W11" s="20"/>
-      <c r="X11" s="20"/>
-      <c r="Y11" s="20">
+      <c r="U11" s="22"/>
+      <c r="V11" s="22"/>
+      <c r="W11" s="22"/>
+      <c r="X11" s="22"/>
+      <c r="Y11" s="22">
         <f>Y9</f>
         <v>17</v>
       </c>
-      <c r="Z11" s="20"/>
-      <c r="AA11" s="20"/>
-      <c r="AB11" s="20"/>
-      <c r="AC11" s="20"/>
-      <c r="AD11" s="20">
+      <c r="Z11" s="22"/>
+      <c r="AA11" s="22"/>
+      <c r="AB11" s="22"/>
+      <c r="AC11" s="22"/>
+      <c r="AD11" s="22">
         <f>LOOKUP(AD9,'Data package'!$A$84:$A$88,'Data package'!$B$84:$B$88)</f>
         <v>1</v>
       </c>
-      <c r="AE11" s="20"/>
-      <c r="AF11" s="20"/>
+      <c r="AE11" s="22"/>
+      <c r="AF11" s="22"/>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
@@ -3864,46 +3864,46 @@
       <c r="AF14" s="25"/>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26" t="s">
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="J15" s="26"/>
-      <c r="K15" s="26"/>
-      <c r="L15" s="26"/>
-      <c r="M15" s="26"/>
-      <c r="N15" s="26"/>
-      <c r="O15" s="26"/>
-      <c r="P15" s="26"/>
-      <c r="Q15" s="26" t="s">
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="24"/>
+      <c r="N15" s="24"/>
+      <c r="O15" s="24"/>
+      <c r="P15" s="24"/>
+      <c r="Q15" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="R15" s="26"/>
-      <c r="S15" s="26"/>
-      <c r="T15" s="26"/>
-      <c r="U15" s="26"/>
-      <c r="V15" s="26"/>
-      <c r="W15" s="26"/>
-      <c r="X15" s="26"/>
-      <c r="Y15" s="26" t="s">
+      <c r="R15" s="24"/>
+      <c r="S15" s="24"/>
+      <c r="T15" s="24"/>
+      <c r="U15" s="24"/>
+      <c r="V15" s="24"/>
+      <c r="W15" s="24"/>
+      <c r="X15" s="24"/>
+      <c r="Y15" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="Z15" s="26"/>
-      <c r="AA15" s="26"/>
-      <c r="AB15" s="26"/>
-      <c r="AC15" s="26"/>
-      <c r="AD15" s="26"/>
-      <c r="AE15" s="26"/>
-      <c r="AF15" s="26"/>
+      <c r="Z15" s="24"/>
+      <c r="AA15" s="24"/>
+      <c r="AB15" s="24"/>
+      <c r="AC15" s="24"/>
+      <c r="AD15" s="24"/>
+      <c r="AE15" s="24"/>
+      <c r="AF15" s="24"/>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
@@ -4004,203 +4004,203 @@
       </c>
     </row>
     <row r="17" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22" t="s">
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="J17" s="22"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="22"/>
-      <c r="M17" s="22"/>
-      <c r="N17" s="22" t="s">
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="20"/>
+      <c r="N17" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="O17" s="22"/>
-      <c r="P17" s="22"/>
-      <c r="Q17" s="22" t="s">
+      <c r="O17" s="20"/>
+      <c r="P17" s="20"/>
+      <c r="Q17" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="R17" s="22"/>
-      <c r="S17" s="22"/>
-      <c r="T17" s="22" t="s">
+      <c r="R17" s="20"/>
+      <c r="S17" s="20"/>
+      <c r="T17" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="U17" s="22"/>
-      <c r="V17" s="22"/>
-      <c r="W17" s="22"/>
-      <c r="X17" s="22"/>
-      <c r="Y17" s="22" t="s">
+      <c r="U17" s="20"/>
+      <c r="V17" s="20"/>
+      <c r="W17" s="20"/>
+      <c r="X17" s="20"/>
+      <c r="Y17" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z17" s="22"/>
-      <c r="AA17" s="22"/>
-      <c r="AB17" s="22"/>
-      <c r="AC17" s="22"/>
-      <c r="AD17" s="22" t="s">
+      <c r="Z17" s="20"/>
+      <c r="AA17" s="20"/>
+      <c r="AB17" s="20"/>
+      <c r="AC17" s="20"/>
+      <c r="AD17" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="AE17" s="22"/>
-      <c r="AF17" s="22"/>
+      <c r="AE17" s="20"/>
+      <c r="AF17" s="20"/>
     </row>
     <row r="18" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A18" s="22">
+      <c r="A18" s="20">
         <v>5</v>
       </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22">
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20">
         <v>8</v>
       </c>
-      <c r="J18" s="22"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="22"/>
-      <c r="N18" s="22">
-        <v>0</v>
-      </c>
-      <c r="O18" s="22"/>
-      <c r="P18" s="22"/>
-      <c r="Q18" s="22">
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="20">
+        <v>0</v>
+      </c>
+      <c r="O18" s="20"/>
+      <c r="P18" s="20"/>
+      <c r="Q18" s="20">
         <v>3</v>
       </c>
-      <c r="R18" s="22"/>
-      <c r="S18" s="22"/>
-      <c r="T18" s="22">
+      <c r="R18" s="20"/>
+      <c r="S18" s="20"/>
+      <c r="T18" s="20">
         <v>19</v>
       </c>
-      <c r="U18" s="22"/>
-      <c r="V18" s="22"/>
-      <c r="W18" s="22"/>
-      <c r="X18" s="22"/>
-      <c r="Y18" s="22">
+      <c r="U18" s="20"/>
+      <c r="V18" s="20"/>
+      <c r="W18" s="20"/>
+      <c r="X18" s="20"/>
+      <c r="Y18" s="20">
         <v>17</v>
       </c>
-      <c r="Z18" s="22"/>
-      <c r="AA18" s="22"/>
-      <c r="AB18" s="22"/>
-      <c r="AC18" s="22"/>
-      <c r="AD18" s="22">
-        <v>0</v>
-      </c>
-      <c r="AE18" s="22"/>
-      <c r="AF18" s="22"/>
+      <c r="Z18" s="20"/>
+      <c r="AA18" s="20"/>
+      <c r="AB18" s="20"/>
+      <c r="AC18" s="20"/>
+      <c r="AD18" s="20">
+        <v>0</v>
+      </c>
+      <c r="AE18" s="20"/>
+      <c r="AF18" s="20"/>
     </row>
     <row r="19" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22" t="s">
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="J19" s="22"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="22"/>
-      <c r="M19" s="22"/>
-      <c r="N19" s="22" t="s">
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="20"/>
+      <c r="N19" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="O19" s="22"/>
-      <c r="P19" s="22"/>
-      <c r="Q19" s="22" t="s">
+      <c r="O19" s="20"/>
+      <c r="P19" s="20"/>
+      <c r="Q19" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="R19" s="22"/>
-      <c r="S19" s="22"/>
-      <c r="T19" s="22" t="s">
+      <c r="R19" s="20"/>
+      <c r="S19" s="20"/>
+      <c r="T19" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="U19" s="22"/>
-      <c r="V19" s="22"/>
-      <c r="W19" s="22"/>
-      <c r="X19" s="22"/>
-      <c r="Y19" s="22" t="s">
+      <c r="U19" s="20"/>
+      <c r="V19" s="20"/>
+      <c r="W19" s="20"/>
+      <c r="X19" s="20"/>
+      <c r="Y19" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="Z19" s="22"/>
-      <c r="AA19" s="22"/>
-      <c r="AB19" s="22"/>
-      <c r="AC19" s="22"/>
-      <c r="AD19" s="22" t="s">
+      <c r="Z19" s="20"/>
+      <c r="AA19" s="20"/>
+      <c r="AB19" s="20"/>
+      <c r="AC19" s="20"/>
+      <c r="AD19" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="AE19" s="22"/>
-      <c r="AF19" s="22"/>
+      <c r="AE19" s="20"/>
+      <c r="AF19" s="20"/>
     </row>
     <row r="20" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A20" s="22">
+      <c r="A20" s="20">
         <f>A18</f>
         <v>5</v>
       </c>
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="23">
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="21">
         <f>'Data package'!$B$31*I18+'Data package'!$B$28</f>
         <v>3.3870967741935485</v>
       </c>
-      <c r="J20" s="23"/>
-      <c r="K20" s="23"/>
-      <c r="L20" s="23"/>
-      <c r="M20" s="23"/>
-      <c r="N20" s="20">
+      <c r="J20" s="21"/>
+      <c r="K20" s="21"/>
+      <c r="L20" s="21"/>
+      <c r="M20" s="21"/>
+      <c r="N20" s="22">
         <f ca="1">LOOKUP(N18,'Data package'!$D$21:$D$24,'Data package'!$E$22:$E$35)</f>
         <v>0</v>
       </c>
-      <c r="O20" s="20"/>
-      <c r="P20" s="20"/>
-      <c r="Q20" s="24">
+      <c r="O20" s="22"/>
+      <c r="P20" s="22"/>
+      <c r="Q20" s="23">
         <f>100/(2^3-1)*Q18</f>
         <v>42.857142857142861</v>
       </c>
-      <c r="R20" s="24"/>
-      <c r="S20" s="24"/>
-      <c r="T20" s="24">
+      <c r="R20" s="23"/>
+      <c r="S20" s="23"/>
+      <c r="T20" s="23">
         <f>'Data package'!$B$40*T18+'Data package'!$B$37</f>
         <v>22.903225806451616</v>
       </c>
-      <c r="U20" s="20"/>
-      <c r="V20" s="20"/>
-      <c r="W20" s="20"/>
-      <c r="X20" s="20"/>
-      <c r="Y20" s="20">
+      <c r="U20" s="22"/>
+      <c r="V20" s="22"/>
+      <c r="W20" s="22"/>
+      <c r="X20" s="22"/>
+      <c r="Y20" s="22">
         <f>Y18</f>
         <v>17</v>
       </c>
-      <c r="Z20" s="20"/>
-      <c r="AA20" s="20"/>
-      <c r="AB20" s="20"/>
-      <c r="AC20" s="20"/>
-      <c r="AD20" s="20">
+      <c r="Z20" s="22"/>
+      <c r="AA20" s="22"/>
+      <c r="AB20" s="22"/>
+      <c r="AC20" s="22"/>
+      <c r="AD20" s="22">
         <f>LOOKUP(AD18,'Data package'!$A$84:$A$88,'Data package'!$B$84:$B$88)</f>
         <v>1</v>
       </c>
-      <c r="AE20" s="20"/>
-      <c r="AF20" s="20"/>
+      <c r="AE20" s="22"/>
+      <c r="AF20" s="22"/>
     </row>
     <row r="23" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A23" s="25" t="s">
@@ -4239,126 +4239,126 @@
       <c r="AF23" s="25"/>
     </row>
     <row r="24" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A24" s="26" t="s">
+      <c r="A24" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26" t="s">
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="J24" s="26"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="26"/>
-      <c r="M24" s="26"/>
-      <c r="N24" s="26"/>
-      <c r="O24" s="26"/>
-      <c r="P24" s="26"/>
-      <c r="Q24" s="26" t="s">
+      <c r="J24" s="24"/>
+      <c r="K24" s="24"/>
+      <c r="L24" s="24"/>
+      <c r="M24" s="24"/>
+      <c r="N24" s="24"/>
+      <c r="O24" s="24"/>
+      <c r="P24" s="24"/>
+      <c r="Q24" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="R24" s="26"/>
-      <c r="S24" s="26"/>
-      <c r="T24" s="26"/>
-      <c r="U24" s="26"/>
-      <c r="V24" s="26"/>
-      <c r="W24" s="26"/>
-      <c r="X24" s="26"/>
-      <c r="Y24" s="26" t="s">
+      <c r="R24" s="24"/>
+      <c r="S24" s="24"/>
+      <c r="T24" s="24"/>
+      <c r="U24" s="24"/>
+      <c r="V24" s="24"/>
+      <c r="W24" s="24"/>
+      <c r="X24" s="24"/>
+      <c r="Y24" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="Z24" s="26"/>
-      <c r="AA24" s="26"/>
-      <c r="AB24" s="26"/>
-      <c r="AC24" s="26"/>
-      <c r="AD24" s="26"/>
-      <c r="AE24" s="26"/>
-      <c r="AF24" s="26"/>
-      <c r="AG24" s="21">
+      <c r="Z24" s="24"/>
+      <c r="AA24" s="24"/>
+      <c r="AB24" s="24"/>
+      <c r="AC24" s="24"/>
+      <c r="AD24" s="24"/>
+      <c r="AE24" s="24"/>
+      <c r="AF24" s="24"/>
+      <c r="AG24" s="35">
         <v>59</v>
       </c>
-      <c r="AH24" s="21"/>
-      <c r="AI24" s="21"/>
-      <c r="AJ24" s="21"/>
-      <c r="AK24" s="21"/>
-      <c r="AL24" s="21"/>
-      <c r="AM24" s="21"/>
-      <c r="AN24" s="21"/>
-      <c r="AO24" s="21">
+      <c r="AH24" s="35"/>
+      <c r="AI24" s="35"/>
+      <c r="AJ24" s="35"/>
+      <c r="AK24" s="35"/>
+      <c r="AL24" s="35"/>
+      <c r="AM24" s="35"/>
+      <c r="AN24" s="35"/>
+      <c r="AO24" s="35">
         <v>96</v>
       </c>
-      <c r="AP24" s="21"/>
-      <c r="AQ24" s="21"/>
-      <c r="AR24" s="21"/>
-      <c r="AS24" s="21"/>
-      <c r="AT24" s="21"/>
-      <c r="AU24" s="21"/>
-      <c r="AV24" s="21"/>
-      <c r="AW24" s="21">
+      <c r="AP24" s="35"/>
+      <c r="AQ24" s="35"/>
+      <c r="AR24" s="35"/>
+      <c r="AS24" s="35"/>
+      <c r="AT24" s="35"/>
+      <c r="AU24" s="35"/>
+      <c r="AV24" s="35"/>
+      <c r="AW24" s="35">
         <v>65</v>
       </c>
-      <c r="AX24" s="21"/>
-      <c r="AY24" s="21"/>
-      <c r="AZ24" s="21"/>
-      <c r="BA24" s="21"/>
-      <c r="BB24" s="21"/>
-      <c r="BC24" s="21"/>
-      <c r="BD24" s="21"/>
-      <c r="BE24" s="21" t="s">
+      <c r="AX24" s="35"/>
+      <c r="AY24" s="35"/>
+      <c r="AZ24" s="35"/>
+      <c r="BA24" s="35"/>
+      <c r="BB24" s="35"/>
+      <c r="BC24" s="35"/>
+      <c r="BD24" s="35"/>
+      <c r="BE24" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="BF24" s="21"/>
-      <c r="BG24" s="21"/>
-      <c r="BH24" s="21"/>
-      <c r="BI24" s="21"/>
-      <c r="BJ24" s="21"/>
-      <c r="BK24" s="21"/>
-      <c r="BL24" s="21"/>
-      <c r="BM24" s="21" t="s">
+      <c r="BF24" s="35"/>
+      <c r="BG24" s="35"/>
+      <c r="BH24" s="35"/>
+      <c r="BI24" s="35"/>
+      <c r="BJ24" s="35"/>
+      <c r="BK24" s="35"/>
+      <c r="BL24" s="35"/>
+      <c r="BM24" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="BN24" s="21"/>
-      <c r="BO24" s="21"/>
-      <c r="BP24" s="21"/>
-      <c r="BQ24" s="21"/>
-      <c r="BR24" s="21"/>
-      <c r="BS24" s="21"/>
-      <c r="BT24" s="21"/>
-      <c r="BU24" s="21">
+      <c r="BN24" s="35"/>
+      <c r="BO24" s="35"/>
+      <c r="BP24" s="35"/>
+      <c r="BQ24" s="35"/>
+      <c r="BR24" s="35"/>
+      <c r="BS24" s="35"/>
+      <c r="BT24" s="35"/>
+      <c r="BU24" s="35">
         <v>69</v>
       </c>
-      <c r="BV24" s="21"/>
-      <c r="BW24" s="21"/>
-      <c r="BX24" s="21"/>
-      <c r="BY24" s="21"/>
-      <c r="BZ24" s="21"/>
-      <c r="CA24" s="21"/>
-      <c r="CB24" s="21"/>
-      <c r="CC24" s="21" t="s">
+      <c r="BV24" s="35"/>
+      <c r="BW24" s="35"/>
+      <c r="BX24" s="35"/>
+      <c r="BY24" s="35"/>
+      <c r="BZ24" s="35"/>
+      <c r="CA24" s="35"/>
+      <c r="CB24" s="35"/>
+      <c r="CC24" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="CD24" s="21"/>
-      <c r="CE24" s="21"/>
-      <c r="CF24" s="21"/>
-      <c r="CG24" s="21"/>
-      <c r="CH24" s="21"/>
-      <c r="CI24" s="21"/>
-      <c r="CJ24" s="21"/>
-      <c r="CK24" s="21" t="s">
+      <c r="CD24" s="35"/>
+      <c r="CE24" s="35"/>
+      <c r="CF24" s="35"/>
+      <c r="CG24" s="35"/>
+      <c r="CH24" s="35"/>
+      <c r="CI24" s="35"/>
+      <c r="CJ24" s="35"/>
+      <c r="CK24" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="CL24" s="21"/>
-      <c r="CM24" s="21"/>
-      <c r="CN24" s="21"/>
-      <c r="CO24" s="21"/>
-      <c r="CP24" s="21"/>
-      <c r="CQ24" s="21"/>
-      <c r="CR24" s="21"/>
+      <c r="CL24" s="35"/>
+      <c r="CM24" s="35"/>
+      <c r="CN24" s="35"/>
+      <c r="CO24" s="35"/>
+      <c r="CP24" s="35"/>
+      <c r="CQ24" s="35"/>
+      <c r="CR24" s="35"/>
     </row>
     <row r="25" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A25" s="7">
@@ -4651,180 +4651,180 @@
       </c>
     </row>
     <row r="26" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22" t="s">
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="J26" s="22"/>
-      <c r="K26" s="22"/>
-      <c r="L26" s="22"/>
-      <c r="M26" s="22"/>
-      <c r="N26" s="22" t="s">
+      <c r="J26" s="20"/>
+      <c r="K26" s="20"/>
+      <c r="L26" s="20"/>
+      <c r="M26" s="20"/>
+      <c r="N26" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="O26" s="22"/>
-      <c r="P26" s="22"/>
-      <c r="Q26" s="22" t="s">
+      <c r="O26" s="20"/>
+      <c r="P26" s="20"/>
+      <c r="Q26" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="R26" s="22"/>
-      <c r="S26" s="22"/>
-      <c r="T26" s="22" t="s">
+      <c r="R26" s="20"/>
+      <c r="S26" s="20"/>
+      <c r="T26" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="U26" s="22"/>
-      <c r="V26" s="22"/>
-      <c r="W26" s="22"/>
-      <c r="X26" s="22"/>
-      <c r="Y26" s="22" t="s">
+      <c r="U26" s="20"/>
+      <c r="V26" s="20"/>
+      <c r="W26" s="20"/>
+      <c r="X26" s="20"/>
+      <c r="Y26" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z26" s="22"/>
-      <c r="AA26" s="22"/>
-      <c r="AB26" s="22"/>
-      <c r="AC26" s="22"/>
-      <c r="AD26" s="22" t="s">
+      <c r="Z26" s="20"/>
+      <c r="AA26" s="20"/>
+      <c r="AB26" s="20"/>
+      <c r="AC26" s="20"/>
+      <c r="AD26" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="AE26" s="22"/>
-      <c r="AF26" s="22"/>
-      <c r="AG26" s="20" t="s">
+      <c r="AE26" s="20"/>
+      <c r="AF26" s="20"/>
+      <c r="AG26" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="AH26" s="20"/>
-      <c r="AI26" s="20"/>
-      <c r="AJ26" s="20"/>
-      <c r="AK26" s="20"/>
-      <c r="AL26" s="20"/>
-      <c r="AM26" s="20"/>
-      <c r="AN26" s="20"/>
-      <c r="AO26" s="20" t="s">
+      <c r="AH26" s="22"/>
+      <c r="AI26" s="22"/>
+      <c r="AJ26" s="22"/>
+      <c r="AK26" s="22"/>
+      <c r="AL26" s="22"/>
+      <c r="AM26" s="22"/>
+      <c r="AN26" s="22"/>
+      <c r="AO26" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="AP26" s="20"/>
-      <c r="AQ26" s="20"/>
-      <c r="AR26" s="20"/>
-      <c r="AS26" s="20"/>
-      <c r="AT26" s="20"/>
-      <c r="AU26" s="20"/>
-      <c r="AV26" s="20"/>
-      <c r="AW26" s="20" t="s">
+      <c r="AP26" s="22"/>
+      <c r="AQ26" s="22"/>
+      <c r="AR26" s="22"/>
+      <c r="AS26" s="22"/>
+      <c r="AT26" s="22"/>
+      <c r="AU26" s="22"/>
+      <c r="AV26" s="22"/>
+      <c r="AW26" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="AX26" s="20"/>
-      <c r="AY26" s="20"/>
-      <c r="AZ26" s="20"/>
-      <c r="BA26" s="20"/>
-      <c r="BB26" s="20"/>
-      <c r="BC26" s="20"/>
-      <c r="BD26" s="20"/>
-      <c r="BE26" s="20" t="s">
+      <c r="AX26" s="22"/>
+      <c r="AY26" s="22"/>
+      <c r="AZ26" s="22"/>
+      <c r="BA26" s="22"/>
+      <c r="BB26" s="22"/>
+      <c r="BC26" s="22"/>
+      <c r="BD26" s="22"/>
+      <c r="BE26" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="BF26" s="20"/>
-      <c r="BG26" s="20"/>
-      <c r="BH26" s="20"/>
-      <c r="BI26" s="20"/>
-      <c r="BJ26" s="20"/>
-      <c r="BK26" s="20"/>
-      <c r="BL26" s="20"/>
-      <c r="BM26" s="20" t="s">
+      <c r="BF26" s="22"/>
+      <c r="BG26" s="22"/>
+      <c r="BH26" s="22"/>
+      <c r="BI26" s="22"/>
+      <c r="BJ26" s="22"/>
+      <c r="BK26" s="22"/>
+      <c r="BL26" s="22"/>
+      <c r="BM26" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="BN26" s="20"/>
-      <c r="BO26" s="20"/>
-      <c r="BP26" s="20"/>
-      <c r="BQ26" s="20"/>
-      <c r="BR26" s="20"/>
-      <c r="BS26" s="20"/>
-      <c r="BT26" s="20"/>
-      <c r="BU26" s="20" t="s">
+      <c r="BN26" s="22"/>
+      <c r="BO26" s="22"/>
+      <c r="BP26" s="22"/>
+      <c r="BQ26" s="22"/>
+      <c r="BR26" s="22"/>
+      <c r="BS26" s="22"/>
+      <c r="BT26" s="22"/>
+      <c r="BU26" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="BV26" s="20"/>
-      <c r="BW26" s="20"/>
-      <c r="BX26" s="20"/>
-      <c r="BY26" s="20"/>
-      <c r="BZ26" s="20"/>
-      <c r="CA26" s="20"/>
-      <c r="CB26" s="20"/>
-      <c r="CC26" s="20" t="s">
+      <c r="BV26" s="22"/>
+      <c r="BW26" s="22"/>
+      <c r="BX26" s="22"/>
+      <c r="BY26" s="22"/>
+      <c r="BZ26" s="22"/>
+      <c r="CA26" s="22"/>
+      <c r="CB26" s="22"/>
+      <c r="CC26" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="CD26" s="20"/>
-      <c r="CE26" s="20"/>
-      <c r="CF26" s="20"/>
-      <c r="CG26" s="20"/>
-      <c r="CH26" s="20"/>
-      <c r="CI26" s="20"/>
-      <c r="CJ26" s="20"/>
-      <c r="CK26" s="20" t="s">
+      <c r="CD26" s="22"/>
+      <c r="CE26" s="22"/>
+      <c r="CF26" s="22"/>
+      <c r="CG26" s="22"/>
+      <c r="CH26" s="22"/>
+      <c r="CI26" s="22"/>
+      <c r="CJ26" s="22"/>
+      <c r="CK26" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="CL26" s="20"/>
-      <c r="CM26" s="20"/>
-      <c r="CN26" s="20"/>
-      <c r="CO26" s="20"/>
-      <c r="CP26" s="20"/>
-      <c r="CQ26" s="20"/>
-      <c r="CR26" s="20"/>
+      <c r="CL26" s="22"/>
+      <c r="CM26" s="22"/>
+      <c r="CN26" s="22"/>
+      <c r="CO26" s="22"/>
+      <c r="CP26" s="22"/>
+      <c r="CQ26" s="22"/>
+      <c r="CR26" s="22"/>
     </row>
     <row r="27" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A27" s="22">
+      <c r="A27" s="20">
         <v>10</v>
       </c>
-      <c r="B27" s="22"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22">
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20">
         <v>8</v>
       </c>
-      <c r="J27" s="22"/>
-      <c r="K27" s="22"/>
-      <c r="L27" s="22"/>
-      <c r="M27" s="22"/>
-      <c r="N27" s="22">
-        <v>0</v>
-      </c>
-      <c r="O27" s="22"/>
-      <c r="P27" s="22"/>
-      <c r="Q27" s="22">
+      <c r="J27" s="20"/>
+      <c r="K27" s="20"/>
+      <c r="L27" s="20"/>
+      <c r="M27" s="20"/>
+      <c r="N27" s="20">
+        <v>0</v>
+      </c>
+      <c r="O27" s="20"/>
+      <c r="P27" s="20"/>
+      <c r="Q27" s="20">
         <v>3</v>
       </c>
-      <c r="R27" s="22"/>
-      <c r="S27" s="22"/>
-      <c r="T27" s="22">
+      <c r="R27" s="20"/>
+      <c r="S27" s="20"/>
+      <c r="T27" s="20">
         <v>19</v>
       </c>
-      <c r="U27" s="22"/>
-      <c r="V27" s="22"/>
-      <c r="W27" s="22"/>
-      <c r="X27" s="22"/>
-      <c r="Y27" s="22">
+      <c r="U27" s="20"/>
+      <c r="V27" s="20"/>
+      <c r="W27" s="20"/>
+      <c r="X27" s="20"/>
+      <c r="Y27" s="20">
         <v>21</v>
       </c>
-      <c r="Z27" s="22"/>
-      <c r="AA27" s="22"/>
-      <c r="AB27" s="22"/>
-      <c r="AC27" s="22"/>
-      <c r="AD27" s="22">
-        <v>0</v>
-      </c>
-      <c r="AE27" s="22"/>
-      <c r="AF27" s="22"/>
+      <c r="Z27" s="20"/>
+      <c r="AA27" s="20"/>
+      <c r="AB27" s="20"/>
+      <c r="AC27" s="20"/>
+      <c r="AD27" s="20">
+        <v>0</v>
+      </c>
+      <c r="AE27" s="20"/>
+      <c r="AF27" s="20"/>
       <c r="AG27">
         <f>AN25</f>
         <v>1</v>
@@ -5083,267 +5083,267 @@
       </c>
     </row>
     <row r="28" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A28" s="22" t="s">
+      <c r="A28" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22" t="s">
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="J28" s="22"/>
-      <c r="K28" s="22"/>
-      <c r="L28" s="22"/>
-      <c r="M28" s="22"/>
-      <c r="N28" s="22" t="s">
+      <c r="J28" s="20"/>
+      <c r="K28" s="20"/>
+      <c r="L28" s="20"/>
+      <c r="M28" s="20"/>
+      <c r="N28" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="O28" s="22"/>
-      <c r="P28" s="22"/>
-      <c r="Q28" s="22" t="s">
+      <c r="O28" s="20"/>
+      <c r="P28" s="20"/>
+      <c r="Q28" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="R28" s="22"/>
-      <c r="S28" s="22"/>
-      <c r="T28" s="22" t="s">
+      <c r="R28" s="20"/>
+      <c r="S28" s="20"/>
+      <c r="T28" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="U28" s="22"/>
-      <c r="V28" s="22"/>
-      <c r="W28" s="22"/>
-      <c r="X28" s="22"/>
-      <c r="Y28" s="22" t="s">
+      <c r="U28" s="20"/>
+      <c r="V28" s="20"/>
+      <c r="W28" s="20"/>
+      <c r="X28" s="20"/>
+      <c r="Y28" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="Z28" s="22"/>
-      <c r="AA28" s="22"/>
-      <c r="AB28" s="22"/>
-      <c r="AC28" s="22"/>
-      <c r="AD28" s="22" t="s">
+      <c r="Z28" s="20"/>
+      <c r="AA28" s="20"/>
+      <c r="AB28" s="20"/>
+      <c r="AC28" s="20"/>
+      <c r="AD28" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="AE28" s="22"/>
-      <c r="AF28" s="22"/>
-      <c r="AG28" s="20" t="s">
+      <c r="AE28" s="20"/>
+      <c r="AF28" s="20"/>
+      <c r="AG28" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="AH28" s="20"/>
-      <c r="AI28" s="20"/>
-      <c r="AJ28" s="20"/>
-      <c r="AK28" s="20"/>
-      <c r="AL28" s="20"/>
-      <c r="AM28" s="20" t="s">
+      <c r="AH28" s="22"/>
+      <c r="AI28" s="22"/>
+      <c r="AJ28" s="22"/>
+      <c r="AK28" s="22"/>
+      <c r="AL28" s="22"/>
+      <c r="AM28" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="AN28" s="20"/>
-      <c r="AO28" s="20"/>
-      <c r="AP28" s="20"/>
-      <c r="AQ28" s="20"/>
-      <c r="AR28" s="20"/>
-      <c r="AS28" s="20" t="s">
+      <c r="AN28" s="22"/>
+      <c r="AO28" s="22"/>
+      <c r="AP28" s="22"/>
+      <c r="AQ28" s="22"/>
+      <c r="AR28" s="22"/>
+      <c r="AS28" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="AT28" s="20"/>
-      <c r="AU28" s="20"/>
-      <c r="AV28" s="20"/>
-      <c r="AW28" s="20"/>
-      <c r="AX28" s="20"/>
-      <c r="AY28" s="20" t="s">
+      <c r="AT28" s="22"/>
+      <c r="AU28" s="22"/>
+      <c r="AV28" s="22"/>
+      <c r="AW28" s="22"/>
+      <c r="AX28" s="22"/>
+      <c r="AY28" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="AZ28" s="20"/>
-      <c r="BA28" s="20"/>
-      <c r="BB28" s="20"/>
-      <c r="BC28" s="20"/>
-      <c r="BD28" s="20"/>
-      <c r="BE28" s="20" t="s">
+      <c r="AZ28" s="22"/>
+      <c r="BA28" s="22"/>
+      <c r="BB28" s="22"/>
+      <c r="BC28" s="22"/>
+      <c r="BD28" s="22"/>
+      <c r="BE28" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="BF28" s="20"/>
-      <c r="BG28" s="20"/>
-      <c r="BH28" s="20"/>
-      <c r="BI28" s="20"/>
-      <c r="BJ28" s="20"/>
-      <c r="BK28" s="20" t="s">
+      <c r="BF28" s="22"/>
+      <c r="BG28" s="22"/>
+      <c r="BH28" s="22"/>
+      <c r="BI28" s="22"/>
+      <c r="BJ28" s="22"/>
+      <c r="BK28" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="BL28" s="20"/>
-      <c r="BM28" s="20"/>
-      <c r="BN28" s="20"/>
-      <c r="BO28" s="20"/>
-      <c r="BP28" s="20"/>
-      <c r="BQ28" s="20" t="s">
+      <c r="BL28" s="22"/>
+      <c r="BM28" s="22"/>
+      <c r="BN28" s="22"/>
+      <c r="BO28" s="22"/>
+      <c r="BP28" s="22"/>
+      <c r="BQ28" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="BR28" s="20"/>
-      <c r="BS28" s="20"/>
-      <c r="BT28" s="20"/>
-      <c r="BU28" s="20"/>
-      <c r="BV28" s="20"/>
-      <c r="BW28" s="20" t="s">
+      <c r="BR28" s="22"/>
+      <c r="BS28" s="22"/>
+      <c r="BT28" s="22"/>
+      <c r="BU28" s="22"/>
+      <c r="BV28" s="22"/>
+      <c r="BW28" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="BX28" s="20"/>
-      <c r="BY28" s="20"/>
-      <c r="BZ28" s="20"/>
-      <c r="CA28" s="20"/>
-      <c r="CB28" s="20"/>
-      <c r="CC28" s="20" t="s">
+      <c r="BX28" s="22"/>
+      <c r="BY28" s="22"/>
+      <c r="BZ28" s="22"/>
+      <c r="CA28" s="22"/>
+      <c r="CB28" s="22"/>
+      <c r="CC28" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="CD28" s="20"/>
-      <c r="CE28" s="20"/>
-      <c r="CF28" s="20"/>
-      <c r="CG28" s="20"/>
-      <c r="CH28" s="20"/>
-      <c r="CI28" s="20" t="s">
+      <c r="CD28" s="22"/>
+      <c r="CE28" s="22"/>
+      <c r="CF28" s="22"/>
+      <c r="CG28" s="22"/>
+      <c r="CH28" s="22"/>
+      <c r="CI28" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="CJ28" s="20"/>
-      <c r="CK28" s="20"/>
-      <c r="CL28" s="20"/>
-      <c r="CM28" s="20"/>
-      <c r="CN28" s="20"/>
+      <c r="CJ28" s="22"/>
+      <c r="CK28" s="22"/>
+      <c r="CL28" s="22"/>
+      <c r="CM28" s="22"/>
+      <c r="CN28" s="22"/>
     </row>
     <row r="29" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A29" s="22">
+      <c r="A29" s="20">
         <f>A27</f>
         <v>10</v>
       </c>
-      <c r="B29" s="22"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="23">
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="21">
         <f>'Data package'!$B$31*I27+'Data package'!$B$28</f>
         <v>3.3870967741935485</v>
       </c>
-      <c r="J29" s="23"/>
-      <c r="K29" s="23"/>
-      <c r="L29" s="23"/>
-      <c r="M29" s="23"/>
-      <c r="N29" s="20">
+      <c r="J29" s="21"/>
+      <c r="K29" s="21"/>
+      <c r="L29" s="21"/>
+      <c r="M29" s="21"/>
+      <c r="N29" s="22">
         <f ca="1">LOOKUP(N27,'Data package'!$D$21:$D$24,'Data package'!$E$22:$E$35)</f>
         <v>0</v>
       </c>
-      <c r="O29" s="20"/>
-      <c r="P29" s="20"/>
-      <c r="Q29" s="24">
+      <c r="O29" s="22"/>
+      <c r="P29" s="22"/>
+      <c r="Q29" s="23">
         <f>100/(2^3-1)*Q27</f>
         <v>42.857142857142861</v>
       </c>
-      <c r="R29" s="24"/>
-      <c r="S29" s="24"/>
-      <c r="T29" s="24">
+      <c r="R29" s="23"/>
+      <c r="S29" s="23"/>
+      <c r="T29" s="23">
         <f>'Data package'!$B$40*T27+'Data package'!$B$37</f>
         <v>22.903225806451616</v>
       </c>
-      <c r="U29" s="20"/>
-      <c r="V29" s="20"/>
-      <c r="W29" s="20"/>
-      <c r="X29" s="20"/>
-      <c r="Y29" s="20">
+      <c r="U29" s="22"/>
+      <c r="V29" s="22"/>
+      <c r="W29" s="22"/>
+      <c r="X29" s="22"/>
+      <c r="Y29" s="22">
         <f>Y27</f>
         <v>21</v>
       </c>
-      <c r="Z29" s="20"/>
-      <c r="AA29" s="20"/>
-      <c r="AB29" s="20"/>
-      <c r="AC29" s="20"/>
-      <c r="AD29" s="20">
+      <c r="Z29" s="22"/>
+      <c r="AA29" s="22"/>
+      <c r="AB29" s="22"/>
+      <c r="AC29" s="22"/>
+      <c r="AD29" s="22">
         <f>LOOKUP(AD27,'Data package'!$A$84:$A$88,'Data package'!$B$84:$B$88)</f>
         <v>1</v>
       </c>
-      <c r="AE29" s="20"/>
-      <c r="AF29" s="20"/>
-      <c r="AG29" s="20" t="s">
+      <c r="AE29" s="22"/>
+      <c r="AF29" s="22"/>
+      <c r="AG29" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="AH29" s="20"/>
-      <c r="AI29" s="20"/>
-      <c r="AJ29" s="20"/>
-      <c r="AK29" s="20"/>
-      <c r="AL29" s="20"/>
-      <c r="AM29" s="20" t="s">
+      <c r="AH29" s="22"/>
+      <c r="AI29" s="22"/>
+      <c r="AJ29" s="22"/>
+      <c r="AK29" s="22"/>
+      <c r="AL29" s="22"/>
+      <c r="AM29" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="AN29" s="20"/>
-      <c r="AO29" s="20"/>
-      <c r="AP29" s="20"/>
-      <c r="AQ29" s="20"/>
-      <c r="AR29" s="20"/>
-      <c r="AS29" s="20" t="s">
+      <c r="AN29" s="22"/>
+      <c r="AO29" s="22"/>
+      <c r="AP29" s="22"/>
+      <c r="AQ29" s="22"/>
+      <c r="AR29" s="22"/>
+      <c r="AS29" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="AT29" s="20"/>
-      <c r="AU29" s="20"/>
-      <c r="AV29" s="20"/>
-      <c r="AW29" s="20"/>
-      <c r="AX29" s="20"/>
-      <c r="AY29" s="20" t="s">
+      <c r="AT29" s="22"/>
+      <c r="AU29" s="22"/>
+      <c r="AV29" s="22"/>
+      <c r="AW29" s="22"/>
+      <c r="AX29" s="22"/>
+      <c r="AY29" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="AZ29" s="20"/>
-      <c r="BA29" s="20"/>
-      <c r="BB29" s="20"/>
-      <c r="BC29" s="20"/>
-      <c r="BD29" s="20"/>
-      <c r="BE29" s="20" t="s">
+      <c r="AZ29" s="22"/>
+      <c r="BA29" s="22"/>
+      <c r="BB29" s="22"/>
+      <c r="BC29" s="22"/>
+      <c r="BD29" s="22"/>
+      <c r="BE29" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="BF29" s="20"/>
-      <c r="BG29" s="20"/>
-      <c r="BH29" s="20"/>
-      <c r="BI29" s="20"/>
-      <c r="BJ29" s="20"/>
-      <c r="BK29" s="20" t="s">
+      <c r="BF29" s="22"/>
+      <c r="BG29" s="22"/>
+      <c r="BH29" s="22"/>
+      <c r="BI29" s="22"/>
+      <c r="BJ29" s="22"/>
+      <c r="BK29" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="BL29" s="20"/>
-      <c r="BM29" s="20"/>
-      <c r="BN29" s="20"/>
-      <c r="BO29" s="20"/>
-      <c r="BP29" s="20"/>
-      <c r="BQ29" s="20" t="s">
+      <c r="BL29" s="22"/>
+      <c r="BM29" s="22"/>
+      <c r="BN29" s="22"/>
+      <c r="BO29" s="22"/>
+      <c r="BP29" s="22"/>
+      <c r="BQ29" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="BR29" s="20"/>
-      <c r="BS29" s="20"/>
-      <c r="BT29" s="20"/>
-      <c r="BU29" s="20"/>
-      <c r="BV29" s="20"/>
-      <c r="BW29" s="20" t="s">
+      <c r="BR29" s="22"/>
+      <c r="BS29" s="22"/>
+      <c r="BT29" s="22"/>
+      <c r="BU29" s="22"/>
+      <c r="BV29" s="22"/>
+      <c r="BW29" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="BX29" s="20"/>
-      <c r="BY29" s="20"/>
-      <c r="BZ29" s="20"/>
-      <c r="CA29" s="20"/>
-      <c r="CB29" s="20"/>
-      <c r="CC29" s="20" t="s">
+      <c r="BX29" s="22"/>
+      <c r="BY29" s="22"/>
+      <c r="BZ29" s="22"/>
+      <c r="CA29" s="22"/>
+      <c r="CB29" s="22"/>
+      <c r="CC29" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="CD29" s="20"/>
-      <c r="CE29" s="20"/>
-      <c r="CF29" s="20"/>
-      <c r="CG29" s="20"/>
-      <c r="CH29" s="20"/>
-      <c r="CI29" s="20" t="s">
+      <c r="CD29" s="22"/>
+      <c r="CE29" s="22"/>
+      <c r="CF29" s="22"/>
+      <c r="CG29" s="22"/>
+      <c r="CH29" s="22"/>
+      <c r="CI29" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="CJ29" s="20"/>
-      <c r="CK29" s="20"/>
-      <c r="CL29" s="20"/>
-      <c r="CM29" s="20"/>
-      <c r="CN29" s="20"/>
+      <c r="CJ29" s="22"/>
+      <c r="CK29" s="22"/>
+      <c r="CL29" s="22"/>
+      <c r="CM29" s="22"/>
+      <c r="CN29" s="22"/>
     </row>
     <row r="30" spans="1:96" x14ac:dyDescent="0.3">
       <c r="AG30">
@@ -5588,229 +5588,255 @@
       </c>
     </row>
     <row r="31" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="AG31" s="20" t="s">
+      <c r="AG31" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="AH31" s="20"/>
-      <c r="AI31" s="20"/>
-      <c r="AJ31" s="20"/>
-      <c r="AK31" s="20"/>
-      <c r="AL31" s="20"/>
-      <c r="AM31" s="20" t="s">
+      <c r="AH31" s="22"/>
+      <c r="AI31" s="22"/>
+      <c r="AJ31" s="22"/>
+      <c r="AK31" s="22"/>
+      <c r="AL31" s="22"/>
+      <c r="AM31" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="AN31" s="20"/>
-      <c r="AO31" s="20"/>
-      <c r="AP31" s="20"/>
-      <c r="AQ31" s="20"/>
-      <c r="AR31" s="20"/>
-      <c r="AS31" s="20" t="s">
+      <c r="AN31" s="22"/>
+      <c r="AO31" s="22"/>
+      <c r="AP31" s="22"/>
+      <c r="AQ31" s="22"/>
+      <c r="AR31" s="22"/>
+      <c r="AS31" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="AT31" s="20"/>
-      <c r="AU31" s="20"/>
-      <c r="AV31" s="20"/>
-      <c r="AW31" s="20"/>
-      <c r="AX31" s="20"/>
-      <c r="AY31" s="20" t="s">
+      <c r="AT31" s="22"/>
+      <c r="AU31" s="22"/>
+      <c r="AV31" s="22"/>
+      <c r="AW31" s="22"/>
+      <c r="AX31" s="22"/>
+      <c r="AY31" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="AZ31" s="20"/>
-      <c r="BA31" s="20"/>
-      <c r="BB31" s="20"/>
-      <c r="BC31" s="20"/>
-      <c r="BD31" s="20"/>
-      <c r="BE31" s="20" t="s">
+      <c r="AZ31" s="22"/>
+      <c r="BA31" s="22"/>
+      <c r="BB31" s="22"/>
+      <c r="BC31" s="22"/>
+      <c r="BD31" s="22"/>
+      <c r="BE31" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="BF31" s="20"/>
-      <c r="BG31" s="20"/>
-      <c r="BH31" s="20"/>
-      <c r="BI31" s="20"/>
-      <c r="BJ31" s="20"/>
-      <c r="BK31" s="20" t="s">
+      <c r="BF31" s="22"/>
+      <c r="BG31" s="22"/>
+      <c r="BH31" s="22"/>
+      <c r="BI31" s="22"/>
+      <c r="BJ31" s="22"/>
+      <c r="BK31" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="BL31" s="20"/>
-      <c r="BM31" s="20"/>
-      <c r="BN31" s="20"/>
-      <c r="BO31" s="20"/>
-      <c r="BP31" s="20"/>
-      <c r="BQ31" s="20" t="s">
+      <c r="BL31" s="22"/>
+      <c r="BM31" s="22"/>
+      <c r="BN31" s="22"/>
+      <c r="BO31" s="22"/>
+      <c r="BP31" s="22"/>
+      <c r="BQ31" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="BR31" s="20"/>
-      <c r="BS31" s="20"/>
-      <c r="BT31" s="20"/>
-      <c r="BU31" s="20"/>
-      <c r="BV31" s="20"/>
-      <c r="BW31" s="20" t="s">
+      <c r="BR31" s="22"/>
+      <c r="BS31" s="22"/>
+      <c r="BT31" s="22"/>
+      <c r="BU31" s="22"/>
+      <c r="BV31" s="22"/>
+      <c r="BW31" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="BX31" s="20"/>
-      <c r="BY31" s="20"/>
-      <c r="BZ31" s="20"/>
-      <c r="CA31" s="20"/>
-      <c r="CB31" s="20"/>
-      <c r="CC31" s="20" t="s">
+      <c r="BX31" s="22"/>
+      <c r="BY31" s="22"/>
+      <c r="BZ31" s="22"/>
+      <c r="CA31" s="22"/>
+      <c r="CB31" s="22"/>
+      <c r="CC31" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="CD31" s="20"/>
-      <c r="CE31" s="20"/>
-      <c r="CF31" s="20"/>
-      <c r="CG31" s="20"/>
-      <c r="CH31" s="20"/>
-      <c r="CI31" s="20" t="s">
+      <c r="CD31" s="22"/>
+      <c r="CE31" s="22"/>
+      <c r="CF31" s="22"/>
+      <c r="CG31" s="22"/>
+      <c r="CH31" s="22"/>
+      <c r="CI31" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="CJ31" s="20"/>
-      <c r="CK31" s="20"/>
-      <c r="CL31" s="20"/>
-      <c r="CM31" s="20"/>
-      <c r="CN31" s="20"/>
+      <c r="CJ31" s="22"/>
+      <c r="CK31" s="22"/>
+      <c r="CL31" s="22"/>
+      <c r="CM31" s="22"/>
+      <c r="CN31" s="22"/>
     </row>
     <row r="32" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="AG32" s="20">
+      <c r="AG32" s="22">
         <v>25</v>
       </c>
-      <c r="AH32" s="20"/>
-      <c r="AI32" s="20"/>
-      <c r="AJ32" s="20"/>
-      <c r="AK32" s="20"/>
-      <c r="AL32" s="20"/>
-      <c r="AM32" s="20">
+      <c r="AH32" s="22"/>
+      <c r="AI32" s="22"/>
+      <c r="AJ32" s="22"/>
+      <c r="AK32" s="22"/>
+      <c r="AL32" s="22"/>
+      <c r="AM32" s="22">
         <v>25</v>
       </c>
-      <c r="AN32" s="20"/>
-      <c r="AO32" s="20"/>
-      <c r="AP32" s="20"/>
-      <c r="AQ32" s="20"/>
-      <c r="AR32" s="20"/>
-      <c r="AS32" s="20">
+      <c r="AN32" s="22"/>
+      <c r="AO32" s="22"/>
+      <c r="AP32" s="22"/>
+      <c r="AQ32" s="22"/>
+      <c r="AR32" s="22"/>
+      <c r="AS32" s="22">
         <v>25</v>
       </c>
-      <c r="AT32" s="20"/>
-      <c r="AU32" s="20"/>
-      <c r="AV32" s="20"/>
-      <c r="AW32" s="20"/>
-      <c r="AX32" s="20"/>
-      <c r="AY32" s="20">
+      <c r="AT32" s="22"/>
+      <c r="AU32" s="22"/>
+      <c r="AV32" s="22"/>
+      <c r="AW32" s="22"/>
+      <c r="AX32" s="22"/>
+      <c r="AY32" s="22">
         <v>25</v>
       </c>
-      <c r="AZ32" s="20"/>
-      <c r="BA32" s="20"/>
-      <c r="BB32" s="20"/>
-      <c r="BC32" s="20"/>
-      <c r="BD32" s="20"/>
-      <c r="BE32" s="20">
+      <c r="AZ32" s="22"/>
+      <c r="BA32" s="22"/>
+      <c r="BB32" s="22"/>
+      <c r="BC32" s="22"/>
+      <c r="BD32" s="22"/>
+      <c r="BE32" s="22">
         <v>26</v>
       </c>
-      <c r="BF32" s="20"/>
-      <c r="BG32" s="20"/>
-      <c r="BH32" s="20"/>
-      <c r="BI32" s="20"/>
-      <c r="BJ32" s="20"/>
-      <c r="BK32" s="20">
+      <c r="BF32" s="22"/>
+      <c r="BG32" s="22"/>
+      <c r="BH32" s="22"/>
+      <c r="BI32" s="22"/>
+      <c r="BJ32" s="22"/>
+      <c r="BK32" s="22">
         <v>26</v>
       </c>
-      <c r="BL32" s="20"/>
-      <c r="BM32" s="20"/>
-      <c r="BN32" s="20"/>
-      <c r="BO32" s="20"/>
-      <c r="BP32" s="20"/>
-      <c r="BQ32" s="20">
+      <c r="BL32" s="22"/>
+      <c r="BM32" s="22"/>
+      <c r="BN32" s="22"/>
+      <c r="BO32" s="22"/>
+      <c r="BP32" s="22"/>
+      <c r="BQ32" s="22">
         <v>26</v>
       </c>
-      <c r="BR32" s="20"/>
-      <c r="BS32" s="20"/>
-      <c r="BT32" s="20"/>
-      <c r="BU32" s="20"/>
-      <c r="BV32" s="20"/>
-      <c r="BW32" s="20">
+      <c r="BR32" s="22"/>
+      <c r="BS32" s="22"/>
+      <c r="BT32" s="22"/>
+      <c r="BU32" s="22"/>
+      <c r="BV32" s="22"/>
+      <c r="BW32" s="22">
         <v>26</v>
       </c>
-      <c r="BX32" s="20"/>
-      <c r="BY32" s="20"/>
-      <c r="BZ32" s="20"/>
-      <c r="CA32" s="20"/>
-      <c r="CB32" s="20"/>
-      <c r="CC32" s="20">
+      <c r="BX32" s="22"/>
+      <c r="BY32" s="22"/>
+      <c r="BZ32" s="22"/>
+      <c r="CA32" s="22"/>
+      <c r="CB32" s="22"/>
+      <c r="CC32" s="22">
         <v>26</v>
       </c>
-      <c r="CD32" s="20"/>
-      <c r="CE32" s="20"/>
-      <c r="CF32" s="20"/>
-      <c r="CG32" s="20"/>
-      <c r="CH32" s="20"/>
-      <c r="CI32" s="20">
+      <c r="CD32" s="22"/>
+      <c r="CE32" s="22"/>
+      <c r="CF32" s="22"/>
+      <c r="CG32" s="22"/>
+      <c r="CH32" s="22"/>
+      <c r="CI32" s="22">
         <v>26</v>
       </c>
-      <c r="CJ32" s="20"/>
-      <c r="CK32" s="20"/>
-      <c r="CL32" s="20"/>
-      <c r="CM32" s="20"/>
-      <c r="CN32" s="20"/>
+      <c r="CJ32" s="22"/>
+      <c r="CK32" s="22"/>
+      <c r="CL32" s="22"/>
+      <c r="CM32" s="22"/>
+      <c r="CN32" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="166">
-    <mergeCell ref="Y19:AC19"/>
-    <mergeCell ref="AD19:AF19"/>
-    <mergeCell ref="A20:H20"/>
-    <mergeCell ref="I20:M20"/>
-    <mergeCell ref="N20:P20"/>
-    <mergeCell ref="Q20:S20"/>
-    <mergeCell ref="T20:X20"/>
-    <mergeCell ref="Y20:AC20"/>
-    <mergeCell ref="AD20:AF20"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="I19:M19"/>
-    <mergeCell ref="N19:P19"/>
-    <mergeCell ref="Q19:S19"/>
-    <mergeCell ref="T19:X19"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="I15:P15"/>
-    <mergeCell ref="Q15:X15"/>
-    <mergeCell ref="Y15:AF15"/>
-    <mergeCell ref="A14:AF14"/>
-    <mergeCell ref="Y17:AC17"/>
-    <mergeCell ref="AD17:AF17"/>
-    <mergeCell ref="A18:H18"/>
-    <mergeCell ref="I18:M18"/>
-    <mergeCell ref="N18:P18"/>
-    <mergeCell ref="Q18:S18"/>
-    <mergeCell ref="T18:X18"/>
-    <mergeCell ref="Y18:AC18"/>
-    <mergeCell ref="AD18:AF18"/>
-    <mergeCell ref="A17:H17"/>
-    <mergeCell ref="I17:M17"/>
-    <mergeCell ref="N17:P17"/>
-    <mergeCell ref="Q17:S17"/>
-    <mergeCell ref="T17:X17"/>
-    <mergeCell ref="I11:M11"/>
-    <mergeCell ref="A11:H11"/>
-    <mergeCell ref="I10:M10"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="AD10:AF10"/>
-    <mergeCell ref="Y10:AC10"/>
-    <mergeCell ref="T10:X10"/>
-    <mergeCell ref="Q10:S10"/>
-    <mergeCell ref="N10:P10"/>
-    <mergeCell ref="AD11:AF11"/>
-    <mergeCell ref="Y11:AC11"/>
-    <mergeCell ref="T11:X11"/>
-    <mergeCell ref="Q11:S11"/>
-    <mergeCell ref="N11:P11"/>
-    <mergeCell ref="Q6:X6"/>
-    <mergeCell ref="Y6:AF6"/>
-    <mergeCell ref="AD9:AF9"/>
-    <mergeCell ref="AD8:AF8"/>
-    <mergeCell ref="Y9:AC9"/>
-    <mergeCell ref="Y8:AC8"/>
-    <mergeCell ref="N9:P9"/>
-    <mergeCell ref="Q8:S8"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="T8:X8"/>
-    <mergeCell ref="T9:X9"/>
+    <mergeCell ref="BK32:BP32"/>
+    <mergeCell ref="BQ32:BV32"/>
+    <mergeCell ref="BW32:CB32"/>
+    <mergeCell ref="CC32:CH32"/>
+    <mergeCell ref="CI32:CN32"/>
+    <mergeCell ref="AG32:AL32"/>
+    <mergeCell ref="AM32:AR32"/>
+    <mergeCell ref="AS32:AX32"/>
+    <mergeCell ref="AY32:BD32"/>
+    <mergeCell ref="BE32:BJ32"/>
+    <mergeCell ref="BK31:BP31"/>
+    <mergeCell ref="BQ31:BV31"/>
+    <mergeCell ref="BW31:CB31"/>
+    <mergeCell ref="CC31:CH31"/>
+    <mergeCell ref="CI31:CN31"/>
+    <mergeCell ref="AG31:AL31"/>
+    <mergeCell ref="AM31:AR31"/>
+    <mergeCell ref="AS31:AX31"/>
+    <mergeCell ref="AY31:BD31"/>
+    <mergeCell ref="BE31:BJ31"/>
+    <mergeCell ref="BK29:BP29"/>
+    <mergeCell ref="BQ29:BV29"/>
+    <mergeCell ref="BW29:CB29"/>
+    <mergeCell ref="CC29:CH29"/>
+    <mergeCell ref="CI29:CN29"/>
+    <mergeCell ref="AG29:AL29"/>
+    <mergeCell ref="AM29:AR29"/>
+    <mergeCell ref="AS29:AX29"/>
+    <mergeCell ref="AY29:BD29"/>
+    <mergeCell ref="BE29:BJ29"/>
+    <mergeCell ref="BK28:BP28"/>
+    <mergeCell ref="BQ28:BV28"/>
+    <mergeCell ref="BW28:CB28"/>
+    <mergeCell ref="CC28:CH28"/>
+    <mergeCell ref="CI28:CN28"/>
+    <mergeCell ref="AG28:AL28"/>
+    <mergeCell ref="AM28:AR28"/>
+    <mergeCell ref="AS28:AX28"/>
+    <mergeCell ref="AY28:BD28"/>
+    <mergeCell ref="BE28:BJ28"/>
+    <mergeCell ref="BU24:CB24"/>
+    <mergeCell ref="CC24:CJ24"/>
+    <mergeCell ref="CK24:CR24"/>
+    <mergeCell ref="AG26:AN26"/>
+    <mergeCell ref="AO26:AV26"/>
+    <mergeCell ref="AW26:BD26"/>
+    <mergeCell ref="BE26:BL26"/>
+    <mergeCell ref="BM26:BT26"/>
+    <mergeCell ref="BU26:CB26"/>
+    <mergeCell ref="CC26:CJ26"/>
+    <mergeCell ref="CK26:CR26"/>
+    <mergeCell ref="AG24:AN24"/>
+    <mergeCell ref="AO24:AV24"/>
+    <mergeCell ref="AW24:BD24"/>
+    <mergeCell ref="BE24:BL24"/>
+    <mergeCell ref="BM24:BT24"/>
+    <mergeCell ref="Y28:AC28"/>
+    <mergeCell ref="AD28:AF28"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="I29:M29"/>
+    <mergeCell ref="N29:P29"/>
+    <mergeCell ref="Q29:S29"/>
+    <mergeCell ref="T29:X29"/>
+    <mergeCell ref="Y29:AC29"/>
+    <mergeCell ref="AD29:AF29"/>
+    <mergeCell ref="A28:H28"/>
+    <mergeCell ref="I28:M28"/>
+    <mergeCell ref="N28:P28"/>
+    <mergeCell ref="Q28:S28"/>
+    <mergeCell ref="T28:X28"/>
+    <mergeCell ref="Y26:AC26"/>
+    <mergeCell ref="AD26:AF26"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="I27:M27"/>
+    <mergeCell ref="N27:P27"/>
+    <mergeCell ref="Q27:S27"/>
+    <mergeCell ref="T27:X27"/>
+    <mergeCell ref="Y27:AC27"/>
+    <mergeCell ref="AD27:AF27"/>
+    <mergeCell ref="A26:H26"/>
+    <mergeCell ref="I26:M26"/>
+    <mergeCell ref="N26:P26"/>
+    <mergeCell ref="Q26:S26"/>
+    <mergeCell ref="T26:X26"/>
     <mergeCell ref="A23:AF23"/>
     <mergeCell ref="A24:H24"/>
     <mergeCell ref="I24:P24"/>
@@ -5835,90 +5861,64 @@
     <mergeCell ref="I8:M8"/>
     <mergeCell ref="N8:P8"/>
     <mergeCell ref="I9:M9"/>
-    <mergeCell ref="Y26:AC26"/>
-    <mergeCell ref="AD26:AF26"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="I27:M27"/>
-    <mergeCell ref="N27:P27"/>
-    <mergeCell ref="Q27:S27"/>
-    <mergeCell ref="T27:X27"/>
-    <mergeCell ref="Y27:AC27"/>
-    <mergeCell ref="AD27:AF27"/>
-    <mergeCell ref="A26:H26"/>
-    <mergeCell ref="I26:M26"/>
-    <mergeCell ref="N26:P26"/>
-    <mergeCell ref="Q26:S26"/>
-    <mergeCell ref="T26:X26"/>
-    <mergeCell ref="Y28:AC28"/>
-    <mergeCell ref="AD28:AF28"/>
-    <mergeCell ref="A29:H29"/>
-    <mergeCell ref="I29:M29"/>
-    <mergeCell ref="N29:P29"/>
-    <mergeCell ref="Q29:S29"/>
-    <mergeCell ref="T29:X29"/>
-    <mergeCell ref="Y29:AC29"/>
-    <mergeCell ref="AD29:AF29"/>
-    <mergeCell ref="A28:H28"/>
-    <mergeCell ref="I28:M28"/>
-    <mergeCell ref="N28:P28"/>
-    <mergeCell ref="Q28:S28"/>
-    <mergeCell ref="T28:X28"/>
-    <mergeCell ref="BU24:CB24"/>
-    <mergeCell ref="CC24:CJ24"/>
-    <mergeCell ref="CK24:CR24"/>
-    <mergeCell ref="AG26:AN26"/>
-    <mergeCell ref="AO26:AV26"/>
-    <mergeCell ref="AW26:BD26"/>
-    <mergeCell ref="BE26:BL26"/>
-    <mergeCell ref="BM26:BT26"/>
-    <mergeCell ref="BU26:CB26"/>
-    <mergeCell ref="CC26:CJ26"/>
-    <mergeCell ref="CK26:CR26"/>
-    <mergeCell ref="AG24:AN24"/>
-    <mergeCell ref="AO24:AV24"/>
-    <mergeCell ref="AW24:BD24"/>
-    <mergeCell ref="BE24:BL24"/>
-    <mergeCell ref="BM24:BT24"/>
-    <mergeCell ref="BK28:BP28"/>
-    <mergeCell ref="BQ28:BV28"/>
-    <mergeCell ref="BW28:CB28"/>
-    <mergeCell ref="CC28:CH28"/>
-    <mergeCell ref="CI28:CN28"/>
-    <mergeCell ref="AG28:AL28"/>
-    <mergeCell ref="AM28:AR28"/>
-    <mergeCell ref="AS28:AX28"/>
-    <mergeCell ref="AY28:BD28"/>
-    <mergeCell ref="BE28:BJ28"/>
-    <mergeCell ref="BK29:BP29"/>
-    <mergeCell ref="BQ29:BV29"/>
-    <mergeCell ref="BW29:CB29"/>
-    <mergeCell ref="CC29:CH29"/>
-    <mergeCell ref="CI29:CN29"/>
-    <mergeCell ref="AG29:AL29"/>
-    <mergeCell ref="AM29:AR29"/>
-    <mergeCell ref="AS29:AX29"/>
-    <mergeCell ref="AY29:BD29"/>
-    <mergeCell ref="BE29:BJ29"/>
-    <mergeCell ref="BK31:BP31"/>
-    <mergeCell ref="BQ31:BV31"/>
-    <mergeCell ref="BW31:CB31"/>
-    <mergeCell ref="CC31:CH31"/>
-    <mergeCell ref="CI31:CN31"/>
-    <mergeCell ref="AG31:AL31"/>
-    <mergeCell ref="AM31:AR31"/>
-    <mergeCell ref="AS31:AX31"/>
-    <mergeCell ref="AY31:BD31"/>
-    <mergeCell ref="BE31:BJ31"/>
-    <mergeCell ref="BK32:BP32"/>
-    <mergeCell ref="BQ32:BV32"/>
-    <mergeCell ref="BW32:CB32"/>
-    <mergeCell ref="CC32:CH32"/>
-    <mergeCell ref="CI32:CN32"/>
-    <mergeCell ref="AG32:AL32"/>
-    <mergeCell ref="AM32:AR32"/>
-    <mergeCell ref="AS32:AX32"/>
-    <mergeCell ref="AY32:BD32"/>
-    <mergeCell ref="BE32:BJ32"/>
+    <mergeCell ref="Q6:X6"/>
+    <mergeCell ref="Y6:AF6"/>
+    <mergeCell ref="AD9:AF9"/>
+    <mergeCell ref="AD8:AF8"/>
+    <mergeCell ref="Y9:AC9"/>
+    <mergeCell ref="Y8:AC8"/>
+    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="T8:X8"/>
+    <mergeCell ref="T9:X9"/>
+    <mergeCell ref="I11:M11"/>
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="I10:M10"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="AD10:AF10"/>
+    <mergeCell ref="Y10:AC10"/>
+    <mergeCell ref="T10:X10"/>
+    <mergeCell ref="Q10:S10"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="AD11:AF11"/>
+    <mergeCell ref="Y11:AC11"/>
+    <mergeCell ref="T11:X11"/>
+    <mergeCell ref="Q11:S11"/>
+    <mergeCell ref="N11:P11"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="I15:P15"/>
+    <mergeCell ref="Q15:X15"/>
+    <mergeCell ref="Y15:AF15"/>
+    <mergeCell ref="A14:AF14"/>
+    <mergeCell ref="Y17:AC17"/>
+    <mergeCell ref="AD17:AF17"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="I18:M18"/>
+    <mergeCell ref="N18:P18"/>
+    <mergeCell ref="Q18:S18"/>
+    <mergeCell ref="T18:X18"/>
+    <mergeCell ref="Y18:AC18"/>
+    <mergeCell ref="AD18:AF18"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="I17:M17"/>
+    <mergeCell ref="N17:P17"/>
+    <mergeCell ref="Q17:S17"/>
+    <mergeCell ref="T17:X17"/>
+    <mergeCell ref="Y19:AC19"/>
+    <mergeCell ref="AD19:AF19"/>
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="I20:M20"/>
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="Q20:S20"/>
+    <mergeCell ref="T20:X20"/>
+    <mergeCell ref="Y20:AC20"/>
+    <mergeCell ref="AD20:AF20"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="I19:M19"/>
+    <mergeCell ref="N19:P19"/>
+    <mergeCell ref="Q19:S19"/>
+    <mergeCell ref="T19:X19"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -5947,11 +5947,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
       <c r="E1" s="7">
         <v>0.5</v>
       </c>
@@ -6777,28 +6777,28 @@
       <c r="S2" s="7"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="33" t="s">
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="34"/>
-      <c r="N3" s="33" t="s">
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="O3" s="34"/>
-      <c r="P3" s="35"/>
+      <c r="O3" s="33"/>
+      <c r="P3" s="34"/>
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
       <c r="S3" s="7"/>
@@ -6865,10 +6865,10 @@
       <c r="O6" s="25"/>
       <c r="P6" s="25"/>
       <c r="Q6" s="7"/>
-      <c r="R6" s="22" t="s">
+      <c r="R6" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="S6" s="22"/>
+      <c r="S6" s="20"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
@@ -6920,18 +6920,18 @@
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
-      <c r="I8" s="22" t="s">
+      <c r="I8" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="22" t="s">
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="O8" s="22"/>
-      <c r="P8" s="22"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
       <c r="Q8" s="7"/>
       <c r="R8" s="7"/>
       <c r="S8" s="7"/>
@@ -6945,18 +6945,18 @@
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
-      <c r="I9" s="22">
+      <c r="I9" s="20">
         <v>17</v>
       </c>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="22">
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20">
         <v>4</v>
       </c>
-      <c r="O9" s="22"/>
-      <c r="P9" s="22"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
       <c r="Q9" s="7"/>
       <c r="R9" s="7"/>
       <c r="S9" s="7"/>
@@ -6975,11 +6975,11 @@
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
-      <c r="N10" s="22" t="s">
+      <c r="N10" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="O10" s="22"/>
-      <c r="P10" s="22"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
       <c r="Q10" s="7"/>
       <c r="R10" s="7"/>
       <c r="S10" s="7"/>
@@ -6998,18 +6998,24 @@
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
-      <c r="N11" s="23">
+      <c r="N11" s="21">
         <f>100/(2^3-1)*N9</f>
         <v>57.142857142857146</v>
       </c>
-      <c r="O11" s="23"/>
-      <c r="P11" s="23"/>
+      <c r="O11" s="21"/>
+      <c r="P11" s="21"/>
       <c r="Q11" s="7"/>
       <c r="R11" s="7"/>
       <c r="S11" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="I3:M3"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="I6:P6"/>
     <mergeCell ref="N11:P11"/>
     <mergeCell ref="R7:S7"/>
     <mergeCell ref="I8:M8"/>
@@ -7017,12 +7023,6 @@
     <mergeCell ref="I9:M9"/>
     <mergeCell ref="N9:P9"/>
     <mergeCell ref="N10:P10"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="I3:M3"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="I6:P6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>